<commit_message>
Added co-product handling method
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Box\Research\Interactive SCSA\IBR-development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F5400E-3AF7-4E6F-B8A6-5DB8943207CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FA6C6A-D306-4F7B-BE07-A2396B42291C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="313">
   <si>
     <t>NG</t>
   </si>
@@ -1202,6 +1202,9 @@
   </si>
   <si>
     <t>Feedstock</t>
+  </si>
+  <si>
+    <t>Corn Stover</t>
   </si>
 </sst>
 </file>
@@ -4115,10 +4118,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F07116-128C-456A-A5F4-E4321BD8FA65}">
-  <dimension ref="A1:BZ37"/>
+  <dimension ref="A1:CA37"/>
   <sheetViews>
     <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+      <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4127,7 +4130,7 @@
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="102" t="s">
         <v>223</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A2" s="103" t="s">
         <v>291</v>
       </c>
@@ -4149,7 +4152,7 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A3" s="104" t="s">
         <v>292</v>
       </c>
@@ -4160,7 +4163,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:78" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:79" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A5" s="83" t="s">
         <v>226</v>
       </c>
@@ -4255,148 +4258,151 @@
         <v>302</v>
       </c>
       <c r="AF5" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="AG5" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="AG5" s="20" t="s">
+      <c r="AH5" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="AH5" s="20" t="s">
+      <c r="AI5" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="AI5" s="20" t="s">
+      <c r="AJ5" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="AJ5" s="20" t="s">
+      <c r="AK5" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="AK5" s="20" t="s">
+      <c r="AL5" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="AL5" s="20" t="s">
+      <c r="AM5" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="AM5" s="20" t="s">
+      <c r="AN5" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="AN5" s="20" t="s">
+      <c r="AO5" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="AO5" s="20" t="s">
+      <c r="AP5" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="AP5" s="20" t="s">
+      <c r="AQ5" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="AQ5" s="20" t="s">
+      <c r="AR5" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="AR5" s="20" t="s">
+      <c r="AS5" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="AS5" s="20" t="s">
+      <c r="AT5" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="AT5" s="20" t="s">
+      <c r="AU5" s="20" t="s">
         <v>262</v>
       </c>
-      <c r="AU5" s="20" t="s">
+      <c r="AV5" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="AV5" s="20" t="s">
+      <c r="AW5" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="AW5" s="20" t="s">
+      <c r="AX5" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="AX5" s="20" t="s">
+      <c r="AY5" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="AY5" s="20" t="s">
+      <c r="AZ5" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="AZ5" s="20" t="s">
+      <c r="BA5" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="BA5" s="20" t="s">
+      <c r="BB5" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="BB5" s="20" t="s">
+      <c r="BC5" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="BC5" s="20" t="s">
+      <c r="BD5" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="BD5" s="20" t="s">
+      <c r="BE5" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="BE5" s="20" t="s">
+      <c r="BF5" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="BF5" s="20" t="s">
+      <c r="BG5" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="BG5" s="20" t="s">
+      <c r="BH5" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="BH5" s="20" t="s">
+      <c r="BI5" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="BI5" s="20" t="s">
+      <c r="BJ5" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="BJ5" s="20" t="s">
+      <c r="BK5" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="BK5" s="20" t="s">
+      <c r="BL5" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="BL5" s="20" t="s">
+      <c r="BM5" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="BM5" s="20" t="s">
+      <c r="BN5" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="BN5" s="20" t="s">
+      <c r="BO5" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="BO5" s="20" t="s">
+      <c r="BP5" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="BP5" s="20" t="s">
+      <c r="BQ5" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="BQ5" s="20" t="s">
+      <c r="BR5" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="BR5" s="20" t="s">
+      <c r="BS5" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="BS5" s="20" t="s">
+      <c r="BT5" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="BT5" s="20" t="s">
+      <c r="BU5" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="BU5" s="20" t="s">
+      <c r="BV5" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="BV5" s="20" t="s">
+      <c r="BW5" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="BW5" s="20" t="s">
+      <c r="BX5" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="BX5" s="20" t="s">
+      <c r="BY5" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="BY5" s="20" t="s">
+      <c r="BZ5" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="BZ5" s="21" t="s">
+      <c r="CA5" s="21" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A6" s="84" t="s">
         <v>289</v>
       </c>
@@ -4469,23 +4475,23 @@
       <c r="AH6" s="87"/>
       <c r="AI6" s="87"/>
       <c r="AJ6" s="87"/>
-      <c r="AK6" s="86">
+      <c r="AK6" s="87"/>
+      <c r="AL6" s="86">
         <v>150000</v>
       </c>
-      <c r="AL6" s="87"/>
-      <c r="AM6" s="82"/>
-      <c r="AN6" s="87"/>
+      <c r="AM6" s="87"/>
+      <c r="AN6" s="82"/>
       <c r="AO6" s="87"/>
       <c r="AP6" s="87"/>
       <c r="AQ6" s="87"/>
-      <c r="AR6" s="88">
-        <v>100000</v>
-      </c>
+      <c r="AR6" s="87"/>
       <c r="AS6" s="88">
         <v>100000</v>
       </c>
-      <c r="AT6" s="89"/>
-      <c r="AU6" s="87"/>
+      <c r="AT6" s="88">
+        <v>100000</v>
+      </c>
+      <c r="AU6" s="89"/>
       <c r="AV6" s="87"/>
       <c r="AW6" s="87"/>
       <c r="AX6" s="87"/>
@@ -4502,29 +4508,30 @@
       <c r="BI6" s="87"/>
       <c r="BJ6" s="87"/>
       <c r="BK6" s="87"/>
-      <c r="BL6" s="82"/>
-      <c r="BM6" s="87"/>
-      <c r="BN6" s="90">
+      <c r="BL6" s="87"/>
+      <c r="BM6" s="82"/>
+      <c r="BN6" s="87"/>
+      <c r="BO6" s="90">
         <v>100000</v>
       </c>
-      <c r="BO6" s="82"/>
-      <c r="BP6" s="91">
+      <c r="BP6" s="82"/>
+      <c r="BQ6" s="91">
         <v>90000</v>
       </c>
-      <c r="BQ6" s="87"/>
-      <c r="BR6" s="82"/>
-      <c r="BS6" s="91">
+      <c r="BR6" s="87"/>
+      <c r="BS6" s="82"/>
+      <c r="BT6" s="91">
         <v>80000</v>
       </c>
-      <c r="BT6" s="87"/>
       <c r="BU6" s="87"/>
       <c r="BV6" s="87"/>
       <c r="BW6" s="87"/>
       <c r="BX6" s="87"/>
       <c r="BY6" s="87"/>
-      <c r="BZ6" s="92"/>
-    </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BZ6" s="87"/>
+      <c r="CA6" s="92"/>
+    </row>
+    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A7" s="84" t="s">
         <v>290</v>
       </c>
@@ -4617,16 +4624,16 @@
       <c r="AF7" s="86">
         <v>20000</v>
       </c>
-      <c r="AG7" s="87"/>
+      <c r="AG7" s="86">
+        <v>20000</v>
+      </c>
       <c r="AH7" s="87"/>
       <c r="AI7" s="87"/>
-      <c r="AJ7" s="86">
+      <c r="AJ7" s="87"/>
+      <c r="AK7" s="86">
         <v>20000</v>
       </c>
-      <c r="AK7" s="87"/>
-      <c r="AL7" s="86">
-        <v>20000</v>
-      </c>
+      <c r="AL7" s="87"/>
       <c r="AM7" s="86">
         <v>20000</v>
       </c>
@@ -4634,17 +4641,17 @@
         <v>20000</v>
       </c>
       <c r="AO7" s="86">
+        <v>20000</v>
+      </c>
+      <c r="AP7" s="86">
         <v>30000</v>
       </c>
-      <c r="AP7" s="87"/>
-      <c r="AQ7" s="86">
+      <c r="AQ7" s="87"/>
+      <c r="AR7" s="86">
         <v>30000</v>
       </c>
-      <c r="AR7" s="86">
+      <c r="AS7" s="86">
         <v>22500</v>
-      </c>
-      <c r="AS7" s="86">
-        <v>20000</v>
       </c>
       <c r="AT7" s="86">
         <v>20000</v>
@@ -4652,11 +4659,13 @@
       <c r="AU7" s="86">
         <v>20000</v>
       </c>
-      <c r="AV7" s="87"/>
-      <c r="AW7" s="86">
+      <c r="AV7" s="86">
+        <v>20000</v>
+      </c>
+      <c r="AW7" s="87"/>
+      <c r="AX7" s="86">
         <v>22500</v>
       </c>
-      <c r="AX7" s="87"/>
       <c r="AY7" s="87"/>
       <c r="AZ7" s="87"/>
       <c r="BA7" s="87"/>
@@ -4667,38 +4676,39 @@
       <c r="BF7" s="87"/>
       <c r="BG7" s="87"/>
       <c r="BH7" s="87"/>
-      <c r="BI7" s="86">
+      <c r="BI7" s="87"/>
+      <c r="BJ7" s="86">
         <v>20000</v>
       </c>
-      <c r="BJ7" s="87"/>
-      <c r="BK7" s="86">
+      <c r="BK7" s="87"/>
+      <c r="BL7" s="86">
         <v>20000</v>
       </c>
-      <c r="BL7" s="87"/>
-      <c r="BM7" s="86"/>
-      <c r="BN7" s="87"/>
-      <c r="BO7" s="82"/>
-      <c r="BP7" s="86">
+      <c r="BM7" s="87"/>
+      <c r="BN7" s="86"/>
+      <c r="BO7" s="87"/>
+      <c r="BP7" s="82"/>
+      <c r="BQ7" s="86">
         <v>19000</v>
       </c>
-      <c r="BQ7" s="86">
+      <c r="BR7" s="86">
         <v>20000</v>
       </c>
-      <c r="BR7" s="82"/>
-      <c r="BS7" s="86">
+      <c r="BS7" s="82"/>
+      <c r="BT7" s="86">
         <v>18000</v>
       </c>
-      <c r="BT7" s="86">
+      <c r="BU7" s="86">
         <v>20000</v>
       </c>
-      <c r="BU7" s="87"/>
       <c r="BV7" s="87"/>
       <c r="BW7" s="87"/>
       <c r="BX7" s="87"/>
       <c r="BY7" s="87"/>
-      <c r="BZ7" s="92"/>
-    </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BZ7" s="87"/>
+      <c r="CA7" s="92"/>
+    </row>
+    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A8" s="84" t="s">
         <v>224</v>
       </c>
@@ -4792,26 +4802,26 @@
       <c r="AE8" s="132">
         <v>20.889521999999999</v>
       </c>
-      <c r="AF8" s="86">
+      <c r="AF8" s="132">
+        <v>17.684999999999999</v>
+      </c>
+      <c r="AG8" s="86">
         <v>17.5</v>
       </c>
-      <c r="AG8" s="86">
+      <c r="AH8" s="86">
         <v>25</v>
-      </c>
-      <c r="AH8" s="86">
-        <v>17</v>
       </c>
       <c r="AI8" s="86">
         <v>17</v>
       </c>
       <c r="AJ8" s="86">
+        <v>17</v>
+      </c>
+      <c r="AK8" s="86">
         <v>15</v>
       </c>
-      <c r="AK8" s="86">
+      <c r="AL8" s="86">
         <v>25</v>
-      </c>
-      <c r="AL8" s="86">
-        <v>15</v>
       </c>
       <c r="AM8" s="86">
         <v>15</v>
@@ -4820,7 +4830,7 @@
         <v>15</v>
       </c>
       <c r="AO8" s="86">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AP8" s="86">
         <v>25</v>
@@ -4838,10 +4848,10 @@
         <v>25</v>
       </c>
       <c r="AU8" s="86">
+        <v>25</v>
+      </c>
+      <c r="AV8" s="86">
         <v>24</v>
-      </c>
-      <c r="AV8" s="86">
-        <v>25</v>
       </c>
       <c r="AW8" s="86">
         <v>25</v>
@@ -4859,7 +4869,7 @@
         <v>25</v>
       </c>
       <c r="BB8" s="86">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="BC8" s="86">
         <v>23</v>
@@ -4880,59 +4890,62 @@
         <v>23</v>
       </c>
       <c r="BI8" s="86">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="BJ8" s="86">
         <v>25</v>
       </c>
       <c r="BK8" s="86">
+        <v>25</v>
+      </c>
+      <c r="BL8" s="86">
         <v>20</v>
       </c>
-      <c r="BL8" s="93">
+      <c r="BM8" s="93">
         <v>23</v>
       </c>
-      <c r="BM8" s="86">
+      <c r="BN8" s="86">
         <v>21.75</v>
       </c>
-      <c r="BN8" s="82"/>
-      <c r="BO8" s="94">
+      <c r="BO8" s="82"/>
+      <c r="BP8" s="94">
         <v>23</v>
       </c>
-      <c r="BP8" s="86">
+      <c r="BQ8" s="86">
         <v>22</v>
       </c>
-      <c r="BQ8" s="90">
+      <c r="BR8" s="90">
         <v>17.62</v>
       </c>
-      <c r="BR8" s="94">
+      <c r="BS8" s="94">
         <v>17.68</v>
       </c>
-      <c r="BS8" s="86">
+      <c r="BT8" s="86">
         <v>20</v>
       </c>
-      <c r="BT8" s="86">
+      <c r="BU8" s="86">
         <v>17.62</v>
       </c>
-      <c r="BU8" s="86">
+      <c r="BV8" s="86">
         <v>24</v>
-      </c>
-      <c r="BV8" s="86">
-        <v>15</v>
       </c>
       <c r="BW8" s="86">
         <v>15</v>
       </c>
       <c r="BX8" s="86">
+        <v>15</v>
+      </c>
+      <c r="BY8" s="86">
         <v>21</v>
       </c>
-      <c r="BY8" s="86">
+      <c r="BZ8" s="86">
         <v>24</v>
       </c>
-      <c r="BZ8" s="95">
+      <c r="CA8" s="95">
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A9" s="96" t="s">
         <v>225</v>
       </c>
@@ -4980,9 +4993,7 @@
       <c r="AG9" s="97"/>
       <c r="AH9" s="97"/>
       <c r="AI9" s="97"/>
-      <c r="AJ9" s="98">
-        <v>8</v>
-      </c>
+      <c r="AJ9" s="97"/>
       <c r="AK9" s="98">
         <v>8</v>
       </c>
@@ -4995,22 +5006,22 @@
       <c r="AN9" s="98">
         <v>8</v>
       </c>
-      <c r="AO9" s="97"/>
+      <c r="AO9" s="98">
+        <v>8</v>
+      </c>
       <c r="AP9" s="97"/>
       <c r="AQ9" s="97"/>
-      <c r="AR9" s="99"/>
+      <c r="AR9" s="97"/>
       <c r="AS9" s="99"/>
       <c r="AT9" s="99"/>
-      <c r="AU9" s="97"/>
-      <c r="AV9" s="98">
+      <c r="AU9" s="99"/>
+      <c r="AV9" s="97"/>
+      <c r="AW9" s="98">
         <v>8</v>
       </c>
-      <c r="AW9" s="97"/>
       <c r="AX9" s="97"/>
       <c r="AY9" s="97"/>
-      <c r="AZ9" s="98">
-        <v>8</v>
-      </c>
+      <c r="AZ9" s="97"/>
       <c r="BA9" s="98">
         <v>8</v>
       </c>
@@ -5035,37 +5046,40 @@
       <c r="BH9" s="98">
         <v>8</v>
       </c>
-      <c r="BI9" s="97"/>
+      <c r="BI9" s="98">
+        <v>8</v>
+      </c>
       <c r="BJ9" s="97"/>
-      <c r="BK9" s="97">
+      <c r="BK9" s="97"/>
+      <c r="BL9" s="97">
         <v>5</v>
       </c>
-      <c r="BL9" s="100">
+      <c r="BM9" s="100">
         <v>8</v>
       </c>
-      <c r="BM9" s="97"/>
-      <c r="BN9" s="99"/>
+      <c r="BN9" s="97"/>
       <c r="BO9" s="99"/>
-      <c r="BP9" s="97"/>
+      <c r="BP9" s="99"/>
       <c r="BQ9" s="97"/>
-      <c r="BR9" s="99"/>
-      <c r="BS9" s="97"/>
+      <c r="BR9" s="97"/>
+      <c r="BS9" s="99"/>
       <c r="BT9" s="97"/>
       <c r="BU9" s="97"/>
-      <c r="BV9" s="97">
+      <c r="BV9" s="97"/>
+      <c r="BW9" s="97">
         <v>8</v>
       </c>
-      <c r="BW9" s="97"/>
       <c r="BX9" s="97"/>
       <c r="BY9" s="97"/>
-      <c r="BZ9" s="101"/>
-    </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BZ9" s="97"/>
+      <c r="CA9" s="101"/>
+    </row>
+    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A11" s="126" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
       <c r="B12" s="140" t="s">
         <v>293</v>
       </c>
@@ -5083,7 +5097,7 @@
       <c r="L12" s="106"/>
       <c r="M12" s="107"/>
     </row>
-    <row r="13" spans="1:78" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
       <c r="B13" s="141"/>
       <c r="C13" s="108" t="s">
         <v>1</v>
@@ -5119,7 +5133,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A14" s="120" t="s">
         <v>22</v>
       </c>
@@ -5160,7 +5174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A15" s="84" t="s">
         <v>23</v>
       </c>
@@ -5201,7 +5215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A16" s="84" t="s">
         <v>7</v>
       </c>
@@ -6682,7 +6696,7 @@
   <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B2" sqref="B2:P2"/>
     </sheetView>
   </sheetViews>
@@ -10083,10 +10097,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2275C5-799F-4B1B-8AD1-776CB314922E}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10094,15 +10108,18 @@
     <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>301</v>
       </c>
       <c r="C1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -10112,8 +10129,11 @@
       <c r="C2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>128</v>
       </c>
@@ -10123,8 +10143,11 @@
       <c r="C3" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -10134,8 +10157,11 @@
       <c r="C4" s="38">
         <v>362403.00757167325</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="38">
+        <v>362403.00757167325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -10145,8 +10171,11 @@
       <c r="C5" s="38">
         <v>344979.42656462023</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="38">
+        <v>344979.42656462023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -10156,8 +10185,11 @@
       <c r="C6" s="38">
         <v>24381.856026689315</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="38">
+        <v>24381.856026689315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -10167,8 +10199,11 @@
       <c r="C7" s="38">
         <v>254462.26606022959</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="38">
+        <v>254462.26606022959</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -10178,8 +10213,11 @@
       <c r="C8" s="38">
         <v>66135.304477701342</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="38">
+        <v>66135.304477701342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -10189,8 +10227,11 @@
       <c r="C9" s="38">
         <v>59.889274923371126</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" s="38">
+        <v>59.889274923371126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10200,8 +10241,11 @@
       <c r="C10">
         <v>24.470884336712146</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>24.470884336712146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -10211,8 +10255,11 @@
       <c r="C11">
         <v>34.134614130073174</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>34.134614130073174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -10222,8 +10269,11 @@
       <c r="C12">
         <v>-15.759603589368934</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <v>-15.759603589368934</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -10233,8 +10283,11 @@
       <c r="C13">
         <v>8.6858851249063438</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <v>8.6858851249063438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -10244,8 +10297,11 @@
       <c r="C14">
         <v>6.9883164862451217</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>6.9883164862451217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -10255,8 +10311,11 @@
       <c r="C15">
         <v>58.328462296040968</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <v>58.328462296040968</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -10266,8 +10325,11 @@
       <c r="C16">
         <v>0.49662761207225459</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>0.49662761207225459</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -10277,8 +10339,11 @@
       <c r="C17">
         <v>1.1283578872130025</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>1.1283578872130025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -10288,8 +10353,11 @@
       <c r="C18">
         <v>57.127332585038609</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>57.127332585038609</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10299,8 +10367,11 @@
       <c r="C19">
         <v>-82.715827114534676</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <v>-82.715827114534676</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10310,8 +10381,11 @@
       <c r="C20">
         <v>22763.019075759898</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>22763.019075759898</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -10321,6 +10395,7 @@
       <c r="C22" s="7" t="s">
         <v>79</v>
       </c>
+      <c r="D22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10538,7 +10613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
   <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added renewable diesel and renewable gasoline to the properties and lookup table files
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53F9DF87-7B86-4CDC-80D8-C572173B06FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D972D4-1253-4106-ACCC-0101A2DB4CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="6" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="304">
   <si>
     <t>Diesel</t>
   </si>
@@ -1738,6 +1738,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1747,7 +1748,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2449,7 +2449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
@@ -2513,7 +2513,7 @@
       <c r="S1" s="125" t="s">
         <v>295</v>
       </c>
-      <c r="T1" s="134" t="s">
+      <c r="T1" s="131" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3270,22 +3270,22 @@
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="131" t="s">
+      <c r="B17" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="131"/>
-      <c r="I17" s="131"/>
-      <c r="J17" s="131"/>
-      <c r="K17" s="131"/>
-      <c r="L17" s="131"/>
-      <c r="M17" s="131"/>
-      <c r="N17" s="131"/>
-      <c r="O17" s="131"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="132"/>
+      <c r="G17" s="132"/>
+      <c r="H17" s="132"/>
+      <c r="I17" s="132"/>
+      <c r="J17" s="132"/>
+      <c r="K17" s="132"/>
+      <c r="L17" s="132"/>
+      <c r="M17" s="132"/>
+      <c r="N17" s="132"/>
+      <c r="O17" s="132"/>
       <c r="P17" t="s">
         <v>81</v>
       </c>
@@ -4716,7 +4716,7 @@
       </c>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.35">
-      <c r="B12" s="132" t="s">
+      <c r="B12" s="133" t="s">
         <v>282</v>
       </c>
       <c r="C12" s="97" t="s">
@@ -4734,7 +4734,7 @@
       <c r="M12" s="99"/>
     </row>
     <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="133"/>
+      <c r="B13" s="134"/>
       <c r="C13" s="100" t="s">
         <v>0</v>
       </c>
@@ -5222,7 +5222,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="112"/>
-      <c r="B25" s="132" t="s">
+      <c r="B25" s="133" t="s">
         <v>282</v>
       </c>
       <c r="C25" s="97" t="s">
@@ -5241,7 +5241,7 @@
     </row>
     <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="76"/>
-      <c r="B26" s="133"/>
+      <c r="B26" s="134"/>
       <c r="C26" s="100" t="s">
         <v>0</v>
       </c>
@@ -6122,11 +6122,11 @@
       <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="131" t="s">
+      <c r="B22" s="132" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="131"/>
-      <c r="D22" s="131"/>
+      <c r="C22" s="132"/>
+      <c r="D22" s="132"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
@@ -8433,39 +8433,39 @@
       <c r="A23" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="131" t="s">
+      <c r="B23" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="131"/>
-      <c r="H23" s="131"/>
-      <c r="I23" s="131"/>
-      <c r="J23" s="131"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="131"/>
-      <c r="M23" s="131"/>
-      <c r="N23" s="131"/>
-      <c r="O23" s="131"/>
-      <c r="P23" s="131"/>
-      <c r="Q23" s="131"/>
-      <c r="R23" s="131"/>
-      <c r="S23" s="131"/>
-      <c r="T23" s="131"/>
-      <c r="U23" s="131"/>
-      <c r="V23" s="131"/>
-      <c r="W23" s="131"/>
-      <c r="X23" s="131"/>
-      <c r="Y23" s="131"/>
-      <c r="Z23" s="131"/>
-      <c r="AA23" s="131"/>
-      <c r="AB23" s="131"/>
-      <c r="AC23" s="131"/>
-      <c r="AD23" s="131"/>
-      <c r="AE23" s="131"/>
-      <c r="AF23" s="131"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="132"/>
+      <c r="G23" s="132"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="132"/>
+      <c r="J23" s="132"/>
+      <c r="K23" s="132"/>
+      <c r="L23" s="132"/>
+      <c r="M23" s="132"/>
+      <c r="N23" s="132"/>
+      <c r="O23" s="132"/>
+      <c r="P23" s="132"/>
+      <c r="Q23" s="132"/>
+      <c r="R23" s="132"/>
+      <c r="S23" s="132"/>
+      <c r="T23" s="132"/>
+      <c r="U23" s="132"/>
+      <c r="V23" s="132"/>
+      <c r="W23" s="132"/>
+      <c r="X23" s="132"/>
+      <c r="Y23" s="132"/>
+      <c r="Z23" s="132"/>
+      <c r="AA23" s="132"/>
+      <c r="AB23" s="132"/>
+      <c r="AC23" s="132"/>
+      <c r="AD23" s="132"/>
+      <c r="AE23" s="132"/>
+      <c r="AF23" s="132"/>
       <c r="AG23" t="s">
         <v>70</v>
       </c>
@@ -9542,22 +9542,22 @@
       <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="131" t="s">
+      <c r="B23" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="131"/>
-      <c r="H23" s="131"/>
-      <c r="I23" s="131"/>
-      <c r="J23" s="131"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="131"/>
-      <c r="M23" s="131"/>
-      <c r="N23" s="131"/>
-      <c r="O23" s="131"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="132"/>
+      <c r="G23" s="132"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="132"/>
+      <c r="J23" s="132"/>
+      <c r="K23" s="132"/>
+      <c r="L23" s="132"/>
+      <c r="M23" s="132"/>
+      <c r="N23" s="132"/>
+      <c r="O23" s="132"/>
       <c r="P23" t="s">
         <v>81</v>
       </c>
@@ -10088,10 +10088,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10549,466 +10549,469 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="B42">
-        <v>38.180512527472686</v>
+        <v>40.669004600898425</v>
       </c>
       <c r="C42">
-        <v>747.6070630111235</v>
+        <v>793.37856525946859</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B43">
-        <v>37.300256882262083</v>
+        <v>38.180512527472686</v>
       </c>
       <c r="C43">
-        <v>716.69892648380858</v>
+        <v>747.6070630111235</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B44">
-        <v>36.889328265240245</v>
+        <v>37.300256882262083</v>
       </c>
       <c r="C44">
-        <v>744.70116983334174</v>
+        <v>716.69892648380858</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B45">
-        <v>39.429337036099838</v>
+        <v>36.889328265240245</v>
       </c>
       <c r="C45">
-        <v>756.99999999999989</v>
+        <v>744.70116983334174</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B46">
-        <v>10.040313081123244</v>
+        <v>39.429337036099838</v>
       </c>
       <c r="C46">
-        <v>70.798124695046326</v>
+        <v>756.99999999999989</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B47">
-        <v>30.792488052730107</v>
+        <v>10.040313081123244</v>
       </c>
       <c r="C47">
-        <v>742.58779297677324</v>
+        <v>70.798124695046326</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B48">
-        <v>31.839314137909518</v>
+        <v>30.792488052730107</v>
       </c>
       <c r="C48">
-        <v>742.32362086970215</v>
+        <v>742.58779297677324</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B49">
-        <v>33.077070766926674</v>
+        <v>31.839314137909518</v>
       </c>
       <c r="C49">
-        <v>769.53334789802227</v>
+        <v>742.32362086970215</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B50">
-        <v>31.263230600468017</v>
+        <v>33.077070766926674</v>
       </c>
       <c r="C50">
-        <v>584.61287294827434</v>
+        <v>769.53334789802227</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B51">
-        <v>29.646904789703584</v>
+        <v>31.263230600468017</v>
       </c>
       <c r="C51">
-        <v>559.51652277652283</v>
+        <v>584.61287294827434</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B52">
-        <v>31.510123545085804</v>
+        <v>29.646904789703584</v>
       </c>
       <c r="C52">
-        <v>595.17975723111715</v>
+        <v>559.51652277652283</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B53">
-        <v>27.734307445397814</v>
+        <v>31.510123545085804</v>
       </c>
       <c r="C53">
-        <v>507.21044557645126</v>
+        <v>595.17975723111715</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B54">
-        <v>27.548680827882244</v>
+        <v>27.734307445397814</v>
       </c>
       <c r="C54">
-        <v>668.88377510394514</v>
+        <v>507.21044557645126</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B55">
-        <v>34.60609523247426</v>
+        <v>27.548680827882244</v>
       </c>
       <c r="C55">
-        <v>654.80340179705718</v>
+        <v>668.88377510394514</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B56">
-        <v>36.455478031346189</v>
+        <v>34.60609523247426</v>
       </c>
       <c r="C56">
-        <v>688.85095964480468</v>
+        <v>654.80340179705718</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B57">
-        <v>38.505872853524245</v>
+        <v>36.455478031346189</v>
       </c>
       <c r="C57">
-        <v>737.59071339941693</v>
+        <v>688.85095964480468</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B58">
-        <v>39.773165285279561</v>
+        <v>38.505872853524245</v>
       </c>
       <c r="C58">
-        <v>765.47381512866104</v>
+        <v>737.59071339941693</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B59">
-        <v>38.281904677575831</v>
+        <v>39.773165285279561</v>
       </c>
       <c r="C59">
-        <v>731.67589538225809</v>
+        <v>765.47381512866104</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B60">
-        <v>31.369932808387436</v>
+        <v>38.281904677575831</v>
       </c>
       <c r="C60">
-        <v>800.00032424653136</v>
+        <v>731.67589538225809</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B61">
-        <v>38.180512527472686</v>
+        <v>31.369932808387436</v>
       </c>
       <c r="C61">
-        <v>747.6070630111235</v>
+        <v>800.00032424653136</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B62">
-        <v>47.141813661363628</v>
+        <v>38.180512527472686</v>
       </c>
       <c r="C62">
-        <v>0.77692265667854898</v>
+        <v>747.6070630111235</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>179</v>
+      </c>
+      <c r="B63">
+        <v>47.141813661363628</v>
+      </c>
+      <c r="C63">
+        <v>0.77692265667854898</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>180</v>
       </c>
-      <c r="B63">
+      <c r="B64">
         <v>49.999999999999993</v>
       </c>
-      <c r="C63">
+      <c r="C64">
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="67" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <v>119.98674372549019</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>9.0052398842286357E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>181</v>
-      </c>
-      <c r="B65">
-        <v>0</v>
-      </c>
-      <c r="C65">
-        <v>1.9768383817590991</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B66">
-        <v>48.885121247479262</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>0.88356773166440861</v>
+        <v>1.9768383817590991</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B67">
-        <v>22.648458746153963</v>
+        <v>48.885121247479262</v>
+      </c>
+      <c r="C67">
+        <v>0.88356773166440861</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B68">
-        <v>26.329529071139479</v>
+        <v>22.648458746153963</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B69">
-        <v>18.707371337693861</v>
+        <v>26.329529071139479</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B70">
-        <v>12.566427590816895</v>
+        <v>18.707371337693861</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B71">
-        <v>26.329529071139479</v>
+        <v>12.566427590816895</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B72">
-        <v>11.566786665057547</v>
+        <v>26.329529071139479</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B73">
-        <v>31.342185540824094</v>
+        <v>11.566786665057547</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B74">
-        <v>31.0106439692332</v>
+        <v>31.342185540824094</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B75">
-        <v>28.609127685562171</v>
+        <v>31.0106439692332</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B76">
-        <v>33.012627597074328</v>
+        <v>28.609127685562171</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B77">
-        <v>17.905547955535493</v>
+        <v>33.012627597074328</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B78">
-        <v>18.52542695399616</v>
+        <v>17.905547955535493</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B79">
-        <v>16.801860958276258</v>
+        <v>18.52542695399616</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B80">
-        <v>17.842745955691449</v>
+        <v>16.801860958276258</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B81">
-        <v>17.11470795749937</v>
+        <v>17.842745955691449</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B82">
-        <v>20.107106950068403</v>
+        <v>17.11470795749937</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B83">
-        <v>18.52542695399616</v>
+        <v>20.107106950068403</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B84">
-        <v>17.444999956679162</v>
+        <v>18.52542695399616</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B85">
-        <v>15.647058823529411</v>
+        <v>17.444999956679162</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B86">
-        <v>14.4</v>
+        <v>15.647058823529411</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B87">
-        <v>22.000366940104676</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B88">
-        <v>14.864999999999997</v>
+        <v>22.000366940104676</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B89">
-        <v>16.758749999999999</v>
+        <v>14.864999999999997</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B90">
         <v>16.758749999999999</v>
@@ -11016,33 +11019,41 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B91">
-        <v>13.036809815950916</v>
+        <v>16.758749999999999</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>207</v>
+      </c>
+      <c r="B92">
+        <v>13.036809815950916</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>208</v>
       </c>
-      <c r="B92">
+      <c r="B93">
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="67" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="67" t="s">
         <v>211</v>
       </c>
-      <c r="C93">
+      <c r="C94">
         <v>1000</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>66</v>
       </c>
-      <c r="C94">
+      <c r="C95">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added emissions from RD and RG distribution (loss factor not added yet)
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE3A8BD-9AD9-4590-A12A-8731FA8FD551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AAEF1E-4951-4BCE-BBCD-212EB89D06EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="318">
   <si>
     <t>NG</t>
   </si>
@@ -1211,6 +1211,15 @@
   </si>
   <si>
     <t>Empty</t>
+  </si>
+  <si>
+    <t>Fuel Distribution</t>
+  </si>
+  <si>
+    <t>Fuel Distribution and Vehicle Operation</t>
+  </si>
+  <si>
+    <t>Need to add energy and water</t>
   </si>
 </sst>
 </file>
@@ -1804,6 +1813,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1813,11 +1827,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2517,19 +2526,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="8"/>
-    <col min="9" max="9" width="9.140625" style="145"/>
+    <col min="1" max="1" width="8.7265625" style="8"/>
+    <col min="9" max="9" width="9.1796875" style="142"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="26.5" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2545,13 +2554,13 @@
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="143" t="s">
+      <c r="G1" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="143" t="s">
+      <c r="H1" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="143" t="s">
+      <c r="I1" s="140" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -2597,10 +2606,22 @@
         <v>165</v>
       </c>
       <c r="X1" s="121" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y1" s="121" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z1" s="121" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="AA1" s="121" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB1" s="121" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="78.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -2617,13 +2638,13 @@
       <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="144" t="s">
+      <c r="G2" s="141" t="s">
         <v>313</v>
       </c>
-      <c r="H2" s="144" t="s">
+      <c r="H2" s="141" t="s">
         <v>314</v>
       </c>
-      <c r="I2" s="144" t="s">
+      <c r="I2" s="141" t="s">
         <v>312</v>
       </c>
       <c r="J2" s="70" t="s">
@@ -2669,10 +2690,22 @@
         <v>312</v>
       </c>
       <c r="X2" s="139" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y2" s="139" t="s">
+        <v>316</v>
+      </c>
+      <c r="Z2" s="139" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA2" s="139" t="s">
+        <v>315</v>
+      </c>
+      <c r="AB2" s="139" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>126</v>
       </c>
@@ -2691,13 +2724,13 @@
       <c r="F3" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="144" t="s">
+      <c r="G3" s="141" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="144" t="s">
+      <c r="H3" s="141" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="144" t="s">
+      <c r="I3" s="141" t="s">
         <v>125</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -2740,7 +2773,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>22</v>
       </c>
@@ -2759,13 +2792,13 @@
       <c r="F4" s="4">
         <v>41.5</v>
       </c>
-      <c r="G4" s="145">
+      <c r="G4" s="142">
         <v>5.8123534639999992</v>
       </c>
-      <c r="H4" s="145">
+      <c r="H4" s="142">
         <v>7.3235653640000002</v>
       </c>
-      <c r="I4" s="145">
+      <c r="I4" s="142">
         <v>41.750349867302674</v>
       </c>
       <c r="J4" s="71">
@@ -2803,10 +2836,24 @@
         <v>53.597474630288403</v>
       </c>
       <c r="X4">
+        <v>0.12380376798091507</v>
+      </c>
+      <c r="Y4">
+        <f>W4+X4</f>
+        <v>53.72127839826932</v>
+      </c>
+      <c r="Z4">
         <v>40.352647182660228</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA4">
+        <v>1.4111608204643369E-2</v>
+      </c>
+      <c r="AB4">
+        <f>Z4+AA4</f>
+        <v>40.366758790864871</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -2825,13 +2872,13 @@
       <c r="F5" s="4">
         <v>200.11</v>
       </c>
-      <c r="G5" s="145">
+      <c r="G5" s="142">
         <v>161.77639492999998</v>
       </c>
-      <c r="H5" s="145">
+      <c r="H5" s="142">
         <v>203.83825762999999</v>
       </c>
-      <c r="I5" s="145">
+      <c r="I5" s="142">
         <v>993.80073264760836</v>
       </c>
       <c r="J5" s="71">
@@ -2869,10 +2916,24 @@
         <v>639.10415070792988</v>
       </c>
       <c r="X5">
+        <v>0.53001711985689259</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" ref="Y5:Y15" si="0">W5+X5</f>
+        <v>639.63416782778677</v>
+      </c>
+      <c r="Z5">
         <v>993.80073264760836</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA5">
+        <v>0.19579254162294349</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" ref="AB5:AB15" si="1">Z5+AA5</f>
+        <v>993.99652518923131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -2891,13 +2952,13 @@
       <c r="F6" s="4">
         <v>434.31</v>
       </c>
-      <c r="G6" s="145">
+      <c r="G6" s="142">
         <v>101.53518337</v>
       </c>
-      <c r="H6" s="145">
+      <c r="H6" s="142">
         <v>127.93433107000001</v>
       </c>
-      <c r="I6" s="145">
+      <c r="I6" s="142">
         <v>27.387619255967515</v>
       </c>
       <c r="J6" s="71">
@@ -2935,10 +2996,24 @@
         <v>19.208734314891956</v>
       </c>
       <c r="X6">
+        <v>1.4390708093838975</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>20.647805124275852</v>
+      </c>
+      <c r="Z6">
         <v>27.387619255967515</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA6">
+        <v>0.13356807901983217</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="1"/>
+        <v>27.521187334987346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>24</v>
       </c>
@@ -2957,13 +3032,13 @@
       <c r="F7" s="4">
         <v>29.83</v>
       </c>
-      <c r="G7" s="145">
+      <c r="G7" s="142">
         <v>5.4409986930000001</v>
       </c>
-      <c r="H7" s="145">
+      <c r="H7" s="142">
         <v>6.8556583530000008</v>
       </c>
-      <c r="I7" s="145">
+      <c r="I7" s="142">
         <v>9.458769751780995</v>
       </c>
       <c r="J7" s="71">
@@ -3001,10 +3076,24 @@
         <v>8.0441472410106218</v>
       </c>
       <c r="X7">
+        <v>6.8025222126898502E-2</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="0"/>
+        <v>8.1121724631375205</v>
+      </c>
+      <c r="Z7">
         <v>9.458769751780995</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA7">
+        <v>7.5116168079741932E-3</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="1"/>
+        <v>9.4662813685889695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -3023,13 +3112,13 @@
       <c r="F8" s="4">
         <v>28.935099999999998</v>
       </c>
-      <c r="G8" s="145">
+      <c r="G8" s="142">
         <v>0.9282486969999999</v>
       </c>
-      <c r="H8" s="145">
+      <c r="H8" s="142">
         <v>1.1695933580000002</v>
       </c>
-      <c r="I8" s="145">
+      <c r="I8" s="142">
         <v>1.8922698715311803</v>
       </c>
       <c r="J8" s="71">
@@ -3067,10 +3156,24 @@
         <v>1.728649515788488</v>
       </c>
       <c r="X8">
+        <v>4.6442748659862865E-2</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="0"/>
+        <v>1.7750922644483509</v>
+      </c>
+      <c r="Z8">
         <v>1.8922698715311803</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA8">
+        <v>2.1809956805283149E-3</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="1"/>
+        <v>1.8944508672117086</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>26</v>
       </c>
@@ -3089,13 +3192,13 @@
       <c r="F9" s="4">
         <v>0.54242117555469049</v>
       </c>
-      <c r="G9" s="145">
+      <c r="G9" s="142">
         <v>0.54469976400000064</v>
       </c>
-      <c r="H9" s="145">
+      <c r="H9" s="142">
         <v>0.54469976400000064</v>
       </c>
-      <c r="I9" s="145">
+      <c r="I9" s="142">
         <v>0.54469976387990116</v>
       </c>
       <c r="J9" s="71">
@@ -3133,10 +3236,24 @@
         <v>0.47886752155609885</v>
       </c>
       <c r="X9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0.22128373782612412</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="0"/>
+        <v>0.700151259382223</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>5.3987418408876558E-3</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="1"/>
+        <v>5.3987418408876558E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>27</v>
       </c>
@@ -3155,13 +3272,13 @@
       <c r="F10" s="4">
         <v>16.290461299999997</v>
       </c>
-      <c r="G10" s="145">
+      <c r="G10" s="142">
         <v>3.1580813000000013E-2</v>
       </c>
-      <c r="H10" s="145">
+      <c r="H10" s="142">
         <v>3.9791824000000003E-2</v>
       </c>
-      <c r="I10" s="145">
+      <c r="I10" s="142">
         <v>0.51210428280035414</v>
       </c>
       <c r="J10" s="71">
@@ -3199,10 +3316,24 @@
         <v>0.47390947465623479</v>
       </c>
       <c r="X10">
+        <v>4.2404984619842561E-3</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="0"/>
+        <v>0.47814997311821905</v>
+      </c>
+      <c r="Z10">
         <v>0.51210428280035414</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA10">
+        <v>2.0959176112987082E-4</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="1"/>
+        <v>0.51231387456148403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
@@ -3221,13 +3352,13 @@
       <c r="F11" s="4">
         <v>10.098349899999999</v>
       </c>
-      <c r="G11" s="145">
+      <c r="G11" s="142">
         <v>5.8681168000000006E-2</v>
       </c>
-      <c r="H11" s="145">
+      <c r="H11" s="142">
         <v>7.3938271E-2</v>
       </c>
-      <c r="I11" s="145">
+      <c r="I11" s="142">
         <v>7.6630038890183744E-2</v>
       </c>
       <c r="J11" s="71">
@@ -3265,10 +3396,24 @@
         <v>0.24585827527712426</v>
       </c>
       <c r="X11">
+        <v>2.0700811243651359E-2</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="0"/>
+        <v>0.26655908652077559</v>
+      </c>
+      <c r="Z11">
         <v>7.6630038890183744E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA11">
+        <v>3.7216049065244534E-4</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="1"/>
+        <v>7.7002199380836189E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>29</v>
       </c>
@@ -3287,13 +3432,13 @@
       <c r="F12" s="4">
         <v>0.62999999523162842</v>
       </c>
-      <c r="G12" s="145">
+      <c r="G12" s="142">
         <v>0.79687950000000285</v>
       </c>
-      <c r="H12" s="145">
+      <c r="H12" s="142">
         <v>1.0040682000000061</v>
       </c>
-      <c r="I12" s="145">
+      <c r="I12" s="142">
         <v>0</v>
       </c>
       <c r="J12" s="71">
@@ -3331,10 +3476,24 @@
         <v>3.4141251927898666</v>
       </c>
       <c r="X12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1.0718762615156343</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="0"/>
+        <v>4.4860014543055007</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0.11248755052026857</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="1"/>
+        <v>0.11248755052026857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>30</v>
       </c>
@@ -3353,13 +3512,13 @@
       <c r="F13" s="4">
         <v>0.92000001668930043</v>
       </c>
-      <c r="G13" s="145">
+      <c r="G13" s="142">
         <v>0.10695653399999999</v>
       </c>
-      <c r="H13" s="145">
+      <c r="H13" s="142">
         <v>0.13476523299999998</v>
       </c>
-      <c r="I13" s="145">
+      <c r="I13" s="142">
         <v>0.18877324129794976</v>
       </c>
       <c r="J13" s="71">
@@ -3397,10 +3556,24 @@
         <v>0.91142919415811929</v>
       </c>
       <c r="X13">
+        <v>1.1802078079887578E-2</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="0"/>
+        <v>0.92323127223800683</v>
+      </c>
+      <c r="Z13">
         <v>0.18877324129794976</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA13">
+        <v>3.4778154884700514E-4</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="1"/>
+        <v>0.18912102284679677</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>31</v>
       </c>
@@ -3419,13 +3592,13 @@
       <c r="F14" s="5">
         <v>77753.520071052437</v>
       </c>
-      <c r="G14" s="145">
+      <c r="G14" s="142">
         <v>77924.526169999997</v>
       </c>
-      <c r="H14" s="145">
+      <c r="H14" s="142">
         <v>77853.149250000002</v>
       </c>
-      <c r="I14" s="145">
+      <c r="I14" s="142">
         <v>77380.440267223457</v>
       </c>
       <c r="J14" s="5">
@@ -3475,10 +3648,24 @@
         <v>71783.505317547926</v>
       </c>
       <c r="X14">
+        <v>611.91676387079497</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="0"/>
+        <v>72395.422081418714</v>
+      </c>
+      <c r="Z14">
         <v>74927.07400875607</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA14">
+        <v>92.564589004961775</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="1"/>
+        <v>75019.638597761033</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>32</v>
       </c>
@@ -3488,7 +3675,7 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15" s="145">
+      <c r="I15" s="142">
         <v>0</v>
       </c>
       <c r="J15" s="69"/>
@@ -3503,40 +3690,57 @@
       <c r="W15">
         <v>-72964.246146966863</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
+        <f t="shared" si="0"/>
+        <v>-72964.246146966863</v>
+      </c>
+      <c r="Z15">
         <v>-76614.526624731123</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AB15">
+        <f t="shared" si="1"/>
+        <v>-76614.526624731123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
       <c r="P16" s="74"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="140" t="s">
+      <c r="B17" s="143" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="140"/>
-      <c r="D17" s="140"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="140"/>
-      <c r="I17" s="140"/>
-      <c r="J17" s="140"/>
-      <c r="K17" s="140"/>
-      <c r="L17" s="140"/>
-      <c r="M17" s="140"/>
-      <c r="N17" s="140"/>
-      <c r="O17" s="140"/>
-      <c r="P17" s="140"/>
-      <c r="Q17" s="140"/>
-      <c r="R17" s="140"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="143"/>
+      <c r="E17" s="143"/>
+      <c r="F17" s="143"/>
+      <c r="G17" s="143"/>
+      <c r="H17" s="143"/>
+      <c r="I17" s="143"/>
+      <c r="J17" s="143"/>
+      <c r="K17" s="143"/>
+      <c r="L17" s="143"/>
+      <c r="M17" s="143"/>
+      <c r="N17" s="143"/>
+      <c r="O17" s="143"/>
+      <c r="P17" s="143"/>
+      <c r="Q17" s="143"/>
+      <c r="R17" s="143"/>
       <c r="S17" t="s">
         <v>90</v>
       </c>
+      <c r="X17" s="76" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y17" s="76"/>
+      <c r="Z17" s="76"/>
+      <c r="AA17" s="76" t="s">
+        <v>317</v>
+      </c>
+      <c r="AB17" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3556,12 +3760,12 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="128"/>
       <c r="B1" s="67" t="s">
         <v>93</v>
@@ -3585,7 +3789,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="67" t="s">
         <v>93</v>
       </c>
@@ -3611,7 +3815,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="67" t="s">
         <v>94</v>
       </c>
@@ -3637,7 +3841,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="67" t="s">
         <v>95</v>
       </c>
@@ -3663,7 +3867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="67" t="s">
         <v>96</v>
       </c>
@@ -3689,7 +3893,7 @@
         <v>2204.6226218487759</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="67" t="s">
         <v>295</v>
       </c>
@@ -3715,7 +3919,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="127" t="s">
         <v>296</v>
       </c>
@@ -3741,7 +3945,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="127" t="s">
         <v>297</v>
       </c>
@@ -3780,9 +3984,9 @@
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>97</v>
       </c>
@@ -3802,7 +4006,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="65" t="s">
         <v>98</v>
       </c>
@@ -3822,7 +4026,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="65" t="s">
         <v>99</v>
       </c>
@@ -3842,7 +4046,7 @@
         <v>28316.847000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>100</v>
       </c>
@@ -3862,7 +4066,7 @@
         <v>28.316846999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>101</v>
       </c>
@@ -3882,7 +4086,7 @@
         <v>7.4805211375990615</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="66" t="s">
         <v>102</v>
       </c>
@@ -3915,9 +4119,9 @@
       <selection activeCell="B2" sqref="B2:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>103</v>
       </c>
@@ -3946,7 +4150,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="65" t="s">
         <v>104</v>
       </c>
@@ -3975,7 +4179,7 @@
         <v>2684519.5376862194</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="65" t="s">
         <v>105</v>
       </c>
@@ -4004,7 +4208,7 @@
         <v>2684.5195376862198</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>106</v>
       </c>
@@ -4033,7 +4237,7 @@
         <v>2.6845195376862194</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>107</v>
       </c>
@@ -4062,7 +4266,7 @@
         <v>745.69987157950538</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="65" t="s">
         <v>108</v>
       </c>
@@ -4091,7 +4295,7 @@
         <v>0.74569987157950535</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="65" t="s">
         <v>109</v>
       </c>
@@ -4120,7 +4324,7 @@
         <v>2544.4335839531336</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="65" t="s">
         <v>110</v>
       </c>
@@ -4149,7 +4353,7 @@
         <v>2.5444335839531337E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="66" t="s">
         <v>111</v>
       </c>
@@ -4191,9 +4395,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="128" t="s">
         <v>112</v>
       </c>
@@ -4216,7 +4420,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="67" t="s">
         <v>113</v>
       </c>
@@ -4239,7 +4443,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="67" t="s">
         <v>114</v>
       </c>
@@ -4262,7 +4466,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="67" t="s">
         <v>115</v>
       </c>
@@ -4285,7 +4489,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="67" t="s">
         <v>116</v>
       </c>
@@ -4308,7 +4512,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="67" t="s">
         <v>117</v>
       </c>
@@ -4331,7 +4535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="127" t="s">
         <v>298</v>
       </c>
@@ -4367,13 +4571,13 @@
       <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="102" t="s">
         <v>221</v>
       </c>
@@ -4384,7 +4588,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A2" s="103" t="s">
         <v>289</v>
       </c>
@@ -4395,7 +4599,7 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A3" s="104" t="s">
         <v>290</v>
       </c>
@@ -4406,7 +4610,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:79" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A5" s="83" t="s">
         <v>224</v>
       </c>
@@ -4645,7 +4849,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A6" s="84" t="s">
         <v>287</v>
       </c>
@@ -4774,7 +4978,7 @@
       <c r="BZ6" s="87"/>
       <c r="CA6" s="92"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A7" s="84" t="s">
         <v>288</v>
       </c>
@@ -4951,7 +5155,7 @@
       <c r="BZ7" s="87"/>
       <c r="CA7" s="92"/>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A8" s="84" t="s">
         <v>222</v>
       </c>
@@ -5188,7 +5392,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A9" s="96" t="s">
         <v>223</v>
       </c>
@@ -5317,13 +5521,13 @@
       <c r="BZ9" s="97"/>
       <c r="CA9" s="101"/>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A11" s="126" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="B12" s="141" t="s">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
+      <c r="B12" s="144" t="s">
         <v>291</v>
       </c>
       <c r="C12" s="105" t="s">
@@ -5340,8 +5544,8 @@
       <c r="L12" s="106"/>
       <c r="M12" s="107"/>
     </row>
-    <row r="13" spans="1:79" ht="39" x14ac:dyDescent="0.25">
-      <c r="B13" s="142"/>
+    <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="145"/>
       <c r="C13" s="108" t="s">
         <v>1</v>
       </c>
@@ -5376,7 +5580,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A14" s="120" t="s">
         <v>22</v>
       </c>
@@ -5417,7 +5621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A15" s="84" t="s">
         <v>23</v>
       </c>
@@ -5458,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A16" s="84" t="s">
         <v>7</v>
       </c>
@@ -5499,7 +5703,7 @@
         <v>76.151387532990128</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="84" t="s">
         <v>24</v>
       </c>
@@ -5540,7 +5744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="84" t="s">
         <v>25</v>
       </c>
@@ -5581,7 +5785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="84" t="s">
         <v>26</v>
       </c>
@@ -5622,7 +5826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="121" t="s">
         <v>27</v>
       </c>
@@ -5663,7 +5867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="121" t="s">
         <v>28</v>
       </c>
@@ -5704,7 +5908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="84" t="s">
         <v>29</v>
       </c>
@@ -5745,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="84" t="s">
         <v>30</v>
       </c>
@@ -5786,7 +5990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="96" t="s">
         <v>31</v>
       </c>
@@ -5827,9 +6031,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="120"/>
-      <c r="B25" s="141" t="s">
+      <c r="B25" s="144" t="s">
         <v>291</v>
       </c>
       <c r="C25" s="105" t="s">
@@ -5846,9 +6050,9 @@
       <c r="L25" s="106"/>
       <c r="M25" s="107"/>
     </row>
-    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="84"/>
-      <c r="B26" s="142"/>
+      <c r="B26" s="145"/>
       <c r="C26" s="108" t="s">
         <v>1</v>
       </c>
@@ -5883,7 +6087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="120" t="s">
         <v>22</v>
       </c>
@@ -5924,7 +6128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="84" t="s">
         <v>23</v>
       </c>
@@ -5965,7 +6169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="84" t="s">
         <v>7</v>
       </c>
@@ -6006,7 +6210,7 @@
         <v>95.950748291567578</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="84" t="s">
         <v>24</v>
       </c>
@@ -6047,7 +6251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="84" t="s">
         <v>25</v>
       </c>
@@ -6088,7 +6292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="84" t="s">
         <v>26</v>
       </c>
@@ -6129,7 +6333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="121" t="s">
         <v>27</v>
       </c>
@@ -6170,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="121" t="s">
         <v>28</v>
       </c>
@@ -6211,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="84" t="s">
         <v>29</v>
       </c>
@@ -6252,7 +6456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="84" t="s">
         <v>30</v>
       </c>
@@ -6293,7 +6497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="96" t="s">
         <v>31</v>
       </c>
@@ -6351,9 +6555,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -6362,7 +6566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="123" t="s">
         <v>8</v>
       </c>
@@ -6373,7 +6577,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="123" t="s">
         <v>9</v>
       </c>
@@ -6384,7 +6588,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="123" t="s">
         <v>10</v>
       </c>
@@ -6395,7 +6599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="123" t="s">
         <v>11</v>
       </c>
@@ -6406,7 +6610,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="123" t="s">
         <v>12</v>
       </c>
@@ -6417,7 +6621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="123" t="s">
         <v>13</v>
       </c>
@@ -6442,12 +6646,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -6455,7 +6659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6466,7 +6670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -6477,7 +6681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -6488,7 +6692,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -6499,7 +6703,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -6510,7 +6714,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -6534,13 +6738,13 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -6554,7 +6758,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="136" t="s">
         <v>123</v>
       </c>
@@ -6571,7 +6775,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>126</v>
       </c>
@@ -6588,7 +6792,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -6605,7 +6809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -6622,7 +6826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6639,7 +6843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -6656,7 +6860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -6673,7 +6877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -6690,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -6707,7 +6911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -6724,7 +6928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -6741,7 +6945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -6758,7 +6962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -6775,7 +6979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -6792,7 +6996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -6809,7 +7013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -6826,7 +7030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -6843,7 +7047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -6860,7 +7064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -6877,111 +7081,111 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E21" s="38"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="140" t="s">
+      <c r="B22" s="143" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="140"/>
-      <c r="D22" s="140"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="143"/>
+      <c r="D22" s="143"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -7006,17 +7210,17 @@
       <selection pane="topRight" activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A1" s="19"/>
       <c r="B1" s="20" t="s">
         <v>311</v>
@@ -7121,7 +7325,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>123</v>
       </c>
@@ -7228,7 +7432,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>126</v>
       </c>
@@ -7335,7 +7539,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -7442,7 +7646,7 @@
         <v>22.768308419908244</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -7549,7 +7753,7 @@
         <v>14.313720661890066</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -7656,7 +7860,7 @@
         <v>1.01369654150063</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7763,7 +7967,7 @@
         <v>11.762225607448672</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -7870,7 +8074,7 @@
         <v>1.537798512940765</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -7977,7 +8181,7 @@
         <v>1.0524015417807536E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
         <v>59</v>
       </c>
@@ -8014,7 +8218,7 @@
       <c r="AF10" s="38"/>
       <c r="AH10" s="29"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>60</v>
       </c>
@@ -8121,7 +8325,7 @@
         <v>1.5332925780409926E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
         <v>61</v>
       </c>
@@ -8228,7 +8432,7 @@
         <v>1.0670036531779258E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>62</v>
       </c>
@@ -8335,7 +8539,7 @@
         <v>2.2646336328392878E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>63</v>
       </c>
@@ -8442,7 +8646,7 @@
         <v>4.1715536368739541E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>64</v>
       </c>
@@ -8549,7 +8753,7 @@
         <v>1.5575235226667416E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>65</v>
       </c>
@@ -8656,7 +8860,7 @@
         <v>6.4089140933905775E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
         <v>66</v>
       </c>
@@ -8763,7 +8967,7 @@
         <v>1.8129502103015302E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>67</v>
       </c>
@@ -8870,7 +9074,7 @@
         <v>2.6305516438756624E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" s="24" t="s">
         <v>68</v>
       </c>
@@ -8977,7 +9181,7 @@
         <v>2.5803232307925993E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="24" t="s">
         <v>69</v>
       </c>
@@ -9084,7 +9288,7 @@
         <v>1.0018145421706144E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
         <v>70</v>
       </c>
@@ -9191,43 +9395,43 @@
         <v>1.1117032316949111</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="143" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="140"/>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="140"/>
-      <c r="J23" s="140"/>
-      <c r="K23" s="140"/>
-      <c r="L23" s="140"/>
-      <c r="M23" s="140"/>
-      <c r="N23" s="140"/>
-      <c r="O23" s="140"/>
-      <c r="P23" s="140"/>
-      <c r="Q23" s="140"/>
-      <c r="R23" s="140"/>
-      <c r="S23" s="140"/>
-      <c r="T23" s="140"/>
-      <c r="U23" s="140"/>
-      <c r="V23" s="140"/>
-      <c r="W23" s="140"/>
-      <c r="X23" s="140"/>
-      <c r="Y23" s="140"/>
-      <c r="Z23" s="140"/>
-      <c r="AA23" s="140"/>
-      <c r="AB23" s="140"/>
-      <c r="AC23" s="140"/>
-      <c r="AD23" s="140"/>
-      <c r="AE23" s="140"/>
-      <c r="AF23" s="140"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="143"/>
+      <c r="E23" s="143"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="143"/>
+      <c r="I23" s="143"/>
+      <c r="J23" s="143"/>
+      <c r="K23" s="143"/>
+      <c r="L23" s="143"/>
+      <c r="M23" s="143"/>
+      <c r="N23" s="143"/>
+      <c r="O23" s="143"/>
+      <c r="P23" s="143"/>
+      <c r="Q23" s="143"/>
+      <c r="R23" s="143"/>
+      <c r="S23" s="143"/>
+      <c r="T23" s="143"/>
+      <c r="U23" s="143"/>
+      <c r="V23" s="143"/>
+      <c r="W23" s="143"/>
+      <c r="X23" s="143"/>
+      <c r="Y23" s="143"/>
+      <c r="Z23" s="143"/>
+      <c r="AA23" s="143"/>
+      <c r="AB23" s="143"/>
+      <c r="AC23" s="143"/>
+      <c r="AD23" s="143"/>
+      <c r="AE23" s="143"/>
+      <c r="AF23" s="143"/>
       <c r="AI23" t="s">
         <v>305</v>
       </c>
@@ -9249,9 +9453,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
@@ -9259,7 +9463,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>34</v>
       </c>
@@ -9268,7 +9472,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>35</v>
       </c>
@@ -9277,7 +9481,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
@@ -9286,7 +9490,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
@@ -9295,7 +9499,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="39" t="s">
         <v>79</v>
       </c>
@@ -9316,12 +9520,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="8"/>
+    <col min="1" max="1" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -9371,7 +9575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="78.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -9422,7 +9626,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>126</v>
       </c>
@@ -9475,7 +9679,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="123" t="s">
         <v>8</v>
       </c>
@@ -9526,7 +9730,7 @@
       </c>
       <c r="Q4" s="125"/>
     </row>
-    <row r="5" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="123" t="s">
         <v>9</v>
       </c>
@@ -9577,7 +9781,7 @@
       </c>
       <c r="Q5" s="125"/>
     </row>
-    <row r="6" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="123" t="s">
         <v>10</v>
       </c>
@@ -9628,7 +9832,7 @@
       </c>
       <c r="Q6" s="125"/>
     </row>
-    <row r="7" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="123" t="s">
         <v>11</v>
       </c>
@@ -9679,7 +9883,7 @@
       </c>
       <c r="Q7" s="125"/>
     </row>
-    <row r="8" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="123" t="s">
         <v>12</v>
       </c>
@@ -9730,7 +9934,7 @@
       </c>
       <c r="Q8" s="125"/>
     </row>
-    <row r="9" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="123" t="s">
         <v>13</v>
       </c>
@@ -9781,7 +9985,7 @@
       </c>
       <c r="Q9" s="125"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
@@ -9832,7 +10036,7 @@
       </c>
       <c r="Q10" s="73"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>23</v>
       </c>
@@ -9883,7 +10087,7 @@
       </c>
       <c r="Q11" s="73"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
@@ -9934,7 +10138,7 @@
       </c>
       <c r="Q12" s="73"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -9985,7 +10189,7 @@
       </c>
       <c r="Q13" s="73"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
@@ -10036,7 +10240,7 @@
       </c>
       <c r="Q14" s="73"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -10087,7 +10291,7 @@
       </c>
       <c r="Q15" s="73"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -10138,7 +10342,7 @@
       </c>
       <c r="Q16" s="73"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
@@ -10189,7 +10393,7 @@
       </c>
       <c r="Q17" s="73"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
@@ -10240,7 +10444,7 @@
       </c>
       <c r="Q18" s="73"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>30</v>
       </c>
@@ -10291,7 +10495,7 @@
       </c>
       <c r="Q19" s="73"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>31</v>
       </c>
@@ -10346,7 +10550,7 @@
         <v>3.3478260869565215</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>32</v>
       </c>
@@ -10360,30 +10564,30 @@
       <c r="N21" s="69"/>
       <c r="O21" s="69"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="M22" s="74"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="143" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="140"/>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="140"/>
-      <c r="J23" s="140"/>
-      <c r="K23" s="140"/>
-      <c r="L23" s="140"/>
-      <c r="M23" s="140"/>
-      <c r="N23" s="140"/>
-      <c r="O23" s="140"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="143"/>
+      <c r="E23" s="143"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="143"/>
+      <c r="I23" s="143"/>
+      <c r="J23" s="143"/>
+      <c r="K23" s="143"/>
+      <c r="L23" s="143"/>
+      <c r="M23" s="143"/>
+      <c r="N23" s="143"/>
+      <c r="O23" s="143"/>
       <c r="P23" t="s">
         <v>90</v>
       </c>
@@ -10406,12 +10610,12 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>299</v>
       </c>
@@ -10422,7 +10626,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -10436,7 +10640,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>126</v>
       </c>
@@ -10450,7 +10654,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -10464,7 +10668,7 @@
         <v>362403.00757167325</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -10478,7 +10682,7 @@
         <v>344979.42656462023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -10492,7 +10696,7 @@
         <v>24381.856026689315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -10506,7 +10710,7 @@
         <v>254462.26606022959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -10520,7 +10724,7 @@
         <v>66135.304477701342</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -10534,7 +10738,7 @@
         <v>59.889274923371126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10548,7 +10752,7 @@
         <v>24.470884336712146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -10562,7 +10766,7 @@
         <v>34.134614130073174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -10576,7 +10780,7 @@
         <v>-15.759603589368934</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -10590,7 +10794,7 @@
         <v>8.6858851249063438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -10604,7 +10808,7 @@
         <v>6.9883164862451217</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -10618,7 +10822,7 @@
         <v>58.328462296040968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -10632,7 +10836,7 @@
         <v>0.49662761207225459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -10646,7 +10850,7 @@
         <v>1.1283578872130025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -10660,7 +10864,7 @@
         <v>57.127332585038609</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10674,7 +10878,7 @@
         <v>-82.715827114534676</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10688,7 +10892,7 @@
         <v>22763.019075759898</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -10713,9 +10917,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -10723,7 +10927,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="67" t="s">
         <v>93</v>
       </c>
@@ -10731,7 +10935,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="67" t="s">
         <v>94</v>
       </c>
@@ -10739,7 +10943,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="67" t="s">
         <v>95</v>
       </c>
@@ -10747,7 +10951,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="67" t="s">
         <v>96</v>
       </c>
@@ -10755,7 +10959,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="67" t="s">
         <v>295</v>
       </c>
@@ -10763,7 +10967,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="67" t="s">
         <v>98</v>
       </c>
@@ -10771,7 +10975,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="67" t="s">
         <v>99</v>
       </c>
@@ -10779,7 +10983,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="67" t="s">
         <v>100</v>
       </c>
@@ -10787,7 +10991,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="67" t="s">
         <v>101</v>
       </c>
@@ -10795,7 +10999,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="67" t="s">
         <v>102</v>
       </c>
@@ -10803,7 +11007,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="67" t="s">
         <v>104</v>
       </c>
@@ -10811,7 +11015,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="67" t="s">
         <v>105</v>
       </c>
@@ -10819,7 +11023,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="67" t="s">
         <v>106</v>
       </c>
@@ -10827,7 +11031,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="67" t="s">
         <v>107</v>
       </c>
@@ -10835,7 +11039,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="67" t="s">
         <v>108</v>
       </c>
@@ -10843,7 +11047,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="67" t="s">
         <v>109</v>
       </c>
@@ -10851,7 +11055,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="67" t="s">
         <v>110</v>
       </c>
@@ -10859,7 +11063,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="67" t="s">
         <v>111</v>
       </c>
@@ -10867,7 +11071,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="67" t="s">
         <v>113</v>
       </c>
@@ -10875,7 +11079,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="67" t="s">
         <v>114</v>
       </c>
@@ -10883,7 +11087,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="67" t="s">
         <v>115</v>
       </c>
@@ -10891,7 +11095,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="67" t="s">
         <v>116</v>
       </c>
@@ -10899,7 +11103,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="67" t="s">
         <v>117</v>
       </c>
@@ -10920,12 +11124,12 @@
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="75" t="s">
         <v>187</v>
       </c>
@@ -10933,7 +11137,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -10944,7 +11148,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -10955,7 +11159,7 @@
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="76" t="s">
         <v>128</v>
       </c>
@@ -10966,7 +11170,7 @@
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="76" t="s">
         <v>129</v>
       </c>
@@ -10977,7 +11181,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="76" t="s">
         <v>130</v>
       </c>
@@ -10988,7 +11192,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="76" t="s">
         <v>131</v>
       </c>
@@ -10999,7 +11203,7 @@
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="76" t="s">
         <v>132</v>
       </c>
@@ -11010,7 +11214,7 @@
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="76" t="s">
         <v>133</v>
       </c>
@@ -11021,7 +11225,7 @@
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="76" t="s">
         <v>134</v>
       </c>
@@ -11032,7 +11236,7 @@
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="76" t="s">
         <v>135</v>
       </c>
@@ -11043,7 +11247,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -11054,7 +11258,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="76" t="s">
         <v>137</v>
       </c>
@@ -11065,7 +11269,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="76" t="s">
         <v>138</v>
       </c>
@@ -11076,7 +11280,7 @@
         <v>755.86244135709444</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="76" t="s">
         <v>139</v>
       </c>
@@ -11087,7 +11291,7 @@
         <v>762.55920427134606</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="76" t="s">
         <v>140</v>
       </c>
@@ -11098,7 +11302,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="76" t="s">
         <v>141</v>
       </c>
@@ -11109,7 +11313,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="76" t="s">
         <v>142</v>
       </c>
@@ -11120,7 +11324,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="75" t="s">
         <v>1</v>
       </c>
@@ -11131,7 +11335,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>143</v>
       </c>
@@ -11142,7 +11346,7 @@
         <v>725.15243391008278</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>144</v>
       </c>
@@ -11153,7 +11357,7 @@
         <v>748.62596861099109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -11164,7 +11368,7 @@
         <v>801.99999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -11175,7 +11379,7 @@
         <v>791.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>147</v>
       </c>
@@ -11186,7 +11390,7 @@
         <v>700.32025584540236</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -11197,7 +11401,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>149</v>
       </c>
@@ -11208,7 +11412,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -11219,7 +11423,7 @@
         <v>794.1013538556316</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>151</v>
       </c>
@@ -11230,7 +11434,7 @@
         <v>789.34625592835232</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>152</v>
       </c>
@@ -11241,7 +11445,7 @@
         <v>809.68750817282455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>153</v>
       </c>
@@ -11252,7 +11456,7 @@
         <v>783.00612535864673</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>154</v>
       </c>
@@ -11263,7 +11467,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>155</v>
       </c>
@@ -11274,7 +11478,7 @@
         <v>508.00296189766453</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>156</v>
       </c>
@@ -11285,7 +11489,7 @@
         <v>428.22298556220187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>157</v>
       </c>
@@ -11296,7 +11500,7 @@
         <v>665.18536560495022</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>158</v>
       </c>
@@ -11307,7 +11511,7 @@
         <v>859.88020851632757</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>159</v>
       </c>
@@ -11318,7 +11522,7 @@
         <v>887.88245186586084</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>160</v>
       </c>
@@ -11329,7 +11533,7 @@
         <v>797.00724703341325</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -11340,7 +11544,7 @@
         <v>748.92792354647884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>162</v>
       </c>
@@ -11351,7 +11555,7 @@
         <v>778.77937164550963</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>163</v>
       </c>
@@ -11362,7 +11566,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>164</v>
       </c>
@@ -11373,7 +11577,7 @@
         <v>798.04417121416941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>243</v>
       </c>
@@ -11384,7 +11588,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -11395,7 +11599,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>166</v>
       </c>
@@ -11406,7 +11610,7 @@
         <v>716.69892648380858</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>167</v>
       </c>
@@ -11417,7 +11621,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -11428,7 +11632,7 @@
         <v>756.99999999999989</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -11439,7 +11643,7 @@
         <v>70.798124695046326</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -11450,7 +11654,7 @@
         <v>742.58779297677324</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -11461,7 +11665,7 @@
         <v>742.32362086970215</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>172</v>
       </c>
@@ -11472,7 +11676,7 @@
         <v>769.53334789802227</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>173</v>
       </c>
@@ -11483,7 +11687,7 @@
         <v>584.61287294827434</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>174</v>
       </c>
@@ -11494,7 +11698,7 @@
         <v>559.51652277652283</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>175</v>
       </c>
@@ -11505,7 +11709,7 @@
         <v>595.17975723111715</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>176</v>
       </c>
@@ -11516,7 +11720,7 @@
         <v>507.21044557645126</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>177</v>
       </c>
@@ -11527,7 +11731,7 @@
         <v>668.88377510394514</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>178</v>
       </c>
@@ -11538,7 +11742,7 @@
         <v>654.80340179705718</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>179</v>
       </c>
@@ -11549,7 +11753,7 @@
         <v>688.85095964480468</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>180</v>
       </c>
@@ -11560,7 +11764,7 @@
         <v>737.59071339941693</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>181</v>
       </c>
@@ -11571,7 +11775,7 @@
         <v>765.47381512866104</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -11582,7 +11786,7 @@
         <v>731.67589538225809</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>183</v>
       </c>
@@ -11593,7 +11797,7 @@
         <v>800.00032424653136</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>184</v>
       </c>
@@ -11604,7 +11808,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>188</v>
       </c>
@@ -11615,7 +11819,7 @@
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>189</v>
       </c>
@@ -11626,7 +11830,7 @@
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="75" t="s">
         <v>89</v>
       </c>
@@ -11637,7 +11841,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -11648,7 +11852,7 @@
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -11659,7 +11863,7 @@
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>192</v>
       </c>
@@ -11667,7 +11871,7 @@
         <v>22.648458746153963</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -11675,7 +11879,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>194</v>
       </c>
@@ -11683,7 +11887,7 @@
         <v>18.707371337693861</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -11691,7 +11895,7 @@
         <v>12.566427590816895</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>196</v>
       </c>
@@ -11699,7 +11903,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>197</v>
       </c>
@@ -11707,7 +11911,7 @@
         <v>11.566786665057547</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -11715,7 +11919,7 @@
         <v>31.342185540824094</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>199</v>
       </c>
@@ -11723,7 +11927,7 @@
         <v>31.0106439692332</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>200</v>
       </c>
@@ -11731,7 +11935,7 @@
         <v>28.609127685562171</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -11739,7 +11943,7 @@
         <v>33.012627597074328</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>202</v>
       </c>
@@ -11747,7 +11951,7 @@
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>203</v>
       </c>
@@ -11755,7 +11959,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -11763,7 +11967,7 @@
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -11771,7 +11975,7 @@
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -11779,7 +11983,7 @@
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -11787,7 +11991,7 @@
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>208</v>
       </c>
@@ -11795,7 +11999,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>209</v>
       </c>
@@ -11803,7 +12007,7 @@
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -11811,7 +12015,7 @@
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>211</v>
       </c>
@@ -11819,7 +12023,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>212</v>
       </c>
@@ -11827,7 +12031,7 @@
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>213</v>
       </c>
@@ -11835,7 +12039,7 @@
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -11843,7 +12047,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -11851,7 +12055,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>216</v>
       </c>
@@ -11859,7 +12063,7 @@
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -11867,7 +12071,7 @@
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="75" t="s">
         <v>220</v>
       </c>
@@ -11875,7 +12079,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
1. Modified the basis on which multiple main products are combined (now based on coproduct handling method); 2. Changed how biorefinery-level results are calculated for displacement method are calculated so that it shows consistent value when allocation methods are used
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AAEF1E-4951-4BCE-BBCD-212EB89D06EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487FC5B5-E97A-4711-BBEE-D84D1AE3CD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView minimized="1" xWindow="53640" yWindow="11415" windowWidth="2040" windowHeight="720" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -1538,7 +1538,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1827,6 +1827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2528,17 +2529,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AD6" sqref="AD6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="8"/>
-    <col min="9" max="9" width="9.1796875" style="142"/>
+    <col min="1" max="1" width="8.7109375" style="8"/>
+    <col min="9" max="9" width="9.140625" style="142"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -2705,7 +2706,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>126</v>
       </c>
@@ -2773,7 +2774,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>22</v>
       </c>
@@ -2853,7 +2854,7 @@
         <v>40.366758790864871</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -2933,7 +2934,7 @@
         <v>993.99652518923131</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>27.521187334987346</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>24</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>9.4662813685889695</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -3173,7 +3174,7 @@
         <v>1.8944508672117086</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>26</v>
       </c>
@@ -3253,7 +3254,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>27</v>
       </c>
@@ -3333,7 +3334,7 @@
         <v>0.51231387456148403</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>7.7002199380836189E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>29</v>
       </c>
@@ -3493,7 +3494,7 @@
         <v>0.11248755052026857</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>30</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>0.18912102284679677</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>31</v>
       </c>
@@ -3640,7 +3641,7 @@
         <f>-12*6/(12*6+10*1+4*16)*44/12</f>
         <v>-1.8082191780821917</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="146">
         <f>-12*6/(12*6+8*1+5*16)*44/12</f>
         <v>-1.6500000000000001</v>
       </c>
@@ -3665,7 +3666,7 @@
         <v>75019.638597761033</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>32</v>
       </c>
@@ -3702,11 +3703,11 @@
         <v>-76614.526624731123</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="P16" s="74"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -3760,12 +3761,12 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="128"/>
       <c r="B1" s="67" t="s">
         <v>93</v>
@@ -3789,7 +3790,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
         <v>93</v>
       </c>
@@ -3815,7 +3816,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
         <v>94</v>
       </c>
@@ -3841,7 +3842,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
         <v>95</v>
       </c>
@@ -3867,7 +3868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
         <v>96</v>
       </c>
@@ -3893,7 +3894,7 @@
         <v>2204.6226218487759</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="67" t="s">
         <v>295</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="127" t="s">
         <v>296</v>
       </c>
@@ -3945,7 +3946,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="127" t="s">
         <v>297</v>
       </c>
@@ -3984,9 +3985,9 @@
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>97</v>
       </c>
@@ -4006,7 +4007,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
         <v>98</v>
       </c>
@@ -4026,7 +4027,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>99</v>
       </c>
@@ -4046,7 +4047,7 @@
         <v>28316.847000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
         <v>100</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>28.316846999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
         <v>101</v>
       </c>
@@ -4086,7 +4087,7 @@
         <v>7.4805211375990615</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
         <v>102</v>
       </c>
@@ -4119,9 +4120,9 @@
       <selection activeCell="B2" sqref="B2:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>103</v>
       </c>
@@ -4150,7 +4151,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
         <v>104</v>
       </c>
@@ -4179,7 +4180,7 @@
         <v>2684519.5376862194</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>105</v>
       </c>
@@ -4208,7 +4209,7 @@
         <v>2684.5195376862198</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
         <v>106</v>
       </c>
@@ -4237,7 +4238,7 @@
         <v>2.6845195376862194</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
         <v>107</v>
       </c>
@@ -4266,7 +4267,7 @@
         <v>745.69987157950538</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
         <v>108</v>
       </c>
@@ -4295,7 +4296,7 @@
         <v>0.74569987157950535</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
         <v>109</v>
       </c>
@@ -4324,7 +4325,7 @@
         <v>2544.4335839531336</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="65" t="s">
         <v>110</v>
       </c>
@@ -4353,7 +4354,7 @@
         <v>2.5444335839531337E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
         <v>111</v>
       </c>
@@ -4395,9 +4396,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="128" t="s">
         <v>112</v>
       </c>
@@ -4420,7 +4421,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
         <v>113</v>
       </c>
@@ -4443,7 +4444,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
         <v>114</v>
       </c>
@@ -4466,7 +4467,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
         <v>115</v>
       </c>
@@ -4489,7 +4490,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
         <v>116</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="67" t="s">
         <v>117</v>
       </c>
@@ -4535,7 +4536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="127" t="s">
         <v>298</v>
       </c>
@@ -4571,13 +4572,13 @@
       <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="102" t="s">
         <v>221</v>
       </c>
@@ -4588,7 +4589,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>289</v>
       </c>
@@ -4599,7 +4600,7 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="104" t="s">
         <v>290</v>
       </c>
@@ -4610,7 +4611,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:79" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A5" s="83" t="s">
         <v>224</v>
       </c>
@@ -4849,7 +4850,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A6" s="84" t="s">
         <v>287</v>
       </c>
@@ -4978,7 +4979,7 @@
       <c r="BZ6" s="87"/>
       <c r="CA6" s="92"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A7" s="84" t="s">
         <v>288</v>
       </c>
@@ -5155,7 +5156,7 @@
       <c r="BZ7" s="87"/>
       <c r="CA7" s="92"/>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A8" s="84" t="s">
         <v>222</v>
       </c>
@@ -5392,7 +5393,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A9" s="96" t="s">
         <v>223</v>
       </c>
@@ -5521,12 +5522,12 @@
       <c r="BZ9" s="97"/>
       <c r="CA9" s="101"/>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A11" s="126" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B12" s="144" t="s">
         <v>291</v>
       </c>
@@ -5544,7 +5545,7 @@
       <c r="L12" s="106"/>
       <c r="M12" s="107"/>
     </row>
-    <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:79" ht="39" x14ac:dyDescent="0.25">
       <c r="B13" s="145"/>
       <c r="C13" s="108" t="s">
         <v>1</v>
@@ -5580,7 +5581,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A14" s="120" t="s">
         <v>22</v>
       </c>
@@ -5621,7 +5622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A15" s="84" t="s">
         <v>23</v>
       </c>
@@ -5662,7 +5663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A16" s="84" t="s">
         <v>7</v>
       </c>
@@ -5703,7 +5704,7 @@
         <v>76.151387532990128</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="84" t="s">
         <v>24</v>
       </c>
@@ -5744,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="84" t="s">
         <v>25</v>
       </c>
@@ -5785,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="84" t="s">
         <v>26</v>
       </c>
@@ -5826,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="121" t="s">
         <v>27</v>
       </c>
@@ -5867,7 +5868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="121" t="s">
         <v>28</v>
       </c>
@@ -5908,7 +5909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="84" t="s">
         <v>29</v>
       </c>
@@ -5949,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="84" t="s">
         <v>30</v>
       </c>
@@ -5990,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="96" t="s">
         <v>31</v>
       </c>
@@ -6031,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="120"/>
       <c r="B25" s="144" t="s">
         <v>291</v>
@@ -6050,7 +6051,7 @@
       <c r="L25" s="106"/>
       <c r="M25" s="107"/>
     </row>
-    <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A26" s="84"/>
       <c r="B26" s="145"/>
       <c r="C26" s="108" t="s">
@@ -6087,7 +6088,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="120" t="s">
         <v>22</v>
       </c>
@@ -6128,7 +6129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="84" t="s">
         <v>23</v>
       </c>
@@ -6169,7 +6170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="84" t="s">
         <v>7</v>
       </c>
@@ -6210,7 +6211,7 @@
         <v>95.950748291567578</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="84" t="s">
         <v>24</v>
       </c>
@@ -6251,7 +6252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="84" t="s">
         <v>25</v>
       </c>
@@ -6292,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="84" t="s">
         <v>26</v>
       </c>
@@ -6333,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="121" t="s">
         <v>27</v>
       </c>
@@ -6374,7 +6375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="121" t="s">
         <v>28</v>
       </c>
@@ -6415,7 +6416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="84" t="s">
         <v>29</v>
       </c>
@@ -6456,7 +6457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="84" t="s">
         <v>30</v>
       </c>
@@ -6497,7 +6498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="96" t="s">
         <v>31</v>
       </c>
@@ -6555,9 +6556,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -6566,7 +6567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="123" t="s">
         <v>8</v>
       </c>
@@ -6577,7 +6578,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="123" t="s">
         <v>9</v>
       </c>
@@ -6588,7 +6589,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="123" t="s">
         <v>10</v>
       </c>
@@ -6599,7 +6600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="123" t="s">
         <v>11</v>
       </c>
@@ -6610,7 +6611,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="123" t="s">
         <v>12</v>
       </c>
@@ -6621,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="123" t="s">
         <v>13</v>
       </c>
@@ -6646,12 +6647,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -6659,7 +6660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6670,7 +6671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -6681,7 +6682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -6692,7 +6693,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -6703,7 +6704,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -6714,7 +6715,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -6738,13 +6739,13 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -6758,7 +6759,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="136" t="s">
         <v>123</v>
       </c>
@@ -6775,7 +6776,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>126</v>
       </c>
@@ -6792,7 +6793,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -6809,7 +6810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -6826,7 +6827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6843,7 +6844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -6860,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -6877,7 +6878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -6894,7 +6895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -6911,7 +6912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -6928,7 +6929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -6945,7 +6946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -6962,7 +6963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -6979,7 +6980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -6996,7 +6997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -7013,7 +7014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -7030,7 +7031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -7047,7 +7048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -7064,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -7081,10 +7082,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E21" s="38"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -7094,98 +7095,98 @@
       <c r="C22" s="143"/>
       <c r="D22" s="143"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -7210,17 +7211,17 @@
       <selection pane="topRight" activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" customWidth="1"/>
-    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
       <c r="B1" s="20" t="s">
         <v>311</v>
@@ -7325,7 +7326,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>123</v>
       </c>
@@ -7432,7 +7433,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>126</v>
       </c>
@@ -7539,7 +7540,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -7646,7 +7647,7 @@
         <v>22.768308419908244</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -7753,7 +7754,7 @@
         <v>14.313720661890066</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -7860,7 +7861,7 @@
         <v>1.01369654150063</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7967,7 +7968,7 @@
         <v>11.762225607448672</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -8074,7 +8075,7 @@
         <v>1.537798512940765</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -8181,7 +8182,7 @@
         <v>1.0524015417807536E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>59</v>
       </c>
@@ -8218,7 +8219,7 @@
       <c r="AF10" s="38"/>
       <c r="AH10" s="29"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>60</v>
       </c>
@@ -8325,7 +8326,7 @@
         <v>1.5332925780409926E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>61</v>
       </c>
@@ -8432,7 +8433,7 @@
         <v>1.0670036531779258E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>62</v>
       </c>
@@ -8539,7 +8540,7 @@
         <v>2.2646336328392878E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>63</v>
       </c>
@@ -8646,7 +8647,7 @@
         <v>4.1715536368739541E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>64</v>
       </c>
@@ -8753,7 +8754,7 @@
         <v>1.5575235226667416E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>65</v>
       </c>
@@ -8860,7 +8861,7 @@
         <v>6.4089140933905775E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>66</v>
       </c>
@@ -8967,7 +8968,7 @@
         <v>1.8129502103015302E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>67</v>
       </c>
@@ -9074,7 +9075,7 @@
         <v>2.6305516438756624E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>68</v>
       </c>
@@ -9181,7 +9182,7 @@
         <v>2.5803232307925993E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>69</v>
       </c>
@@ -9288,7 +9289,7 @@
         <v>1.0018145421706144E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>70</v>
       </c>
@@ -9395,7 +9396,7 @@
         <v>1.1117032316949111</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -9453,9 +9454,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
@@ -9463,7 +9464,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>34</v>
       </c>
@@ -9472,7 +9473,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>35</v>
       </c>
@@ -9481,7 +9482,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
@@ -9490,7 +9491,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
@@ -9499,7 +9500,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
         <v>79</v>
       </c>
@@ -9520,12 +9521,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="8.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -9575,7 +9576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -9626,7 +9627,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>126</v>
       </c>
@@ -9679,7 +9680,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="123" t="s">
         <v>8</v>
       </c>
@@ -9730,7 +9731,7 @@
       </c>
       <c r="Q4" s="125"/>
     </row>
-    <row r="5" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="123" t="s">
         <v>9</v>
       </c>
@@ -9781,7 +9782,7 @@
       </c>
       <c r="Q5" s="125"/>
     </row>
-    <row r="6" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="123" t="s">
         <v>10</v>
       </c>
@@ -9832,7 +9833,7 @@
       </c>
       <c r="Q6" s="125"/>
     </row>
-    <row r="7" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="123" t="s">
         <v>11</v>
       </c>
@@ -9883,7 +9884,7 @@
       </c>
       <c r="Q7" s="125"/>
     </row>
-    <row r="8" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="123" t="s">
         <v>12</v>
       </c>
@@ -9934,7 +9935,7 @@
       </c>
       <c r="Q8" s="125"/>
     </row>
-    <row r="9" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="123" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="123" t="s">
         <v>13</v>
       </c>
@@ -9985,7 +9986,7 @@
       </c>
       <c r="Q9" s="125"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
@@ -10036,7 +10037,7 @@
       </c>
       <c r="Q10" s="73"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>23</v>
       </c>
@@ -10087,7 +10088,7 @@
       </c>
       <c r="Q11" s="73"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
@@ -10138,7 +10139,7 @@
       </c>
       <c r="Q12" s="73"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -10189,7 +10190,7 @@
       </c>
       <c r="Q13" s="73"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
@@ -10240,7 +10241,7 @@
       </c>
       <c r="Q14" s="73"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -10291,7 +10292,7 @@
       </c>
       <c r="Q15" s="73"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -10342,7 +10343,7 @@
       </c>
       <c r="Q16" s="73"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
@@ -10393,7 +10394,7 @@
       </c>
       <c r="Q17" s="73"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
@@ -10444,7 +10445,7 @@
       </c>
       <c r="Q18" s="73"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>30</v>
       </c>
@@ -10495,7 +10496,7 @@
       </c>
       <c r="Q19" s="73"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>31</v>
       </c>
@@ -10550,7 +10551,7 @@
         <v>3.3478260869565215</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>32</v>
       </c>
@@ -10564,11 +10565,11 @@
       <c r="N21" s="69"/>
       <c r="O21" s="69"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="M22" s="74"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
@@ -10610,12 +10611,12 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>299</v>
       </c>
@@ -10626,7 +10627,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -10640,7 +10641,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>126</v>
       </c>
@@ -10654,7 +10655,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -10668,7 +10669,7 @@
         <v>362403.00757167325</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -10682,7 +10683,7 @@
         <v>344979.42656462023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -10696,7 +10697,7 @@
         <v>24381.856026689315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -10710,7 +10711,7 @@
         <v>254462.26606022959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -10724,7 +10725,7 @@
         <v>66135.304477701342</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -10738,7 +10739,7 @@
         <v>59.889274923371126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10752,7 +10753,7 @@
         <v>24.470884336712146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -10766,7 +10767,7 @@
         <v>34.134614130073174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -10780,7 +10781,7 @@
         <v>-15.759603589368934</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -10794,7 +10795,7 @@
         <v>8.6858851249063438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -10808,7 +10809,7 @@
         <v>6.9883164862451217</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -10822,7 +10823,7 @@
         <v>58.328462296040968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -10836,7 +10837,7 @@
         <v>0.49662761207225459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -10850,7 +10851,7 @@
         <v>1.1283578872130025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -10864,7 +10865,7 @@
         <v>57.127332585038609</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10878,7 +10879,7 @@
         <v>-82.715827114534676</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10892,7 +10893,7 @@
         <v>22763.019075759898</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -10917,9 +10918,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -10927,7 +10928,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
         <v>93</v>
       </c>
@@ -10935,7 +10936,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
         <v>94</v>
       </c>
@@ -10943,7 +10944,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
         <v>95</v>
       </c>
@@ -10951,7 +10952,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
         <v>96</v>
       </c>
@@ -10959,7 +10960,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="67" t="s">
         <v>295</v>
       </c>
@@ -10967,7 +10968,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="67" t="s">
         <v>98</v>
       </c>
@@ -10975,7 +10976,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="s">
         <v>99</v>
       </c>
@@ -10983,7 +10984,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
         <v>100</v>
       </c>
@@ -10991,7 +10992,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
         <v>101</v>
       </c>
@@ -10999,7 +11000,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
         <v>102</v>
       </c>
@@ -11007,7 +11008,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="67" t="s">
         <v>104</v>
       </c>
@@ -11015,7 +11016,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="67" t="s">
         <v>105</v>
       </c>
@@ -11023,7 +11024,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="67" t="s">
         <v>106</v>
       </c>
@@ -11031,7 +11032,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
         <v>107</v>
       </c>
@@ -11039,7 +11040,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
         <v>108</v>
       </c>
@@ -11047,7 +11048,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="67" t="s">
         <v>109</v>
       </c>
@@ -11055,7 +11056,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
         <v>110</v>
       </c>
@@ -11063,7 +11064,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="67" t="s">
         <v>111</v>
       </c>
@@ -11071,7 +11072,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="67" t="s">
         <v>113</v>
       </c>
@@ -11079,7 +11080,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="67" t="s">
         <v>114</v>
       </c>
@@ -11087,7 +11088,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="67" t="s">
         <v>115</v>
       </c>
@@ -11095,7 +11096,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="67" t="s">
         <v>116</v>
       </c>
@@ -11103,7 +11104,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="67" t="s">
         <v>117</v>
       </c>
@@ -11120,16 +11121,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="75" t="s">
         <v>187</v>
       </c>
@@ -11137,7 +11138,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -11148,7 +11149,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -11159,7 +11160,7 @@
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
         <v>128</v>
       </c>
@@ -11170,7 +11171,7 @@
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="76" t="s">
         <v>129</v>
       </c>
@@ -11181,7 +11182,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
         <v>130</v>
       </c>
@@ -11192,7 +11193,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>131</v>
       </c>
@@ -11203,7 +11204,7 @@
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
         <v>132</v>
       </c>
@@ -11214,7 +11215,7 @@
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="76" t="s">
         <v>133</v>
       </c>
@@ -11225,7 +11226,7 @@
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="76" t="s">
         <v>134</v>
       </c>
@@ -11236,7 +11237,7 @@
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="76" t="s">
         <v>135</v>
       </c>
@@ -11247,7 +11248,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -11258,7 +11259,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="76" t="s">
         <v>137</v>
       </c>
@@ -11269,7 +11270,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="76" t="s">
         <v>138</v>
       </c>
@@ -11280,7 +11281,7 @@
         <v>755.86244135709444</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="76" t="s">
         <v>139</v>
       </c>
@@ -11291,7 +11292,7 @@
         <v>762.55920427134606</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="76" t="s">
         <v>140</v>
       </c>
@@ -11302,7 +11303,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="76" t="s">
         <v>141</v>
       </c>
@@ -11313,7 +11314,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="76" t="s">
         <v>142</v>
       </c>
@@ -11324,7 +11325,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
         <v>1</v>
       </c>
@@ -11335,7 +11336,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>143</v>
       </c>
@@ -11346,7 +11347,7 @@
         <v>725.15243391008278</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>144</v>
       </c>
@@ -11357,7 +11358,7 @@
         <v>748.62596861099109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -11368,7 +11369,7 @@
         <v>801.99999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -11379,7 +11380,7 @@
         <v>791.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>147</v>
       </c>
@@ -11390,7 +11391,7 @@
         <v>700.32025584540236</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -11401,7 +11402,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>149</v>
       </c>
@@ -11412,7 +11413,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -11423,7 +11424,7 @@
         <v>794.1013538556316</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>151</v>
       </c>
@@ -11434,7 +11435,7 @@
         <v>789.34625592835232</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>152</v>
       </c>
@@ -11445,7 +11446,7 @@
         <v>809.68750817282455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>153</v>
       </c>
@@ -11456,7 +11457,7 @@
         <v>783.00612535864673</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>154</v>
       </c>
@@ -11467,7 +11468,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>155</v>
       </c>
@@ -11478,7 +11479,7 @@
         <v>508.00296189766453</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>156</v>
       </c>
@@ -11489,7 +11490,7 @@
         <v>428.22298556220187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>157</v>
       </c>
@@ -11500,7 +11501,7 @@
         <v>665.18536560495022</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>158</v>
       </c>
@@ -11511,7 +11512,7 @@
         <v>859.88020851632757</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>159</v>
       </c>
@@ -11522,7 +11523,7 @@
         <v>887.88245186586084</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>160</v>
       </c>
@@ -11533,7 +11534,7 @@
         <v>797.00724703341325</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -11544,7 +11545,7 @@
         <v>748.92792354647884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>162</v>
       </c>
@@ -11555,7 +11556,7 @@
         <v>778.77937164550963</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>163</v>
       </c>
@@ -11566,7 +11567,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>164</v>
       </c>
@@ -11577,18 +11578,18 @@
         <v>798.04417121416941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>243</v>
       </c>
-      <c r="B42">
-        <v>43.400833892223638</v>
+      <c r="B42" s="76">
+        <v>43.995102738357922</v>
       </c>
       <c r="C42">
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -11599,7 +11600,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>166</v>
       </c>
@@ -11610,7 +11611,7 @@
         <v>716.69892648380858</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>167</v>
       </c>
@@ -11621,7 +11622,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -11632,7 +11633,7 @@
         <v>756.99999999999989</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -11643,7 +11644,7 @@
         <v>70.798124695046326</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -11654,7 +11655,7 @@
         <v>742.58779297677324</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -11665,7 +11666,7 @@
         <v>742.32362086970215</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>172</v>
       </c>
@@ -11676,7 +11677,7 @@
         <v>769.53334789802227</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>173</v>
       </c>
@@ -11687,7 +11688,7 @@
         <v>584.61287294827434</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>174</v>
       </c>
@@ -11698,7 +11699,7 @@
         <v>559.51652277652283</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>175</v>
       </c>
@@ -11709,7 +11710,7 @@
         <v>595.17975723111715</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>176</v>
       </c>
@@ -11720,7 +11721,7 @@
         <v>507.21044557645126</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>177</v>
       </c>
@@ -11731,7 +11732,7 @@
         <v>668.88377510394514</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>178</v>
       </c>
@@ -11742,7 +11743,7 @@
         <v>654.80340179705718</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>179</v>
       </c>
@@ -11753,7 +11754,7 @@
         <v>688.85095964480468</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>180</v>
       </c>
@@ -11764,7 +11765,7 @@
         <v>737.59071339941693</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>181</v>
       </c>
@@ -11775,7 +11776,7 @@
         <v>765.47381512866104</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -11786,7 +11787,7 @@
         <v>731.67589538225809</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>183</v>
       </c>
@@ -11797,7 +11798,7 @@
         <v>800.00032424653136</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>184</v>
       </c>
@@ -11808,7 +11809,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>188</v>
       </c>
@@ -11819,7 +11820,7 @@
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>189</v>
       </c>
@@ -11830,7 +11831,7 @@
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="75" t="s">
         <v>89</v>
       </c>
@@ -11841,7 +11842,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>190</v>
       </c>
@@ -11852,7 +11853,7 @@
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -11863,7 +11864,7 @@
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>192</v>
       </c>
@@ -11871,7 +11872,7 @@
         <v>22.648458746153963</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -11879,7 +11880,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>194</v>
       </c>
@@ -11887,7 +11888,7 @@
         <v>18.707371337693861</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -11895,7 +11896,7 @@
         <v>12.566427590816895</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>196</v>
       </c>
@@ -11903,7 +11904,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>197</v>
       </c>
@@ -11911,7 +11912,7 @@
         <v>11.566786665057547</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -11919,7 +11920,7 @@
         <v>31.342185540824094</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>199</v>
       </c>
@@ -11927,7 +11928,7 @@
         <v>31.0106439692332</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>200</v>
       </c>
@@ -11935,7 +11936,7 @@
         <v>28.609127685562171</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -11943,7 +11944,7 @@
         <v>33.012627597074328</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>202</v>
       </c>
@@ -11951,7 +11952,7 @@
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>203</v>
       </c>
@@ -11959,7 +11960,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -11967,7 +11968,7 @@
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -11975,7 +11976,7 @@
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -11983,7 +11984,7 @@
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -11991,7 +11992,7 @@
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>208</v>
       </c>
@@ -11999,7 +12000,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>209</v>
       </c>
@@ -12007,7 +12008,7 @@
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -12015,7 +12016,7 @@
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>211</v>
       </c>
@@ -12023,7 +12024,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>212</v>
       </c>
@@ -12031,7 +12032,7 @@
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>213</v>
       </c>
@@ -12039,7 +12040,7 @@
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -12047,7 +12048,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -12055,7 +12056,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>216</v>
       </c>
@@ -12063,7 +12064,7 @@
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -12071,7 +12072,7 @@
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="75" t="s">
         <v>220</v>
       </c>
@@ -12079,7 +12080,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
1. Corrected the way of incorporating RD distribution loss factor; 2. Added energy use and water consumption for the end use table; 3. The results of the biochem and sludge HTL pathways are verified
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5110E05B-6322-4CE0-96C6-53F810537B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF6C703-666E-44A0-8ABA-4D58EAD13099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="MT2T">[2]Fuel_Specs!$D$175</definedName>
     <definedName name="t2g">Other!$B$8</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="334">
   <si>
     <t>NG</t>
   </si>
@@ -1870,6 +1870,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1879,8 +1881,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2580,16 +2580,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="25.08984375" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1796875" style="142"/>
+    <col min="28" max="28" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="26.5" x14ac:dyDescent="0.35">
@@ -2837,1006 +2839,1504 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1.1729999780654907</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.2010000000000001</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2.0270000000000001</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.25800000000000001</v>
-      </c>
-      <c r="F4" s="4">
-        <v>41.5</v>
-      </c>
-      <c r="G4" s="142">
-        <v>5.8123534639999992</v>
-      </c>
-      <c r="H4" s="142">
-        <v>7.3235653640000002</v>
-      </c>
-      <c r="I4" s="142">
-        <v>41.750349867302674</v>
-      </c>
-      <c r="J4" s="71">
-        <v>2.54</v>
-      </c>
-      <c r="K4" s="71">
-        <v>2.54</v>
-      </c>
-      <c r="L4" s="71">
-        <v>1.056</v>
-      </c>
-      <c r="M4" s="71">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="N4" s="71">
-        <v>1.056</v>
-      </c>
-      <c r="O4" s="71">
-        <v>130.05799999999999</v>
-      </c>
-      <c r="P4" s="71">
-        <v>2.5</v>
-      </c>
-      <c r="Q4" s="72">
-        <v>100</v>
-      </c>
-      <c r="R4" s="73">
-        <v>2.54</v>
-      </c>
-      <c r="S4" s="73">
-        <v>0.69343623523370912</v>
-      </c>
-      <c r="T4" s="73">
-        <v>0</v>
-      </c>
-      <c r="U4" s="73"/>
-      <c r="X4">
-        <v>53.597474630288403</v>
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="R4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="S4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="T4" s="70"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="134"/>
+      <c r="W4" s="134"/>
+      <c r="X4" s="3">
+        <v>1000000</v>
       </c>
       <c r="Y4">
-        <v>0.12380376798091507</v>
+        <v>9216.8702699702171</v>
       </c>
       <c r="Z4">
         <f>X4+Y4</f>
-        <v>53.72127839826932</v>
-      </c>
-      <c r="AA4">
-        <v>40.352647182660228</v>
+        <v>1009216.8702699703</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1000000</v>
       </c>
       <c r="AB4">
-        <v>1.4111608204643369E-2</v>
+        <v>1250.309002469897</v>
       </c>
       <c r="AC4">
         <f>AA4+AB4</f>
-        <v>40.366758790864871</v>
+        <v>1001250.3090024699</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="4">
-        <v>16.686000823974609</v>
-      </c>
-      <c r="C5" s="4">
-        <v>25.114999999999998</v>
-      </c>
-      <c r="D5" s="4">
-        <v>526.19200000000001</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1.56</v>
-      </c>
-      <c r="F5" s="4">
-        <v>200.11</v>
-      </c>
-      <c r="G5" s="142">
-        <v>161.77639492999998</v>
-      </c>
-      <c r="H5" s="142">
-        <v>203.83825762999999</v>
-      </c>
-      <c r="I5" s="142">
-        <v>993.80073264760836</v>
-      </c>
-      <c r="J5" s="71">
-        <v>22.21</v>
-      </c>
-      <c r="K5" s="71">
-        <v>24.97</v>
-      </c>
-      <c r="L5" s="71">
-        <v>41.286000000000001</v>
-      </c>
-      <c r="M5" s="71">
-        <v>14.532999999999999</v>
-      </c>
-      <c r="N5" s="71">
-        <v>41.286000000000001</v>
-      </c>
-      <c r="O5" s="71">
-        <v>660.91099999999994</v>
-      </c>
-      <c r="P5" s="71">
-        <v>26</v>
-      </c>
-      <c r="Q5" s="72">
-        <v>50</v>
-      </c>
-      <c r="R5" s="73">
-        <v>22.21</v>
-      </c>
-      <c r="S5" s="73">
-        <v>0.90633720079240732</v>
-      </c>
-      <c r="T5" s="73">
-        <v>0</v>
-      </c>
-      <c r="U5" s="73"/>
-      <c r="X5">
-        <v>639.10415070792988</v>
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="R5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="S5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="134"/>
+      <c r="W5" s="134"/>
+      <c r="X5" s="3">
+        <v>0</v>
       </c>
       <c r="Y5">
-        <v>0.53001711985689259</v>
+        <v>8027.464959570797</v>
       </c>
       <c r="Z5">
-        <f t="shared" ref="Z5:Z15" si="0">X5+Y5</f>
-        <v>639.63416782778677</v>
-      </c>
-      <c r="AA5">
-        <v>993.80073264760836</v>
+        <f>X5+Y5</f>
+        <v>8027.464959570797</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
       </c>
       <c r="AB5">
-        <v>0.19579254162294349</v>
+        <v>1199.1725344773329</v>
       </c>
       <c r="AC5">
-        <f t="shared" ref="AC5:AC15" si="1">AA5+AB5</f>
-        <v>993.99652518923131</v>
+        <f t="shared" ref="AC5:AC9" si="0">AA5+AB5</f>
+        <v>1199.1725344773329</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4">
-        <v>82.224998474121094</v>
-      </c>
-      <c r="C6" s="4">
-        <v>66.543000000000006</v>
-      </c>
-      <c r="D6" s="4">
-        <v>267.89</v>
-      </c>
-      <c r="E6" s="4">
-        <v>256.41199999999998</v>
-      </c>
-      <c r="F6" s="4">
-        <v>434.31</v>
-      </c>
-      <c r="G6" s="142">
-        <v>101.53518337</v>
-      </c>
-      <c r="H6" s="142">
-        <v>127.93433107000001</v>
-      </c>
-      <c r="I6" s="142">
-        <v>27.387619255967515</v>
-      </c>
-      <c r="J6" s="71">
-        <v>36.4</v>
-      </c>
-      <c r="K6" s="71">
-        <v>41.05</v>
-      </c>
-      <c r="L6" s="71">
-        <v>31.969000000000001</v>
-      </c>
-      <c r="M6" s="71">
-        <v>17.425000000000001</v>
-      </c>
-      <c r="N6" s="71">
-        <v>31.969000000000001</v>
-      </c>
-      <c r="O6" s="71">
-        <v>752.81600000000003</v>
-      </c>
-      <c r="P6" s="71">
-        <v>48.900001525878899</v>
-      </c>
-      <c r="Q6" s="72">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="70"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="134"/>
+      <c r="X6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>1664.7217341019561</v>
+      </c>
+      <c r="Z6">
+        <f>X6+Y6</f>
+        <v>1664.7217341019561</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>8.0912620107395146</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="0"/>
+        <v>8.0912620107395146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="R7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="S7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="T7" s="70"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="134"/>
+      <c r="W7" s="134"/>
+      <c r="X7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>2963.4305044075732</v>
+      </c>
+      <c r="Z7">
+        <f>X7+Y7</f>
+        <v>2963.4305044075732</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>124.60248498831356</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="0"/>
+        <v>124.60248498831356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="70"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="134"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>3399.3127210612679</v>
+      </c>
+      <c r="Z8">
+        <f>X8+Y8</f>
+        <v>3399.3127210612679</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>1066.4787874782799</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="0"/>
+        <v>1066.4787874782799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="134"/>
+      <c r="W9" s="134"/>
+      <c r="X9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0.56134131706501467</v>
+      </c>
+      <c r="Z9">
+        <f>X9+Y9</f>
+        <v>0.56134131706501467</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>2.3217600680931635E-2</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="0"/>
+        <v>2.3217600680931635E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1.1729999780654907</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="F10" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="G10" s="142">
+        <v>5.8123534639999992</v>
+      </c>
+      <c r="H10" s="142">
+        <v>7.3235653640000002</v>
+      </c>
+      <c r="I10" s="142">
+        <v>41.750349867302674</v>
+      </c>
+      <c r="J10" s="71">
+        <v>2.54</v>
+      </c>
+      <c r="K10" s="71">
+        <v>2.54</v>
+      </c>
+      <c r="L10" s="71">
+        <v>1.056</v>
+      </c>
+      <c r="M10" s="71">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="N10" s="71">
+        <v>1.056</v>
+      </c>
+      <c r="O10" s="71">
+        <v>130.05799999999999</v>
+      </c>
+      <c r="P10" s="71">
+        <v>2.5</v>
+      </c>
+      <c r="Q10" s="72">
         <v>100</v>
       </c>
-      <c r="R6" s="73">
-        <v>13.296832</v>
-      </c>
-      <c r="S6" s="73">
-        <v>1.1820623069568268</v>
-      </c>
-      <c r="T6" s="73">
-        <v>0</v>
-      </c>
-      <c r="U6" s="73"/>
-      <c r="X6">
-        <v>19.208734314891956</v>
-      </c>
-      <c r="Y6">
-        <v>1.4390708093838975</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="0"/>
-        <v>20.647805124275852</v>
-      </c>
-      <c r="AA6">
-        <v>27.387619255967515</v>
-      </c>
-      <c r="AB6">
-        <v>0.13356807901983217</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" si="1"/>
-        <v>27.521187334987346</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4">
-        <v>6.4169999999999998</v>
-      </c>
-      <c r="C7" s="4">
-        <v>8.4039999999999999</v>
-      </c>
-      <c r="D7" s="4">
-        <v>22.539000000000001</v>
-      </c>
-      <c r="E7" s="4">
-        <v>25.943999999999999</v>
-      </c>
-      <c r="F7" s="4">
-        <v>29.83</v>
-      </c>
-      <c r="G7" s="142">
-        <v>5.4409986930000001</v>
-      </c>
-      <c r="H7" s="142">
-        <v>6.8556583530000008</v>
-      </c>
-      <c r="I7" s="142">
-        <v>9.458769751780995</v>
-      </c>
-      <c r="J7" s="71">
-        <v>3.5070000000000001</v>
-      </c>
-      <c r="K7" s="71">
-        <v>3.5070000000000001</v>
-      </c>
-      <c r="L7" s="71">
-        <v>3.5750000000000002</v>
-      </c>
-      <c r="M7" s="71">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="N7" s="71">
-        <v>3.5750000000000002</v>
-      </c>
-      <c r="O7" s="71">
-        <v>7.1970000000000001</v>
-      </c>
-      <c r="P7" s="71">
-        <v>3.7000000476837154</v>
-      </c>
-      <c r="Q7" s="72">
-        <v>90</v>
-      </c>
-      <c r="R7" s="73">
-        <v>3.2150660000000002</v>
-      </c>
-      <c r="S7" s="73">
-        <v>0.86769042919929373</v>
-      </c>
-      <c r="T7" s="73">
-        <v>0</v>
-      </c>
-      <c r="U7" s="73"/>
-      <c r="X7">
-        <v>8.0441472410106218</v>
-      </c>
-      <c r="Y7">
-        <v>6.8025222126898502E-2</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="0"/>
-        <v>8.1121724631375205</v>
-      </c>
-      <c r="AA7">
-        <v>9.458769751780995</v>
-      </c>
-      <c r="AB7">
-        <v>7.5116168079741932E-3</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="1"/>
-        <v>9.4662813685889695</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4">
-        <v>5.03</v>
-      </c>
-      <c r="C8" s="4">
-        <v>7.5220000000000002</v>
-      </c>
-      <c r="D8" s="4">
-        <v>22.3</v>
-      </c>
-      <c r="E8" s="4">
-        <v>6.5739999999999998</v>
-      </c>
-      <c r="F8" s="4">
-        <v>28.935099999999998</v>
-      </c>
-      <c r="G8" s="142">
-        <v>0.9282486969999999</v>
-      </c>
-      <c r="H8" s="142">
-        <v>1.1695933580000002</v>
-      </c>
-      <c r="I8" s="142">
-        <v>1.8922698715311803</v>
-      </c>
-      <c r="J8" s="71">
-        <v>3.5070000000000001</v>
-      </c>
-      <c r="K8" s="71">
-        <v>3.5070000000000001</v>
-      </c>
-      <c r="L8" s="71">
-        <v>3.5750000000000002</v>
-      </c>
-      <c r="M8" s="71">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="N8" s="71">
-        <v>3.5750000000000002</v>
-      </c>
-      <c r="O8" s="71">
-        <v>7.1970000000000001</v>
-      </c>
-      <c r="P8" s="71">
-        <v>3.7000000476837154</v>
-      </c>
-      <c r="Q8" s="72">
-        <v>90</v>
-      </c>
-      <c r="R8" s="73">
-        <v>3.2150660000000002</v>
-      </c>
-      <c r="S8" s="73">
-        <v>0.83613317023827116</v>
-      </c>
-      <c r="T8" s="73">
-        <v>0</v>
-      </c>
-      <c r="U8" s="73"/>
-      <c r="X8">
-        <v>1.728649515788488</v>
-      </c>
-      <c r="Y8">
-        <v>4.6442748659862865E-2</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="0"/>
-        <v>1.7750922644483509</v>
-      </c>
-      <c r="AA8">
-        <v>1.8922698715311803</v>
-      </c>
-      <c r="AB8">
-        <v>2.1809956805283149E-3</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="1"/>
-        <v>1.8944508672117086</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.54242117555469049</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.54242117555469049</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.54242117555469049</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.54242117555469049</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.54242117555469049</v>
-      </c>
-      <c r="G9" s="142">
-        <v>0.54469976400000064</v>
-      </c>
-      <c r="H9" s="142">
-        <v>0.54469976400000064</v>
-      </c>
-      <c r="I9" s="142">
-        <v>0.54469976387990116</v>
-      </c>
-      <c r="J9" s="71">
-        <v>0.26856561546286878</v>
-      </c>
-      <c r="K9" s="71">
-        <v>0.26856561546286878</v>
-      </c>
-      <c r="L9" s="71">
-        <v>0.26856561546286878</v>
-      </c>
-      <c r="M9" s="71">
-        <v>0.26856561546286878</v>
-      </c>
-      <c r="N9" s="71">
-        <v>0.26856561546286878</v>
-      </c>
-      <c r="O9" s="71">
-        <v>0.26856561546286878</v>
-      </c>
-      <c r="P9" s="71">
-        <v>0.26856561546286878</v>
-      </c>
-      <c r="Q9" s="72">
-        <v>30</v>
-      </c>
-      <c r="R9" s="73">
-        <v>0.32149299999999997</v>
-      </c>
-      <c r="S9" s="73">
-        <v>1.9503787502411295E-2</v>
-      </c>
-      <c r="T9" s="73">
-        <v>0</v>
-      </c>
-      <c r="U9" s="73"/>
-      <c r="X9">
-        <v>0.47886752155609885</v>
-      </c>
-      <c r="Y9">
-        <v>0.22128373782612412</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="0"/>
-        <v>0.700151259382223</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <v>5.3987418408876558E-3</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="1"/>
-        <v>5.3987418408876558E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.503</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.75219999999999998</v>
-      </c>
-      <c r="D10" s="4">
-        <v>18.129899999999999</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="F10" s="4">
-        <v>16.290461299999997</v>
-      </c>
-      <c r="G10" s="142">
-        <v>3.1580813000000013E-2</v>
-      </c>
-      <c r="H10" s="142">
-        <v>3.9791824000000003E-2</v>
-      </c>
-      <c r="I10" s="142">
-        <v>0.51210428280035414</v>
-      </c>
-      <c r="J10" s="71">
-        <v>0.57865500000000003</v>
-      </c>
-      <c r="K10" s="71">
-        <v>0.57865500000000003</v>
-      </c>
-      <c r="L10" s="71">
-        <v>0.103675</v>
-      </c>
-      <c r="M10" s="71">
-        <v>3.8569999999999998E-3</v>
-      </c>
-      <c r="N10" s="71">
-        <v>0.103675</v>
-      </c>
-      <c r="O10" s="71">
-        <v>1.4394</v>
-      </c>
-      <c r="P10" s="71">
-        <v>3.5150000452995296</v>
-      </c>
-      <c r="Q10" s="71">
-        <v>14.85</v>
-      </c>
       <c r="R10" s="73">
-        <v>0.53048589000000002</v>
-      </c>
-      <c r="S10" s="73"/>
+        <v>2.54</v>
+      </c>
+      <c r="S10" s="73">
+        <v>0.69343623523370912</v>
+      </c>
       <c r="T10" s="73">
         <v>0</v>
       </c>
       <c r="U10" s="73"/>
       <c r="X10">
-        <v>0.47390947465623479</v>
+        <v>53.597474630288403</v>
       </c>
       <c r="Y10">
-        <v>4.2404984619842561E-3</v>
+        <v>0.12380376798091507</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="0"/>
-        <v>0.47814997311821905</v>
+        <f>X10+Y10</f>
+        <v>53.72127839826932</v>
       </c>
       <c r="AA10">
-        <v>0.51210428280035414</v>
+        <v>40.352647182660228</v>
       </c>
       <c r="AB10">
-        <v>2.0959176112987082E-4</v>
+        <v>1.4111608204643369E-2</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="1"/>
-        <v>0.51231387456148403</v>
+        <f>AA10+AB10</f>
+        <v>40.366758790864871</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>28</v>
+      <c r="A11" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="B11" s="4">
-        <v>1.2575000000000001</v>
+        <v>16.686000823974609</v>
       </c>
       <c r="C11" s="4">
-        <v>1.8805000000000001</v>
+        <v>25.114999999999998</v>
       </c>
       <c r="D11" s="4">
-        <v>4.0363000000000007</v>
+        <v>526.19200000000001</v>
       </c>
       <c r="E11" s="4">
-        <v>1.6435</v>
+        <v>1.56</v>
       </c>
       <c r="F11" s="4">
-        <v>10.098349899999999</v>
+        <v>200.11</v>
       </c>
       <c r="G11" s="142">
-        <v>5.8681168000000006E-2</v>
+        <v>161.77639492999998</v>
       </c>
       <c r="H11" s="142">
-        <v>7.3938271E-2</v>
+        <v>203.83825762999999</v>
       </c>
       <c r="I11" s="142">
-        <v>7.6630038890183744E-2</v>
+        <v>993.80073264760836</v>
       </c>
       <c r="J11" s="71">
-        <v>1.5009959999999998</v>
+        <v>22.21</v>
       </c>
       <c r="K11" s="71">
-        <v>1.5009959999999998</v>
+        <v>24.97</v>
       </c>
       <c r="L11" s="71">
-        <v>2.431</v>
+        <v>41.286000000000001</v>
       </c>
       <c r="M11" s="71">
-        <v>9.0440000000000006E-2</v>
+        <v>14.532999999999999</v>
       </c>
       <c r="N11" s="71">
-        <v>2.431</v>
+        <v>41.286000000000001</v>
       </c>
       <c r="O11" s="71">
-        <v>3.0803159999999998</v>
+        <v>660.91099999999994</v>
       </c>
       <c r="P11" s="71">
-        <v>0.18500000238418576</v>
-      </c>
-      <c r="Q11" s="71">
-        <v>38.519999999999996</v>
+        <v>26</v>
+      </c>
+      <c r="Q11" s="72">
+        <v>50</v>
       </c>
       <c r="R11" s="73">
-        <v>1.3760482479999998</v>
-      </c>
-      <c r="S11" s="73"/>
+        <v>22.21</v>
+      </c>
+      <c r="S11" s="73">
+        <v>0.90633720079240732</v>
+      </c>
       <c r="T11" s="73">
         <v>0</v>
       </c>
       <c r="U11" s="73"/>
       <c r="X11">
-        <v>0.24585827527712426</v>
+        <v>639.10415070792988</v>
       </c>
       <c r="Y11">
-        <v>2.0700811243651359E-2</v>
+        <v>0.53001711985689259</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="0"/>
-        <v>0.26655908652077559</v>
+        <f t="shared" ref="Z11:Z21" si="1">X11+Y11</f>
+        <v>639.63416782778677</v>
       </c>
       <c r="AA11">
-        <v>7.6630038890183744E-2</v>
+        <v>993.80073264760836</v>
       </c>
       <c r="AB11">
-        <v>3.7216049065244534E-4</v>
+        <v>0.19579254162294349</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="1"/>
-        <v>7.7002199380836189E-2</v>
+        <f t="shared" ref="AC11:AC21" si="2">AA11+AB11</f>
+        <v>993.99652518923131</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B12" s="4">
-        <v>0.18000000715255737</v>
+        <v>82.224998474121094</v>
       </c>
       <c r="C12" s="4">
-        <v>0.76300000000000001</v>
+        <v>66.543000000000006</v>
       </c>
       <c r="D12" s="4">
-        <v>4.2210000000000001</v>
+        <v>267.89</v>
       </c>
       <c r="E12" s="4">
-        <v>3.024</v>
+        <v>256.41199999999998</v>
       </c>
       <c r="F12" s="4">
-        <v>0.62999999523162842</v>
+        <v>434.31</v>
       </c>
       <c r="G12" s="142">
-        <v>0.79687950000000285</v>
+        <v>101.53518337</v>
       </c>
       <c r="H12" s="142">
-        <v>1.0040682000000061</v>
+        <v>127.93433107000001</v>
       </c>
       <c r="I12" s="142">
-        <v>0</v>
+        <v>27.387619255967515</v>
       </c>
       <c r="J12" s="71">
-        <v>1.06</v>
+        <v>36.4</v>
       </c>
       <c r="K12" s="71">
-        <v>1.06</v>
+        <v>41.05</v>
       </c>
       <c r="L12" s="71">
-        <v>1.056</v>
+        <v>31.969000000000001</v>
       </c>
       <c r="M12" s="71">
-        <v>1.1419999999999999</v>
+        <v>17.425000000000001</v>
       </c>
       <c r="N12" s="71">
-        <v>1.056</v>
+        <v>31.969000000000001</v>
       </c>
       <c r="O12" s="71">
-        <v>392.35399999999998</v>
+        <v>752.81600000000003</v>
       </c>
       <c r="P12" s="71">
-        <v>49</v>
+        <v>48.900001525878899</v>
       </c>
       <c r="Q12" s="72">
-        <v>2.85</v>
+        <v>100</v>
       </c>
       <c r="R12" s="73">
-        <v>1.06</v>
-      </c>
-      <c r="S12" s="73"/>
+        <v>13.296832</v>
+      </c>
+      <c r="S12" s="73">
+        <v>1.1820623069568268</v>
+      </c>
       <c r="T12" s="73">
         <v>0</v>
       </c>
       <c r="U12" s="73"/>
       <c r="X12">
-        <v>3.4141251927898666</v>
+        <v>19.208734314891956</v>
       </c>
       <c r="Y12">
-        <v>1.0718762615156343</v>
+        <v>1.4390708093838975</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="0"/>
-        <v>4.4860014543055007</v>
+        <f t="shared" si="1"/>
+        <v>20.647805124275852</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>27.387619255967515</v>
       </c>
       <c r="AB12">
-        <v>0.11248755052026857</v>
+        <v>0.13356807901983217</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="1"/>
-        <v>0.11248755052026857</v>
+        <f t="shared" si="2"/>
+        <v>27.521187334987346</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4">
-        <v>0.38999998569488525</v>
+        <v>6.4169999999999998</v>
       </c>
       <c r="C13" s="4">
-        <v>0.91800000000000004</v>
+        <v>8.4039999999999999</v>
       </c>
       <c r="D13" s="4">
-        <v>0.6</v>
+        <v>22.539000000000001</v>
       </c>
       <c r="E13" s="4">
-        <v>0.60299999999999998</v>
+        <v>25.943999999999999</v>
       </c>
       <c r="F13" s="4">
-        <v>0.92000001668930043</v>
+        <v>29.83</v>
       </c>
       <c r="G13" s="142">
-        <v>0.10695653399999999</v>
+        <v>5.4409986930000001</v>
       </c>
       <c r="H13" s="142">
-        <v>0.13476523299999998</v>
+        <v>6.8556583530000008</v>
       </c>
       <c r="I13" s="142">
-        <v>0.18877324129794976</v>
+        <v>9.458769751780995</v>
       </c>
       <c r="J13" s="71">
-        <v>0.75</v>
+        <v>3.5070000000000001</v>
       </c>
       <c r="K13" s="71">
-        <v>0.35</v>
+        <v>3.5070000000000001</v>
       </c>
       <c r="L13" s="71">
-        <v>0.10199999999999999</v>
+        <v>3.5750000000000002</v>
       </c>
       <c r="M13" s="71">
-        <v>0.11899999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="N13" s="71">
-        <v>0.10199999999999999</v>
+        <v>3.5750000000000002</v>
       </c>
       <c r="O13" s="71">
-        <v>0.111</v>
+        <v>7.1970000000000001</v>
       </c>
       <c r="P13" s="71">
-        <v>1.1000000238418579</v>
+        <v>3.7000000476837154</v>
       </c>
       <c r="Q13" s="72">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="R13" s="73">
-        <v>0.40123199999999998</v>
-      </c>
-      <c r="S13" s="73"/>
+        <v>3.2150660000000002</v>
+      </c>
+      <c r="S13" s="73">
+        <v>0.86769042919929373</v>
+      </c>
       <c r="T13" s="73">
         <v>0</v>
       </c>
       <c r="U13" s="73"/>
       <c r="X13">
-        <v>0.91142919415811929</v>
+        <v>8.0441472410106218</v>
       </c>
       <c r="Y13">
-        <v>1.1802078079887578E-2</v>
+        <v>6.8025222126898502E-2</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="0"/>
-        <v>0.92323127223800683</v>
+        <f t="shared" si="1"/>
+        <v>8.1121724631375205</v>
       </c>
       <c r="AA13">
-        <v>0.18877324129794976</v>
+        <v>9.458769751780995</v>
       </c>
       <c r="AB13">
-        <v>3.4778154884700514E-4</v>
+        <v>7.5116168079741932E-3</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="1"/>
-        <v>0.18912102284679677</v>
+        <f t="shared" si="2"/>
+        <v>9.4662813685889695</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4">
+        <v>5.03</v>
+      </c>
+      <c r="C14" s="4">
+        <v>7.5220000000000002</v>
+      </c>
+      <c r="D14" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6.5739999999999998</v>
+      </c>
+      <c r="F14" s="4">
+        <v>28.935099999999998</v>
+      </c>
+      <c r="G14" s="142">
+        <v>0.9282486969999999</v>
+      </c>
+      <c r="H14" s="142">
+        <v>1.1695933580000002</v>
+      </c>
+      <c r="I14" s="142">
+        <v>1.8922698715311803</v>
+      </c>
+      <c r="J14" s="71">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="K14" s="71">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="L14" s="71">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="M14" s="71">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="N14" s="71">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="O14" s="71">
+        <v>7.1970000000000001</v>
+      </c>
+      <c r="P14" s="71">
+        <v>3.7000000476837154</v>
+      </c>
+      <c r="Q14" s="72">
+        <v>90</v>
+      </c>
+      <c r="R14" s="73">
+        <v>3.2150660000000002</v>
+      </c>
+      <c r="S14" s="73">
+        <v>0.83613317023827116</v>
+      </c>
+      <c r="T14" s="73">
+        <v>0</v>
+      </c>
+      <c r="U14" s="73"/>
+      <c r="X14">
+        <v>1.728649515788488</v>
+      </c>
+      <c r="Y14">
+        <v>4.6442748659862865E-2</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="1"/>
+        <v>1.7750922644483509</v>
+      </c>
+      <c r="AA14">
+        <v>1.8922698715311803</v>
+      </c>
+      <c r="AB14">
+        <v>2.1809956805283149E-3</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="2"/>
+        <v>1.8944508672117086</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.54242117555469049</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.54242117555469049</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.54242117555469049</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.54242117555469049</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.54242117555469049</v>
+      </c>
+      <c r="G15" s="142">
+        <v>0.54469976400000064</v>
+      </c>
+      <c r="H15" s="142">
+        <v>0.54469976400000064</v>
+      </c>
+      <c r="I15" s="142">
+        <v>0.54469976387990116</v>
+      </c>
+      <c r="J15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="K15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="L15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="M15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="N15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="O15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="P15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="Q15" s="72">
+        <v>30</v>
+      </c>
+      <c r="R15" s="73">
+        <v>0.32149299999999997</v>
+      </c>
+      <c r="S15" s="73">
+        <v>1.9503787502411295E-2</v>
+      </c>
+      <c r="T15" s="73">
+        <v>0</v>
+      </c>
+      <c r="U15" s="73"/>
+      <c r="X15">
+        <v>0.47886752155609885</v>
+      </c>
+      <c r="Y15">
+        <v>0.22128373782612412</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="1"/>
+        <v>0.700151259382223</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>5.3987418408876558E-3</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="2"/>
+        <v>5.3987418408876558E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.503</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.75219999999999998</v>
+      </c>
+      <c r="D16" s="4">
+        <v>18.129899999999999</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.65739999999999998</v>
+      </c>
+      <c r="F16" s="4">
+        <v>16.290461299999997</v>
+      </c>
+      <c r="G16" s="142">
+        <v>3.1580813000000013E-2</v>
+      </c>
+      <c r="H16" s="142">
+        <v>3.9791824000000003E-2</v>
+      </c>
+      <c r="I16" s="142">
+        <v>0.51210428280035414</v>
+      </c>
+      <c r="J16" s="71">
+        <v>0.57865500000000003</v>
+      </c>
+      <c r="K16" s="71">
+        <v>0.57865500000000003</v>
+      </c>
+      <c r="L16" s="71">
+        <v>0.103675</v>
+      </c>
+      <c r="M16" s="71">
+        <v>3.8569999999999998E-3</v>
+      </c>
+      <c r="N16" s="71">
+        <v>0.103675</v>
+      </c>
+      <c r="O16" s="71">
+        <v>1.4394</v>
+      </c>
+      <c r="P16" s="71">
+        <v>3.5150000452995296</v>
+      </c>
+      <c r="Q16" s="71">
+        <v>14.85</v>
+      </c>
+      <c r="R16" s="73">
+        <v>0.53048589000000002</v>
+      </c>
+      <c r="S16" s="73"/>
+      <c r="T16" s="73">
+        <v>0</v>
+      </c>
+      <c r="U16" s="73"/>
+      <c r="X16">
+        <v>0.47390947465623479</v>
+      </c>
+      <c r="Y16">
+        <v>4.2404984619842561E-3</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="1"/>
+        <v>0.47814997311821905</v>
+      </c>
+      <c r="AA16">
+        <v>0.51210428280035414</v>
+      </c>
+      <c r="AB16">
+        <v>2.0959176112987082E-4</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="2"/>
+        <v>0.51231387456148403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1.2575000000000001</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.8805000000000001</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4.0363000000000007</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.6435</v>
+      </c>
+      <c r="F17" s="4">
+        <v>10.098349899999999</v>
+      </c>
+      <c r="G17" s="142">
+        <v>5.8681168000000006E-2</v>
+      </c>
+      <c r="H17" s="142">
+        <v>7.3938271E-2</v>
+      </c>
+      <c r="I17" s="142">
+        <v>7.6630038890183744E-2</v>
+      </c>
+      <c r="J17" s="71">
+        <v>1.5009959999999998</v>
+      </c>
+      <c r="K17" s="71">
+        <v>1.5009959999999998</v>
+      </c>
+      <c r="L17" s="71">
+        <v>2.431</v>
+      </c>
+      <c r="M17" s="71">
+        <v>9.0440000000000006E-2</v>
+      </c>
+      <c r="N17" s="71">
+        <v>2.431</v>
+      </c>
+      <c r="O17" s="71">
+        <v>3.0803159999999998</v>
+      </c>
+      <c r="P17" s="71">
+        <v>0.18500000238418576</v>
+      </c>
+      <c r="Q17" s="71">
+        <v>38.519999999999996</v>
+      </c>
+      <c r="R17" s="73">
+        <v>1.3760482479999998</v>
+      </c>
+      <c r="S17" s="73"/>
+      <c r="T17" s="73">
+        <v>0</v>
+      </c>
+      <c r="U17" s="73"/>
+      <c r="X17">
+        <v>0.24585827527712426</v>
+      </c>
+      <c r="Y17">
+        <v>2.0700811243651359E-2</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="1"/>
+        <v>0.26655908652077559</v>
+      </c>
+      <c r="AA17">
+        <v>7.6630038890183744E-2</v>
+      </c>
+      <c r="AB17">
+        <v>3.7216049065244534E-4</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="2"/>
+        <v>7.7002199380836189E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.18000000715255737</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="D18" s="4">
+        <v>4.2210000000000001</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3.024</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.62999999523162842</v>
+      </c>
+      <c r="G18" s="142">
+        <v>0.79687950000000285</v>
+      </c>
+      <c r="H18" s="142">
+        <v>1.0040682000000061</v>
+      </c>
+      <c r="I18" s="142">
+        <v>0</v>
+      </c>
+      <c r="J18" s="71">
+        <v>1.06</v>
+      </c>
+      <c r="K18" s="71">
+        <v>1.06</v>
+      </c>
+      <c r="L18" s="71">
+        <v>1.056</v>
+      </c>
+      <c r="M18" s="71">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="N18" s="71">
+        <v>1.056</v>
+      </c>
+      <c r="O18" s="71">
+        <v>392.35399999999998</v>
+      </c>
+      <c r="P18" s="71">
+        <v>49</v>
+      </c>
+      <c r="Q18" s="72">
+        <v>2.85</v>
+      </c>
+      <c r="R18" s="73">
+        <v>1.06</v>
+      </c>
+      <c r="S18" s="73"/>
+      <c r="T18" s="73">
+        <v>0</v>
+      </c>
+      <c r="U18" s="73"/>
+      <c r="X18">
+        <v>3.4141251927898666</v>
+      </c>
+      <c r="Y18">
+        <v>1.0718762615156343</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="1"/>
+        <v>4.4860014543055007</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0.11248755052026857</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="2"/>
+        <v>0.11248755052026857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.38999998569488525</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.92000001668930043</v>
+      </c>
+      <c r="G19" s="142">
+        <v>0.10695653399999999</v>
+      </c>
+      <c r="H19" s="142">
+        <v>0.13476523299999998</v>
+      </c>
+      <c r="I19" s="142">
+        <v>0.18877324129794976</v>
+      </c>
+      <c r="J19" s="71">
+        <v>0.75</v>
+      </c>
+      <c r="K19" s="71">
+        <v>0.35</v>
+      </c>
+      <c r="L19" s="71">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="M19" s="71">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="N19" s="71">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="O19" s="71">
+        <v>0.111</v>
+      </c>
+      <c r="P19" s="71">
+        <v>1.1000000238418579</v>
+      </c>
+      <c r="Q19" s="72">
+        <v>0</v>
+      </c>
+      <c r="R19" s="73">
+        <v>0.40123199999999998</v>
+      </c>
+      <c r="S19" s="73"/>
+      <c r="T19" s="73">
+        <v>0</v>
+      </c>
+      <c r="U19" s="73"/>
+      <c r="X19">
+        <v>0.91142919415811929</v>
+      </c>
+      <c r="Y19">
+        <v>1.1802078079887578E-2</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="1"/>
+        <v>0.92323127223800683</v>
+      </c>
+      <c r="AA19">
+        <v>0.18877324129794976</v>
+      </c>
+      <c r="AB19">
+        <v>3.4778154884700514E-4</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" si="2"/>
+        <v>0.18912102284679677</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B20" s="2">
         <v>78168.681100745569</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C20" s="2">
         <v>78153.745013896463</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D20" s="2">
         <v>77354.254432944086</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E20" s="2">
         <v>78187.481280563123</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F20" s="5">
         <v>77753.520071052437</v>
       </c>
-      <c r="G14" s="142">
+      <c r="G20" s="142">
         <v>77924.526169999997</v>
       </c>
-      <c r="H14" s="142">
+      <c r="H20" s="142">
         <v>77853.149250000002</v>
       </c>
-      <c r="I14" s="142">
+      <c r="I20" s="142">
         <v>77380.440267223457</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J20" s="5">
         <v>59366.949503269869</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K20" s="5">
         <v>59362.612360412735</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L20" s="5">
         <v>59341.609065174642</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M20" s="5">
         <v>59385.872043746065</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N20" s="2">
         <v>59341.609065174642</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O20" s="5">
         <v>56889.786903269873</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P20" s="5">
         <v>59229.283455650831</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="Q20" s="5">
         <v>59014.60666993654</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R20" s="2">
         <v>59366.949503269869</v>
       </c>
-      <c r="S14" s="149">
+      <c r="S20" s="146">
         <v>59412.682265174597</v>
       </c>
-      <c r="T14" s="122">
+      <c r="T20" s="122">
         <f>12/106*44/12</f>
         <v>0.41509433962264147</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U20" s="2">
         <f>12*7/(12*7+8*1)*44/12</f>
         <v>3.3478260869565215</v>
       </c>
-      <c r="V14">
+      <c r="V20">
         <f>-12*6/(12*6+10*1+4*16)*44/12</f>
         <v>-1.8082191780821917</v>
       </c>
-      <c r="W14" s="144">
+      <c r="W20" s="144">
         <f>-12*6/(12*6+8*1+5*16)*44/12</f>
         <v>-1.6500000000000001</v>
       </c>
-      <c r="X14">
+      <c r="X20">
         <v>71783.505317547926</v>
       </c>
-      <c r="Y14">
+      <c r="Y20">
         <v>611.91676387079497</v>
       </c>
-      <c r="Z14">
-        <f t="shared" si="0"/>
+      <c r="Z20">
+        <f t="shared" si="1"/>
         <v>72395.422081418714</v>
       </c>
-      <c r="AA14">
+      <c r="AA20">
         <v>74927.07400875607</v>
       </c>
-      <c r="AB14">
+      <c r="AB20">
         <v>92.564589004961775</v>
       </c>
-      <c r="AC14">
+      <c r="AC20">
+        <f t="shared" si="2"/>
+        <v>75019.638597761033</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="142">
+        <v>0</v>
+      </c>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="69"/>
+      <c r="Q21" s="69"/>
+      <c r="R21" s="69"/>
+      <c r="S21" s="69"/>
+      <c r="X21">
+        <v>-72964.246146966863</v>
+      </c>
+      <c r="Z21">
         <f t="shared" si="1"/>
-        <v>75019.638597761033</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="142">
-        <v>0</v>
-      </c>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="69"/>
-      <c r="X15">
         <v>-72964.246146966863</v>
       </c>
-      <c r="Z15">
-        <f t="shared" si="0"/>
-        <v>-72964.246146966863</v>
-      </c>
-      <c r="AA15">
+      <c r="AA21">
         <v>-76614.526624731123</v>
       </c>
-      <c r="AC15">
-        <f t="shared" si="1"/>
+      <c r="AC21">
+        <f t="shared" si="2"/>
         <v>-76614.526624731123</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="P16" s="74"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A22" s="12"/>
+      <c r="P22" s="74"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="145" t="s">
+      <c r="B23" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="145"/>
-      <c r="D17" s="145"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="145"/>
-      <c r="G17" s="145"/>
-      <c r="H17" s="145"/>
-      <c r="I17" s="145"/>
-      <c r="J17" s="145"/>
-      <c r="K17" s="145"/>
-      <c r="L17" s="145"/>
-      <c r="M17" s="145"/>
-      <c r="N17" s="145"/>
-      <c r="O17" s="145"/>
-      <c r="P17" s="145"/>
-      <c r="Q17" s="145"/>
-      <c r="R17" s="145"/>
-      <c r="S17" s="143" t="s">
+      <c r="C23" s="147"/>
+      <c r="D23" s="147"/>
+      <c r="E23" s="147"/>
+      <c r="F23" s="147"/>
+      <c r="G23" s="147"/>
+      <c r="H23" s="147"/>
+      <c r="I23" s="147"/>
+      <c r="J23" s="147"/>
+      <c r="K23" s="147"/>
+      <c r="L23" s="147"/>
+      <c r="M23" s="147"/>
+      <c r="N23" s="147"/>
+      <c r="O23" s="147"/>
+      <c r="P23" s="147"/>
+      <c r="Q23" s="147"/>
+      <c r="R23" s="147"/>
+      <c r="S23" s="143" t="s">
         <v>332</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T23" t="s">
         <v>90</v>
       </c>
-      <c r="Y17" s="76" t="s">
+      <c r="Y23" s="76" t="s">
         <v>317</v>
       </c>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76" t="s">
+      <c r="Z23" s="76"/>
+      <c r="AA23" s="76"/>
+      <c r="AB23" s="76" t="s">
         <v>317</v>
       </c>
-      <c r="AC17" s="76"/>
+      <c r="AC23" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B17:R17"/>
+    <mergeCell ref="B23:R23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5619,7 +6119,7 @@
       </c>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.35">
-      <c r="B12" s="146" t="s">
+      <c r="B12" s="148" t="s">
         <v>291</v>
       </c>
       <c r="C12" s="105" t="s">
@@ -5637,7 +6137,7 @@
       <c r="M12" s="107"/>
     </row>
     <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="147"/>
+      <c r="B13" s="149"/>
       <c r="C13" s="108" t="s">
         <v>1</v>
       </c>
@@ -6125,7 +6625,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="120"/>
-      <c r="B25" s="146" t="s">
+      <c r="B25" s="148" t="s">
         <v>291</v>
       </c>
       <c r="C25" s="105" t="s">
@@ -6144,7 +6644,7 @@
     </row>
     <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="84"/>
-      <c r="B26" s="147"/>
+      <c r="B26" s="149"/>
       <c r="C26" s="108" t="s">
         <v>1</v>
       </c>
@@ -6826,8 +7326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8031,11 +8531,11 @@
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="145" t="s">
+      <c r="B22" s="147" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="145"/>
-      <c r="D22" s="145"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="147"/>
       <c r="K22" s="38"/>
       <c r="L22" s="38"/>
       <c r="M22" s="38"/>
@@ -8347,16 +8847,16 @@
       <c r="AK1" t="s">
         <v>324</v>
       </c>
-      <c r="AL1" s="148" t="s">
+      <c r="AL1" s="145" t="s">
         <v>327</v>
       </c>
-      <c r="AM1" s="148" t="s">
+      <c r="AM1" s="145" t="s">
         <v>328</v>
       </c>
-      <c r="AN1" s="148" t="s">
+      <c r="AN1" s="145" t="s">
         <v>329</v>
       </c>
-      <c r="AO1" s="148" t="s">
+      <c r="AO1" s="145" t="s">
         <v>326</v>
       </c>
     </row>
@@ -10776,39 +11276,39 @@
       <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="145" t="s">
+      <c r="B23" s="147" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="145"/>
-      <c r="D23" s="145"/>
-      <c r="E23" s="145"/>
-      <c r="F23" s="145"/>
-      <c r="G23" s="145"/>
-      <c r="H23" s="145"/>
-      <c r="I23" s="145"/>
-      <c r="J23" s="145"/>
-      <c r="K23" s="145"/>
-      <c r="L23" s="145"/>
-      <c r="M23" s="145"/>
-      <c r="N23" s="145"/>
-      <c r="O23" s="145"/>
-      <c r="P23" s="145"/>
-      <c r="Q23" s="145"/>
-      <c r="R23" s="145"/>
-      <c r="S23" s="145"/>
-      <c r="T23" s="145"/>
-      <c r="U23" s="145"/>
-      <c r="V23" s="145"/>
-      <c r="W23" s="145"/>
-      <c r="X23" s="145"/>
-      <c r="Y23" s="145"/>
-      <c r="Z23" s="145"/>
-      <c r="AA23" s="145"/>
-      <c r="AB23" s="145"/>
-      <c r="AC23" s="145"/>
-      <c r="AD23" s="145"/>
-      <c r="AE23" s="145"/>
-      <c r="AF23" s="145"/>
+      <c r="C23" s="147"/>
+      <c r="D23" s="147"/>
+      <c r="E23" s="147"/>
+      <c r="F23" s="147"/>
+      <c r="G23" s="147"/>
+      <c r="H23" s="147"/>
+      <c r="I23" s="147"/>
+      <c r="J23" s="147"/>
+      <c r="K23" s="147"/>
+      <c r="L23" s="147"/>
+      <c r="M23" s="147"/>
+      <c r="N23" s="147"/>
+      <c r="O23" s="147"/>
+      <c r="P23" s="147"/>
+      <c r="Q23" s="147"/>
+      <c r="R23" s="147"/>
+      <c r="S23" s="147"/>
+      <c r="T23" s="147"/>
+      <c r="U23" s="147"/>
+      <c r="V23" s="147"/>
+      <c r="W23" s="147"/>
+      <c r="X23" s="147"/>
+      <c r="Y23" s="147"/>
+      <c r="Z23" s="147"/>
+      <c r="AA23" s="147"/>
+      <c r="AB23" s="147"/>
+      <c r="AC23" s="147"/>
+      <c r="AD23" s="147"/>
+      <c r="AE23" s="147"/>
+      <c r="AF23" s="147"/>
       <c r="AI23" t="s">
         <v>305</v>
       </c>
@@ -11967,22 +12467,22 @@
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="145" t="s">
+      <c r="B23" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="145"/>
-      <c r="D23" s="145"/>
-      <c r="E23" s="145"/>
-      <c r="F23" s="145"/>
-      <c r="G23" s="145"/>
-      <c r="H23" s="145"/>
-      <c r="I23" s="145"/>
-      <c r="J23" s="145"/>
-      <c r="K23" s="145"/>
-      <c r="L23" s="145"/>
-      <c r="M23" s="145"/>
-      <c r="N23" s="145"/>
-      <c r="O23" s="145"/>
+      <c r="C23" s="147"/>
+      <c r="D23" s="147"/>
+      <c r="E23" s="147"/>
+      <c r="F23" s="147"/>
+      <c r="G23" s="147"/>
+      <c r="H23" s="147"/>
+      <c r="I23" s="147"/>
+      <c r="J23" s="147"/>
+      <c r="K23" s="147"/>
+      <c r="L23" s="147"/>
+      <c r="M23" s="147"/>
+      <c r="N23" s="147"/>
+      <c r="O23" s="147"/>
       <c r="P23" t="s">
         <v>90</v>
       </c>
@@ -12515,8 +13015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12977,7 +13477,7 @@
         <v>243</v>
       </c>
       <c r="B42" s="76">
-        <v>43.995102738357922</v>
+        <v>44.291949816853993</v>
       </c>
       <c r="C42">
         <v>793.37856525946859</v>

</xml_diff>

<commit_message>
Re-implemented quick sensitivity analysis for renewable electricity share
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF6C703-666E-44A0-8ABA-4D58EAD13099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39799C9E-0D40-456E-915D-EEA3D1E95D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="335">
   <si>
     <t>NG</t>
   </si>
@@ -1268,6 +1268,9 @@
   </si>
   <si>
     <t>Biocrude</t>
+  </si>
+  <si>
+    <t>Electricity_Renewable</t>
   </si>
 </sst>
 </file>
@@ -2582,7 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AB9" sqref="AB9"/>
     </sheetView>
@@ -2907,7 +2910,7 @@
         <v>9216.8702699702171</v>
       </c>
       <c r="Z4">
-        <f>X4+Y4</f>
+        <f t="shared" ref="Z4:Z10" si="0">X4+Y4</f>
         <v>1009216.8702699703</v>
       </c>
       <c r="AA4" s="3">
@@ -2990,7 +2993,7 @@
         <v>8027.464959570797</v>
       </c>
       <c r="Z5">
-        <f>X5+Y5</f>
+        <f t="shared" si="0"/>
         <v>8027.464959570797</v>
       </c>
       <c r="AA5" s="3">
@@ -3000,7 +3003,7 @@
         <v>1199.1725344773329</v>
       </c>
       <c r="AC5">
-        <f t="shared" ref="AC5:AC9" si="0">AA5+AB5</f>
+        <f t="shared" ref="AC5:AC9" si="1">AA5+AB5</f>
         <v>1199.1725344773329</v>
       </c>
     </row>
@@ -3073,7 +3076,7 @@
         <v>1664.7217341019561</v>
       </c>
       <c r="Z6">
-        <f>X6+Y6</f>
+        <f t="shared" si="0"/>
         <v>1664.7217341019561</v>
       </c>
       <c r="AA6" s="3">
@@ -3083,7 +3086,7 @@
         <v>8.0912620107395146</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0912620107395146</v>
       </c>
     </row>
@@ -3156,7 +3159,7 @@
         <v>2963.4305044075732</v>
       </c>
       <c r="Z7">
-        <f>X7+Y7</f>
+        <f t="shared" si="0"/>
         <v>2963.4305044075732</v>
       </c>
       <c r="AA7" s="3">
@@ -3166,7 +3169,7 @@
         <v>124.60248498831356</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124.60248498831356</v>
       </c>
     </row>
@@ -3239,7 +3242,7 @@
         <v>3399.3127210612679</v>
       </c>
       <c r="Z8">
-        <f>X8+Y8</f>
+        <f t="shared" si="0"/>
         <v>3399.3127210612679</v>
       </c>
       <c r="AA8" s="3">
@@ -3249,7 +3252,7 @@
         <v>1066.4787874782799</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1066.4787874782799</v>
       </c>
     </row>
@@ -3322,7 +3325,7 @@
         <v>0.56134131706501467</v>
       </c>
       <c r="Z9">
-        <f>X9+Y9</f>
+        <f t="shared" si="0"/>
         <v>0.56134131706501467</v>
       </c>
       <c r="AA9" s="3">
@@ -3332,7 +3335,7 @@
         <v>2.3217600680931635E-2</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3217600680931635E-2</v>
       </c>
     </row>
@@ -3405,7 +3408,7 @@
         <v>0.12380376798091507</v>
       </c>
       <c r="Z10">
-        <f>X10+Y10</f>
+        <f t="shared" si="0"/>
         <v>53.72127839826932</v>
       </c>
       <c r="AA10">
@@ -3488,7 +3491,7 @@
         <v>0.53001711985689259</v>
       </c>
       <c r="Z11">
-        <f t="shared" ref="Z11:Z21" si="1">X11+Y11</f>
+        <f t="shared" ref="Z11:Z21" si="2">X11+Y11</f>
         <v>639.63416782778677</v>
       </c>
       <c r="AA11">
@@ -3498,7 +3501,7 @@
         <v>0.19579254162294349</v>
       </c>
       <c r="AC11">
-        <f t="shared" ref="AC11:AC21" si="2">AA11+AB11</f>
+        <f t="shared" ref="AC11:AC21" si="3">AA11+AB11</f>
         <v>993.99652518923131</v>
       </c>
     </row>
@@ -3571,7 +3574,7 @@
         <v>1.4390708093838975</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.647805124275852</v>
       </c>
       <c r="AA12">
@@ -3581,7 +3584,7 @@
         <v>0.13356807901983217</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.521187334987346</v>
       </c>
     </row>
@@ -3654,7 +3657,7 @@
         <v>6.8025222126898502E-2</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.1121724631375205</v>
       </c>
       <c r="AA13">
@@ -3664,7 +3667,7 @@
         <v>7.5116168079741932E-3</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.4662813685889695</v>
       </c>
     </row>
@@ -3737,7 +3740,7 @@
         <v>4.6442748659862865E-2</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7750922644483509</v>
       </c>
       <c r="AA14">
@@ -3747,7 +3750,7 @@
         <v>2.1809956805283149E-3</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8944508672117086</v>
       </c>
     </row>
@@ -3820,7 +3823,7 @@
         <v>0.22128373782612412</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.700151259382223</v>
       </c>
       <c r="AA15">
@@ -3830,7 +3833,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.3987418408876558E-3</v>
       </c>
     </row>
@@ -3901,7 +3904,7 @@
         <v>4.2404984619842561E-3</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.47814997311821905</v>
       </c>
       <c r="AA16">
@@ -3911,7 +3914,7 @@
         <v>2.0959176112987082E-4</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.51231387456148403</v>
       </c>
     </row>
@@ -3982,7 +3985,7 @@
         <v>2.0700811243651359E-2</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26655908652077559</v>
       </c>
       <c r="AA17">
@@ -3992,7 +3995,7 @@
         <v>3.7216049065244534E-4</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.7002199380836189E-2</v>
       </c>
     </row>
@@ -4063,7 +4066,7 @@
         <v>1.0718762615156343</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.4860014543055007</v>
       </c>
       <c r="AA18">
@@ -4073,7 +4076,7 @@
         <v>0.11248755052026857</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.11248755052026857</v>
       </c>
     </row>
@@ -4144,7 +4147,7 @@
         <v>1.1802078079887578E-2</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92323127223800683</v>
       </c>
       <c r="AA19">
@@ -4154,7 +4157,7 @@
         <v>3.4778154884700514E-4</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.18912102284679677</v>
       </c>
     </row>
@@ -4239,7 +4242,7 @@
         <v>611.91676387079497</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72395.422081418714</v>
       </c>
       <c r="AA20">
@@ -4249,7 +4252,7 @@
         <v>92.564589004961775</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75019.638597761033</v>
       </c>
     </row>
@@ -4280,14 +4283,14 @@
         <v>-72964.246146966863</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-72964.246146966863</v>
       </c>
       <c r="AA21">
         <v>-76614.526624731123</v>
       </c>
       <c r="AC21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-76614.526624731123</v>
       </c>
     </row>
@@ -7324,19 +7327,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -7344,55 +7348,58 @@
         <v>88</v>
       </c>
       <c r="D1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>243</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>320</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>333</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>30</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>31</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="136" t="s">
         <v>123</v>
       </c>
@@ -7409,10 +7416,10 @@
         <v>185</v>
       </c>
       <c r="F2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" t="s">
         <v>321</v>
-      </c>
-      <c r="G2" t="s">
-        <v>318</v>
       </c>
       <c r="H2" t="s">
         <v>318</v>
@@ -7450,8 +7457,11 @@
       <c r="S2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>126</v>
       </c>
@@ -7468,7 +7478,7 @@
         <v>125</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="G3" t="s">
         <v>93</v>
@@ -7509,8 +7519,11 @@
       <c r="S3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -7520,19 +7533,19 @@
       <c r="C4" s="68">
         <v>2030788.9805523627</v>
       </c>
-      <c r="D4" s="68">
+      <c r="D4" s="76">
+        <v>0</v>
+      </c>
+      <c r="E4" s="68">
         <v>104261.00625785353</v>
       </c>
-      <c r="E4" s="76">
-        <v>0</v>
-      </c>
       <c r="F4" s="76">
         <v>0</v>
       </c>
       <c r="G4" s="76">
         <v>0</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="76">
         <v>0</v>
       </c>
       <c r="I4" s="38">
@@ -7568,8 +7581,11 @@
       <c r="S4" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -7579,19 +7595,19 @@
       <c r="C5" s="68">
         <v>1595100.2772139744</v>
       </c>
-      <c r="D5" s="68">
+      <c r="D5" s="76">
+        <v>0</v>
+      </c>
+      <c r="E5" s="68">
         <v>103489.85649124274</v>
       </c>
-      <c r="E5" s="76">
-        <v>0</v>
-      </c>
       <c r="F5" s="76">
         <v>0</v>
       </c>
       <c r="G5" s="76">
         <v>0</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="76">
         <v>0</v>
       </c>
       <c r="I5" s="38">
@@ -7627,8 +7643,11 @@
       <c r="S5" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -7638,19 +7657,19 @@
       <c r="C6" s="68">
         <v>610146.06903376419</v>
       </c>
-      <c r="D6" s="68">
+      <c r="D6" s="76">
+        <v>0</v>
+      </c>
+      <c r="E6" s="68">
         <v>1078.8033372105469</v>
       </c>
-      <c r="E6" s="76">
-        <v>0</v>
-      </c>
       <c r="F6" s="76">
         <v>0</v>
       </c>
       <c r="G6" s="76">
         <v>0</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="76">
         <v>0</v>
       </c>
       <c r="I6" s="38">
@@ -7686,8 +7705,11 @@
       <c r="S6" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T6" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7697,19 +7719,19 @@
       <c r="C7" s="68">
         <v>958187.72206407064</v>
       </c>
-      <c r="D7" s="68">
+      <c r="D7" s="76">
+        <v>0</v>
+      </c>
+      <c r="E7" s="68">
         <v>98380.297877359611</v>
       </c>
-      <c r="E7" s="76">
-        <v>0</v>
-      </c>
       <c r="F7" s="76">
         <v>0</v>
       </c>
       <c r="G7" s="76">
         <v>0</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="76">
         <v>0</v>
       </c>
       <c r="I7" s="38">
@@ -7745,8 +7767,11 @@
       <c r="S7" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -7756,19 +7781,19 @@
       <c r="C8" s="68">
         <v>26766.486116139466</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="76">
+        <v>0</v>
+      </c>
+      <c r="E8" s="68">
         <v>4030.7552766725985</v>
       </c>
-      <c r="E8" s="76">
-        <v>0</v>
-      </c>
       <c r="F8" s="76">
         <v>0</v>
       </c>
       <c r="G8" s="76">
         <v>0</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="76">
         <v>0</v>
       </c>
       <c r="I8" s="38">
@@ -7804,8 +7829,11 @@
       <c r="S8" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T8" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -7815,19 +7843,19 @@
       <c r="C9" s="68">
         <v>181.94958337414994</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="76">
+        <v>0</v>
+      </c>
+      <c r="E9" s="68">
         <v>3.211633491944839</v>
       </c>
-      <c r="E9" s="76">
-        <v>0</v>
-      </c>
       <c r="F9" s="76">
         <v>0</v>
       </c>
       <c r="G9" s="76">
         <v>0</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="76">
         <v>0</v>
       </c>
       <c r="I9" s="38">
@@ -7863,8 +7891,11 @@
       <c r="S9" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T9" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -7874,24 +7905,24 @@
       <c r="C10">
         <v>14.163040112750402</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="76">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>10.287405417696785</v>
       </c>
-      <c r="E10" s="76">
-        <v>0</v>
-      </c>
       <c r="F10" s="76">
         <v>0</v>
       </c>
       <c r="G10" s="76">
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="76">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
-      <c r="I10" s="38">
-        <v>0</v>
-      </c>
       <c r="J10" s="38">
         <v>0</v>
       </c>
@@ -7922,8 +7953,11 @@
       <c r="S10" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T10" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -7933,27 +7967,27 @@
       <c r="C11">
         <v>49.808169492725952</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="76">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>31.26772994989345</v>
       </c>
-      <c r="E11" s="76">
-        <v>0</v>
-      </c>
       <c r="F11" s="76">
         <v>0</v>
       </c>
       <c r="G11" s="76">
         <v>0</v>
       </c>
-      <c r="H11" s="38">
-        <v>0</v>
-      </c>
-      <c r="I11">
+      <c r="H11" s="76">
+        <v>0</v>
+      </c>
+      <c r="I11" s="38">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="J11" s="38">
-        <v>0</v>
-      </c>
       <c r="K11" s="38">
         <v>0</v>
       </c>
@@ -7981,8 +8015,11 @@
       <c r="S11" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T11" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -7992,30 +8029,30 @@
       <c r="C12">
         <v>89.209957975971022</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="76">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>36.291301237350226</v>
       </c>
-      <c r="E12" s="76">
-        <v>0</v>
-      </c>
       <c r="F12" s="76">
         <v>0</v>
       </c>
       <c r="G12" s="76">
         <v>0</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="76">
         <v>0</v>
       </c>
       <c r="I12" s="38">
         <v>0</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="38">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>1</v>
       </c>
-      <c r="K12" s="38">
-        <v>0</v>
-      </c>
       <c r="L12" s="38">
         <v>0</v>
       </c>
@@ -8040,8 +8077,11 @@
       <c r="S12" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T12" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -8051,19 +8091,19 @@
       <c r="C13">
         <v>13.192309126038818</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="76">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>0.42153625660303229</v>
       </c>
-      <c r="E13" s="76">
-        <v>0</v>
-      </c>
       <c r="F13" s="76">
         <v>0</v>
       </c>
       <c r="G13" s="76">
         <v>0</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="76">
         <v>0</v>
       </c>
       <c r="I13" s="38">
@@ -8072,12 +8112,12 @@
       <c r="J13" s="38">
         <v>0</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="38">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>1</v>
       </c>
-      <c r="L13" s="38">
-        <v>0</v>
-      </c>
       <c r="M13" s="38">
         <v>0</v>
       </c>
@@ -8099,8 +8139,11 @@
       <c r="S13" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T13" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -8110,19 +8153,19 @@
       <c r="C14">
         <v>7.5508397631511279</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="76">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>0.37894052180007021</v>
       </c>
-      <c r="E14" s="76">
-        <v>0</v>
-      </c>
       <c r="F14" s="76">
         <v>0</v>
       </c>
       <c r="G14" s="76">
         <v>0</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="76">
         <v>0</v>
       </c>
       <c r="I14" s="38">
@@ -8134,12 +8177,12 @@
       <c r="K14" s="38">
         <v>0</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="38">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>1</v>
       </c>
-      <c r="M14" s="38">
-        <v>0</v>
-      </c>
       <c r="N14" s="38">
         <v>0</v>
       </c>
@@ -8158,8 +8201,11 @@
       <c r="S14" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T14" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -8169,19 +8215,19 @@
       <c r="C15">
         <v>76.085922807953608</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="76">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>11.120378048826899</v>
       </c>
-      <c r="E15" s="76">
-        <v>0</v>
-      </c>
       <c r="F15" s="76">
         <v>0</v>
       </c>
       <c r="G15" s="76">
         <v>0</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="76">
         <v>0</v>
       </c>
       <c r="I15" s="38">
@@ -8196,12 +8242,12 @@
       <c r="L15" s="38">
         <v>0</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="38">
+        <v>0</v>
+      </c>
+      <c r="N15">
         <v>1</v>
       </c>
-      <c r="N15" s="38">
-        <v>0</v>
-      </c>
       <c r="O15" s="38">
         <v>0</v>
       </c>
@@ -8217,8 +8263,11 @@
       <c r="S15" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T15" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -8228,19 +8277,19 @@
       <c r="C16">
         <v>0.4314302688983046</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="76">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>9.919204253941645E-2</v>
       </c>
-      <c r="E16" s="76">
-        <v>0</v>
-      </c>
       <c r="F16" s="76">
         <v>0</v>
       </c>
       <c r="G16" s="76">
         <v>0</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="76">
         <v>0</v>
       </c>
       <c r="I16" s="38">
@@ -8258,12 +8307,12 @@
       <c r="M16" s="38">
         <v>0</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="38">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <v>1</v>
       </c>
-      <c r="O16" s="38">
-        <v>0</v>
-      </c>
       <c r="P16" s="38">
         <v>0</v>
       </c>
@@ -8276,8 +8325,11 @@
       <c r="S16" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T16" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -8287,19 +8339,19 @@
       <c r="C17">
         <v>2.13733672790991</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="76">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>0.14325167839344721</v>
       </c>
-      <c r="E17" s="76">
-        <v>0</v>
-      </c>
       <c r="F17" s="76">
         <v>0</v>
       </c>
       <c r="G17" s="76">
         <v>0</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="76">
         <v>0</v>
       </c>
       <c r="I17" s="38">
@@ -8320,12 +8372,12 @@
       <c r="N17" s="38">
         <v>0</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="38">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <v>1</v>
       </c>
-      <c r="P17" s="38">
-        <v>0</v>
-      </c>
       <c r="Q17" s="38">
         <v>0</v>
       </c>
@@ -8335,8 +8387,11 @@
       <c r="S17" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T17" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -8346,19 +8401,19 @@
       <c r="C18">
         <v>264.62635507778742</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="76">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>216.35815892748519</v>
       </c>
-      <c r="E18" s="76">
-        <v>0</v>
-      </c>
       <c r="F18" s="76">
         <v>0</v>
       </c>
       <c r="G18" s="76">
         <v>0</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="76">
         <v>0</v>
       </c>
       <c r="I18" s="38">
@@ -8382,20 +8437,23 @@
       <c r="O18" s="38">
         <v>0</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <v>1</v>
       </c>
-      <c r="Q18" s="38">
-        <v>0</v>
-      </c>
       <c r="R18" s="38">
         <v>0</v>
       </c>
       <c r="S18" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T18" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -8405,19 +8463,19 @@
       <c r="C19">
         <v>2.3934466638424041</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="76">
+        <v>0</v>
+      </c>
+      <c r="E19">
         <v>1.4196658578962942</v>
       </c>
-      <c r="E19" s="76">
-        <v>0</v>
-      </c>
       <c r="F19" s="76">
         <v>0</v>
       </c>
       <c r="G19" s="76">
         <v>0</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="76">
         <v>0</v>
       </c>
       <c r="I19" s="38">
@@ -8444,17 +8502,20 @@
       <c r="P19" s="38">
         <v>0</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="38">
+        <v>0</v>
+      </c>
+      <c r="R19">
         <v>1</v>
       </c>
-      <c r="R19" s="38">
-        <v>0</v>
-      </c>
       <c r="S19" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T19" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -8464,19 +8525,19 @@
       <c r="C20">
         <v>120183.90410917185</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="76">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>6135.9109157721377</v>
       </c>
-      <c r="E20" s="76">
-        <v>0</v>
-      </c>
       <c r="F20" s="76">
         <v>0</v>
       </c>
       <c r="G20" s="76">
         <v>0</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="76">
         <v>0</v>
       </c>
       <c r="I20" s="38">
@@ -8506,18 +8567,20 @@
       <c r="Q20" s="38">
         <v>0</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="38">
+        <v>0</v>
+      </c>
+      <c r="S20">
         <v>1</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E21" s="38"/>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
-      <c r="J21" s="38"/>
+      <c r="H21" s="38"/>
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
@@ -8526,8 +8589,9 @@
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S21" s="38"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -8536,7 +8600,7 @@
       </c>
       <c r="C22" s="147"/>
       <c r="D22" s="147"/>
-      <c r="K22" s="38"/>
+      <c r="E22" s="147"/>
       <c r="L22" s="38"/>
       <c r="M22" s="38"/>
       <c r="N22" s="38"/>
@@ -8544,9 +8608,9 @@
       <c r="P22" s="38"/>
       <c r="Q22" s="38"/>
       <c r="R22" s="38"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="K23" s="38"/>
+      <c r="S22" s="38"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
@@ -8554,8 +8618,9 @@
       <c r="P23" s="38"/>
       <c r="Q23" s="38"/>
       <c r="R23" s="38"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S23" s="38"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -8563,15 +8628,16 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="L24" s="38"/>
+      <c r="I24" s="6"/>
       <c r="M24" s="38"/>
       <c r="N24" s="38"/>
       <c r="O24" s="38"/>
       <c r="P24" s="38"/>
       <c r="Q24" s="38"/>
       <c r="R24" s="38"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S24" s="38"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -8579,14 +8645,15 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="M25" s="38"/>
+      <c r="I25" s="3"/>
       <c r="N25" s="38"/>
       <c r="O25" s="38"/>
       <c r="P25" s="38"/>
       <c r="Q25" s="38"/>
       <c r="R25" s="38"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S25" s="38"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -8594,13 +8661,14 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="N26" s="38"/>
+      <c r="I26" s="4"/>
       <c r="O26" s="38"/>
       <c r="P26" s="38"/>
       <c r="Q26" s="38"/>
       <c r="R26" s="38"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S26" s="38"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -8608,12 +8676,13 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="O27" s="38"/>
+      <c r="I27" s="4"/>
       <c r="P27" s="38"/>
       <c r="Q27" s="38"/>
       <c r="R27" s="38"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S27" s="38"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -8621,11 +8690,12 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="P28" s="38"/>
+      <c r="I28" s="4"/>
       <c r="Q28" s="38"/>
       <c r="R28" s="38"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S28" s="38"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -8633,10 +8703,11 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="Q29" s="38"/>
+      <c r="I29" s="4"/>
       <c r="R29" s="38"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S29" s="38"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -8644,9 +8715,10 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="R30" s="38"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I30" s="4"/>
+      <c r="S30" s="38"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -8654,8 +8726,9 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -8663,8 +8736,9 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -8672,8 +8746,9 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -8681,8 +8756,9 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -8690,17 +8766,19 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H36" s="2"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -8708,10 +8786,11 @@
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added postprocessing funciton and fixed the order of the bars
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39799C9E-0D40-456E-915D-EEA3D1E95D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004F3BA0-4FE1-4EAE-8E51-47311D46F94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -70,6 +70,10 @@
     <author>tc={34D340DC-D67A-4CAE-8C20-051ACF44D0B9}</author>
     <author>tc={84A790D2-B4B9-4265-BD79-AAB8D56817C1}</author>
     <author>tc={1637977C-8F1B-4736-AFF4-BC85BB25E877}</author>
+    <author>tc={AEEC40CA-3288-4896-9A88-AB2AB3314A84}</author>
+    <author>tc={18F5452D-DD29-49E9-AA32-C6698F56C629}</author>
+    <author>tc={2C8587DB-B33F-47F4-B13B-33B4A46987E0}</author>
+    <author>tc={7C7F111C-24AE-475B-B4AD-4A8AD1795C98}</author>
   </authors>
   <commentList>
     <comment ref="J2" authorId="0" shapeId="0" xr:uid="{7EC4C7E0-FF9B-4515-8E61-AA65D5664E9D}">
@@ -103,6 +107,44 @@
       </text>
     </comment>
     <comment ref="P2" authorId="3" shapeId="0" xr:uid="{1637977C-8F1B-4736-AFF4-BC85BB25E877}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CO and CH4 emissions are calculated from CO2 emissions and ratios developed from Kuipers and Jarvis (1996). </t>
+      </text>
+    </comment>
+    <comment ref="T2" authorId="4" shapeId="0" xr:uid="{AEEC40CA-3288-4896-9A88-AB2AB3314A84}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Emsisions factors are for large industrial boilers. 
+Calculated utility boiler results in g/kWh in Electric sheet are based on the inputs here. 
+Also, utility boiler results in g/kWh are inputted separately into Electric sheet.</t>
+      </text>
+    </comment>
+    <comment ref="V2" authorId="5" shapeId="0" xr:uid="{18F5452D-DD29-49E9-AA32-C6698F56C629}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Emsisions factors are for large turbines. 
+Calculated turbine results in g/kWh in Electric sheet are based on the inputs here. 
+Also, turbine results in g/kWh are inputted separately into Electric sheet.</t>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="6" shapeId="0" xr:uid="{2C8587DB-B33F-47F4-B13B-33B4A46987E0}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Calculated CC turbine results in g/kWh in Electric sheet are based on the inputs here. 
+Also, CC turbine results in g/kWh are inputted separately into Electric sheet.
+</t>
+      </text>
+    </comment>
+    <comment ref="Z2" authorId="7" shapeId="0" xr:uid="{7C7F111C-24AE-475B-B4AD-4A8AD1795C98}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -266,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="338">
   <si>
     <t>NG</t>
   </si>
@@ -1271,6 +1313,15 @@
   </si>
   <si>
     <t>Electricity_Renewable</t>
+  </si>
+  <si>
+    <t>Renewable Natural Gas</t>
+  </si>
+  <si>
+    <t>RNG tab, intermediate NG from landfill gas</t>
+  </si>
+  <si>
+    <t>Biogenic CO2 calculated by carbon balance</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1341,7 @@
     <numFmt numFmtId="172" formatCode="#,##0.0000000000"/>
     <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1336,6 +1387,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1589,7 +1646,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1875,6 +1932,9 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2517,6 +2577,24 @@
   <threadedComment ref="P2" personId="{865AB77A-77F7-42CA-A3DE-E71A2578FA95}" id="{1637977C-8F1B-4736-AFF4-BC85BB25E877}">
     <text xml:space="preserve">CO and CH4 emissions are calculated from CO2 emissions and ratios developed from Kuipers and Jarvis (1996). </text>
   </threadedComment>
+  <threadedComment ref="T2" personId="{52F93C99-6E2F-47FF-A86C-9CFC6703D7FF}" id="{AEEC40CA-3288-4896-9A88-AB2AB3314A84}">
+    <text>Emsisions factors are for large industrial boilers. 
+Calculated utility boiler results in g/kWh in Electric sheet are based on the inputs here. 
+Also, utility boiler results in g/kWh are inputted separately into Electric sheet.</text>
+  </threadedComment>
+  <threadedComment ref="V2" personId="{52F93C99-6E2F-47FF-A86C-9CFC6703D7FF}" id="{18F5452D-DD29-49E9-AA32-C6698F56C629}">
+    <text>Emsisions factors are for large turbines. 
+Calculated turbine results in g/kWh in Electric sheet are based on the inputs here. 
+Also, turbine results in g/kWh are inputted separately into Electric sheet.</text>
+  </threadedComment>
+  <threadedComment ref="W2" personId="{52F93C99-6E2F-47FF-A86C-9CFC6703D7FF}" id="{2C8587DB-B33F-47F4-B13B-33B4A46987E0}">
+    <text xml:space="preserve">Calculated CC turbine results in g/kWh in Electric sheet are based on the inputs here. 
+Also, CC turbine results in g/kWh are inputted separately into Electric sheet.
+</text>
+  </threadedComment>
+  <threadedComment ref="Z2" personId="{865AB77A-77F7-42CA-A3DE-E71A2578FA95}" id="{7C7F111C-24AE-475B-B4AD-4A8AD1795C98}">
+    <text xml:space="preserve">CO and CH4 emissions are calculated from CO2 emissions and ratios developed from Kuipers and Jarvis (1996). </text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2583,21 +2661,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
-  <dimension ref="A1:AC23"/>
+  <dimension ref="A1:AM23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB9" sqref="AB9"/>
+      <selection pane="topRight" activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.08984375" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1796875" style="142"/>
-    <col min="28" max="28" width="13.7265625" customWidth="1"/>
+    <col min="38" max="38" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" ht="26.5" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2653,37 +2731,67 @@
         <v>14</v>
       </c>
       <c r="T1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="AD1" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="AF1" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="W1" s="133" t="s">
+      <c r="AG1" s="133" t="s">
         <v>304</v>
       </c>
-      <c r="X1" s="121" t="s">
+      <c r="AH1" s="121" t="s">
         <v>165</v>
       </c>
-      <c r="Y1" s="121" t="s">
+      <c r="AI1" s="121" t="s">
         <v>165</v>
       </c>
-      <c r="Z1" s="121" t="s">
+      <c r="AJ1" s="121" t="s">
         <v>165</v>
       </c>
-      <c r="AA1" s="121" t="s">
+      <c r="AK1" s="121" t="s">
         <v>243</v>
       </c>
-      <c r="AB1" s="121" t="s">
+      <c r="AL1" s="121" t="s">
         <v>243</v>
       </c>
-      <c r="AC1" s="121" t="s">
+      <c r="AM1" s="121" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="78.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -2740,37 +2848,67 @@
         <v>331</v>
       </c>
       <c r="T2" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="U2" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="V2" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="W2" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="X2" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y2" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z2" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB2" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC2" s="70" t="s">
+        <v>331</v>
+      </c>
+      <c r="AD2" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="U2" s="70" t="s">
+      <c r="AE2" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="V2" s="135" t="s">
+      <c r="AF2" s="135" t="s">
         <v>307</v>
       </c>
-      <c r="W2" s="135" t="s">
+      <c r="AG2" s="135" t="s">
         <v>307</v>
       </c>
-      <c r="X2" s="139" t="s">
+      <c r="AH2" s="139" t="s">
         <v>312</v>
       </c>
-      <c r="Y2" s="139" t="s">
+      <c r="AI2" s="139" t="s">
         <v>315</v>
       </c>
-      <c r="Z2" s="139" t="s">
+      <c r="AJ2" s="139" t="s">
         <v>316</v>
       </c>
-      <c r="AA2" s="139" t="s">
+      <c r="AK2" s="139" t="s">
         <v>312</v>
       </c>
-      <c r="AB2" s="139" t="s">
+      <c r="AL2" s="139" t="s">
         <v>315</v>
       </c>
-      <c r="AC2" s="139" t="s">
+      <c r="AM2" s="139" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>126</v>
       </c>
@@ -2828,20 +2966,50 @@
       <c r="S3" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="T3" s="70" t="s">
+      <c r="T3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD3" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="70" t="s">
+      <c r="AE3" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="V3" s="134" t="s">
+      <c r="AF3" s="134" t="s">
         <v>93</v>
       </c>
-      <c r="W3" s="134" t="s">
+      <c r="AG3" s="134" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2899,32 +3067,62 @@
       <c r="S4" s="3">
         <v>1000000</v>
       </c>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-      <c r="V4" s="134"/>
-      <c r="W4" s="134"/>
+      <c r="T4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="V4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="W4" s="3">
+        <v>1000000</v>
+      </c>
       <c r="X4" s="3">
         <v>1000000</v>
       </c>
-      <c r="Y4">
-        <v>9216.8702699702171</v>
-      </c>
-      <c r="Z4">
-        <f t="shared" ref="Z4:Z10" si="0">X4+Y4</f>
-        <v>1009216.8702699703</v>
+      <c r="Y4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1000000</v>
       </c>
       <c r="AA4" s="3">
         <v>1000000</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AD4" s="70"/>
+      <c r="AE4" s="70"/>
+      <c r="AF4" s="134"/>
+      <c r="AG4" s="134"/>
+      <c r="AH4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AI4">
+        <v>9216.8702699702171</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" ref="AJ4:AJ10" si="0">AH4+AI4</f>
+        <v>1009216.8702699703</v>
+      </c>
+      <c r="AK4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AL4">
         <v>1250.309002469897</v>
       </c>
-      <c r="AC4">
-        <f>AA4+AB4</f>
+      <c r="AM4">
+        <f>AK4+AL4</f>
         <v>1001250.3090024699</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2982,32 +3180,62 @@
       <c r="S5" s="3">
         <v>1000000</v>
       </c>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="134"/>
-      <c r="W5" s="134"/>
+      <c r="T5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="U5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="V5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="W5" s="3">
+        <v>1000000</v>
+      </c>
       <c r="X5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y5">
+        <v>1000000</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AD5" s="70"/>
+      <c r="AE5" s="70"/>
+      <c r="AF5" s="134"/>
+      <c r="AG5" s="134"/>
+      <c r="AH5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI5">
         <v>8027.464959570797</v>
       </c>
-      <c r="Z5">
+      <c r="AJ5">
         <f t="shared" si="0"/>
         <v>8027.464959570797</v>
       </c>
-      <c r="AA5" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB5">
+      <c r="AK5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL5">
         <v>1199.1725344773329</v>
       </c>
-      <c r="AC5">
-        <f t="shared" ref="AC5:AC9" si="1">AA5+AB5</f>
+      <c r="AM5">
+        <f t="shared" ref="AM5:AM9" si="1">AK5+AL5</f>
         <v>1199.1725344773329</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3065,32 +3293,62 @@
       <c r="S6" s="3">
         <v>0</v>
       </c>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
-      <c r="V6" s="134"/>
-      <c r="W6" s="134"/>
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
       <c r="X6" s="3">
         <v>0</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="70"/>
+      <c r="AE6" s="70"/>
+      <c r="AF6" s="134"/>
+      <c r="AG6" s="134"/>
+      <c r="AH6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI6">
         <v>1664.7217341019561</v>
       </c>
-      <c r="Z6">
+      <c r="AJ6">
         <f t="shared" si="0"/>
         <v>1664.7217341019561</v>
       </c>
-      <c r="AA6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB6">
+      <c r="AK6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL6">
         <v>8.0912620107395146</v>
       </c>
-      <c r="AC6">
+      <c r="AM6">
         <f t="shared" si="1"/>
         <v>8.0912620107395146</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3148,32 +3406,62 @@
       <c r="S7" s="3">
         <v>1000000</v>
       </c>
-      <c r="T7" s="70"/>
-      <c r="U7" s="70"/>
-      <c r="V7" s="134"/>
-      <c r="W7" s="134"/>
+      <c r="T7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="U7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="V7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="W7" s="3">
+        <v>1000000</v>
+      </c>
       <c r="X7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y7">
+        <v>1000000</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AD7" s="70"/>
+      <c r="AE7" s="70"/>
+      <c r="AF7" s="134"/>
+      <c r="AG7" s="134"/>
+      <c r="AH7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI7">
         <v>2963.4305044075732</v>
       </c>
-      <c r="Z7">
+      <c r="AJ7">
         <f t="shared" si="0"/>
         <v>2963.4305044075732</v>
       </c>
-      <c r="AA7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB7">
+      <c r="AK7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL7">
         <v>124.60248498831356</v>
       </c>
-      <c r="AC7">
+      <c r="AM7">
         <f t="shared" si="1"/>
         <v>124.60248498831356</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3231,32 +3519,62 @@
       <c r="S8" s="3">
         <v>0</v>
       </c>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="134"/>
-      <c r="W8" s="134"/>
+      <c r="T8" s="3">
+        <v>0</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0</v>
+      </c>
       <c r="X8" s="3">
         <v>0</v>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="70"/>
+      <c r="AE8" s="70"/>
+      <c r="AF8" s="134"/>
+      <c r="AG8" s="134"/>
+      <c r="AH8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI8">
         <v>3399.3127210612679</v>
       </c>
-      <c r="Z8">
+      <c r="AJ8">
         <f t="shared" si="0"/>
         <v>3399.3127210612679</v>
       </c>
-      <c r="AA8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB8">
+      <c r="AK8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL8">
         <v>1066.4787874782799</v>
       </c>
-      <c r="AC8">
+      <c r="AM8">
         <f t="shared" si="1"/>
         <v>1066.4787874782799</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3314,32 +3632,62 @@
       <c r="S9" s="3">
         <v>0</v>
       </c>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="134"/>
-      <c r="W9" s="134"/>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0</v>
+      </c>
       <c r="X9" s="3">
         <v>0</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="70"/>
+      <c r="AE9" s="70"/>
+      <c r="AF9" s="134"/>
+      <c r="AG9" s="134"/>
+      <c r="AH9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI9">
         <v>0.56134131706501467</v>
       </c>
-      <c r="Z9">
+      <c r="AJ9">
         <f t="shared" si="0"/>
         <v>0.56134131706501467</v>
       </c>
-      <c r="AA9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB9">
+      <c r="AK9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL9">
         <v>2.3217600680931635E-2</v>
       </c>
-      <c r="AC9">
+      <c r="AM9">
         <f t="shared" si="1"/>
         <v>2.3217600680931635E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
@@ -3397,32 +3745,62 @@
       <c r="S10" s="73">
         <v>0.69343623523370912</v>
       </c>
-      <c r="T10" s="73">
-        <v>0</v>
-      </c>
-      <c r="U10" s="73"/>
-      <c r="X10">
+      <c r="T10" s="71">
+        <v>2.54</v>
+      </c>
+      <c r="U10" s="71">
+        <v>2.54</v>
+      </c>
+      <c r="V10" s="71">
+        <v>1.056</v>
+      </c>
+      <c r="W10" s="71">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X10" s="71">
+        <v>1.056</v>
+      </c>
+      <c r="Y10" s="71">
+        <v>130.05799999999999</v>
+      </c>
+      <c r="Z10" s="71">
+        <v>2.5</v>
+      </c>
+      <c r="AA10" s="72">
+        <v>100</v>
+      </c>
+      <c r="AB10" s="73">
+        <v>2.54</v>
+      </c>
+      <c r="AC10" s="73">
+        <v>0.69343623523370912</v>
+      </c>
+      <c r="AD10" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="73"/>
+      <c r="AH10">
         <v>53.597474630288403</v>
       </c>
-      <c r="Y10">
+      <c r="AI10">
         <v>0.12380376798091507</v>
       </c>
-      <c r="Z10">
+      <c r="AJ10">
         <f t="shared" si="0"/>
         <v>53.72127839826932</v>
       </c>
-      <c r="AA10">
+      <c r="AK10">
         <v>40.352647182660228</v>
       </c>
-      <c r="AB10">
+      <c r="AL10">
         <v>1.4111608204643369E-2</v>
       </c>
-      <c r="AC10">
-        <f>AA10+AB10</f>
+      <c r="AM10">
+        <f>AK10+AL10</f>
         <v>40.366758790864871</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>23</v>
       </c>
@@ -3480,32 +3858,62 @@
       <c r="S11" s="73">
         <v>0.90633720079240732</v>
       </c>
-      <c r="T11" s="73">
-        <v>0</v>
-      </c>
-      <c r="U11" s="73"/>
-      <c r="X11">
+      <c r="T11" s="71">
+        <v>22.21</v>
+      </c>
+      <c r="U11" s="71">
+        <v>24.97</v>
+      </c>
+      <c r="V11" s="71">
+        <v>41.286000000000001</v>
+      </c>
+      <c r="W11" s="71">
+        <v>14.532999999999999</v>
+      </c>
+      <c r="X11" s="71">
+        <v>41.286000000000001</v>
+      </c>
+      <c r="Y11" s="71">
+        <v>660.91099999999994</v>
+      </c>
+      <c r="Z11" s="71">
+        <v>26</v>
+      </c>
+      <c r="AA11" s="72">
+        <v>50</v>
+      </c>
+      <c r="AB11" s="73">
+        <v>22.21</v>
+      </c>
+      <c r="AC11" s="73">
+        <v>0.90633720079240732</v>
+      </c>
+      <c r="AD11" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="73"/>
+      <c r="AH11">
         <v>639.10415070792988</v>
       </c>
-      <c r="Y11">
+      <c r="AI11">
         <v>0.53001711985689259</v>
       </c>
-      <c r="Z11">
-        <f t="shared" ref="Z11:Z21" si="2">X11+Y11</f>
+      <c r="AJ11">
+        <f t="shared" ref="AJ11:AJ21" si="2">AH11+AI11</f>
         <v>639.63416782778677</v>
       </c>
-      <c r="AA11">
+      <c r="AK11">
         <v>993.80073264760836</v>
       </c>
-      <c r="AB11">
+      <c r="AL11">
         <v>0.19579254162294349</v>
       </c>
-      <c r="AC11">
-        <f t="shared" ref="AC11:AC21" si="3">AA11+AB11</f>
+      <c r="AM11">
+        <f t="shared" ref="AM11:AM21" si="3">AK11+AL11</f>
         <v>993.99652518923131</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
@@ -3563,32 +3971,62 @@
       <c r="S12" s="73">
         <v>1.1820623069568268</v>
       </c>
-      <c r="T12" s="73">
-        <v>0</v>
-      </c>
-      <c r="U12" s="73"/>
-      <c r="X12">
+      <c r="T12" s="71">
+        <v>36.4</v>
+      </c>
+      <c r="U12" s="71">
+        <v>41.05</v>
+      </c>
+      <c r="V12" s="71">
+        <v>31.969000000000001</v>
+      </c>
+      <c r="W12" s="71">
+        <v>17.425000000000001</v>
+      </c>
+      <c r="X12" s="71">
+        <v>31.969000000000001</v>
+      </c>
+      <c r="Y12" s="71">
+        <v>752.81600000000003</v>
+      </c>
+      <c r="Z12" s="71">
+        <v>48.900001525878899</v>
+      </c>
+      <c r="AA12" s="72">
+        <v>100</v>
+      </c>
+      <c r="AB12" s="73">
+        <v>13.296832</v>
+      </c>
+      <c r="AC12" s="73">
+        <v>1.1820623069568268</v>
+      </c>
+      <c r="AD12" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="73"/>
+      <c r="AH12">
         <v>19.208734314891956</v>
       </c>
-      <c r="Y12">
+      <c r="AI12">
         <v>1.4390708093838975</v>
       </c>
-      <c r="Z12">
+      <c r="AJ12">
         <f t="shared" si="2"/>
         <v>20.647805124275852</v>
       </c>
-      <c r="AA12">
+      <c r="AK12">
         <v>27.387619255967515</v>
       </c>
-      <c r="AB12">
+      <c r="AL12">
         <v>0.13356807901983217</v>
       </c>
-      <c r="AC12">
+      <c r="AM12">
         <f t="shared" si="3"/>
         <v>27.521187334987346</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -3646,32 +4084,62 @@
       <c r="S13" s="73">
         <v>0.86769042919929373</v>
       </c>
-      <c r="T13" s="73">
-        <v>0</v>
-      </c>
-      <c r="U13" s="73"/>
-      <c r="X13">
+      <c r="T13" s="71">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="U13" s="71">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="V13" s="71">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="W13" s="71">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="X13" s="71">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="Y13" s="71">
+        <v>7.1970000000000001</v>
+      </c>
+      <c r="Z13" s="71">
+        <v>3.7000000476837154</v>
+      </c>
+      <c r="AA13" s="72">
+        <v>90</v>
+      </c>
+      <c r="AB13" s="73">
+        <v>3.2150660000000002</v>
+      </c>
+      <c r="AC13" s="73">
+        <v>0.86769042919929373</v>
+      </c>
+      <c r="AD13" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="73"/>
+      <c r="AH13">
         <v>8.0441472410106218</v>
       </c>
-      <c r="Y13">
+      <c r="AI13">
         <v>6.8025222126898502E-2</v>
       </c>
-      <c r="Z13">
+      <c r="AJ13">
         <f t="shared" si="2"/>
         <v>8.1121724631375205</v>
       </c>
-      <c r="AA13">
+      <c r="AK13">
         <v>9.458769751780995</v>
       </c>
-      <c r="AB13">
+      <c r="AL13">
         <v>7.5116168079741932E-3</v>
       </c>
-      <c r="AC13">
+      <c r="AM13">
         <f t="shared" si="3"/>
         <v>9.4662813685889695</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
@@ -3729,32 +4197,62 @@
       <c r="S14" s="73">
         <v>0.83613317023827116</v>
       </c>
-      <c r="T14" s="73">
-        <v>0</v>
-      </c>
-      <c r="U14" s="73"/>
-      <c r="X14">
+      <c r="T14" s="71">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="U14" s="71">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="V14" s="71">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="W14" s="71">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="X14" s="71">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="Y14" s="71">
+        <v>7.1970000000000001</v>
+      </c>
+      <c r="Z14" s="71">
+        <v>3.7000000476837154</v>
+      </c>
+      <c r="AA14" s="72">
+        <v>90</v>
+      </c>
+      <c r="AB14" s="73">
+        <v>3.2150660000000002</v>
+      </c>
+      <c r="AC14" s="73">
+        <v>0.83613317023827116</v>
+      </c>
+      <c r="AD14" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="73"/>
+      <c r="AH14">
         <v>1.728649515788488</v>
       </c>
-      <c r="Y14">
+      <c r="AI14">
         <v>4.6442748659862865E-2</v>
       </c>
-      <c r="Z14">
+      <c r="AJ14">
         <f t="shared" si="2"/>
         <v>1.7750922644483509</v>
       </c>
-      <c r="AA14">
+      <c r="AK14">
         <v>1.8922698715311803</v>
       </c>
-      <c r="AB14">
+      <c r="AL14">
         <v>2.1809956805283149E-3</v>
       </c>
-      <c r="AC14">
+      <c r="AM14">
         <f t="shared" si="3"/>
         <v>1.8944508672117086</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -3812,32 +4310,62 @@
       <c r="S15" s="73">
         <v>1.9503787502411295E-2</v>
       </c>
-      <c r="T15" s="73">
-        <v>0</v>
-      </c>
-      <c r="U15" s="73"/>
-      <c r="X15">
+      <c r="T15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="U15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="V15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="W15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="X15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="Y15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="Z15" s="71">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="AA15" s="72">
+        <v>30</v>
+      </c>
+      <c r="AB15" s="73">
+        <v>0.32149299999999997</v>
+      </c>
+      <c r="AC15" s="73">
+        <v>1.9503787502411295E-2</v>
+      </c>
+      <c r="AD15" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="73"/>
+      <c r="AH15">
         <v>0.47886752155609885</v>
       </c>
-      <c r="Y15">
+      <c r="AI15">
         <v>0.22128373782612412</v>
       </c>
-      <c r="Z15">
+      <c r="AJ15">
         <f t="shared" si="2"/>
         <v>0.700151259382223</v>
       </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15">
+      <c r="AK15">
+        <v>0</v>
+      </c>
+      <c r="AL15">
         <v>5.3987418408876558E-3</v>
       </c>
-      <c r="AC15">
+      <c r="AM15">
         <f t="shared" si="3"/>
         <v>5.3987418408876558E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -3893,32 +4421,60 @@
         <v>0.53048589000000002</v>
       </c>
       <c r="S16" s="73"/>
-      <c r="T16" s="73">
-        <v>0</v>
-      </c>
-      <c r="U16" s="73"/>
-      <c r="X16">
+      <c r="T16" s="71">
+        <v>0.57865500000000003</v>
+      </c>
+      <c r="U16" s="71">
+        <v>0.57865500000000003</v>
+      </c>
+      <c r="V16" s="71">
+        <v>0.103675</v>
+      </c>
+      <c r="W16" s="71">
+        <v>3.8569999999999998E-3</v>
+      </c>
+      <c r="X16" s="71">
+        <v>0.103675</v>
+      </c>
+      <c r="Y16" s="71">
+        <v>1.4394</v>
+      </c>
+      <c r="Z16" s="71">
+        <v>3.5150000452995296</v>
+      </c>
+      <c r="AA16" s="71">
+        <v>14.85</v>
+      </c>
+      <c r="AB16" s="73">
+        <v>0.53048589000000002</v>
+      </c>
+      <c r="AC16" s="73"/>
+      <c r="AD16" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="73"/>
+      <c r="AH16">
         <v>0.47390947465623479</v>
       </c>
-      <c r="Y16">
+      <c r="AI16">
         <v>4.2404984619842561E-3</v>
       </c>
-      <c r="Z16">
+      <c r="AJ16">
         <f t="shared" si="2"/>
         <v>0.47814997311821905</v>
       </c>
-      <c r="AA16">
+      <c r="AK16">
         <v>0.51210428280035414</v>
       </c>
-      <c r="AB16">
+      <c r="AL16">
         <v>2.0959176112987082E-4</v>
       </c>
-      <c r="AC16">
+      <c r="AM16">
         <f t="shared" si="3"/>
         <v>0.51231387456148403</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
@@ -3974,32 +4530,60 @@
         <v>1.3760482479999998</v>
       </c>
       <c r="S17" s="73"/>
-      <c r="T17" s="73">
-        <v>0</v>
-      </c>
-      <c r="U17" s="73"/>
-      <c r="X17">
+      <c r="T17" s="71">
+        <v>1.5009959999999998</v>
+      </c>
+      <c r="U17" s="71">
+        <v>1.5009959999999998</v>
+      </c>
+      <c r="V17" s="71">
+        <v>2.431</v>
+      </c>
+      <c r="W17" s="71">
+        <v>9.0440000000000006E-2</v>
+      </c>
+      <c r="X17" s="71">
+        <v>2.431</v>
+      </c>
+      <c r="Y17" s="71">
+        <v>3.0803159999999998</v>
+      </c>
+      <c r="Z17" s="71">
+        <v>0.18500000238418576</v>
+      </c>
+      <c r="AA17" s="71">
+        <v>38.519999999999996</v>
+      </c>
+      <c r="AB17" s="73">
+        <v>1.3760482479999998</v>
+      </c>
+      <c r="AC17" s="73"/>
+      <c r="AD17" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="73"/>
+      <c r="AH17">
         <v>0.24585827527712426</v>
       </c>
-      <c r="Y17">
+      <c r="AI17">
         <v>2.0700811243651359E-2</v>
       </c>
-      <c r="Z17">
+      <c r="AJ17">
         <f t="shared" si="2"/>
         <v>0.26655908652077559</v>
       </c>
-      <c r="AA17">
+      <c r="AK17">
         <v>7.6630038890183744E-2</v>
       </c>
-      <c r="AB17">
+      <c r="AL17">
         <v>3.7216049065244534E-4</v>
       </c>
-      <c r="AC17">
+      <c r="AM17">
         <f t="shared" si="3"/>
         <v>7.7002199380836189E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
@@ -4055,32 +4639,60 @@
         <v>1.06</v>
       </c>
       <c r="S18" s="73"/>
-      <c r="T18" s="73">
-        <v>0</v>
-      </c>
-      <c r="U18" s="73"/>
-      <c r="X18">
+      <c r="T18" s="71">
+        <v>1.06</v>
+      </c>
+      <c r="U18" s="71">
+        <v>1.06</v>
+      </c>
+      <c r="V18" s="71">
+        <v>1.056</v>
+      </c>
+      <c r="W18" s="71">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="X18" s="71">
+        <v>1.056</v>
+      </c>
+      <c r="Y18" s="71">
+        <v>392.35399999999998</v>
+      </c>
+      <c r="Z18" s="71">
+        <v>49</v>
+      </c>
+      <c r="AA18" s="72">
+        <v>2.85</v>
+      </c>
+      <c r="AB18" s="73">
+        <v>1.06</v>
+      </c>
+      <c r="AC18" s="73"/>
+      <c r="AD18" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="73"/>
+      <c r="AH18">
         <v>3.4141251927898666</v>
       </c>
-      <c r="Y18">
+      <c r="AI18">
         <v>1.0718762615156343</v>
       </c>
-      <c r="Z18">
+      <c r="AJ18">
         <f t="shared" si="2"/>
         <v>4.4860014543055007</v>
       </c>
-      <c r="AA18">
-        <v>0</v>
-      </c>
-      <c r="AB18">
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
         <v>0.11248755052026857</v>
       </c>
-      <c r="AC18">
+      <c r="AM18">
         <f t="shared" si="3"/>
         <v>0.11248755052026857</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>30</v>
       </c>
@@ -4136,32 +4748,60 @@
         <v>0.40123199999999998</v>
       </c>
       <c r="S19" s="73"/>
-      <c r="T19" s="73">
-        <v>0</v>
-      </c>
-      <c r="U19" s="73"/>
-      <c r="X19">
+      <c r="T19" s="71">
+        <v>0.75</v>
+      </c>
+      <c r="U19" s="71">
+        <v>0.35</v>
+      </c>
+      <c r="V19" s="71">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="W19" s="71">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="X19" s="71">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="Y19" s="71">
+        <v>0.111</v>
+      </c>
+      <c r="Z19" s="71">
+        <v>1.1000000238418579</v>
+      </c>
+      <c r="AA19" s="72">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="73">
+        <v>0.40123199999999998</v>
+      </c>
+      <c r="AC19" s="73"/>
+      <c r="AD19" s="73">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="73"/>
+      <c r="AH19">
         <v>0.91142919415811929</v>
       </c>
-      <c r="Y19">
+      <c r="AI19">
         <v>1.1802078079887578E-2</v>
       </c>
-      <c r="Z19">
+      <c r="AJ19">
         <f t="shared" si="2"/>
         <v>0.92323127223800683</v>
       </c>
-      <c r="AA19">
+      <c r="AK19">
         <v>0.18877324129794976</v>
       </c>
-      <c r="AB19">
+      <c r="AL19">
         <v>3.4778154884700514E-4</v>
       </c>
-      <c r="AC19">
+      <c r="AM19">
         <f t="shared" si="3"/>
         <v>0.18912102284679677</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>31</v>
       </c>
@@ -4219,44 +4859,74 @@
       <c r="S20" s="146">
         <v>59412.682265174597</v>
       </c>
-      <c r="T20" s="122">
+      <c r="T20" s="5">
+        <v>59366.949503269869</v>
+      </c>
+      <c r="U20" s="5">
+        <v>59362.612360412735</v>
+      </c>
+      <c r="V20" s="5">
+        <v>59341.609065174642</v>
+      </c>
+      <c r="W20" s="5">
+        <v>59385.872043746065</v>
+      </c>
+      <c r="X20" s="2">
+        <v>59341.609065174642</v>
+      </c>
+      <c r="Y20" s="5">
+        <v>56889.786903269873</v>
+      </c>
+      <c r="Z20" s="5">
+        <v>59229.283455650831</v>
+      </c>
+      <c r="AA20" s="5">
+        <v>59014.60666993654</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>59366.949503269869</v>
+      </c>
+      <c r="AC20" s="146">
+        <v>59412.682265174597</v>
+      </c>
+      <c r="AD20" s="122">
         <f>12/106*44/12</f>
         <v>0.41509433962264147</v>
       </c>
-      <c r="U20" s="2">
+      <c r="AE20" s="2">
         <f>12*7/(12*7+8*1)*44/12</f>
         <v>3.3478260869565215</v>
       </c>
-      <c r="V20">
+      <c r="AF20">
         <f>-12*6/(12*6+10*1+4*16)*44/12</f>
         <v>-1.8082191780821917</v>
       </c>
-      <c r="W20" s="144">
+      <c r="AG20" s="144">
         <f>-12*6/(12*6+8*1+5*16)*44/12</f>
         <v>-1.6500000000000001</v>
       </c>
-      <c r="X20">
+      <c r="AH20">
         <v>71783.505317547926</v>
       </c>
-      <c r="Y20">
+      <c r="AI20">
         <v>611.91676387079497</v>
       </c>
-      <c r="Z20">
+      <c r="AJ20">
         <f t="shared" si="2"/>
         <v>72395.422081418714</v>
       </c>
-      <c r="AA20">
+      <c r="AK20">
         <v>74927.07400875607</v>
       </c>
-      <c r="AB20">
+      <c r="AL20">
         <v>92.564589004961775</v>
       </c>
-      <c r="AC20">
+      <c r="AM20">
         <f t="shared" si="3"/>
         <v>75019.638597761033</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>32</v>
       </c>
@@ -4279,63 +4949,105 @@
       <c r="Q21" s="69"/>
       <c r="R21" s="69"/>
       <c r="S21" s="69"/>
-      <c r="X21">
+      <c r="T21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="U21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="V21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="W21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="X21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="Y21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="Z21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="AA21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="AB21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="AC21" s="69">
+        <v>-59412.682265174633</v>
+      </c>
+      <c r="AH21">
         <v>-72964.246146966863</v>
       </c>
-      <c r="Z21">
+      <c r="AJ21">
         <f t="shared" si="2"/>
         <v>-72964.246146966863</v>
       </c>
-      <c r="AA21">
+      <c r="AK21">
         <v>-76614.526624731123</v>
       </c>
-      <c r="AC21">
+      <c r="AM21">
         <f t="shared" si="3"/>
         <v>-76614.526624731123</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="P22" s="74"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="147" t="s">
+      <c r="B23" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="147"/>
-      <c r="D23" s="147"/>
-      <c r="E23" s="147"/>
-      <c r="F23" s="147"/>
-      <c r="G23" s="147"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="147"/>
-      <c r="J23" s="147"/>
-      <c r="K23" s="147"/>
-      <c r="L23" s="147"/>
-      <c r="M23" s="147"/>
-      <c r="N23" s="147"/>
-      <c r="O23" s="147"/>
-      <c r="P23" s="147"/>
-      <c r="Q23" s="147"/>
-      <c r="R23" s="147"/>
+      <c r="C23" s="148"/>
+      <c r="D23" s="148"/>
+      <c r="E23" s="148"/>
+      <c r="F23" s="148"/>
+      <c r="G23" s="148"/>
+      <c r="H23" s="148"/>
+      <c r="I23" s="148"/>
+      <c r="J23" s="148"/>
+      <c r="K23" s="148"/>
+      <c r="L23" s="148"/>
+      <c r="M23" s="148"/>
+      <c r="N23" s="148"/>
+      <c r="O23" s="148"/>
+      <c r="P23" s="148"/>
+      <c r="Q23" s="148"/>
+      <c r="R23" s="148"/>
       <c r="S23" s="143" t="s">
         <v>332</v>
       </c>
-      <c r="T23" t="s">
+      <c r="T23" s="147" t="s">
+        <v>337</v>
+      </c>
+      <c r="U23" s="147"/>
+      <c r="V23" s="147"/>
+      <c r="W23" s="147"/>
+      <c r="X23" s="147"/>
+      <c r="Y23" s="147"/>
+      <c r="Z23" s="147"/>
+      <c r="AA23" s="147"/>
+      <c r="AB23" s="147"/>
+      <c r="AC23" s="147"/>
+      <c r="AD23" t="s">
         <v>90</v>
       </c>
-      <c r="Y23" s="76" t="s">
+      <c r="AI23" s="76" t="s">
         <v>317</v>
       </c>
-      <c r="Z23" s="76"/>
-      <c r="AA23" s="76"/>
-      <c r="AB23" s="76" t="s">
+      <c r="AJ23" s="76"/>
+      <c r="AK23" s="76"/>
+      <c r="AL23" s="76" t="s">
         <v>317</v>
       </c>
-      <c r="AC23" s="76"/>
+      <c r="AM23" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6122,7 +6834,7 @@
       </c>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.35">
-      <c r="B12" s="148" t="s">
+      <c r="B12" s="149" t="s">
         <v>291</v>
       </c>
       <c r="C12" s="105" t="s">
@@ -6140,7 +6852,7 @@
       <c r="M12" s="107"/>
     </row>
     <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="149"/>
+      <c r="B13" s="150"/>
       <c r="C13" s="108" t="s">
         <v>1</v>
       </c>
@@ -6628,7 +7340,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="120"/>
-      <c r="B25" s="148" t="s">
+      <c r="B25" s="149" t="s">
         <v>291</v>
       </c>
       <c r="C25" s="105" t="s">
@@ -6647,7 +7359,7 @@
     </row>
     <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="84"/>
-      <c r="B26" s="149"/>
+      <c r="B26" s="150"/>
       <c r="C26" s="108" t="s">
         <v>1</v>
       </c>
@@ -7327,10 +8039,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7340,7 +8052,7 @@
     <col min="4" max="4" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -7354,52 +8066,55 @@
         <v>14</v>
       </c>
       <c r="F1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G1" t="s">
         <v>243</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>320</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>333</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>29</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>30</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>31</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="136" t="s">
         <v>123</v>
       </c>
@@ -7419,10 +8134,10 @@
         <v>185</v>
       </c>
       <c r="G2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" t="s">
         <v>321</v>
-      </c>
-      <c r="H2" t="s">
-        <v>318</v>
       </c>
       <c r="I2" t="s">
         <v>318</v>
@@ -7460,8 +8175,11 @@
       <c r="T2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>126</v>
       </c>
@@ -7481,7 +8199,7 @@
         <v>125</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
         <v>93</v>
@@ -7522,8 +8240,11 @@
       <c r="T3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -7539,7 +8260,7 @@
       <c r="E4" s="68">
         <v>104261.00625785353</v>
       </c>
-      <c r="F4" s="76">
+      <c r="F4" s="68">
         <v>0</v>
       </c>
       <c r="G4" s="76">
@@ -7548,7 +8269,7 @@
       <c r="H4" s="76">
         <v>0</v>
       </c>
-      <c r="I4" s="38">
+      <c r="I4" s="76">
         <v>0</v>
       </c>
       <c r="J4" s="38">
@@ -7584,8 +8305,11 @@
       <c r="T4" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -7601,7 +8325,7 @@
       <c r="E5" s="68">
         <v>103489.85649124274</v>
       </c>
-      <c r="F5" s="76">
+      <c r="F5" s="68">
         <v>0</v>
       </c>
       <c r="G5" s="76">
@@ -7610,7 +8334,7 @@
       <c r="H5" s="76">
         <v>0</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="76">
         <v>0</v>
       </c>
       <c r="J5" s="38">
@@ -7646,8 +8370,11 @@
       <c r="T5" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -7663,7 +8390,7 @@
       <c r="E6" s="68">
         <v>1078.8033372105469</v>
       </c>
-      <c r="F6" s="76">
+      <c r="F6" s="68">
         <v>0</v>
       </c>
       <c r="G6" s="76">
@@ -7672,7 +8399,7 @@
       <c r="H6" s="76">
         <v>0</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="76">
         <v>0</v>
       </c>
       <c r="J6" s="38">
@@ -7708,8 +8435,11 @@
       <c r="T6" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U6" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7725,7 +8455,7 @@
       <c r="E7" s="68">
         <v>98380.297877359611</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="68">
         <v>0</v>
       </c>
       <c r="G7" s="76">
@@ -7734,7 +8464,7 @@
       <c r="H7" s="76">
         <v>0</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="76">
         <v>0</v>
       </c>
       <c r="J7" s="38">
@@ -7770,8 +8500,11 @@
       <c r="T7" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -7787,7 +8520,7 @@
       <c r="E8" s="68">
         <v>4030.7552766725985</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="68">
         <v>0</v>
       </c>
       <c r="G8" s="76">
@@ -7796,7 +8529,7 @@
       <c r="H8" s="76">
         <v>0</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="76">
         <v>0</v>
       </c>
       <c r="J8" s="38">
@@ -7832,8 +8565,11 @@
       <c r="T8" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U8" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -7849,7 +8585,7 @@
       <c r="E9" s="68">
         <v>3.211633491944839</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F9" s="68">
         <v>0</v>
       </c>
       <c r="G9" s="76">
@@ -7858,7 +8594,7 @@
       <c r="H9" s="76">
         <v>0</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="76">
         <v>0</v>
       </c>
       <c r="J9" s="38">
@@ -7894,8 +8630,11 @@
       <c r="T9" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U9" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -7911,8 +8650,8 @@
       <c r="E10">
         <v>10.287405417696785</v>
       </c>
-      <c r="F10" s="76">
-        <v>0</v>
+      <c r="F10">
+        <v>-28.216209696614314</v>
       </c>
       <c r="G10" s="76">
         <v>0</v>
@@ -7920,12 +8659,12 @@
       <c r="H10" s="76">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="76">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="J10" s="38">
-        <v>0</v>
-      </c>
       <c r="K10" s="38">
         <v>0</v>
       </c>
@@ -7956,8 +8695,11 @@
       <c r="T10" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U10" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -7973,8 +8715,8 @@
       <c r="E11">
         <v>31.26772994989345</v>
       </c>
-      <c r="F11" s="76">
-        <v>0</v>
+      <c r="F11">
+        <v>-42.331377382329954</v>
       </c>
       <c r="G11" s="76">
         <v>0</v>
@@ -7982,15 +8724,15 @@
       <c r="H11" s="76">
         <v>0</v>
       </c>
-      <c r="I11" s="38">
-        <v>0</v>
-      </c>
-      <c r="J11">
+      <c r="I11" s="76">
+        <v>0</v>
+      </c>
+      <c r="J11" s="38">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="K11" s="38">
-        <v>0</v>
-      </c>
       <c r="L11" s="38">
         <v>0</v>
       </c>
@@ -8018,8 +8760,11 @@
       <c r="T11" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U11" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -8035,8 +8780,8 @@
       <c r="E12">
         <v>36.291301237350226</v>
       </c>
-      <c r="F12" s="76">
-        <v>0</v>
+      <c r="F12">
+        <v>-13.685436653377941</v>
       </c>
       <c r="G12" s="76">
         <v>0</v>
@@ -8044,18 +8789,18 @@
       <c r="H12" s="76">
         <v>0</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I12" s="76">
         <v>0</v>
       </c>
       <c r="J12" s="38">
         <v>0</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="38">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>1</v>
       </c>
-      <c r="L12" s="38">
-        <v>0</v>
-      </c>
       <c r="M12" s="38">
         <v>0</v>
       </c>
@@ -8080,8 +8825,11 @@
       <c r="T12" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U12" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -8097,8 +8845,8 @@
       <c r="E13">
         <v>0.42153625660303229</v>
       </c>
-      <c r="F13" s="76">
-        <v>0</v>
+      <c r="F13">
+        <v>-5.4061596857689773</v>
       </c>
       <c r="G13" s="76">
         <v>0</v>
@@ -8106,7 +8854,7 @@
       <c r="H13" s="76">
         <v>0</v>
       </c>
-      <c r="I13" s="38">
+      <c r="I13" s="76">
         <v>0</v>
       </c>
       <c r="J13" s="38">
@@ -8115,12 +8863,12 @@
       <c r="K13" s="38">
         <v>0</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="38">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>1</v>
       </c>
-      <c r="M13" s="38">
-        <v>0</v>
-      </c>
       <c r="N13" s="38">
         <v>0</v>
       </c>
@@ -8142,8 +8890,11 @@
       <c r="T13" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U13" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -8159,8 +8910,8 @@
       <c r="E14">
         <v>0.37894052180007021</v>
       </c>
-      <c r="F14" s="76">
-        <v>0</v>
+      <c r="F14">
+        <v>-5.4061596857689773</v>
       </c>
       <c r="G14" s="76">
         <v>0</v>
@@ -8168,7 +8919,7 @@
       <c r="H14" s="76">
         <v>0</v>
       </c>
-      <c r="I14" s="38">
+      <c r="I14" s="76">
         <v>0</v>
       </c>
       <c r="J14" s="38">
@@ -8180,12 +8931,12 @@
       <c r="L14" s="38">
         <v>0</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="38">
+        <v>0</v>
+      </c>
+      <c r="N14">
         <v>1</v>
       </c>
-      <c r="N14" s="38">
-        <v>0</v>
-      </c>
       <c r="O14" s="38">
         <v>0</v>
       </c>
@@ -8204,8 +8955,11 @@
       <c r="T14" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U14" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -8221,8 +8975,8 @@
       <c r="E15">
         <v>11.120378048826899</v>
       </c>
-      <c r="F15" s="76">
-        <v>0</v>
+      <c r="F15">
+        <v>-0.27393692777212614</v>
       </c>
       <c r="G15" s="76">
         <v>0</v>
@@ -8230,7 +8984,7 @@
       <c r="H15" s="76">
         <v>0</v>
       </c>
-      <c r="I15" s="38">
+      <c r="I15" s="76">
         <v>0</v>
       </c>
       <c r="J15" s="38">
@@ -8245,12 +8999,12 @@
       <c r="M15" s="38">
         <v>0</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="38">
+        <v>0</v>
+      </c>
+      <c r="O15">
         <v>1</v>
       </c>
-      <c r="O15" s="38">
-        <v>0</v>
-      </c>
       <c r="P15" s="38">
         <v>0</v>
       </c>
@@ -8266,8 +9020,11 @@
       <c r="T15" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U15" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -8283,8 +9040,8 @@
       <c r="E16">
         <v>9.919204253941645E-2</v>
       </c>
-      <c r="F16" s="76">
-        <v>0</v>
+      <c r="F16">
+        <v>-5.72954763659021</v>
       </c>
       <c r="G16" s="76">
         <v>0</v>
@@ -8292,7 +9049,7 @@
       <c r="H16" s="76">
         <v>0</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="76">
         <v>0</v>
       </c>
       <c r="J16" s="38">
@@ -8310,12 +9067,12 @@
       <c r="N16" s="38">
         <v>0</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="38">
+        <v>0</v>
+      </c>
+      <c r="P16">
         <v>1</v>
       </c>
-      <c r="P16" s="38">
-        <v>0</v>
-      </c>
       <c r="Q16" s="38">
         <v>0</v>
       </c>
@@ -8328,8 +9085,11 @@
       <c r="T16" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U16" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -8345,8 +9105,8 @@
       <c r="E17">
         <v>0.14325167839344721</v>
       </c>
-      <c r="F17" s="76">
-        <v>0</v>
+      <c r="F17">
+        <v>0.13580324168234237</v>
       </c>
       <c r="G17" s="76">
         <v>0</v>
@@ -8354,7 +9114,7 @@
       <c r="H17" s="76">
         <v>0</v>
       </c>
-      <c r="I17" s="38">
+      <c r="I17" s="76">
         <v>0</v>
       </c>
       <c r="J17" s="38">
@@ -8375,12 +9135,12 @@
       <c r="O17" s="38">
         <v>0</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q17">
         <v>1</v>
       </c>
-      <c r="Q17" s="38">
-        <v>0</v>
-      </c>
       <c r="R17" s="38">
         <v>0</v>
       </c>
@@ -8390,8 +9150,11 @@
       <c r="T17" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U17" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -8407,8 +9170,8 @@
       <c r="E18">
         <v>216.35815892748519</v>
       </c>
-      <c r="F18" s="76">
-        <v>0</v>
+      <c r="F18">
+        <v>384.29844655783586</v>
       </c>
       <c r="G18" s="76">
         <v>0</v>
@@ -8416,7 +9179,7 @@
       <c r="H18" s="76">
         <v>0</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I18" s="76">
         <v>0</v>
       </c>
       <c r="J18" s="38">
@@ -8440,20 +9203,23 @@
       <c r="P18" s="38">
         <v>0</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="38">
+        <v>0</v>
+      </c>
+      <c r="R18">
         <v>1</v>
       </c>
-      <c r="R18" s="38">
-        <v>0</v>
-      </c>
       <c r="S18" s="38">
         <v>0</v>
       </c>
       <c r="T18" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U18" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -8469,8 +9235,8 @@
       <c r="E19">
         <v>1.4196658578962942</v>
       </c>
-      <c r="F19" s="76">
-        <v>0</v>
+      <c r="F19">
+        <v>-1.3019529375153069</v>
       </c>
       <c r="G19" s="76">
         <v>0</v>
@@ -8478,7 +9244,7 @@
       <c r="H19" s="76">
         <v>0</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="76">
         <v>0</v>
       </c>
       <c r="J19" s="38">
@@ -8505,17 +9271,20 @@
       <c r="Q19" s="38">
         <v>0</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="38">
+        <v>0</v>
+      </c>
+      <c r="S19">
         <v>1</v>
       </c>
-      <c r="S19" s="38">
-        <v>0</v>
-      </c>
       <c r="T19" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U19" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -8531,8 +9300,8 @@
       <c r="E20">
         <v>6135.9109157721377</v>
       </c>
-      <c r="F20" s="76">
-        <v>0</v>
+      <c r="F20">
+        <v>258.20196307358003</v>
       </c>
       <c r="G20" s="76">
         <v>0</v>
@@ -8540,7 +9309,7 @@
       <c r="H20" s="76">
         <v>0</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="76">
         <v>0</v>
       </c>
       <c r="J20" s="38">
@@ -8570,18 +9339,20 @@
       <c r="R20" s="38">
         <v>0</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="38">
+        <v>0</v>
+      </c>
+      <c r="T20">
         <v>1</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F21" s="38"/>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="G21" s="38"/>
       <c r="H21" s="38"/>
-      <c r="K21" s="38"/>
+      <c r="I21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
       <c r="N21" s="38"/>
@@ -8590,18 +9361,21 @@
       <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
       <c r="S21" s="38"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T21" s="38"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="147" t="s">
+      <c r="B22" s="148" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="147"/>
-      <c r="D22" s="147"/>
-      <c r="E22" s="147"/>
-      <c r="L22" s="38"/>
+      <c r="C22" s="148"/>
+      <c r="D22" s="148"/>
+      <c r="E22" s="148"/>
+      <c r="F22" s="147" t="s">
+        <v>336</v>
+      </c>
       <c r="M22" s="38"/>
       <c r="N22" s="38"/>
       <c r="O22" s="38"/>
@@ -8609,9 +9383,9 @@
       <c r="Q22" s="38"/>
       <c r="R22" s="38"/>
       <c r="S22" s="38"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="L23" s="38"/>
+      <c r="T22" s="38"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
       <c r="O23" s="38"/>
@@ -8619,8 +9393,9 @@
       <c r="Q23" s="38"/>
       <c r="R23" s="38"/>
       <c r="S23" s="38"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T23" s="38"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -8629,15 +9404,16 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="M24" s="38"/>
+      <c r="J24" s="6"/>
       <c r="N24" s="38"/>
       <c r="O24" s="38"/>
       <c r="P24" s="38"/>
       <c r="Q24" s="38"/>
       <c r="R24" s="38"/>
       <c r="S24" s="38"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T24" s="38"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -8646,14 +9422,15 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="N25" s="38"/>
+      <c r="J25" s="3"/>
       <c r="O25" s="38"/>
       <c r="P25" s="38"/>
       <c r="Q25" s="38"/>
       <c r="R25" s="38"/>
       <c r="S25" s="38"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T25" s="38"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -8662,13 +9439,14 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
-      <c r="O26" s="38"/>
+      <c r="J26" s="4"/>
       <c r="P26" s="38"/>
       <c r="Q26" s="38"/>
       <c r="R26" s="38"/>
       <c r="S26" s="38"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T26" s="38"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -8677,12 +9455,13 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
-      <c r="P27" s="38"/>
+      <c r="J27" s="4"/>
       <c r="Q27" s="38"/>
       <c r="R27" s="38"/>
       <c r="S27" s="38"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T27" s="38"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -8691,11 +9470,12 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-      <c r="Q28" s="38"/>
+      <c r="J28" s="4"/>
       <c r="R28" s="38"/>
       <c r="S28" s="38"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T28" s="38"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -8704,10 +9484,11 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="R29" s="38"/>
+      <c r="J29" s="4"/>
       <c r="S29" s="38"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T29" s="38"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -8716,9 +9497,10 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="S30" s="38"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="J30" s="4"/>
+      <c r="T30" s="38"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -8727,8 +9509,9 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -8737,8 +9520,9 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -8747,8 +9531,9 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -8757,8 +9542,9 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -8767,8 +9553,9 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -8776,9 +9563,10 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I36" s="2"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -8787,6 +9575,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11355,39 +12144,39 @@
       <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="147" t="s">
+      <c r="B23" s="148" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="147"/>
-      <c r="D23" s="147"/>
-      <c r="E23" s="147"/>
-      <c r="F23" s="147"/>
-      <c r="G23" s="147"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="147"/>
-      <c r="J23" s="147"/>
-      <c r="K23" s="147"/>
-      <c r="L23" s="147"/>
-      <c r="M23" s="147"/>
-      <c r="N23" s="147"/>
-      <c r="O23" s="147"/>
-      <c r="P23" s="147"/>
-      <c r="Q23" s="147"/>
-      <c r="R23" s="147"/>
-      <c r="S23" s="147"/>
-      <c r="T23" s="147"/>
-      <c r="U23" s="147"/>
-      <c r="V23" s="147"/>
-      <c r="W23" s="147"/>
-      <c r="X23" s="147"/>
-      <c r="Y23" s="147"/>
-      <c r="Z23" s="147"/>
-      <c r="AA23" s="147"/>
-      <c r="AB23" s="147"/>
-      <c r="AC23" s="147"/>
-      <c r="AD23" s="147"/>
-      <c r="AE23" s="147"/>
-      <c r="AF23" s="147"/>
+      <c r="C23" s="148"/>
+      <c r="D23" s="148"/>
+      <c r="E23" s="148"/>
+      <c r="F23" s="148"/>
+      <c r="G23" s="148"/>
+      <c r="H23" s="148"/>
+      <c r="I23" s="148"/>
+      <c r="J23" s="148"/>
+      <c r="K23" s="148"/>
+      <c r="L23" s="148"/>
+      <c r="M23" s="148"/>
+      <c r="N23" s="148"/>
+      <c r="O23" s="148"/>
+      <c r="P23" s="148"/>
+      <c r="Q23" s="148"/>
+      <c r="R23" s="148"/>
+      <c r="S23" s="148"/>
+      <c r="T23" s="148"/>
+      <c r="U23" s="148"/>
+      <c r="V23" s="148"/>
+      <c r="W23" s="148"/>
+      <c r="X23" s="148"/>
+      <c r="Y23" s="148"/>
+      <c r="Z23" s="148"/>
+      <c r="AA23" s="148"/>
+      <c r="AB23" s="148"/>
+      <c r="AC23" s="148"/>
+      <c r="AD23" s="148"/>
+      <c r="AE23" s="148"/>
+      <c r="AF23" s="148"/>
       <c r="AI23" t="s">
         <v>305</v>
       </c>
@@ -12546,22 +13335,22 @@
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="147" t="s">
+      <c r="B23" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="147"/>
-      <c r="D23" s="147"/>
-      <c r="E23" s="147"/>
-      <c r="F23" s="147"/>
-      <c r="G23" s="147"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="147"/>
-      <c r="J23" s="147"/>
-      <c r="K23" s="147"/>
-      <c r="L23" s="147"/>
-      <c r="M23" s="147"/>
-      <c r="N23" s="147"/>
-      <c r="O23" s="147"/>
+      <c r="C23" s="148"/>
+      <c r="D23" s="148"/>
+      <c r="E23" s="148"/>
+      <c r="F23" s="148"/>
+      <c r="G23" s="148"/>
+      <c r="H23" s="148"/>
+      <c r="I23" s="148"/>
+      <c r="J23" s="148"/>
+      <c r="K23" s="148"/>
+      <c r="L23" s="148"/>
+      <c r="M23" s="148"/>
+      <c r="N23" s="148"/>
+      <c r="O23" s="148"/>
       <c r="P23" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Added fossil energy metric
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004F3BA0-4FE1-4EAE-8E51-47311D46F94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08BFD6B-54DD-4A73-B133-CF6DBF879C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -1341,7 +1341,7 @@
     <numFmt numFmtId="172" formatCode="#,##0.0000000000"/>
     <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1387,12 +1387,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2663,8 +2657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:AM23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -9590,9 +9584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
   <dimension ref="A1:AO23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ1" sqref="AJ1:AO1"/>
+      <selection pane="topRight" activeCell="AF27" sqref="AF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10076,7 +10070,7 @@
         <v>0</v>
       </c>
       <c r="AG4">
-        <v>315314.54817417532</v>
+        <v>1315314.5481741754</v>
       </c>
       <c r="AH4" s="25">
         <v>99.15771301835683</v>
@@ -10201,7 +10195,7 @@
         <v>0</v>
       </c>
       <c r="AG5">
-        <v>311743.85319645284</v>
+        <v>1311743.8531964528</v>
       </c>
       <c r="AH5" s="25">
         <v>99.10102802045931</v>
@@ -10451,7 +10445,7 @@
         <v>0</v>
       </c>
       <c r="AG7">
-        <v>301825.3866966911</v>
+        <v>1301825.3866966912</v>
       </c>
       <c r="AH7" s="25">
         <v>87.624663165139467</v>

</xml_diff>

<commit_message>
Added biochem via acids and sludge HTL with NH3 removal
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E38FDF-C065-4C44-8D3C-29148033D131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7721CA53-3755-443D-B165-43A53A5DEC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" activeTab="7" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" activeTab="8" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="341">
   <si>
     <t>NG</t>
   </si>
@@ -1325,6 +1325,12 @@
   </si>
   <si>
     <t>GGE</t>
+  </si>
+  <si>
+    <t>Renewable Diesel - Bichem (BDO)</t>
+  </si>
+  <si>
+    <t>Renewable Diesel - Biochem (Acids)</t>
   </si>
 </sst>
 </file>
@@ -1643,7 +1649,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1932,6 +1938,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1941,13 +1957,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2665,21 +2674,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
-  <dimension ref="A1:AM23"/>
+  <dimension ref="A1:AS23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T24" sqref="T24"/>
+      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.08984375" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1796875" style="142"/>
-    <col min="38" max="38" width="13.7265625" customWidth="1"/>
+    <col min="41" max="41" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" ht="26.5" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2794,8 +2803,26 @@
       <c r="AM1" s="121" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" ht="78.5" x14ac:dyDescent="0.35">
+      <c r="AN1" s="121" t="s">
+        <v>339</v>
+      </c>
+      <c r="AO1" s="121" t="s">
+        <v>339</v>
+      </c>
+      <c r="AP1" s="121" t="s">
+        <v>339</v>
+      </c>
+      <c r="AQ1" s="121" t="s">
+        <v>340</v>
+      </c>
+      <c r="AR1" s="121" t="s">
+        <v>340</v>
+      </c>
+      <c r="AS1" s="121" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" ht="78.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -2911,8 +2938,26 @@
       <c r="AM2" s="139" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN2" s="139" t="s">
+        <v>311</v>
+      </c>
+      <c r="AO2" s="139" t="s">
+        <v>314</v>
+      </c>
+      <c r="AP2" s="139" t="s">
+        <v>315</v>
+      </c>
+      <c r="AQ2" s="139" t="s">
+        <v>311</v>
+      </c>
+      <c r="AR2" s="139" t="s">
+        <v>314</v>
+      </c>
+      <c r="AS2" s="139" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>125</v>
       </c>
@@ -3013,7 +3058,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3125,8 +3170,28 @@
         <f>AK4+AL4</f>
         <v>1001250.3090024699</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AO4">
+        <v>1250.309002469897</v>
+      </c>
+      <c r="AP4">
+        <f>AN4+AO4</f>
+        <v>1001250.3090024699</v>
+      </c>
+      <c r="AQ4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AR4">
+        <v>1250.309002469897</v>
+      </c>
+      <c r="AS4">
+        <f>AQ4+AR4</f>
+        <v>1001250.3090024699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3238,8 +3303,28 @@
         <f t="shared" ref="AM5:AM9" si="1">AK5+AL5</f>
         <v>1199.1725344773329</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>1199.1725344773329</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" ref="AP5:AP9" si="2">AN5+AO5</f>
+        <v>1199.1725344773329</v>
+      </c>
+      <c r="AQ5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>1199.1725344773329</v>
+      </c>
+      <c r="AS5">
+        <f t="shared" ref="AS5:AS9" si="3">AQ5+AR5</f>
+        <v>1199.1725344773329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3351,8 +3436,28 @@
         <f t="shared" si="1"/>
         <v>8.0912620107395146</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>8.0912620107395146</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" si="2"/>
+        <v>8.0912620107395146</v>
+      </c>
+      <c r="AQ6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>8.0912620107395146</v>
+      </c>
+      <c r="AS6">
+        <f t="shared" si="3"/>
+        <v>8.0912620107395146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3464,8 +3569,28 @@
         <f t="shared" si="1"/>
         <v>124.60248498831356</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>124.60248498831356</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" si="2"/>
+        <v>124.60248498831356</v>
+      </c>
+      <c r="AQ7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>124.60248498831356</v>
+      </c>
+      <c r="AS7">
+        <f t="shared" si="3"/>
+        <v>124.60248498831356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3577,8 +3702,28 @@
         <f t="shared" si="1"/>
         <v>1066.4787874782799</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>1066.4787874782799</v>
+      </c>
+      <c r="AP8">
+        <f t="shared" si="2"/>
+        <v>1066.4787874782799</v>
+      </c>
+      <c r="AQ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>1066.4787874782799</v>
+      </c>
+      <c r="AS8">
+        <f t="shared" si="3"/>
+        <v>1066.4787874782799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3690,8 +3835,28 @@
         <f t="shared" si="1"/>
         <v>2.3217600680931635E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>2.3217600680931635E-2</v>
+      </c>
+      <c r="AP9">
+        <f t="shared" si="2"/>
+        <v>2.3217600680931635E-2</v>
+      </c>
+      <c r="AQ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>2.3217600680931635E-2</v>
+      </c>
+      <c r="AS9">
+        <f t="shared" si="3"/>
+        <v>2.3217600680931635E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
@@ -3803,8 +3968,28 @@
         <f>AK10+AL10</f>
         <v>40.366758790864871</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN10">
+        <v>40.352647182660228</v>
+      </c>
+      <c r="AO10">
+        <v>1.4111608204643369E-2</v>
+      </c>
+      <c r="AP10">
+        <f>AN10+AO10</f>
+        <v>40.366758790864871</v>
+      </c>
+      <c r="AQ10">
+        <v>40.352647182660228</v>
+      </c>
+      <c r="AR10">
+        <v>1.4111608204643369E-2</v>
+      </c>
+      <c r="AS10">
+        <f>AQ10+AR10</f>
+        <v>40.366758790864871</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>23</v>
       </c>
@@ -3903,7 +4088,7 @@
         <v>0.53001711985689259</v>
       </c>
       <c r="AJ11">
-        <f t="shared" ref="AJ11:AJ21" si="2">AH11+AI11</f>
+        <f t="shared" ref="AJ11:AJ21" si="4">AH11+AI11</f>
         <v>639.63416782778677</v>
       </c>
       <c r="AK11">
@@ -3913,11 +4098,31 @@
         <v>0.19579254162294349</v>
       </c>
       <c r="AM11">
-        <f t="shared" ref="AM11:AM21" si="3">AK11+AL11</f>
+        <f t="shared" ref="AM11:AM21" si="5">AK11+AL11</f>
         <v>993.99652518923131</v>
       </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN11">
+        <v>993.80073264760836</v>
+      </c>
+      <c r="AO11">
+        <v>0.19579254162294349</v>
+      </c>
+      <c r="AP11">
+        <f t="shared" ref="AP11:AP21" si="6">AN11+AO11</f>
+        <v>993.99652518923131</v>
+      </c>
+      <c r="AQ11">
+        <v>993.80073264760836</v>
+      </c>
+      <c r="AR11">
+        <v>0.19579254162294349</v>
+      </c>
+      <c r="AS11">
+        <f t="shared" ref="AS11:AS21" si="7">AQ11+AR11</f>
+        <v>993.99652518923131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
@@ -4016,7 +4221,7 @@
         <v>1.4390708093838975</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20.647805124275852</v>
       </c>
       <c r="AK12">
@@ -4026,11 +4231,31 @@
         <v>0.13356807901983217</v>
       </c>
       <c r="AM12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>27.521187334987346</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN12">
+        <v>27.387619255967515</v>
+      </c>
+      <c r="AO12">
+        <v>0.13356807901983217</v>
+      </c>
+      <c r="AP12">
+        <f t="shared" si="6"/>
+        <v>27.521187334987346</v>
+      </c>
+      <c r="AQ12">
+        <v>27.387619255967515</v>
+      </c>
+      <c r="AR12">
+        <v>0.13356807901983217</v>
+      </c>
+      <c r="AS12">
+        <f t="shared" si="7"/>
+        <v>27.521187334987346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -4129,7 +4354,7 @@
         <v>6.8025222126898502E-2</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.1121724631375205</v>
       </c>
       <c r="AK13">
@@ -4139,11 +4364,31 @@
         <v>7.5116168079741932E-3</v>
       </c>
       <c r="AM13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.4662813685889695</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN13">
+        <v>9.458769751780995</v>
+      </c>
+      <c r="AO13">
+        <v>7.5116168079741932E-3</v>
+      </c>
+      <c r="AP13">
+        <f t="shared" si="6"/>
+        <v>9.4662813685889695</v>
+      </c>
+      <c r="AQ13">
+        <v>9.458769751780995</v>
+      </c>
+      <c r="AR13">
+        <v>7.5116168079741932E-3</v>
+      </c>
+      <c r="AS13">
+        <f t="shared" si="7"/>
+        <v>9.4662813685889695</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
@@ -4242,7 +4487,7 @@
         <v>4.6442748659862865E-2</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7750922644483509</v>
       </c>
       <c r="AK14">
@@ -4252,11 +4497,31 @@
         <v>2.1809956805283149E-3</v>
       </c>
       <c r="AM14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.8944508672117086</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN14">
+        <v>1.8922698715311803</v>
+      </c>
+      <c r="AO14">
+        <v>2.1809956805283149E-3</v>
+      </c>
+      <c r="AP14">
+        <f t="shared" si="6"/>
+        <v>1.8944508672117086</v>
+      </c>
+      <c r="AQ14">
+        <v>1.8922698715311803</v>
+      </c>
+      <c r="AR14">
+        <v>2.1809956805283149E-3</v>
+      </c>
+      <c r="AS14">
+        <f t="shared" si="7"/>
+        <v>1.8944508672117086</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -4355,7 +4620,7 @@
         <v>0.22128373782612412</v>
       </c>
       <c r="AJ15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.700151259382223</v>
       </c>
       <c r="AK15">
@@ -4365,11 +4630,31 @@
         <v>5.3987418408876558E-3</v>
       </c>
       <c r="AM15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.3987418408876558E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>5.3987418408876558E-3</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="6"/>
+        <v>5.3987418408876558E-3</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15">
+        <v>5.3987418408876558E-3</v>
+      </c>
+      <c r="AS15">
+        <f t="shared" si="7"/>
+        <v>5.3987418408876558E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -4464,7 +4749,7 @@
         <v>4.2404984619842561E-3</v>
       </c>
       <c r="AJ16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.47814997311821905</v>
       </c>
       <c r="AK16">
@@ -4474,11 +4759,31 @@
         <v>2.0959176112987082E-4</v>
       </c>
       <c r="AM16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.51231387456148403</v>
       </c>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN16">
+        <v>0.51210428280035414</v>
+      </c>
+      <c r="AO16">
+        <v>2.0959176112987082E-4</v>
+      </c>
+      <c r="AP16">
+        <f t="shared" si="6"/>
+        <v>0.51231387456148403</v>
+      </c>
+      <c r="AQ16">
+        <v>0.51210428280035414</v>
+      </c>
+      <c r="AR16">
+        <v>2.0959176112987082E-4</v>
+      </c>
+      <c r="AS16">
+        <f t="shared" si="7"/>
+        <v>0.51231387456148403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
@@ -4573,7 +4878,7 @@
         <v>2.0700811243651359E-2</v>
       </c>
       <c r="AJ17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.26655908652077559</v>
       </c>
       <c r="AK17">
@@ -4583,11 +4888,31 @@
         <v>3.7216049065244534E-4</v>
       </c>
       <c r="AM17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.7002199380836189E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN17">
+        <v>7.6630038890183744E-2</v>
+      </c>
+      <c r="AO17">
+        <v>3.7216049065244534E-4</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" si="6"/>
+        <v>7.7002199380836189E-2</v>
+      </c>
+      <c r="AQ17">
+        <v>7.6630038890183744E-2</v>
+      </c>
+      <c r="AR17">
+        <v>3.7216049065244534E-4</v>
+      </c>
+      <c r="AS17">
+        <f t="shared" si="7"/>
+        <v>7.7002199380836189E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
@@ -4682,7 +5007,7 @@
         <v>1.0718762615156343</v>
       </c>
       <c r="AJ18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.4860014543055007</v>
       </c>
       <c r="AK18">
@@ -4692,11 +5017,31 @@
         <v>0.11248755052026857</v>
       </c>
       <c r="AM18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.11248755052026857</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>0.11248755052026857</v>
+      </c>
+      <c r="AP18">
+        <f t="shared" si="6"/>
+        <v>0.11248755052026857</v>
+      </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
+      <c r="AR18">
+        <v>0.11248755052026857</v>
+      </c>
+      <c r="AS18">
+        <f t="shared" si="7"/>
+        <v>0.11248755052026857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>30</v>
       </c>
@@ -4791,7 +5136,7 @@
         <v>1.1802078079887578E-2</v>
       </c>
       <c r="AJ19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.92323127223800683</v>
       </c>
       <c r="AK19">
@@ -4801,11 +5146,31 @@
         <v>3.4778154884700514E-4</v>
       </c>
       <c r="AM19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.18912102284679677</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN19">
+        <v>0.18877324129794976</v>
+      </c>
+      <c r="AO19">
+        <v>3.4778154884700514E-4</v>
+      </c>
+      <c r="AP19">
+        <f t="shared" si="6"/>
+        <v>0.18912102284679677</v>
+      </c>
+      <c r="AQ19">
+        <v>0.18877324129794976</v>
+      </c>
+      <c r="AR19">
+        <v>3.4778154884700514E-4</v>
+      </c>
+      <c r="AS19">
+        <f t="shared" si="7"/>
+        <v>0.18912102284679677</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>31</v>
       </c>
@@ -4916,7 +5281,7 @@
         <v>611.91676387079497</v>
       </c>
       <c r="AJ20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>72395.422081418714</v>
       </c>
       <c r="AK20">
@@ -4926,11 +5291,31 @@
         <v>92.564589004961775</v>
       </c>
       <c r="AM20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>75019.638597761033</v>
       </c>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN20">
+        <v>74927.07400875607</v>
+      </c>
+      <c r="AO20">
+        <v>92.564589004961775</v>
+      </c>
+      <c r="AP20">
+        <f t="shared" si="6"/>
+        <v>75019.638597761033</v>
+      </c>
+      <c r="AQ20">
+        <v>74927.07400875607</v>
+      </c>
+      <c r="AR20">
+        <v>92.564589004961775</v>
+      </c>
+      <c r="AS20">
+        <f t="shared" si="7"/>
+        <v>75019.638597761033</v>
+      </c>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>32</v>
       </c>
@@ -4987,44 +5372,58 @@
         <v>-72964.246146966863</v>
       </c>
       <c r="AJ21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-72964.246146966863</v>
       </c>
       <c r="AK21">
         <v>-76614.526624731123</v>
       </c>
       <c r="AM21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-76614.526624731123</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN21">
+        <v>-76614.526624731123</v>
+      </c>
+      <c r="AP21">
+        <f t="shared" si="6"/>
+        <v>-76614.526624731123</v>
+      </c>
+      <c r="AQ21">
+        <v>-76614.526624731123</v>
+      </c>
+      <c r="AS21">
+        <f t="shared" si="7"/>
+        <v>-76614.526624731123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="P22" s="74"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="148" t="s">
+      <c r="B23" s="152" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="148"/>
-      <c r="D23" s="148"/>
-      <c r="E23" s="148"/>
-      <c r="F23" s="148"/>
-      <c r="G23" s="148"/>
-      <c r="H23" s="148"/>
-      <c r="I23" s="148"/>
-      <c r="J23" s="148"/>
-      <c r="K23" s="148"/>
-      <c r="L23" s="148"/>
-      <c r="M23" s="148"/>
-      <c r="N23" s="148"/>
-      <c r="O23" s="148"/>
-      <c r="P23" s="148"/>
-      <c r="Q23" s="148"/>
-      <c r="R23" s="148"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
+      <c r="H23" s="152"/>
+      <c r="I23" s="152"/>
+      <c r="J23" s="152"/>
+      <c r="K23" s="152"/>
+      <c r="L23" s="152"/>
+      <c r="M23" s="152"/>
+      <c r="N23" s="152"/>
+      <c r="O23" s="152"/>
+      <c r="P23" s="152"/>
+      <c r="Q23" s="152"/>
+      <c r="R23" s="152"/>
       <c r="S23" s="143" t="s">
         <v>331</v>
       </c>
@@ -5048,10 +5447,13 @@
       </c>
       <c r="AJ23" s="76"/>
       <c r="AK23" s="76"/>
-      <c r="AL23" s="76" t="s">
+      <c r="AL23" s="76"/>
+      <c r="AM23" s="76"/>
+      <c r="AN23" s="76"/>
+      <c r="AO23" s="76" t="s">
         <v>316</v>
       </c>
-      <c r="AM23" s="76"/>
+      <c r="AP23" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5466,7 +5868,7 @@
       <c r="I1" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="151" t="s">
+      <c r="J1" s="148" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5565,7 +5967,7 @@
         <v>2.6845195376862194</v>
       </c>
       <c r="J4" s="76">
-        <f t="shared" ref="J4:J6" si="0">$J$7*G4</f>
+        <f t="shared" ref="J4:J5" si="0">$J$7*G4</f>
         <v>122.48143362649999</v>
       </c>
     </row>
@@ -5734,7 +6136,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="152" t="s">
+      <c r="A10" s="149" t="s">
         <v>338</v>
       </c>
       <c r="B10" s="76">
@@ -6918,7 +7320,7 @@
       </c>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.35">
-      <c r="B12" s="149" t="s">
+      <c r="B12" s="153" t="s">
         <v>290</v>
       </c>
       <c r="C12" s="105" t="s">
@@ -6936,7 +7338,7 @@
       <c r="M12" s="107"/>
     </row>
     <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="150"/>
+      <c r="B13" s="154"/>
       <c r="C13" s="108" t="s">
         <v>1</v>
       </c>
@@ -7424,7 +7826,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="120"/>
-      <c r="B25" s="149" t="s">
+      <c r="B25" s="153" t="s">
         <v>290</v>
       </c>
       <c r="C25" s="105" t="s">
@@ -7443,7 +7845,7 @@
     </row>
     <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="84"/>
-      <c r="B26" s="150"/>
+      <c r="B26" s="154"/>
       <c r="C26" s="108" t="s">
         <v>1</v>
       </c>
@@ -8123,10 +8525,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8134,9 +8536,11 @@
     <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="8" max="8" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -8156,49 +8560,55 @@
         <v>242</v>
       </c>
       <c r="H1" t="s">
+        <v>339</v>
+      </c>
+      <c r="I1" t="s">
+        <v>340</v>
+      </c>
+      <c r="J1" t="s">
         <v>319</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>332</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="136" t="s">
         <v>122</v>
       </c>
@@ -8221,13 +8631,13 @@
         <v>184</v>
       </c>
       <c r="H2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I2" t="s">
+        <v>184</v>
+      </c>
+      <c r="J2" t="s">
         <v>320</v>
-      </c>
-      <c r="I2" t="s">
-        <v>317</v>
-      </c>
-      <c r="J2" t="s">
-        <v>317</v>
       </c>
       <c r="K2" t="s">
         <v>317</v>
@@ -8262,8 +8672,14 @@
       <c r="U2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V2" t="s">
+        <v>317</v>
+      </c>
+      <c r="W2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>125</v>
       </c>
@@ -8286,10 +8702,10 @@
         <v>124</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="J3" t="s">
         <v>93</v>
@@ -8327,8 +8743,14 @@
       <c r="U3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V3" t="s">
+        <v>93</v>
+      </c>
+      <c r="W3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -8356,10 +8778,10 @@
       <c r="I4" s="76">
         <v>0</v>
       </c>
-      <c r="J4" s="38">
-        <v>0</v>
-      </c>
-      <c r="K4" s="38">
+      <c r="J4" s="76">
+        <v>0</v>
+      </c>
+      <c r="K4" s="76">
         <v>0</v>
       </c>
       <c r="L4" s="38">
@@ -8392,8 +8814,14 @@
       <c r="U4" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V4" s="38">
+        <v>0</v>
+      </c>
+      <c r="W4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -8421,10 +8849,10 @@
       <c r="I5" s="76">
         <v>0</v>
       </c>
-      <c r="J5" s="38">
-        <v>0</v>
-      </c>
-      <c r="K5" s="38">
+      <c r="J5" s="76">
+        <v>0</v>
+      </c>
+      <c r="K5" s="76">
         <v>0</v>
       </c>
       <c r="L5" s="38">
@@ -8457,8 +8885,14 @@
       <c r="U5" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V5" s="38">
+        <v>0</v>
+      </c>
+      <c r="W5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -8486,10 +8920,10 @@
       <c r="I6" s="76">
         <v>0</v>
       </c>
-      <c r="J6" s="38">
-        <v>0</v>
-      </c>
-      <c r="K6" s="38">
+      <c r="J6" s="76">
+        <v>0</v>
+      </c>
+      <c r="K6" s="76">
         <v>0</v>
       </c>
       <c r="L6" s="38">
@@ -8522,8 +8956,14 @@
       <c r="U6" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V6" s="38">
+        <v>0</v>
+      </c>
+      <c r="W6" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -8551,10 +8991,10 @@
       <c r="I7" s="76">
         <v>0</v>
       </c>
-      <c r="J7" s="38">
-        <v>0</v>
-      </c>
-      <c r="K7" s="38">
+      <c r="J7" s="76">
+        <v>0</v>
+      </c>
+      <c r="K7" s="76">
         <v>0</v>
       </c>
       <c r="L7" s="38">
@@ -8587,8 +9027,14 @@
       <c r="U7" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V7" s="38">
+        <v>0</v>
+      </c>
+      <c r="W7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -8616,10 +9062,10 @@
       <c r="I8" s="76">
         <v>0</v>
       </c>
-      <c r="J8" s="38">
-        <v>0</v>
-      </c>
-      <c r="K8" s="38">
+      <c r="J8" s="76">
+        <v>0</v>
+      </c>
+      <c r="K8" s="76">
         <v>0</v>
       </c>
       <c r="L8" s="38">
@@ -8652,8 +9098,14 @@
       <c r="U8" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V8" s="38">
+        <v>0</v>
+      </c>
+      <c r="W8" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -8681,10 +9133,10 @@
       <c r="I9" s="76">
         <v>0</v>
       </c>
-      <c r="J9" s="38">
-        <v>0</v>
-      </c>
-      <c r="K9" s="38">
+      <c r="J9" s="76">
+        <v>0</v>
+      </c>
+      <c r="K9" s="76">
         <v>0</v>
       </c>
       <c r="L9" s="38">
@@ -8717,8 +9169,14 @@
       <c r="U9" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V9" s="38">
+        <v>0</v>
+      </c>
+      <c r="W9" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -8746,15 +9204,15 @@
       <c r="I10" s="76">
         <v>0</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="76">
+        <v>0</v>
+      </c>
+      <c r="K10" s="76">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>1</v>
       </c>
-      <c r="K10" s="38">
-        <v>0</v>
-      </c>
-      <c r="L10" s="38">
-        <v>0</v>
-      </c>
       <c r="M10" s="38">
         <v>0</v>
       </c>
@@ -8782,8 +9240,14 @@
       <c r="U10" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V10" s="38">
+        <v>0</v>
+      </c>
+      <c r="W10" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -8811,18 +9275,18 @@
       <c r="I11" s="76">
         <v>0</v>
       </c>
-      <c r="J11" s="38">
-        <v>0</v>
-      </c>
-      <c r="K11">
+      <c r="J11" s="76">
+        <v>0</v>
+      </c>
+      <c r="K11" s="76">
+        <v>0</v>
+      </c>
+      <c r="L11" s="38">
+        <v>0</v>
+      </c>
+      <c r="M11">
         <v>1</v>
       </c>
-      <c r="L11" s="38">
-        <v>0</v>
-      </c>
-      <c r="M11" s="38">
-        <v>0</v>
-      </c>
       <c r="N11" s="38">
         <v>0</v>
       </c>
@@ -8847,8 +9311,14 @@
       <c r="U11" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V11" s="38">
+        <v>0</v>
+      </c>
+      <c r="W11" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -8876,21 +9346,21 @@
       <c r="I12" s="76">
         <v>0</v>
       </c>
-      <c r="J12" s="38">
-        <v>0</v>
-      </c>
-      <c r="K12" s="38">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="J12" s="76">
+        <v>0</v>
+      </c>
+      <c r="K12" s="76">
+        <v>0</v>
+      </c>
+      <c r="L12" s="38">
+        <v>0</v>
+      </c>
+      <c r="M12" s="38">
+        <v>0</v>
+      </c>
+      <c r="N12">
         <v>1</v>
       </c>
-      <c r="M12" s="38">
-        <v>0</v>
-      </c>
-      <c r="N12" s="38">
-        <v>0</v>
-      </c>
       <c r="O12" s="38">
         <v>0</v>
       </c>
@@ -8912,8 +9382,14 @@
       <c r="U12" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V12" s="38">
+        <v>0</v>
+      </c>
+      <c r="W12" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -8941,24 +9417,24 @@
       <c r="I13" s="76">
         <v>0</v>
       </c>
-      <c r="J13" s="38">
-        <v>0</v>
-      </c>
-      <c r="K13" s="38">
+      <c r="J13" s="76">
+        <v>0</v>
+      </c>
+      <c r="K13" s="76">
         <v>0</v>
       </c>
       <c r="L13" s="38">
         <v>0</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="38">
+        <v>0</v>
+      </c>
+      <c r="N13" s="38">
+        <v>0</v>
+      </c>
+      <c r="O13">
         <v>1</v>
       </c>
-      <c r="N13" s="38">
-        <v>0</v>
-      </c>
-      <c r="O13" s="38">
-        <v>0</v>
-      </c>
       <c r="P13" s="38">
         <v>0</v>
       </c>
@@ -8977,8 +9453,14 @@
       <c r="U13" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V13" s="38">
+        <v>0</v>
+      </c>
+      <c r="W13" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -9006,10 +9488,10 @@
       <c r="I14" s="76">
         <v>0</v>
       </c>
-      <c r="J14" s="38">
-        <v>0</v>
-      </c>
-      <c r="K14" s="38">
+      <c r="J14" s="76">
+        <v>0</v>
+      </c>
+      <c r="K14" s="76">
         <v>0</v>
       </c>
       <c r="L14" s="38">
@@ -9018,15 +9500,15 @@
       <c r="M14" s="38">
         <v>0</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="38">
+        <v>0</v>
+      </c>
+      <c r="O14" s="38">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>1</v>
       </c>
-      <c r="O14" s="38">
-        <v>0</v>
-      </c>
-      <c r="P14" s="38">
-        <v>0</v>
-      </c>
       <c r="Q14" s="38">
         <v>0</v>
       </c>
@@ -9042,8 +9524,14 @@
       <c r="U14" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V14" s="38">
+        <v>0</v>
+      </c>
+      <c r="W14" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -9071,10 +9559,10 @@
       <c r="I15" s="76">
         <v>0</v>
       </c>
-      <c r="J15" s="38">
-        <v>0</v>
-      </c>
-      <c r="K15" s="38">
+      <c r="J15" s="76">
+        <v>0</v>
+      </c>
+      <c r="K15" s="76">
         <v>0</v>
       </c>
       <c r="L15" s="38">
@@ -9086,15 +9574,15 @@
       <c r="N15" s="38">
         <v>0</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="38">
+        <v>0</v>
+      </c>
+      <c r="P15" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q15">
         <v>1</v>
       </c>
-      <c r="P15" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="38">
-        <v>0</v>
-      </c>
       <c r="R15" s="38">
         <v>0</v>
       </c>
@@ -9107,8 +9595,14 @@
       <c r="U15" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V15" s="38">
+        <v>0</v>
+      </c>
+      <c r="W15" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -9136,10 +9630,10 @@
       <c r="I16" s="76">
         <v>0</v>
       </c>
-      <c r="J16" s="38">
-        <v>0</v>
-      </c>
-      <c r="K16" s="38">
+      <c r="J16" s="76">
+        <v>0</v>
+      </c>
+      <c r="K16" s="76">
         <v>0</v>
       </c>
       <c r="L16" s="38">
@@ -9154,15 +9648,15 @@
       <c r="O16" s="38">
         <v>0</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="38">
+        <v>0</v>
+      </c>
+      <c r="R16">
         <v>1</v>
       </c>
-      <c r="Q16" s="38">
-        <v>0</v>
-      </c>
-      <c r="R16" s="38">
-        <v>0</v>
-      </c>
       <c r="S16" s="38">
         <v>0</v>
       </c>
@@ -9172,8 +9666,14 @@
       <c r="U16" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V16" s="38">
+        <v>0</v>
+      </c>
+      <c r="W16" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -9201,10 +9701,10 @@
       <c r="I17" s="76">
         <v>0</v>
       </c>
-      <c r="J17" s="38">
-        <v>0</v>
-      </c>
-      <c r="K17" s="38">
+      <c r="J17" s="76">
+        <v>0</v>
+      </c>
+      <c r="K17" s="76">
         <v>0</v>
       </c>
       <c r="L17" s="38">
@@ -9222,23 +9722,29 @@
       <c r="P17" s="38">
         <v>0</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="38">
+        <v>0</v>
+      </c>
+      <c r="R17" s="38">
+        <v>0</v>
+      </c>
+      <c r="S17">
         <v>1</v>
       </c>
-      <c r="R17" s="38">
-        <v>0</v>
-      </c>
-      <c r="S17" s="38">
-        <v>0</v>
-      </c>
       <c r="T17" s="38">
         <v>0</v>
       </c>
       <c r="U17" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V17" s="38">
+        <v>0</v>
+      </c>
+      <c r="W17" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -9266,10 +9772,10 @@
       <c r="I18" s="76">
         <v>0</v>
       </c>
-      <c r="J18" s="38">
-        <v>0</v>
-      </c>
-      <c r="K18" s="38">
+      <c r="J18" s="76">
+        <v>0</v>
+      </c>
+      <c r="K18" s="76">
         <v>0</v>
       </c>
       <c r="L18" s="38">
@@ -9290,20 +9796,26 @@
       <c r="Q18" s="38">
         <v>0</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="38">
+        <v>0</v>
+      </c>
+      <c r="S18" s="38">
+        <v>0</v>
+      </c>
+      <c r="T18">
         <v>1</v>
       </c>
-      <c r="S18" s="38">
-        <v>0</v>
-      </c>
-      <c r="T18" s="38">
-        <v>0</v>
-      </c>
       <c r="U18" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V18" s="38">
+        <v>0</v>
+      </c>
+      <c r="W18" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -9331,10 +9843,10 @@
       <c r="I19" s="76">
         <v>0</v>
       </c>
-      <c r="J19" s="38">
-        <v>0</v>
-      </c>
-      <c r="K19" s="38">
+      <c r="J19" s="76">
+        <v>0</v>
+      </c>
+      <c r="K19" s="76">
         <v>0</v>
       </c>
       <c r="L19" s="38">
@@ -9358,17 +9870,23 @@
       <c r="R19" s="38">
         <v>0</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="38">
+        <v>0</v>
+      </c>
+      <c r="T19" s="38">
+        <v>0</v>
+      </c>
+      <c r="U19">
         <v>1</v>
       </c>
-      <c r="T19" s="38">
-        <v>0</v>
-      </c>
-      <c r="U19" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V19" s="38">
+        <v>0</v>
+      </c>
+      <c r="W19" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -9396,10 +9914,10 @@
       <c r="I20" s="76">
         <v>0</v>
       </c>
-      <c r="J20" s="38">
-        <v>0</v>
-      </c>
-      <c r="K20" s="38">
+      <c r="J20" s="76">
+        <v>0</v>
+      </c>
+      <c r="K20" s="76">
         <v>0</v>
       </c>
       <c r="L20" s="38">
@@ -9426,19 +9944,24 @@
       <c r="S20" s="38">
         <v>0</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="38">
+        <v>0</v>
+      </c>
+      <c r="U20" s="38">
+        <v>0</v>
+      </c>
+      <c r="V20">
         <v>1</v>
       </c>
-      <c r="U20">
+      <c r="W20">
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="G21" s="38"/>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="H21" s="38"/>
       <c r="I21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
       <c r="N21" s="38"/>
       <c r="O21" s="38"/>
       <c r="P21" s="38"/>
@@ -9446,40 +9969,43 @@
       <c r="R21" s="38"/>
       <c r="S21" s="38"/>
       <c r="T21" s="38"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="148" t="s">
+      <c r="B22" s="152" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="148"/>
-      <c r="D22" s="148"/>
-      <c r="E22" s="148"/>
+      <c r="C22" s="152"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="152"/>
       <c r="F22" s="147" t="s">
         <v>335</v>
       </c>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
+      <c r="G22" s="151"/>
       <c r="O22" s="38"/>
       <c r="P22" s="38"/>
       <c r="Q22" s="38"/>
       <c r="R22" s="38"/>
       <c r="S22" s="38"/>
       <c r="T22" s="38"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
+      <c r="U22" s="38"/>
+      <c r="V22" s="38"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="O23" s="38"/>
       <c r="P23" s="38"/>
       <c r="Q23" s="38"/>
       <c r="R23" s="38"/>
       <c r="S23" s="38"/>
       <c r="T23" s="38"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U23" s="38"/>
+      <c r="V23" s="38"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -9489,15 +10015,17 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
       <c r="P24" s="38"/>
       <c r="Q24" s="38"/>
       <c r="R24" s="38"/>
       <c r="S24" s="38"/>
       <c r="T24" s="38"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U24" s="38"/>
+      <c r="V24" s="38"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -9507,14 +10035,16 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
       <c r="Q25" s="38"/>
       <c r="R25" s="38"/>
       <c r="S25" s="38"/>
       <c r="T25" s="38"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U25" s="38"/>
+      <c r="V25" s="38"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -9524,13 +10054,15 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
       <c r="R26" s="38"/>
       <c r="S26" s="38"/>
       <c r="T26" s="38"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -9540,12 +10072,14 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
       <c r="S27" s="38"/>
       <c r="T27" s="38"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U27" s="38"/>
+      <c r="V27" s="38"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -9555,11 +10089,13 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
       <c r="T28" s="38"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="U28" s="38"/>
+      <c r="V28" s="38"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -9569,10 +10105,12 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="S29" s="38"/>
-      <c r="T29" s="38"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="U29" s="38"/>
+      <c r="V29" s="38"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -9582,9 +10120,11 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="T30" s="38"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="V30" s="38"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -9594,8 +10134,10 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -9605,8 +10147,10 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -9616,8 +10160,10 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -9627,8 +10173,10 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -9638,8 +10186,10 @@
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -9648,9 +10198,11 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -9660,6 +10212,8 @@
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12228,39 +12782,39 @@
       <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="148" t="s">
+      <c r="B23" s="152" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="148"/>
-      <c r="D23" s="148"/>
-      <c r="E23" s="148"/>
-      <c r="F23" s="148"/>
-      <c r="G23" s="148"/>
-      <c r="H23" s="148"/>
-      <c r="I23" s="148"/>
-      <c r="J23" s="148"/>
-      <c r="K23" s="148"/>
-      <c r="L23" s="148"/>
-      <c r="M23" s="148"/>
-      <c r="N23" s="148"/>
-      <c r="O23" s="148"/>
-      <c r="P23" s="148"/>
-      <c r="Q23" s="148"/>
-      <c r="R23" s="148"/>
-      <c r="S23" s="148"/>
-      <c r="T23" s="148"/>
-      <c r="U23" s="148"/>
-      <c r="V23" s="148"/>
-      <c r="W23" s="148"/>
-      <c r="X23" s="148"/>
-      <c r="Y23" s="148"/>
-      <c r="Z23" s="148"/>
-      <c r="AA23" s="148"/>
-      <c r="AB23" s="148"/>
-      <c r="AC23" s="148"/>
-      <c r="AD23" s="148"/>
-      <c r="AE23" s="148"/>
-      <c r="AF23" s="148"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
+      <c r="H23" s="152"/>
+      <c r="I23" s="152"/>
+      <c r="J23" s="152"/>
+      <c r="K23" s="152"/>
+      <c r="L23" s="152"/>
+      <c r="M23" s="152"/>
+      <c r="N23" s="152"/>
+      <c r="O23" s="152"/>
+      <c r="P23" s="152"/>
+      <c r="Q23" s="152"/>
+      <c r="R23" s="152"/>
+      <c r="S23" s="152"/>
+      <c r="T23" s="152"/>
+      <c r="U23" s="152"/>
+      <c r="V23" s="152"/>
+      <c r="W23" s="152"/>
+      <c r="X23" s="152"/>
+      <c r="Y23" s="152"/>
+      <c r="Z23" s="152"/>
+      <c r="AA23" s="152"/>
+      <c r="AB23" s="152"/>
+      <c r="AC23" s="152"/>
+      <c r="AD23" s="152"/>
+      <c r="AE23" s="152"/>
+      <c r="AF23" s="152"/>
       <c r="AI23" t="s">
         <v>304</v>
       </c>
@@ -13419,22 +13973,22 @@
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="148" t="s">
+      <c r="B23" s="152" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="148"/>
-      <c r="D23" s="148"/>
-      <c r="E23" s="148"/>
-      <c r="F23" s="148"/>
-      <c r="G23" s="148"/>
-      <c r="H23" s="148"/>
-      <c r="I23" s="148"/>
-      <c r="J23" s="148"/>
-      <c r="K23" s="148"/>
-      <c r="L23" s="148"/>
-      <c r="M23" s="148"/>
-      <c r="N23" s="148"/>
-      <c r="O23" s="148"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
+      <c r="H23" s="152"/>
+      <c r="I23" s="152"/>
+      <c r="J23" s="152"/>
+      <c r="K23" s="152"/>
+      <c r="L23" s="152"/>
+      <c r="M23" s="152"/>
+      <c r="N23" s="152"/>
+      <c r="O23" s="152"/>
       <c r="P23" t="s">
         <v>90</v>
       </c>
@@ -13760,7 +14314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912BA9E3-4DC6-4F1B-8852-1658C2A4C23D}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -13919,10 +14473,10 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="151" t="s">
+      <c r="A20" s="148" t="s">
         <v>338</v>
       </c>
-      <c r="B20" s="153" t="s">
+      <c r="B20" s="150" t="s">
         <v>119</v>
       </c>
     </row>
@@ -13973,10 +14527,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14445,500 +14999,522 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>164</v>
-      </c>
-      <c r="B43">
-        <v>38.180512527472686</v>
+        <v>339</v>
+      </c>
+      <c r="B43" s="76">
+        <v>44.291949816853993</v>
       </c>
       <c r="C43">
-        <v>747.6070630111235</v>
+        <v>793.37856525946859</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>165</v>
-      </c>
-      <c r="B44">
-        <v>37.300256882262083</v>
+        <v>340</v>
+      </c>
+      <c r="B44" s="76">
+        <v>43.995102738357922</v>
       </c>
       <c r="C44">
-        <v>716.69892648380858</v>
+        <v>793.37856525946859</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B45">
-        <v>36.889328265240245</v>
+        <v>38.180512527472686</v>
       </c>
       <c r="C45">
-        <v>744.70116983334174</v>
+        <v>747.6070630111235</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B46">
-        <v>39.429337036099838</v>
+        <v>37.300256882262083</v>
       </c>
       <c r="C46">
-        <v>756.99999999999989</v>
+        <v>716.69892648380858</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B47">
-        <v>10.040313081123244</v>
+        <v>36.889328265240245</v>
       </c>
       <c r="C47">
-        <v>70.798124695046326</v>
+        <v>744.70116983334174</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B48">
-        <v>30.792488052730107</v>
+        <v>39.429337036099838</v>
       </c>
       <c r="C48">
-        <v>742.58779297677324</v>
+        <v>756.99999999999989</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B49">
-        <v>31.839314137909518</v>
+        <v>10.040313081123244</v>
       </c>
       <c r="C49">
-        <v>742.32362086970215</v>
+        <v>70.798124695046326</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B50">
-        <v>33.077070766926674</v>
+        <v>30.792488052730107</v>
       </c>
       <c r="C50">
-        <v>769.53334789802227</v>
+        <v>742.58779297677324</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B51">
-        <v>31.263230600468017</v>
+        <v>31.839314137909518</v>
       </c>
       <c r="C51">
-        <v>584.61287294827434</v>
+        <v>742.32362086970215</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B52">
-        <v>29.646904789703584</v>
+        <v>33.077070766926674</v>
       </c>
       <c r="C52">
-        <v>559.51652277652283</v>
+        <v>769.53334789802227</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B53">
-        <v>31.510123545085804</v>
+        <v>31.263230600468017</v>
       </c>
       <c r="C53">
-        <v>595.17975723111715</v>
+        <v>584.61287294827434</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B54">
-        <v>27.734307445397814</v>
+        <v>29.646904789703584</v>
       </c>
       <c r="C54">
-        <v>507.21044557645126</v>
+        <v>559.51652277652283</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B55">
-        <v>27.548680827882244</v>
+        <v>31.510123545085804</v>
       </c>
       <c r="C55">
-        <v>668.88377510394514</v>
+        <v>595.17975723111715</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B56">
-        <v>34.60609523247426</v>
+        <v>27.734307445397814</v>
       </c>
       <c r="C56">
-        <v>654.80340179705718</v>
+        <v>507.21044557645126</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B57">
-        <v>36.455478031346189</v>
+        <v>27.548680827882244</v>
       </c>
       <c r="C57">
-        <v>688.85095964480468</v>
+        <v>668.88377510394514</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B58">
-        <v>38.505872853524245</v>
+        <v>34.60609523247426</v>
       </c>
       <c r="C58">
-        <v>737.59071339941693</v>
+        <v>654.80340179705718</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B59">
-        <v>39.773165285279561</v>
+        <v>36.455478031346189</v>
       </c>
       <c r="C59">
-        <v>765.47381512866104</v>
+        <v>688.85095964480468</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B60">
-        <v>38.281904677575831</v>
+        <v>38.505872853524245</v>
       </c>
       <c r="C60">
-        <v>731.67589538225809</v>
+        <v>737.59071339941693</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B61">
-        <v>31.369932808387436</v>
+        <v>39.773165285279561</v>
       </c>
       <c r="C61">
-        <v>800.00032424653136</v>
+        <v>765.47381512866104</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B62">
-        <v>38.180512527472686</v>
+        <v>38.281904677575831</v>
       </c>
       <c r="C62">
-        <v>747.6070630111235</v>
+        <v>731.67589538225809</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B63">
-        <v>47.141813661363628</v>
+        <v>31.369932808387436</v>
       </c>
       <c r="C63">
-        <v>0.77692265667854898</v>
+        <v>800.00032424653136</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B64">
-        <v>49.999999999999993</v>
+        <v>38.180512527472686</v>
       </c>
       <c r="C64">
-        <v>0.71699999999999986</v>
+        <v>747.6070630111235</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="75" t="s">
-        <v>89</v>
+      <c r="A65" t="s">
+        <v>187</v>
       </c>
       <c r="B65">
-        <v>119.98674372549019</v>
+        <v>47.141813661363628</v>
       </c>
       <c r="C65">
-        <v>9.0052398842286357E-2</v>
+        <v>0.77692265667854898</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>49.999999999999993</v>
       </c>
       <c r="C66">
-        <v>1.9768383817590991</v>
+        <v>0.71699999999999986</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>190</v>
+      <c r="A67" s="75" t="s">
+        <v>89</v>
       </c>
       <c r="B67">
-        <v>48.885121247479262</v>
+        <v>119.98674372549019</v>
       </c>
       <c r="C67">
-        <v>0.88356773166440861</v>
+        <v>9.0052398842286357E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B68">
-        <v>22.648458746153963</v>
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>1.9768383817590991</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B69">
-        <v>26.329529071139479</v>
+        <v>48.885121247479262</v>
+      </c>
+      <c r="C69">
+        <v>0.88356773166440861</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B70">
-        <v>18.707371337693861</v>
+        <v>22.648458746153963</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B71">
-        <v>12.566427590816895</v>
+        <v>26.329529071139479</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B72">
-        <v>26.329529071139479</v>
+        <v>18.707371337693861</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B73">
-        <v>11.566786665057547</v>
+        <v>12.566427590816895</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B74">
-        <v>31.342185540824094</v>
+        <v>26.329529071139479</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B75">
-        <v>31.0106439692332</v>
+        <v>11.566786665057547</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B76">
-        <v>28.609127685562171</v>
+        <v>31.342185540824094</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B77">
-        <v>33.012627597074328</v>
+        <v>31.0106439692332</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B78">
-        <v>17.905547955535493</v>
+        <v>28.609127685562171</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B79">
-        <v>18.52542695399616</v>
+        <v>33.012627597074328</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B80">
-        <v>16.801860958276258</v>
+        <v>17.905547955535493</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B81">
-        <v>17.842745955691449</v>
+        <v>18.52542695399616</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B82">
-        <v>17.11470795749937</v>
+        <v>16.801860958276258</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B83">
-        <v>20.107106950068403</v>
+        <v>17.842745955691449</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B84">
-        <v>18.52542695399616</v>
+        <v>17.11470795749937</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B85">
-        <v>17.444999956679162</v>
+        <v>20.107106950068403</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B86">
-        <v>15.647058823529411</v>
+        <v>18.52542695399616</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B87">
-        <v>14.4</v>
+        <v>17.444999956679162</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B88">
-        <v>22.000366940104676</v>
+        <v>15.647058823529411</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B89">
-        <v>14.864999999999997</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B90">
-        <v>16.758749999999999</v>
+        <v>22.000366940104676</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B91">
-        <v>16.758749999999999</v>
+        <v>14.864999999999997</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B92">
-        <v>13.036809815950916</v>
+        <v>16.758749999999999</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B93">
-        <v>16.462585034013607</v>
+        <v>16.758749999999999</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="75" t="s">
-        <v>219</v>
-      </c>
-      <c r="C94">
-        <v>1000</v>
+      <c r="A94" t="s">
+        <v>215</v>
+      </c>
+      <c r="B94">
+        <v>13.036809815950916</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>216</v>
+      </c>
+      <c r="B95">
+        <v>16.462585034013607</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="75" t="s">
+        <v>219</v>
+      </c>
+      <c r="C96">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>75</v>
       </c>
-      <c r="C95">
+      <c r="C97">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding the CAP pathway ... continued
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BB67BC-B2D0-4C14-9CF4-0E56F0CCBED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3205F58-BADE-40BB-98C4-D3A2870AF62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" firstSheet="3" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="745" firstSheet="3" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="367">
   <si>
     <t>NG</t>
   </si>
@@ -1358,6 +1358,57 @@
   </si>
   <si>
     <t>Algae</t>
+  </si>
+  <si>
+    <t>H3PO4</t>
+  </si>
+  <si>
+    <t>HT Catlysts (HTL)</t>
+  </si>
+  <si>
+    <t>Hydrcracking catalyst  (HTL)</t>
+  </si>
+  <si>
+    <t>Silica</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Dehydration Catalyst</t>
+  </si>
+  <si>
+    <t>Oligomerization Catalyst</t>
+  </si>
+  <si>
+    <t>One step HDO/HI Catalyst</t>
+  </si>
+  <si>
+    <t>Hydrotalcite</t>
+  </si>
+  <si>
+    <t>Ketonization Catalyst (ZrO2)</t>
+  </si>
+  <si>
+    <t>Condensation Catalyst (Niobic Acid)</t>
+  </si>
+  <si>
+    <t>Formic acid</t>
+  </si>
+  <si>
+    <t>H2O2</t>
+  </si>
+  <si>
+    <t>Catalysts and Other Chemicals</t>
+  </si>
+  <si>
+    <t>Toluene Diisocyanate</t>
+  </si>
+  <si>
+    <t>Diethanolamine</t>
+  </si>
+  <si>
+    <t>Surfactant</t>
   </si>
 </sst>
 </file>
@@ -1425,7 +1476,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1489,6 +1540,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1676,7 +1733,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1936,6 +1993,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -10204,11 +10281,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
-  <dimension ref="A1:AU27"/>
+  <dimension ref="A1:BL27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AQ27" sqref="AQ27"/>
+      <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BI27" sqref="BI27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10221,7 +10298,7 @@
     <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
         <v>310</v>
@@ -10235,7 +10312,7 @@
       <c r="E1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="131" t="s">
         <v>40</v>
       </c>
       <c r="G1" s="17" t="s">
@@ -10358,8 +10435,62 @@
       <c r="AT1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU1" s="137" t="s">
+        <v>350</v>
+      </c>
+      <c r="AV1" s="137" t="s">
+        <v>351</v>
+      </c>
+      <c r="AW1" s="137" t="s">
+        <v>352</v>
+      </c>
+      <c r="AX1" s="138" t="s">
+        <v>353</v>
+      </c>
+      <c r="AY1" s="138" t="s">
+        <v>354</v>
+      </c>
+      <c r="AZ1" s="138" t="s">
+        <v>355</v>
+      </c>
+      <c r="BA1" s="138" t="s">
+        <v>356</v>
+      </c>
+      <c r="BB1" s="138" t="s">
+        <v>357</v>
+      </c>
+      <c r="BC1" s="138" t="s">
+        <v>358</v>
+      </c>
+      <c r="BD1" s="138" t="s">
+        <v>359</v>
+      </c>
+      <c r="BE1" s="138" t="s">
+        <v>360</v>
+      </c>
+      <c r="BF1" s="138" t="s">
+        <v>361</v>
+      </c>
+      <c r="BG1" s="138" t="s">
+        <v>362</v>
+      </c>
+      <c r="BH1" s="138" t="s">
+        <v>363</v>
+      </c>
+      <c r="BI1" s="138" t="s">
+        <v>49</v>
+      </c>
+      <c r="BJ1" s="138" t="s">
+        <v>364</v>
+      </c>
+      <c r="BK1" s="138" t="s">
+        <v>365</v>
+      </c>
+      <c r="BL1" s="138" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
@@ -10375,7 +10506,7 @@
       <c r="E2" s="65" t="s">
         <v>307</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="132" t="s">
         <v>307</v>
       </c>
       <c r="G2" s="65" t="s">
@@ -10498,9 +10629,62 @@
       <c r="AT2" s="117" t="s">
         <v>343</v>
       </c>
-      <c r="AU2" s="117"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="AW2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="AX2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="AY2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="AZ2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BA2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BB2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BC2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BD2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BE2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BF2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BG2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BH2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BI2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BJ2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BK2" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="BL2" s="119" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -10516,7 +10700,7 @@
       <c r="E3" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="133" t="s">
         <v>93</v>
       </c>
       <c r="G3" s="20" t="s">
@@ -10639,8 +10823,62 @@
       <c r="AT3" s="20" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AY3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BC3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BE3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BG3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BH3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BI3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BL3" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -10656,7 +10894,7 @@
       <c r="E4" s="22">
         <v>96.173077193221943</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="134">
         <v>24.292168425500595</v>
       </c>
       <c r="G4" s="22">
@@ -10779,8 +11017,62 @@
       <c r="AT4">
         <v>30.295317337266482</v>
       </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU4">
+        <v>15.019429554309164</v>
+      </c>
+      <c r="AV4">
+        <v>39.483586132842049</v>
+      </c>
+      <c r="AW4">
+        <v>39.483586132842049</v>
+      </c>
+      <c r="AX4">
+        <v>0.3581698661381561</v>
+      </c>
+      <c r="AY4">
+        <v>4.3833672938355273E-2</v>
+      </c>
+      <c r="AZ4">
+        <v>196.70295779410594</v>
+      </c>
+      <c r="BA4">
+        <v>196.70295779410594</v>
+      </c>
+      <c r="BB4">
+        <v>196.70295779410594</v>
+      </c>
+      <c r="BC4">
+        <v>196.70295779410594</v>
+      </c>
+      <c r="BD4">
+        <v>196.70295779410594</v>
+      </c>
+      <c r="BE4">
+        <v>196.70295779410594</v>
+      </c>
+      <c r="BF4">
+        <v>39.70337997545861</v>
+      </c>
+      <c r="BG4">
+        <v>16.573687577719323</v>
+      </c>
+      <c r="BH4">
+        <v>196.70295779410594</v>
+      </c>
+      <c r="BI4">
+        <v>2.9101301623725186</v>
+      </c>
+      <c r="BJ4">
+        <v>35.607860000000002</v>
+      </c>
+      <c r="BK4">
+        <v>62.504452652498195</v>
+      </c>
+      <c r="BL4">
+        <v>1708.6819416186172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -10796,7 +11088,7 @@
       <c r="E5" s="22">
         <v>12.434256086332805</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="134">
         <v>23.112834811006994</v>
       </c>
       <c r="G5" s="22">
@@ -10919,8 +11211,62 @@
       <c r="AT5">
         <v>29.831066400462845</v>
       </c>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU5">
+        <v>13.93301632154248</v>
+      </c>
+      <c r="AV5">
+        <v>34.523904822559238</v>
+      </c>
+      <c r="AW5">
+        <v>34.523904822559238</v>
+      </c>
+      <c r="AX5">
+        <v>0.28132753242105452</v>
+      </c>
+      <c r="AY5">
+        <v>3.9756448338327942E-2</v>
+      </c>
+      <c r="AZ5">
+        <v>190.79583917725958</v>
+      </c>
+      <c r="BA5">
+        <v>190.79583917725958</v>
+      </c>
+      <c r="BB5">
+        <v>190.79583917725958</v>
+      </c>
+      <c r="BC5">
+        <v>190.79583917725958</v>
+      </c>
+      <c r="BD5">
+        <v>190.79583917725958</v>
+      </c>
+      <c r="BE5">
+        <v>190.79583917725958</v>
+      </c>
+      <c r="BF5">
+        <v>39.17718902955842</v>
+      </c>
+      <c r="BG5">
+        <v>15.711261044001366</v>
+      </c>
+      <c r="BH5">
+        <v>190.79583917725958</v>
+      </c>
+      <c r="BI5">
+        <v>2.2857862009210681</v>
+      </c>
+      <c r="BJ5">
+        <v>34.146839999999997</v>
+      </c>
+      <c r="BK5">
+        <v>60.353903810734323</v>
+      </c>
+      <c r="BL5">
+        <v>593.4443720738916</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -10936,7 +11282,7 @@
       <c r="E6" s="22">
         <v>0.46325014313213203</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="134">
         <v>1.6501694729418555</v>
       </c>
       <c r="G6" s="22">
@@ -11059,8 +11405,62 @@
       <c r="AT6">
         <v>20.605899142323508</v>
       </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU6">
+        <v>1.5201149893010175</v>
+      </c>
+      <c r="AV6">
+        <v>8.2835881755944225</v>
+      </c>
+      <c r="AW6">
+        <v>8.2835881755944225</v>
+      </c>
+      <c r="AX6">
+        <v>0.1076113461139153</v>
+      </c>
+      <c r="AY6">
+        <v>5.6827199192912457E-3</v>
+      </c>
+      <c r="AZ6">
+        <v>16.802194749958446</v>
+      </c>
+      <c r="BA6">
+        <v>16.802194749958446</v>
+      </c>
+      <c r="BB6">
+        <v>16.802194749958446</v>
+      </c>
+      <c r="BC6">
+        <v>16.802194749958446</v>
+      </c>
+      <c r="BD6">
+        <v>16.802194749958446</v>
+      </c>
+      <c r="BE6">
+        <v>16.802194749958446</v>
+      </c>
+      <c r="BF6">
+        <v>3.8579793740200041</v>
+      </c>
+      <c r="BG6">
+        <v>1.2076769380332584</v>
+      </c>
+      <c r="BH6">
+        <v>16.802194749958446</v>
+      </c>
+      <c r="BI6">
+        <v>0.87434218717556189</v>
+      </c>
+      <c r="BJ6">
+        <v>2.8897429999999997</v>
+      </c>
+      <c r="BK6">
+        <v>3.0069126161037167</v>
+      </c>
+      <c r="BL6">
+        <v>21.022320614309901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -11076,7 +11476,7 @@
       <c r="E7" s="22">
         <v>8.61916794675669</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="134">
         <v>16.483574246246874</v>
       </c>
       <c r="G7" s="22">
@@ -11199,8 +11599,62 @@
       <c r="AT7">
         <v>7.4744027922844962</v>
       </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU7">
+        <v>7.6966652243150877</v>
+      </c>
+      <c r="AV7">
+        <v>25.563238243896706</v>
+      </c>
+      <c r="AW7">
+        <v>25.563238243896706</v>
+      </c>
+      <c r="AX7">
+        <v>0.16899538624321581</v>
+      </c>
+      <c r="AY7">
+        <v>1.2713625725546759E-2</v>
+      </c>
+      <c r="AZ7">
+        <v>156.84426028499615</v>
+      </c>
+      <c r="BA7">
+        <v>156.84426028499615</v>
+      </c>
+      <c r="BB7">
+        <v>156.84426028499615</v>
+      </c>
+      <c r="BC7">
+        <v>156.84426028499615</v>
+      </c>
+      <c r="BD7">
+        <v>156.84426028499615</v>
+      </c>
+      <c r="BE7">
+        <v>156.84426028499615</v>
+      </c>
+      <c r="BF7">
+        <v>18.505024260697184</v>
+      </c>
+      <c r="BG7">
+        <v>14.167331612171793</v>
+      </c>
+      <c r="BH7">
+        <v>156.84426028499615</v>
+      </c>
+      <c r="BI7">
+        <v>1.3730875132261284</v>
+      </c>
+      <c r="BJ7">
+        <v>22.8813</v>
+      </c>
+      <c r="BK7">
+        <v>40.434145515554434</v>
+      </c>
+      <c r="BL7">
+        <v>429.0227371553645</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -11216,7 +11670,7 @@
       <c r="E8" s="22">
         <v>3.3518379964439835</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="134">
         <v>4.9790910918182654</v>
       </c>
       <c r="G8" s="22">
@@ -11339,8 +11793,62 @@
       <c r="AT8">
         <v>1.7507644658548416</v>
       </c>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU8">
+        <v>4.7162361079263766</v>
+      </c>
+      <c r="AV8">
+        <v>0.67707840306811351</v>
+      </c>
+      <c r="AW8">
+        <v>0.67707840306811351</v>
+      </c>
+      <c r="AX8">
+        <v>4.7208000639233794E-3</v>
+      </c>
+      <c r="AY8">
+        <v>2.1360102693489928E-2</v>
+      </c>
+      <c r="AZ8">
+        <v>17.149384142305021</v>
+      </c>
+      <c r="BA8">
+        <v>17.149384142305021</v>
+      </c>
+      <c r="BB8">
+        <v>17.149384142305021</v>
+      </c>
+      <c r="BC8">
+        <v>17.149384142305021</v>
+      </c>
+      <c r="BD8">
+        <v>17.149384142305021</v>
+      </c>
+      <c r="BE8">
+        <v>17.149384142305021</v>
+      </c>
+      <c r="BF8">
+        <v>16.814185394841235</v>
+      </c>
+      <c r="BG8">
+        <v>0.33625249379631927</v>
+      </c>
+      <c r="BH8">
+        <v>17.149384142305021</v>
+      </c>
+      <c r="BI8">
+        <v>3.8356500519377459E-2</v>
+      </c>
+      <c r="BJ8">
+        <v>8.3757970000000004</v>
+      </c>
+      <c r="BK8">
+        <v>16.912845679076177</v>
+      </c>
+      <c r="BL8">
+        <v>143.39931430421726</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -11356,7 +11864,7 @@
       <c r="E9" s="22">
         <v>3.2978238816403618E-2</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="134">
         <v>9.7644290288717555E-3</v>
       </c>
       <c r="G9" s="22">
@@ -11479,8 +11987,62 @@
       <c r="AT9">
         <v>2.9906359464203377E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU9">
+        <v>9.6733337110218535E-3</v>
+      </c>
+      <c r="AV9">
+        <v>2.2061203805970779E-3</v>
+      </c>
+      <c r="AW9">
+        <v>2.2061203805970779E-3</v>
+      </c>
+      <c r="AX9">
+        <v>3.2090413403408869E-5</v>
+      </c>
+      <c r="AY9">
+        <v>1.3460290252513904E-4</v>
+      </c>
+      <c r="AZ9">
+        <v>5.9794753778413525E-3</v>
+      </c>
+      <c r="BA9">
+        <v>5.9794753778413525E-3</v>
+      </c>
+      <c r="BB9">
+        <v>5.9794753778413525E-3</v>
+      </c>
+      <c r="BC9">
+        <v>5.9794753778413525E-3</v>
+      </c>
+      <c r="BD9">
+        <v>5.9794753778413525E-3</v>
+      </c>
+      <c r="BE9">
+        <v>5.9794753778413525E-3</v>
+      </c>
+      <c r="BF9">
+        <v>7.4127995691551001E-4</v>
+      </c>
+      <c r="BG9">
+        <v>5.546552434707912E-4</v>
+      </c>
+      <c r="BH9">
+        <v>5.9794753778413525E-3</v>
+      </c>
+      <c r="BI9">
+        <v>2.6073460890269708E-4</v>
+      </c>
+      <c r="BJ9">
+        <v>1.8195209999999999E-3</v>
+      </c>
+      <c r="BK9">
+        <v>2.1096712000111852E-3</v>
+      </c>
+      <c r="BL9">
+        <v>2.2047543409058148E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>59</v>
       </c>
@@ -11488,7 +12050,7 @@
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
+      <c r="F10" s="135"/>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -11516,7 +12078,7 @@
       <c r="AE10" s="33"/>
       <c r="AH10" s="26"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>60</v>
       </c>
@@ -11532,7 +12094,7 @@
       <c r="E11" s="22">
         <v>7.2867891499553102E-4</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="134">
         <v>1.4518721645225947E-3</v>
       </c>
       <c r="G11" s="22">
@@ -11655,9 +12217,62 @@
       <c r="AT11" s="4">
         <v>1.8584796752811258E-3</v>
       </c>
-      <c r="AU11" s="4"/>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU11">
+        <v>3.2117045106031173E-4</v>
+      </c>
+      <c r="AV11">
+        <v>3.5843366297351307E-4</v>
+      </c>
+      <c r="AW11">
+        <v>3.5843366297351307E-4</v>
+      </c>
+      <c r="AX11">
+        <v>2.4979326901376941E-6</v>
+      </c>
+      <c r="AY11">
+        <v>7.3855385435426911E-7</v>
+      </c>
+      <c r="AZ11">
+        <v>2.8625998452723907E-3</v>
+      </c>
+      <c r="BA11">
+        <v>2.8625998452723907E-3</v>
+      </c>
+      <c r="BB11">
+        <v>2.8625998452723907E-3</v>
+      </c>
+      <c r="BC11">
+        <v>2.8625998452723907E-3</v>
+      </c>
+      <c r="BD11">
+        <v>2.8625998452723907E-3</v>
+      </c>
+      <c r="BE11">
+        <v>2.8625998452723907E-3</v>
+      </c>
+      <c r="BF11">
+        <v>3.2948486894321757E-4</v>
+      </c>
+      <c r="BG11">
+        <v>1.3567144751248743E-4</v>
+      </c>
+      <c r="BH11">
+        <v>2.8625998452723907E-3</v>
+      </c>
+      <c r="BI11">
+        <v>2.0295703107368762E-5</v>
+      </c>
+      <c r="BJ11">
+        <v>1.2273030000000001E-3</v>
+      </c>
+      <c r="BK11">
+        <v>1.7464233094573092E-3</v>
+      </c>
+      <c r="BL11">
+        <v>7.1492853891357677E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -11673,7 +12288,7 @@
       <c r="E12" s="22">
         <v>1.6370311183653559E-3</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="134">
         <v>2.0950301720692433E-3</v>
       </c>
       <c r="G12" s="22">
@@ -11796,9 +12411,62 @@
       <c r="AT12" s="4">
         <v>1.0287707349573311E-3</v>
       </c>
-      <c r="AU12" s="4"/>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU12">
+        <v>9.0118330355885444E-4</v>
+      </c>
+      <c r="AV12">
+        <v>1.4693271978995994E-3</v>
+      </c>
+      <c r="AW12">
+        <v>1.4693271978995994E-3</v>
+      </c>
+      <c r="AX12">
+        <v>8.7846573773233351E-6</v>
+      </c>
+      <c r="AY12">
+        <v>5.4901542023334049E-6</v>
+      </c>
+      <c r="AZ12">
+        <v>9.0357439825093731E-3</v>
+      </c>
+      <c r="BA12">
+        <v>9.0357439825093731E-3</v>
+      </c>
+      <c r="BB12">
+        <v>9.0357439825093731E-3</v>
+      </c>
+      <c r="BC12">
+        <v>9.0357439825093731E-3</v>
+      </c>
+      <c r="BD12">
+        <v>9.0357439825093731E-3</v>
+      </c>
+      <c r="BE12">
+        <v>9.0357439825093731E-3</v>
+      </c>
+      <c r="BF12">
+        <v>1.1738590815362408E-3</v>
+      </c>
+      <c r="BG12">
+        <v>3.5191318979473763E-4</v>
+      </c>
+      <c r="BH12">
+        <v>9.0357439825093731E-3</v>
+      </c>
+      <c r="BI12">
+        <v>7.1375341190752084E-5</v>
+      </c>
+      <c r="BJ12">
+        <v>1.9763879999999999E-3</v>
+      </c>
+      <c r="BK12">
+        <v>2.1003465156061028E-3</v>
+      </c>
+      <c r="BL12">
+        <v>5.0841217516793533E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -11814,7 +12482,7 @@
       <c r="E13" s="22">
         <v>3.7651301520934852E-3</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="134">
         <v>4.8949134111340919E-3</v>
       </c>
       <c r="G13" s="22">
@@ -11937,9 +12605,62 @@
       <c r="AT13" s="4">
         <v>1.3551886660240417E-3</v>
       </c>
-      <c r="AU13" s="4"/>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU13">
+        <v>4.4206261729713833E-3</v>
+      </c>
+      <c r="AV13">
+        <v>2.1147683414910615E-3</v>
+      </c>
+      <c r="AW13">
+        <v>2.1147683414910615E-3</v>
+      </c>
+      <c r="AX13">
+        <v>1.5733943315840347E-5</v>
+      </c>
+      <c r="AY13">
+        <v>8.8882725845278173E-6</v>
+      </c>
+      <c r="AZ13">
+        <v>1.2016331282035468E-2</v>
+      </c>
+      <c r="BA13">
+        <v>1.2016331282035468E-2</v>
+      </c>
+      <c r="BB13">
+        <v>1.2016331282035468E-2</v>
+      </c>
+      <c r="BC13">
+        <v>1.2016331282035468E-2</v>
+      </c>
+      <c r="BD13">
+        <v>1.2016331282035468E-2</v>
+      </c>
+      <c r="BE13">
+        <v>1.2016331282035468E-2</v>
+      </c>
+      <c r="BF13">
+        <v>2.1162595232694635E-3</v>
+      </c>
+      <c r="BG13">
+        <v>5.3462146821994013E-4</v>
+      </c>
+      <c r="BH13">
+        <v>1.2016331282035468E-2</v>
+      </c>
+      <c r="BI13">
+        <v>1.2783828944120282E-4</v>
+      </c>
+      <c r="BJ13">
+        <v>3.2296099999999999E-3</v>
+      </c>
+      <c r="BK13">
+        <v>2.0960223251596816E-3</v>
+      </c>
+      <c r="BL13">
+        <v>9.0564148360102958E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -11955,7 +12676,7 @@
       <c r="E14" s="22">
         <v>2.2562370370703095E-4</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="134">
         <v>1.0582886736867189E-3</v>
       </c>
       <c r="G14" s="22">
@@ -12078,9 +12799,62 @@
       <c r="AT14" s="4">
         <v>9.2590380099334864E-4</v>
       </c>
-      <c r="AU14" s="4"/>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU14">
+        <v>1.0404403176396946E-3</v>
+      </c>
+      <c r="AV14">
+        <v>2.5096719103396089E-4</v>
+      </c>
+      <c r="AW14">
+        <v>2.5096719103396089E-4</v>
+      </c>
+      <c r="AX14">
+        <v>2.326725050694978E-6</v>
+      </c>
+      <c r="AY14">
+        <v>4.9339130582133812E-6</v>
+      </c>
+      <c r="AZ14">
+        <v>1.1155220859685694E-3</v>
+      </c>
+      <c r="BA14">
+        <v>1.1155220859685694E-3</v>
+      </c>
+      <c r="BB14">
+        <v>1.1155220859685694E-3</v>
+      </c>
+      <c r="BC14">
+        <v>1.1155220859685694E-3</v>
+      </c>
+      <c r="BD14">
+        <v>1.1155220859685694E-3</v>
+      </c>
+      <c r="BE14">
+        <v>1.1155220859685694E-3</v>
+      </c>
+      <c r="BF14">
+        <v>1.6389900374865949E-4</v>
+      </c>
+      <c r="BG14">
+        <v>6.2734321278646725E-5</v>
+      </c>
+      <c r="BH14">
+        <v>1.1155220859685694E-3</v>
+      </c>
+      <c r="BI14">
+        <v>1.8904641036896698E-5</v>
+      </c>
+      <c r="BJ14">
+        <v>2.01041E-4</v>
+      </c>
+      <c r="BK14">
+        <v>1.6271341968570853E-4</v>
+      </c>
+      <c r="BL14">
+        <v>6.3347493705224476E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -12096,7 +12870,7 @@
       <c r="E15" s="22">
         <v>1.8438990196320597E-4</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="134">
         <v>8.3472257527739265E-4</v>
       </c>
       <c r="G15" s="22">
@@ -12219,9 +12993,62 @@
       <c r="AT15" s="4">
         <v>4.2364544559550575E-4</v>
       </c>
-      <c r="AU15" s="4"/>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU15">
+        <v>8.1851779459990112E-4</v>
+      </c>
+      <c r="AV15">
+        <v>1.6834887068156192E-4</v>
+      </c>
+      <c r="AW15">
+        <v>1.6834887068156192E-4</v>
+      </c>
+      <c r="AX15">
+        <v>1.3317401724638582E-6</v>
+      </c>
+      <c r="AY15">
+        <v>2.709495694275613E-6</v>
+      </c>
+      <c r="AZ15">
+        <v>8.794358938289306E-4</v>
+      </c>
+      <c r="BA15">
+        <v>8.794358938289306E-4</v>
+      </c>
+      <c r="BB15">
+        <v>8.794358938289306E-4</v>
+      </c>
+      <c r="BC15">
+        <v>8.794358938289306E-4</v>
+      </c>
+      <c r="BD15">
+        <v>8.794358938289306E-4</v>
+      </c>
+      <c r="BE15">
+        <v>8.794358938289306E-4</v>
+      </c>
+      <c r="BF15">
+        <v>1.2732009726717131E-4</v>
+      </c>
+      <c r="BG15">
+        <v>4.7548857062017446E-5</v>
+      </c>
+      <c r="BH15">
+        <v>8.794358938289306E-4</v>
+      </c>
+      <c r="BI15">
+        <v>1.0820388901268849E-5</v>
+      </c>
+      <c r="BJ15">
+        <v>1.60686E-4</v>
+      </c>
+      <c r="BK15">
+        <v>1.2817750979861499E-4</v>
+      </c>
+      <c r="BL15">
+        <v>5.5486300276266073E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -12237,7 +13064,7 @@
       <c r="E16" s="22">
         <v>1.0790959835545997E-3</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="134">
         <v>1.1049620245021844E-2</v>
       </c>
       <c r="G16" s="22">
@@ -12360,9 +13187,62 @@
       <c r="AT16" s="4">
         <v>3.2096943740812676E-3</v>
       </c>
-      <c r="AU16" s="4"/>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU16">
+        <v>1.0940294061138075E-2</v>
+      </c>
+      <c r="AV16">
+        <v>1.0680267428573159E-3</v>
+      </c>
+      <c r="AW16">
+        <v>1.0680267428573159E-3</v>
+      </c>
+      <c r="AX16">
+        <v>1.3419259730132339E-5</v>
+      </c>
+      <c r="AY16">
+        <v>6.7945461187616543E-6</v>
+      </c>
+      <c r="AZ16">
+        <v>6.6987568450597376E-3</v>
+      </c>
+      <c r="BA16">
+        <v>6.6987568450597376E-3</v>
+      </c>
+      <c r="BB16">
+        <v>6.6987568450597376E-3</v>
+      </c>
+      <c r="BC16">
+        <v>6.6987568450597376E-3</v>
+      </c>
+      <c r="BD16">
+        <v>6.6987568450597376E-3</v>
+      </c>
+      <c r="BE16">
+        <v>6.6987568450597376E-3</v>
+      </c>
+      <c r="BF16">
+        <v>1.0391152025580992E-3</v>
+      </c>
+      <c r="BG16">
+        <v>3.0192628867213963E-4</v>
+      </c>
+      <c r="BH16">
+        <v>6.6987568450597376E-3</v>
+      </c>
+      <c r="BI16">
+        <v>1.0903148530732527E-4</v>
+      </c>
+      <c r="BJ16">
+        <v>1.652819E-3</v>
+      </c>
+      <c r="BK16">
+        <v>8.7059200446219169E-4</v>
+      </c>
+      <c r="BL16">
+        <v>1.7710330926649157E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>66</v>
       </c>
@@ -12378,7 +13258,7 @@
       <c r="E17" s="22">
         <v>3.5130761445057097E-5</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="134">
         <v>4.8111856107520034E-5</v>
       </c>
       <c r="G17" s="22">
@@ -12501,9 +13381,62 @@
       <c r="AT17" s="4">
         <v>6.2850617270635867E-6</v>
       </c>
-      <c r="AU17" s="4"/>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU17">
+        <v>4.4946357995072476E-5</v>
+      </c>
+      <c r="AV17">
+        <v>1.5318842808204928E-5</v>
+      </c>
+      <c r="AW17">
+        <v>1.5318842808204928E-5</v>
+      </c>
+      <c r="AX17">
+        <v>7.6091274445080203E-8</v>
+      </c>
+      <c r="AY17">
+        <v>1.0655147070654729E-7</v>
+      </c>
+      <c r="AZ17">
+        <v>1.1024560450050121E-4</v>
+      </c>
+      <c r="BA17">
+        <v>1.1024560450050121E-4</v>
+      </c>
+      <c r="BB17">
+        <v>1.1024560450050121E-4</v>
+      </c>
+      <c r="BC17">
+        <v>1.1024560450050121E-4</v>
+      </c>
+      <c r="BD17">
+        <v>1.1024560450050121E-4</v>
+      </c>
+      <c r="BE17">
+        <v>1.1024560450050121E-4</v>
+      </c>
+      <c r="BF17">
+        <v>1.6678591358774617E-5</v>
+      </c>
+      <c r="BG17">
+        <v>5.1839392164824026E-6</v>
+      </c>
+      <c r="BH17">
+        <v>1.1024560450050121E-4</v>
+      </c>
+      <c r="BI17">
+        <v>6.182416048662768E-7</v>
+      </c>
+      <c r="BJ17">
+        <v>2.4223000000000002E-5</v>
+      </c>
+      <c r="BK17">
+        <v>1.5402460347910774E-5</v>
+      </c>
+      <c r="BL17">
+        <v>2.267359245953986E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>67</v>
       </c>
@@ -12519,7 +13452,7 @@
       <c r="E18" s="22">
         <v>3.1238623176942234E-5</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="134">
         <v>1.0621832498893018E-4</v>
       </c>
       <c r="G18" s="22">
@@ -12642,9 +13575,62 @@
       <c r="AT18" s="4">
         <v>1.6206970607669284E-5</v>
       </c>
-      <c r="AU18" s="4"/>
-    </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU18">
+        <v>9.8395128927191022E-5</v>
+      </c>
+      <c r="AV18">
+        <v>4.8671821414560816E-5</v>
+      </c>
+      <c r="AW18">
+        <v>4.8671821414560816E-5</v>
+      </c>
+      <c r="AX18">
+        <v>3.7696167206867435E-7</v>
+      </c>
+      <c r="AY18">
+        <v>1.5124048468983523E-7</v>
+      </c>
+      <c r="AZ18">
+        <v>2.7268668034746972E-4</v>
+      </c>
+      <c r="BA18">
+        <v>2.7268668034746972E-4</v>
+      </c>
+      <c r="BB18">
+        <v>2.7268668034746972E-4</v>
+      </c>
+      <c r="BC18">
+        <v>2.7268668034746972E-4</v>
+      </c>
+      <c r="BD18">
+        <v>2.7268668034746972E-4</v>
+      </c>
+      <c r="BE18">
+        <v>2.7268668034746972E-4</v>
+      </c>
+      <c r="BF18">
+        <v>4.0251380607755908E-5</v>
+      </c>
+      <c r="BG18">
+        <v>1.375168911277876E-5</v>
+      </c>
+      <c r="BH18">
+        <v>2.7268668034746972E-4</v>
+      </c>
+      <c r="BI18">
+        <v>3.0628135855579789E-6</v>
+      </c>
+      <c r="BJ18">
+        <v>5.9191000000000003E-5</v>
+      </c>
+      <c r="BK18">
+        <v>4.3080929272219695E-5</v>
+      </c>
+      <c r="BL18">
+        <v>1.1238738180435919E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>68</v>
       </c>
@@ -12660,7 +13646,7 @@
       <c r="E19" s="22">
         <v>2.0265281039525424E-3</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="134">
         <v>3.7908790257546046E-3</v>
       </c>
       <c r="G19" s="22">
@@ -12783,9 +13769,62 @@
       <c r="AT19" s="4">
         <v>4.20452167506847E-3</v>
       </c>
-      <c r="AU19" s="4"/>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU19">
+        <v>2.1012190222127122E-3</v>
+      </c>
+      <c r="AV19">
+        <v>6.1328558194932515E-3</v>
+      </c>
+      <c r="AW19">
+        <v>6.1328558194932515E-3</v>
+      </c>
+      <c r="AX19">
+        <v>4.6672099899350148E-5</v>
+      </c>
+      <c r="AY19">
+        <v>4.9809085410593131E-6</v>
+      </c>
+      <c r="AZ19">
+        <v>3.4177296712744172E-2</v>
+      </c>
+      <c r="BA19">
+        <v>3.4177296712744172E-2</v>
+      </c>
+      <c r="BB19">
+        <v>3.4177296712744172E-2</v>
+      </c>
+      <c r="BC19">
+        <v>3.4177296712744172E-2</v>
+      </c>
+      <c r="BD19">
+        <v>3.4177296712744172E-2</v>
+      </c>
+      <c r="BE19">
+        <v>3.4177296712744172E-2</v>
+      </c>
+      <c r="BF19">
+        <v>5.6163768386055567E-3</v>
+      </c>
+      <c r="BG19">
+        <v>2.4549134989312366E-3</v>
+      </c>
+      <c r="BH19">
+        <v>3.4177296712744172E-2</v>
+      </c>
+      <c r="BI19">
+        <v>3.7921081168221991E-4</v>
+      </c>
+      <c r="BJ19">
+        <v>5.8936729999999994E-3</v>
+      </c>
+      <c r="BK19">
+        <v>8.4885067131846726E-3</v>
+      </c>
+      <c r="BL19">
+        <v>8.9030298819192874E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -12801,7 +13840,7 @@
       <c r="E20" s="22">
         <v>2.6985670200181072E-3</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="134">
         <v>3.5321920990798189E-5</v>
       </c>
       <c r="G20" s="22">
@@ -12924,9 +13963,62 @@
       <c r="AT20" s="4">
         <v>1.7149055177278329E-5</v>
       </c>
-      <c r="AU20" s="4"/>
-    </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU20">
+        <v>2.3823858197945876E-5</v>
+      </c>
+      <c r="AV20">
+        <v>5.3785118551802877E-5</v>
+      </c>
+      <c r="AW20">
+        <v>5.3785118551802877E-5</v>
+      </c>
+      <c r="AX20">
+        <v>4.2213173274363571E-7</v>
+      </c>
+      <c r="AY20">
+        <v>5.6664914443380942E-8</v>
+      </c>
+      <c r="AZ20">
+        <v>2.7968853538439578E-4</v>
+      </c>
+      <c r="BA20">
+        <v>2.7968853538439578E-4</v>
+      </c>
+      <c r="BB20">
+        <v>2.7968853538439578E-4</v>
+      </c>
+      <c r="BC20">
+        <v>2.7968853538439578E-4</v>
+      </c>
+      <c r="BD20">
+        <v>2.7968853538439578E-4</v>
+      </c>
+      <c r="BE20">
+        <v>2.7968853538439578E-4</v>
+      </c>
+      <c r="BF20">
+        <v>4.2515389519619327E-5</v>
+      </c>
+      <c r="BG20">
+        <v>1.4517663231511721E-5</v>
+      </c>
+      <c r="BH20">
+        <v>2.7968853538439578E-4</v>
+      </c>
+      <c r="BI20">
+        <v>3.4298203285420399E-6</v>
+      </c>
+      <c r="BJ20">
+        <v>2.0967329999999999E-3</v>
+      </c>
+      <c r="BK20">
+        <v>4.3525227367842782E-5</v>
+      </c>
+      <c r="BL20">
+        <v>6.0967430698154849E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
         <v>70</v>
       </c>
@@ -12942,7 +14034,7 @@
       <c r="E21" s="30">
         <v>0.89131293645591025</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="136">
         <v>1.5403860427603833</v>
       </c>
       <c r="G21" s="30">
@@ -13065,9 +14157,62 @@
       <c r="AT21" s="64">
         <v>0.78372738956644916</v>
       </c>
-      <c r="AU21" s="64"/>
-    </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU21">
+        <v>0.98977076923666552</v>
+      </c>
+      <c r="AV21">
+        <v>2.9906430499306933</v>
+      </c>
+      <c r="AW21">
+        <v>2.9906430499306933</v>
+      </c>
+      <c r="AX21">
+        <v>2.1196812302494747E-2</v>
+      </c>
+      <c r="AY21">
+        <v>3.7719393576396E-3</v>
+      </c>
+      <c r="AZ21">
+        <v>10.954043024257045</v>
+      </c>
+      <c r="BA21">
+        <v>10.954043024257045</v>
+      </c>
+      <c r="BB21">
+        <v>10.954043024257045</v>
+      </c>
+      <c r="BC21">
+        <v>10.954043024257045</v>
+      </c>
+      <c r="BD21">
+        <v>10.954043024257045</v>
+      </c>
+      <c r="BE21">
+        <v>10.954043024257045</v>
+      </c>
+      <c r="BF21">
+        <v>1.885344789686233</v>
+      </c>
+      <c r="BG21">
+        <v>0.99108850050692909</v>
+      </c>
+      <c r="BH21">
+        <v>10.954043024257045</v>
+      </c>
+      <c r="BI21">
+        <v>0.17222409995776983</v>
+      </c>
+      <c r="BJ21">
+        <v>1.9748460000000001</v>
+      </c>
+      <c r="BK21">
+        <v>2.4557188258542357</v>
+      </c>
+      <c r="BL21">
+        <v>29.838516773361853</v>
+      </c>
+    </row>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -13140,8 +14285,62 @@
       <c r="AT23" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AU23" t="s">
+        <v>349</v>
+      </c>
+      <c r="AV23" t="s">
+        <v>349</v>
+      </c>
+      <c r="AW23" t="s">
+        <v>349</v>
+      </c>
+      <c r="AX23" t="s">
+        <v>349</v>
+      </c>
+      <c r="AY23" t="s">
+        <v>349</v>
+      </c>
+      <c r="AZ23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BA23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BB23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BC23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BD23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BE23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BF23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BG23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BH23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BI23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BJ23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BK23" t="s">
+        <v>349</v>
+      </c>
+      <c r="BL23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="27" spans="1:64" x14ac:dyDescent="0.35">
       <c r="AQ27">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
Adding CAP pathway ... Continued
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3205F58-BADE-40BB-98C4-D3A2870AF62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39498F3E-BFA4-4CC0-9836-7E75147DB8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="745" firstSheet="3" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" firstSheet="3" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="370">
   <si>
     <t>NG</t>
   </si>
@@ -1222,9 +1222,6 @@
     <t>Betaketoadipate</t>
   </si>
   <si>
-    <t>EtOH, converted to gram</t>
-  </si>
-  <si>
     <t>Adipic acid</t>
   </si>
   <si>
@@ -1409,13 +1406,25 @@
   </si>
   <si>
     <t>Surfactant</t>
+  </si>
+  <si>
+    <t>Polyurethane</t>
+  </si>
+  <si>
+    <t>Hydrogen for CAP</t>
+  </si>
+  <si>
+    <t>Algae, converted to mmBtu</t>
+  </si>
+  <si>
+    <t>Nitrogen Gas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="12">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1427,6 +1436,7 @@
     <numFmt numFmtId="171" formatCode="#,##0.000000000"/>
     <numFmt numFmtId="172" formatCode="#,##0.0000000000"/>
     <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="174" formatCode="0.00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1476,7 +1486,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1546,6 +1556,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1733,7 +1749,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1984,15 +2000,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2013,6 +2020,26 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2800,34 +2827,34 @@
         <v>14</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AD1" s="6" t="s">
         <v>300</v>
@@ -2836,7 +2863,7 @@
         <v>48</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AG1" s="117" t="s">
         <v>303</v>
@@ -2860,22 +2887,22 @@
         <v>242</v>
       </c>
       <c r="AN1" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AR1" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AS1" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="AQ1" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="AR1" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="AS1" s="6" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:45" ht="78.5" x14ac:dyDescent="0.35">
@@ -2895,13 +2922,13 @@
         <v>20</v>
       </c>
       <c r="G2" s="121" t="s">
+        <v>311</v>
+      </c>
+      <c r="H2" s="121" t="s">
         <v>312</v>
       </c>
-      <c r="H2" s="121" t="s">
-        <v>313</v>
-      </c>
       <c r="I2" s="121" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J2" s="65" t="s">
         <v>80</v>
@@ -2931,7 +2958,7 @@
         <v>86</v>
       </c>
       <c r="S2" s="65" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="T2" s="65" t="s">
         <v>80</v>
@@ -2961,7 +2988,7 @@
         <v>86</v>
       </c>
       <c r="AC2" s="65" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AD2" s="65" t="s">
         <v>91</v>
@@ -2970,46 +2997,46 @@
         <v>92</v>
       </c>
       <c r="AF2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AG2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AH2" s="65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI2" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="AJ2" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="AJ2" s="65" t="s">
-        <v>315</v>
-      </c>
       <c r="AK2" s="65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AL2" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="AM2" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="AM2" s="65" t="s">
-        <v>315</v>
-      </c>
       <c r="AN2" s="65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AO2" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="AP2" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="AP2" s="65" t="s">
-        <v>315</v>
-      </c>
       <c r="AQ2" s="65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AR2" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="AS2" s="65" t="s">
         <v>314</v>
-      </c>
-      <c r="AS2" s="65" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.35">
@@ -5460,30 +5487,30 @@
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="128"/>
-      <c r="K23" s="128"/>
-      <c r="L23" s="128"/>
-      <c r="M23" s="128"/>
-      <c r="N23" s="128"/>
-      <c r="O23" s="128"/>
-      <c r="P23" s="128"/>
-      <c r="Q23" s="128"/>
-      <c r="R23" s="128"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="136"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="136"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="136"/>
+      <c r="J23" s="136"/>
+      <c r="K23" s="136"/>
+      <c r="L23" s="136"/>
+      <c r="M23" s="136"/>
+      <c r="N23" s="136"/>
+      <c r="O23" s="136"/>
+      <c r="P23" s="136"/>
+      <c r="Q23" s="136"/>
+      <c r="R23" s="136"/>
       <c r="S23" s="35" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="T23" s="35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="U23" s="35"/>
       <c r="V23" s="35"/>
@@ -5498,7 +5525,7 @@
         <v>90</v>
       </c>
       <c r="AI23" s="69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AJ23" s="69"/>
       <c r="AK23" s="69"/>
@@ -5506,7 +5533,7 @@
       <c r="AM23" s="69"/>
       <c r="AN23" s="69"/>
       <c r="AO23" s="69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AP23" s="69"/>
     </row>
@@ -5542,7 +5569,7 @@
         <v>94</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E1" s="62" t="s">
         <v>95</v>
@@ -5611,7 +5638,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B4" s="40">
         <v>9.9999999999999995E-7</v>
@@ -5924,7 +5951,7 @@
         <v>110</v>
       </c>
       <c r="J1" s="126" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -6192,7 +6219,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="127" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B10" s="69">
         <f>1/J2</f>
@@ -6553,7 +6580,7 @@
         <v>299</v>
       </c>
       <c r="AF5" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AG5" s="17" t="s">
         <v>245</v>
@@ -7375,7 +7402,7 @@
       </c>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.35">
-      <c r="B12" s="129" t="s">
+      <c r="B12" s="137" t="s">
         <v>290</v>
       </c>
       <c r="C12" s="96" t="s">
@@ -7393,7 +7420,7 @@
       <c r="M12" s="98"/>
     </row>
     <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="130"/>
+      <c r="B13" s="138"/>
       <c r="C13" s="99" t="s">
         <v>1</v>
       </c>
@@ -7881,7 +7908,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="110"/>
-      <c r="B25" s="129" t="s">
+      <c r="B25" s="137" t="s">
         <v>290</v>
       </c>
       <c r="C25" s="96" t="s">
@@ -7900,7 +7927,7 @@
     </row>
     <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="76"/>
-      <c r="B26" s="130"/>
+      <c r="B26" s="138"/>
       <c r="C26" s="99" t="s">
         <v>1</v>
       </c>
@@ -8603,31 +8630,31 @@
         <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H1" t="s">
         <v>242</v>
       </c>
       <c r="I1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J1" t="s">
         <v>339</v>
       </c>
-      <c r="J1" t="s">
-        <v>340</v>
-      </c>
       <c r="K1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M1" t="s">
         <v>22</v>
@@ -8663,7 +8690,7 @@
         <v>31</v>
       </c>
       <c r="X1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
@@ -8698,46 +8725,46 @@
         <v>184</v>
       </c>
       <c r="K2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="R2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="T2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="U2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="V2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="W2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="X2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
@@ -10076,15 +10103,15 @@
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="136" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="128"/>
-      <c r="D22" s="128"/>
-      <c r="E22" s="128"/>
-      <c r="F22" s="128"/>
+      <c r="C22" s="136"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="136"/>
       <c r="G22" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H22" s="35"/>
     </row>
@@ -10281,11 +10308,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
-  <dimension ref="A1:BL27"/>
+  <dimension ref="A1:BN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BI27" sqref="BI27"/>
+      <pane xSplit="1" topLeftCell="AW1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BJ1" sqref="BJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10298,10 +10325,10 @@
     <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>71</v>
@@ -10312,7 +10339,7 @@
       <c r="E1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="131" t="s">
+      <c r="F1" s="128" t="s">
         <v>40</v>
       </c>
       <c r="G1" s="17" t="s">
@@ -10370,7 +10397,7 @@
         <v>56</v>
       </c>
       <c r="Y1" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Z1" s="17" t="s">
         <v>57</v>
@@ -10396,148 +10423,154 @@
       <c r="AG1" t="s">
         <v>89</v>
       </c>
-      <c r="AH1" s="117" t="s">
+      <c r="AH1" s="140" t="s">
+        <v>367</v>
+      </c>
+      <c r="AI1" s="117" t="s">
         <v>303</v>
       </c>
-      <c r="AI1" s="117" t="s">
+      <c r="AJ1" s="140" t="s">
         <v>150</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>321</v>
-      </c>
       <c r="AK1" t="s">
-        <v>323</v>
-      </c>
-      <c r="AL1" s="124" t="s">
+        <v>320</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AM1" s="124" t="s">
+        <v>325</v>
+      </c>
+      <c r="AN1" s="124" t="s">
         <v>326</v>
       </c>
-      <c r="AM1" s="124" t="s">
+      <c r="AO1" s="124" t="s">
         <v>327</v>
       </c>
-      <c r="AN1" s="124" t="s">
-        <v>328</v>
-      </c>
-      <c r="AO1" s="124" t="s">
-        <v>325</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>342</v>
+      <c r="AP1" s="124" t="s">
+        <v>324</v>
       </c>
       <c r="AQ1" t="s">
+        <v>341</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AS1" t="s">
         <v>344</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>345</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>346</v>
       </c>
-      <c r="AT1" t="s">
-        <v>347</v>
-      </c>
-      <c r="AU1" s="137" t="s">
+      <c r="AV1" s="134" t="s">
+        <v>349</v>
+      </c>
+      <c r="AW1" s="134" t="s">
         <v>350</v>
       </c>
-      <c r="AV1" s="137" t="s">
+      <c r="AX1" s="134" t="s">
         <v>351</v>
       </c>
-      <c r="AW1" s="137" t="s">
+      <c r="AY1" s="135" t="s">
         <v>352</v>
       </c>
-      <c r="AX1" s="138" t="s">
+      <c r="AZ1" s="135" t="s">
         <v>353</v>
       </c>
-      <c r="AY1" s="138" t="s">
+      <c r="BA1" s="135" t="s">
         <v>354</v>
       </c>
-      <c r="AZ1" s="138" t="s">
+      <c r="BB1" s="135" t="s">
         <v>355</v>
       </c>
-      <c r="BA1" s="138" t="s">
+      <c r="BC1" s="135" t="s">
         <v>356</v>
       </c>
-      <c r="BB1" s="138" t="s">
+      <c r="BD1" s="135" t="s">
         <v>357</v>
       </c>
-      <c r="BC1" s="138" t="s">
+      <c r="BE1" s="135" t="s">
         <v>358</v>
       </c>
-      <c r="BD1" s="138" t="s">
+      <c r="BF1" s="135" t="s">
         <v>359</v>
       </c>
-      <c r="BE1" s="138" t="s">
+      <c r="BG1" s="135" t="s">
         <v>360</v>
       </c>
-      <c r="BF1" s="138" t="s">
+      <c r="BH1" s="135" t="s">
         <v>361</v>
       </c>
-      <c r="BG1" s="138" t="s">
+      <c r="BI1" s="135" t="s">
         <v>362</v>
       </c>
-      <c r="BH1" s="138" t="s">
+      <c r="BJ1" s="135" t="s">
+        <v>369</v>
+      </c>
+      <c r="BK1" s="135" t="s">
         <v>363</v>
       </c>
-      <c r="BI1" s="138" t="s">
-        <v>49</v>
-      </c>
-      <c r="BJ1" s="138" t="s">
+      <c r="BL1" s="135" t="s">
         <v>364</v>
       </c>
-      <c r="BK1" s="138" t="s">
+      <c r="BM1" s="135" t="s">
         <v>365</v>
       </c>
-      <c r="BL1" s="138" t="s">
+      <c r="BN1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E2" s="65" t="s">
-        <v>307</v>
-      </c>
-      <c r="F2" s="132" t="s">
-        <v>307</v>
+        <v>306</v>
+      </c>
+      <c r="F2" s="129" t="s">
+        <v>306</v>
       </c>
       <c r="G2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P2" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q2" s="65" t="s">
         <v>2</v>
@@ -10555,34 +10588,34 @@
         <v>2</v>
       </c>
       <c r="V2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="W2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="X2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Y2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Z2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AA2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AB2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AC2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AD2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AE2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AF2" s="119" t="s">
         <v>219</v>
@@ -10590,101 +10623,107 @@
       <c r="AG2" s="119" t="s">
         <v>184</v>
       </c>
-      <c r="AH2" s="117" t="s">
-        <v>307</v>
+      <c r="AH2" s="142" t="s">
+        <v>184</v>
       </c>
       <c r="AI2" s="117" t="s">
-        <v>307</v>
-      </c>
-      <c r="AJ2" s="117" t="s">
-        <v>307</v>
+        <v>306</v>
+      </c>
+      <c r="AJ2" s="140" t="s">
+        <v>306</v>
       </c>
       <c r="AK2" s="117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AL2" s="117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM2" s="117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AN2" s="117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AO2" s="117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AP2" s="117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AQ2" s="117" t="s">
-        <v>343</v>
+        <v>306</v>
       </c>
       <c r="AR2" s="117" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AS2" s="117" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AT2" s="117" t="s">
-        <v>343</v>
-      </c>
-      <c r="AU2" s="119" t="s">
-        <v>307</v>
+        <v>342</v>
+      </c>
+      <c r="AU2" s="117" t="s">
+        <v>342</v>
       </c>
       <c r="AV2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AW2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AX2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AY2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AZ2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BA2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BB2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BC2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BD2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BE2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BF2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BG2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BH2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BI2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BJ2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BK2" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BL2" s="119" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+      <c r="BM2" s="119" t="s">
+        <v>306</v>
+      </c>
+      <c r="BN2" s="119" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -10700,7 +10739,7 @@
       <c r="E3" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="133" t="s">
+      <c r="F3" s="130" t="s">
         <v>93</v>
       </c>
       <c r="G3" s="20" t="s">
@@ -10784,13 +10823,13 @@
       <c r="AG3" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="AH3" s="20" t="s">
-        <v>93</v>
+      <c r="AH3" s="141" t="s">
+        <v>109</v>
       </c>
       <c r="AI3" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="AJ3" s="20" t="s">
+      <c r="AJ3" s="141" t="s">
         <v>93</v>
       </c>
       <c r="AK3" s="20" t="s">
@@ -10877,8 +10916,14 @@
       <c r="BL3" s="20" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BM3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN3" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -10894,7 +10939,7 @@
       <c r="E4" s="22">
         <v>96.173077193221943</v>
       </c>
-      <c r="F4" s="134">
+      <c r="F4" s="131">
         <v>24.292168425500595</v>
       </c>
       <c r="G4" s="22">
@@ -10978,62 +11023,62 @@
       <c r="AG4">
         <v>1315314.5481741754</v>
       </c>
-      <c r="AH4" s="22">
+      <c r="AH4" s="140">
+        <v>1577047.8115483243</v>
+      </c>
+      <c r="AI4" s="22">
         <v>99.15771301835683</v>
       </c>
-      <c r="AI4">
-        <v>22.768308419908244</v>
-      </c>
-      <c r="AJ4">
+      <c r="AJ4" s="140">
+        <v>48.309136220851776</v>
+      </c>
+      <c r="AK4">
         <v>19.71853497029684</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>4.713895066511232</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>127.71897395630178</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>39.483586132842056</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>89.569325488930929</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>145.64724186833132</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>24.292168425500595</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>0.50297207180397385</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>26.757444950472731</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>72.594892899575541</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>30.295317337266482</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>15.019429554309164</v>
-      </c>
-      <c r="AV4">
-        <v>39.483586132842049</v>
       </c>
       <c r="AW4">
         <v>39.483586132842049</v>
       </c>
       <c r="AX4">
+        <v>39.483586132842049</v>
+      </c>
+      <c r="AY4">
         <v>0.3581698661381561</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>4.3833672938355273E-2</v>
-      </c>
-      <c r="AZ4">
-        <v>196.70295779410594</v>
       </c>
       <c r="BA4">
         <v>196.70295779410594</v>
@@ -11051,28 +11096,34 @@
         <v>196.70295779410594</v>
       </c>
       <c r="BF4">
+        <v>196.70295779410594</v>
+      </c>
+      <c r="BG4">
         <v>39.70337997545861</v>
       </c>
-      <c r="BG4">
+      <c r="BH4">
         <v>16.573687577719323</v>
       </c>
-      <c r="BH4">
+      <c r="BI4">
         <v>196.70295779410594</v>
       </c>
-      <c r="BI4">
+      <c r="BJ4">
         <v>2.9101301623725186</v>
       </c>
-      <c r="BJ4">
+      <c r="BK4">
         <v>35.607860000000002</v>
       </c>
-      <c r="BK4">
+      <c r="BL4">
         <v>62.504452652498195</v>
       </c>
-      <c r="BL4">
+      <c r="BM4">
         <v>1708.6819416186172</v>
       </c>
-    </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN4">
+        <v>69.378860802973378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -11088,7 +11139,7 @@
       <c r="E5" s="22">
         <v>12.434256086332805</v>
       </c>
-      <c r="F5" s="134">
+      <c r="F5" s="131">
         <v>23.112834811006994</v>
       </c>
       <c r="G5" s="22">
@@ -11172,62 +11223,62 @@
       <c r="AG5">
         <v>1311743.8531964528</v>
       </c>
-      <c r="AH5" s="22">
+      <c r="AH5" s="140">
+        <v>1517324.445253175</v>
+      </c>
+      <c r="AI5" s="22">
         <v>99.10102802045931</v>
       </c>
-      <c r="AI5">
-        <v>14.313720661890066</v>
-      </c>
-      <c r="AJ5">
+      <c r="AJ5" s="140">
+        <v>14.315311187199075</v>
+      </c>
+      <c r="AK5">
         <v>17.330570910222324</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>4.6160147561533957</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>121.57941481743229</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>34.523904822559238</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>84.799946333148981</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>123.61276677668523</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>23.112834811006994</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>0.44760730126075743</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>24.942073667191227</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>69.694323608710306</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>29.831066400462845</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>13.93301632154248</v>
-      </c>
-      <c r="AV5">
-        <v>34.523904822559238</v>
       </c>
       <c r="AW5">
         <v>34.523904822559238</v>
       </c>
       <c r="AX5">
+        <v>34.523904822559238</v>
+      </c>
+      <c r="AY5">
         <v>0.28132753242105452</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>3.9756448338327942E-2</v>
-      </c>
-      <c r="AZ5">
-        <v>190.79583917725958</v>
       </c>
       <c r="BA5">
         <v>190.79583917725958</v>
@@ -11245,28 +11296,34 @@
         <v>190.79583917725958</v>
       </c>
       <c r="BF5">
+        <v>190.79583917725958</v>
+      </c>
+      <c r="BG5">
         <v>39.17718902955842</v>
       </c>
-      <c r="BG5">
+      <c r="BH5">
         <v>15.711261044001366</v>
       </c>
-      <c r="BH5">
+      <c r="BI5">
         <v>190.79583917725958</v>
       </c>
-      <c r="BI5">
+      <c r="BJ5">
         <v>2.2857862009210681</v>
       </c>
-      <c r="BJ5">
+      <c r="BK5">
         <v>34.146839999999997</v>
       </c>
-      <c r="BK5">
+      <c r="BL5">
         <v>60.353903810734323</v>
       </c>
-      <c r="BL5">
+      <c r="BM5">
         <v>593.4443720738916</v>
       </c>
-    </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN5">
+        <v>66.562363858854823</v>
+      </c>
+    </row>
+    <row r="6" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -11282,7 +11339,7 @@
       <c r="E6" s="22">
         <v>0.46325014313213203</v>
       </c>
-      <c r="F6" s="134">
+      <c r="F6" s="131">
         <v>1.6501694729418555</v>
       </c>
       <c r="G6" s="22">
@@ -11366,62 +11423,62 @@
       <c r="AG6">
         <v>4999.13237353164</v>
       </c>
-      <c r="AH6" s="22">
+      <c r="AH6" s="140">
+        <v>83636.313938146748</v>
+      </c>
+      <c r="AI6" s="22">
         <v>7.6154275905965907E-2</v>
       </c>
-      <c r="AI6">
-        <v>1.01369654150063</v>
-      </c>
-      <c r="AJ6">
+      <c r="AJ6" s="140">
+        <v>1.0137246040480141</v>
+      </c>
+      <c r="AK6">
         <v>3.3441377698756791</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>3.8723908230081485</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>10.261050836516857</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>8.2835881755944225</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>29.197535715325103</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>39.708186457607347</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>1.6501694729418555</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>0.17818913929090893</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>17.543672338399276</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>4.0571849924479393</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>20.605899142323508</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>1.5201149893010175</v>
-      </c>
-      <c r="AV6">
-        <v>8.2835881755944225</v>
       </c>
       <c r="AW6">
         <v>8.2835881755944225</v>
       </c>
       <c r="AX6">
+        <v>8.2835881755944225</v>
+      </c>
+      <c r="AY6">
         <v>0.1076113461139153</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>5.6827199192912457E-3</v>
-      </c>
-      <c r="AZ6">
-        <v>16.802194749958446</v>
       </c>
       <c r="BA6">
         <v>16.802194749958446</v>
@@ -11439,28 +11496,34 @@
         <v>16.802194749958446</v>
       </c>
       <c r="BF6">
+        <v>16.802194749958446</v>
+      </c>
+      <c r="BG6">
         <v>3.8579793740200041</v>
       </c>
-      <c r="BG6">
+      <c r="BH6">
         <v>1.2076769380332584</v>
       </c>
-      <c r="BH6">
+      <c r="BI6">
         <v>16.802194749958446</v>
       </c>
-      <c r="BI6">
+      <c r="BJ6">
         <v>0.87434218717556189</v>
       </c>
-      <c r="BJ6">
+      <c r="BK6">
         <v>2.8897429999999997</v>
       </c>
-      <c r="BK6">
+      <c r="BL6">
         <v>3.0069126161037167</v>
       </c>
-      <c r="BL6">
+      <c r="BM6">
         <v>21.022320614309901</v>
       </c>
-    </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN6">
+        <v>3.5388428925359858</v>
+      </c>
+    </row>
+    <row r="7" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -11476,7 +11539,7 @@
       <c r="E7" s="22">
         <v>8.61916794675669</v>
       </c>
-      <c r="F7" s="134">
+      <c r="F7" s="131">
         <v>16.483574246246874</v>
       </c>
       <c r="G7" s="22">
@@ -11560,62 +11623,62 @@
       <c r="AG7">
         <v>1301825.3866966912</v>
       </c>
-      <c r="AH7" s="22">
+      <c r="AH7" s="140">
+        <v>1425319.0641897889</v>
+      </c>
+      <c r="AI7" s="22">
         <v>87.624663165139467</v>
       </c>
-      <c r="AI7">
-        <v>11.762225607448672</v>
-      </c>
-      <c r="AJ7">
+      <c r="AJ7" s="140">
+        <v>11.763196513266807</v>
+      </c>
+      <c r="AK7">
         <v>13.808648364234854</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <v>0.49785115624678716</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>65.13770328951459</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <v>25.563238243896709</v>
       </c>
-      <c r="AN7">
+      <c r="AO7">
         <v>50.092954028495811</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <v>66.003611385435917</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <v>16.483574246246874</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <v>0.13435262332578293</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>7.5034587428535566</v>
       </c>
-      <c r="AS7">
+      <c r="AT7">
         <v>42.044691025692117</v>
       </c>
-      <c r="AT7">
+      <c r="AU7">
         <v>7.4744027922844962</v>
       </c>
-      <c r="AU7">
+      <c r="AV7">
         <v>7.6966652243150877</v>
-      </c>
-      <c r="AV7">
-        <v>25.563238243896706</v>
       </c>
       <c r="AW7">
         <v>25.563238243896706</v>
       </c>
       <c r="AX7">
+        <v>25.563238243896706</v>
+      </c>
+      <c r="AY7">
         <v>0.16899538624321581</v>
       </c>
-      <c r="AY7">
+      <c r="AZ7">
         <v>1.2713625725546759E-2</v>
-      </c>
-      <c r="AZ7">
-        <v>156.84426028499615</v>
       </c>
       <c r="BA7">
         <v>156.84426028499615</v>
@@ -11633,28 +11696,34 @@
         <v>156.84426028499615</v>
       </c>
       <c r="BF7">
+        <v>156.84426028499615</v>
+      </c>
+      <c r="BG7">
         <v>18.505024260697184</v>
       </c>
-      <c r="BG7">
+      <c r="BH7">
         <v>14.167331612171793</v>
       </c>
-      <c r="BH7">
+      <c r="BI7">
         <v>156.84426028499615</v>
       </c>
-      <c r="BI7">
+      <c r="BJ7">
         <v>1.3730875132261284</v>
       </c>
-      <c r="BJ7">
+      <c r="BK7">
         <v>22.8813</v>
       </c>
-      <c r="BK7">
+      <c r="BL7">
         <v>40.434145515554434</v>
       </c>
-      <c r="BL7">
+      <c r="BM7">
         <v>429.0227371553645</v>
       </c>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN7">
+        <v>47.175363754400323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -11670,7 +11739,7 @@
       <c r="E8" s="22">
         <v>3.3518379964439835</v>
       </c>
-      <c r="F8" s="134">
+      <c r="F8" s="131">
         <v>4.9790910918182654</v>
       </c>
       <c r="G8" s="22">
@@ -11754,62 +11823,62 @@
       <c r="AG8">
         <v>4919.3341262300773</v>
       </c>
-      <c r="AH8" s="22">
+      <c r="AH8" s="140">
+        <v>8369.0671252394204</v>
+      </c>
+      <c r="AI8" s="22">
         <v>11.400210579413892</v>
       </c>
-      <c r="AI8">
-        <v>1.537798512940765</v>
-      </c>
-      <c r="AJ8">
+      <c r="AJ8" s="140">
+        <v>1.5383900698842508</v>
+      </c>
+      <c r="AK8">
         <v>0.17778477611178914</v>
       </c>
-      <c r="AK8">
+      <c r="AL8">
         <v>0.24577277689845986</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>46.180660691400824</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <v>0.67707840306811351</v>
       </c>
-      <c r="AN8">
+      <c r="AO8">
         <v>5.5094565893280594</v>
       </c>
-      <c r="AO8">
+      <c r="AP8">
         <v>17.900968933641973</v>
       </c>
-      <c r="AP8">
+      <c r="AQ8">
         <v>4.9790910918182654</v>
       </c>
-      <c r="AQ8">
+      <c r="AR8">
         <v>0.13506553864406559</v>
       </c>
-      <c r="AR8">
+      <c r="AS8">
         <v>-0.10505741406160518</v>
       </c>
-      <c r="AS8">
+      <c r="AT8">
         <v>23.592447590570245</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <v>1.7507644658548416</v>
       </c>
-      <c r="AU8">
+      <c r="AV8">
         <v>4.7162361079263766</v>
-      </c>
-      <c r="AV8">
-        <v>0.67707840306811351</v>
       </c>
       <c r="AW8">
         <v>0.67707840306811351</v>
       </c>
       <c r="AX8">
+        <v>0.67707840306811351</v>
+      </c>
+      <c r="AY8">
         <v>4.7208000639233794E-3</v>
       </c>
-      <c r="AY8">
+      <c r="AZ8">
         <v>2.1360102693489928E-2</v>
-      </c>
-      <c r="AZ8">
-        <v>17.149384142305021</v>
       </c>
       <c r="BA8">
         <v>17.149384142305021</v>
@@ -11827,28 +11896,34 @@
         <v>17.149384142305021</v>
       </c>
       <c r="BF8">
+        <v>17.149384142305021</v>
+      </c>
+      <c r="BG8">
         <v>16.814185394841235</v>
       </c>
-      <c r="BG8">
+      <c r="BH8">
         <v>0.33625249379631927</v>
       </c>
-      <c r="BH8">
+      <c r="BI8">
         <v>17.149384142305021</v>
       </c>
-      <c r="BI8">
+      <c r="BJ8">
         <v>3.8356500519377459E-2</v>
       </c>
-      <c r="BJ8">
+      <c r="BK8">
         <v>8.3757970000000004</v>
       </c>
-      <c r="BK8">
+      <c r="BL8">
         <v>16.912845679076177</v>
       </c>
-      <c r="BL8">
+      <c r="BM8">
         <v>143.39931430421726</v>
       </c>
-    </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN8">
+        <v>15.848157211918526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -11864,7 +11939,7 @@
       <c r="E9" s="22">
         <v>3.2978238816403618E-2</v>
       </c>
-      <c r="F9" s="134">
+      <c r="F9" s="131">
         <v>9.7644290288717555E-3</v>
       </c>
       <c r="G9" s="22">
@@ -11948,62 +12023,62 @@
       <c r="AG9">
         <v>26.022097330325355</v>
       </c>
-      <c r="AH9" s="22">
+      <c r="AH9" s="140">
+        <v>49.472223700978624</v>
+      </c>
+      <c r="AI9" s="22">
         <v>2.8948575569389908E-3</v>
       </c>
-      <c r="AI9">
-        <v>1.0524015417807536E-2</v>
-      </c>
-      <c r="AJ9">
+      <c r="AJ9" s="140">
+        <v>1.0528740521994456E-2</v>
+      </c>
+      <c r="AK9">
         <v>1.0197927155796403E-3</v>
       </c>
-      <c r="AK9">
+      <c r="AL9">
         <v>1.2315095325999179E-3</v>
       </c>
-      <c r="AL9">
+      <c r="AM9">
         <v>9.0227269325247952E-3</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>2.2061203805970784E-3</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>1.0946639202273211E-2</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <v>2.1124691750367366E-2</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <v>9.7644290288717555E-3</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>1.6085915785098235E-4</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>8.6824142776733063E-4</v>
       </c>
-      <c r="AS9">
+      <c r="AT9">
         <v>2.80437679990544E-3</v>
       </c>
-      <c r="AT9">
+      <c r="AU9">
         <v>2.9906359464203377E-4</v>
       </c>
-      <c r="AU9">
+      <c r="AV9">
         <v>9.6733337110218535E-3</v>
-      </c>
-      <c r="AV9">
-        <v>2.2061203805970779E-3</v>
       </c>
       <c r="AW9">
         <v>2.2061203805970779E-3</v>
       </c>
       <c r="AX9">
+        <v>2.2061203805970779E-3</v>
+      </c>
+      <c r="AY9">
         <v>3.2090413403408869E-5</v>
       </c>
-      <c r="AY9">
+      <c r="AZ9">
         <v>1.3460290252513904E-4</v>
-      </c>
-      <c r="AZ9">
-        <v>5.9794753778413525E-3</v>
       </c>
       <c r="BA9">
         <v>5.9794753778413525E-3</v>
@@ -12021,28 +12096,34 @@
         <v>5.9794753778413525E-3</v>
       </c>
       <c r="BF9">
+        <v>5.9794753778413525E-3</v>
+      </c>
+      <c r="BG9">
         <v>7.4127995691551001E-4</v>
       </c>
-      <c r="BG9">
+      <c r="BH9">
         <v>5.546552434707912E-4</v>
       </c>
-      <c r="BH9">
+      <c r="BI9">
         <v>5.9794753778413525E-3</v>
       </c>
-      <c r="BI9">
+      <c r="BJ9">
         <v>2.6073460890269708E-4</v>
       </c>
-      <c r="BJ9">
+      <c r="BK9">
         <v>1.8195209999999999E-3</v>
       </c>
-      <c r="BK9">
+      <c r="BL9">
         <v>2.1096712000111852E-3</v>
       </c>
-      <c r="BL9">
+      <c r="BM9">
         <v>2.2047543409058148E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN9">
+        <v>1.2571786330539047E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>59</v>
       </c>
@@ -12050,7 +12131,7 @@
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="135"/>
+      <c r="F10" s="132"/>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -12076,9 +12157,11 @@
       <c r="AC10" s="33"/>
       <c r="AD10" s="33"/>
       <c r="AE10" s="33"/>
-      <c r="AH10" s="26"/>
-    </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="AH10" s="140"/>
+      <c r="AI10" s="26"/>
+      <c r="AJ10" s="140"/>
+    </row>
+    <row r="11" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>60</v>
       </c>
@@ -12094,7 +12177,7 @@
       <c r="E11" s="22">
         <v>7.2867891499553102E-4</v>
       </c>
-      <c r="F11" s="134">
+      <c r="F11" s="131">
         <v>1.4518721645225947E-3</v>
       </c>
       <c r="G11" s="22">
@@ -12178,62 +12261,62 @@
       <c r="AG11">
         <v>10.275322226239604</v>
       </c>
-      <c r="AH11" s="22">
+      <c r="AH11" s="140">
+        <v>12.100690959036683</v>
+      </c>
+      <c r="AI11" s="22">
         <v>3.2710763129870442E-3</v>
       </c>
-      <c r="AI11">
-        <v>1.5332925780409926E-3</v>
-      </c>
-      <c r="AJ11">
+      <c r="AJ11" s="140">
+        <v>1.5333537460206102E-3</v>
+      </c>
+      <c r="AK11">
         <v>1.7751686943870412E-4</v>
       </c>
-      <c r="AK11">
+      <c r="AL11">
         <v>9.9332879823585071E-5</v>
       </c>
-      <c r="AL11">
+      <c r="AM11">
         <v>1.9062446610619314E-3</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <v>3.5843366297351313E-4</v>
       </c>
-      <c r="AN11">
+      <c r="AO11">
         <v>9.2654664357150532E-4</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <v>1.9786502273731847E-3</v>
       </c>
-      <c r="AP11">
+      <c r="AQ11">
         <v>1.4518721645225947E-3</v>
       </c>
-      <c r="AQ11" s="4">
+      <c r="AR11" s="4">
         <v>8.0635353283643391E-5</v>
       </c>
-      <c r="AR11" s="4">
+      <c r="AS11" s="4">
         <v>2.6011583240220918E-3</v>
       </c>
-      <c r="AS11" s="4">
+      <c r="AT11" s="4">
         <v>1.8924914822510532E-3</v>
       </c>
-      <c r="AT11" s="4">
+      <c r="AU11" s="4">
         <v>1.8584796752811258E-3</v>
       </c>
-      <c r="AU11">
+      <c r="AV11">
         <v>3.2117045106031173E-4</v>
-      </c>
-      <c r="AV11">
-        <v>3.5843366297351307E-4</v>
       </c>
       <c r="AW11">
         <v>3.5843366297351307E-4</v>
       </c>
       <c r="AX11">
+        <v>3.5843366297351307E-4</v>
+      </c>
+      <c r="AY11">
         <v>2.4979326901376941E-6</v>
       </c>
-      <c r="AY11">
+      <c r="AZ11">
         <v>7.3855385435426911E-7</v>
-      </c>
-      <c r="AZ11">
-        <v>2.8625998452723907E-3</v>
       </c>
       <c r="BA11">
         <v>2.8625998452723907E-3</v>
@@ -12251,28 +12334,34 @@
         <v>2.8625998452723907E-3</v>
       </c>
       <c r="BF11">
+        <v>2.8625998452723907E-3</v>
+      </c>
+      <c r="BG11">
         <v>3.2948486894321757E-4</v>
       </c>
-      <c r="BG11">
+      <c r="BH11">
         <v>1.3567144751248743E-4</v>
       </c>
-      <c r="BH11">
+      <c r="BI11">
         <v>2.8625998452723907E-3</v>
       </c>
-      <c r="BI11">
+      <c r="BJ11">
         <v>2.0295703107368762E-5</v>
       </c>
-      <c r="BJ11">
+      <c r="BK11">
         <v>1.2273030000000001E-3</v>
       </c>
-      <c r="BK11">
+      <c r="BL11">
         <v>1.7464233094573092E-3</v>
       </c>
-      <c r="BL11">
+      <c r="BM11">
         <v>7.1492853891357677E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN11">
+        <v>9.6751445371123475E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -12288,7 +12377,7 @@
       <c r="E12" s="22">
         <v>1.6370311183653559E-3</v>
       </c>
-      <c r="F12" s="134">
+      <c r="F12" s="131">
         <v>2.0950301720692433E-3</v>
       </c>
       <c r="G12" s="22">
@@ -12372,62 +12461,62 @@
       <c r="AG12">
         <v>16.062252431105641</v>
       </c>
-      <c r="AH12" s="22">
+      <c r="AH12" s="140">
+        <v>22.481656351880339</v>
+      </c>
+      <c r="AI12" s="22">
         <v>4.4788457908180607E-3</v>
       </c>
-      <c r="AI12">
-        <v>1.0670036531779258E-3</v>
-      </c>
-      <c r="AJ12">
+      <c r="AJ12" s="140">
+        <v>1.0672619853839356E-3</v>
+      </c>
+      <c r="AK12">
         <v>6.8956754673592041E-4</v>
       </c>
-      <c r="AK12">
+      <c r="AL12">
         <v>4.6636829287775221E-4</v>
       </c>
-      <c r="AL12">
+      <c r="AM12">
         <v>1.0464865335871836E-2</v>
       </c>
-      <c r="AM12">
+      <c r="AN12">
         <v>1.4693271978995996E-3</v>
       </c>
-      <c r="AN12">
+      <c r="AO12">
         <v>3.7186845307009622E-3</v>
       </c>
-      <c r="AO12">
+      <c r="AP12">
         <v>1.0678599210148253E-2</v>
       </c>
-      <c r="AP12">
+      <c r="AQ12">
         <v>2.0950301720692433E-3</v>
       </c>
-      <c r="AQ12" s="4">
+      <c r="AR12" s="4">
         <v>1.3527358854509156E-4</v>
       </c>
-      <c r="AR12" s="4">
+      <c r="AS12" s="4">
         <v>1.8821933237997142E-2</v>
       </c>
-      <c r="AS12" s="4">
+      <c r="AT12" s="4">
         <v>4.3426142466434364E-3</v>
       </c>
-      <c r="AT12" s="4">
+      <c r="AU12" s="4">
         <v>1.0287707349573311E-3</v>
       </c>
-      <c r="AU12">
+      <c r="AV12">
         <v>9.0118330355885444E-4</v>
-      </c>
-      <c r="AV12">
-        <v>1.4693271978995994E-3</v>
       </c>
       <c r="AW12">
         <v>1.4693271978995994E-3</v>
       </c>
       <c r="AX12">
+        <v>1.4693271978995994E-3</v>
+      </c>
+      <c r="AY12">
         <v>8.7846573773233351E-6</v>
       </c>
-      <c r="AY12">
+      <c r="AZ12">
         <v>5.4901542023334049E-6</v>
-      </c>
-      <c r="AZ12">
-        <v>9.0357439825093731E-3</v>
       </c>
       <c r="BA12">
         <v>9.0357439825093731E-3</v>
@@ -12445,28 +12534,34 @@
         <v>9.0357439825093731E-3</v>
       </c>
       <c r="BF12">
+        <v>9.0357439825093731E-3</v>
+      </c>
+      <c r="BG12">
         <v>1.1738590815362408E-3</v>
       </c>
-      <c r="BG12">
+      <c r="BH12">
         <v>3.5191318979473763E-4</v>
       </c>
-      <c r="BH12">
+      <c r="BI12">
         <v>9.0357439825093731E-3</v>
       </c>
-      <c r="BI12">
+      <c r="BJ12">
         <v>7.1375341190752084E-5</v>
       </c>
-      <c r="BJ12">
+      <c r="BK12">
         <v>1.9763879999999999E-3</v>
       </c>
-      <c r="BK12">
+      <c r="BL12">
         <v>2.1003465156061028E-3</v>
       </c>
-      <c r="BL12">
+      <c r="BM12">
         <v>5.0841217516793533E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN12">
+        <v>6.9227894123971819E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -12482,7 +12577,7 @@
       <c r="E13" s="22">
         <v>3.7651301520934852E-3</v>
       </c>
-      <c r="F13" s="134">
+      <c r="F13" s="131">
         <v>4.8949134111340919E-3</v>
       </c>
       <c r="G13" s="22">
@@ -12566,62 +12661,62 @@
       <c r="AG13">
         <v>21.007515266850735</v>
       </c>
-      <c r="AH13" s="22">
+      <c r="AH13" s="140">
+        <v>32.505122182253004</v>
+      </c>
+      <c r="AI13" s="22">
         <v>3.5928608420523145E-2</v>
       </c>
-      <c r="AI13">
-        <v>2.2646336328392878E-3</v>
-      </c>
-      <c r="AJ13">
+      <c r="AJ13" s="140">
+        <v>2.2653418147137137E-3</v>
+      </c>
+      <c r="AK13">
         <v>1.0548951025133679E-3</v>
       </c>
-      <c r="AK13">
+      <c r="AL13">
         <v>2.6270665934260057E-4</v>
       </c>
-      <c r="AL13">
+      <c r="AM13">
         <v>1.0484311282441842E-2</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>2.1147683414910615E-3</v>
       </c>
-      <c r="AN13">
+      <c r="AO13">
         <v>2.5599102522421383E-2</v>
       </c>
-      <c r="AO13">
+      <c r="AP13">
         <v>1.2578946144820949E-2</v>
       </c>
-      <c r="AP13">
+      <c r="AQ13">
         <v>4.8949134111340919E-3</v>
       </c>
-      <c r="AQ13" s="4">
+      <c r="AR13" s="4">
         <v>1.5750565532441076E-4</v>
       </c>
-      <c r="AR13" s="4">
+      <c r="AS13" s="4">
         <v>2.3996815097449505E-3</v>
       </c>
-      <c r="AS13" s="4">
+      <c r="AT13" s="4">
         <v>2.1416397844691969E-3</v>
       </c>
-      <c r="AT13" s="4">
+      <c r="AU13" s="4">
         <v>1.3551886660240417E-3</v>
       </c>
-      <c r="AU13">
+      <c r="AV13">
         <v>4.4206261729713833E-3</v>
-      </c>
-      <c r="AV13">
-        <v>2.1147683414910615E-3</v>
       </c>
       <c r="AW13">
         <v>2.1147683414910615E-3</v>
       </c>
       <c r="AX13">
+        <v>2.1147683414910615E-3</v>
+      </c>
+      <c r="AY13">
         <v>1.5733943315840347E-5</v>
       </c>
-      <c r="AY13">
+      <c r="AZ13">
         <v>8.8882725845278173E-6</v>
-      </c>
-      <c r="AZ13">
-        <v>1.2016331282035468E-2</v>
       </c>
       <c r="BA13">
         <v>1.2016331282035468E-2</v>
@@ -12639,28 +12734,34 @@
         <v>1.2016331282035468E-2</v>
       </c>
       <c r="BF13">
+        <v>1.2016331282035468E-2</v>
+      </c>
+      <c r="BG13">
         <v>2.1162595232694635E-3</v>
       </c>
-      <c r="BG13">
+      <c r="BH13">
         <v>5.3462146821994013E-4</v>
       </c>
-      <c r="BH13">
+      <c r="BI13">
         <v>1.2016331282035468E-2</v>
       </c>
-      <c r="BI13">
+      <c r="BJ13">
         <v>1.2783828944120282E-4</v>
       </c>
-      <c r="BJ13">
+      <c r="BK13">
         <v>3.2296099999999999E-3</v>
       </c>
-      <c r="BK13">
+      <c r="BL13">
         <v>2.0960223251596816E-3</v>
       </c>
-      <c r="BL13">
+      <c r="BM13">
         <v>9.0564148360102958E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN13">
+        <v>3.724647449968985E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -12676,7 +12777,7 @@
       <c r="E14" s="22">
         <v>2.2562370370703095E-4</v>
       </c>
-      <c r="F14" s="134">
+      <c r="F14" s="131">
         <v>1.0582886736867189E-3</v>
       </c>
       <c r="G14" s="22">
@@ -12760,62 +12861,62 @@
       <c r="AG14">
         <v>2.8401050053824055</v>
       </c>
-      <c r="AH14" s="22">
+      <c r="AH14" s="140">
+        <v>4.5403634527468109</v>
+      </c>
+      <c r="AI14" s="22">
         <v>3.2848921981275752E-4</v>
       </c>
-      <c r="AI14">
-        <v>4.1715536368739541E-4</v>
-      </c>
-      <c r="AJ14">
+      <c r="AJ14" s="140">
+        <v>4.1719548987732114E-4</v>
+      </c>
+      <c r="AK14">
         <v>1.0277603010773937E-4</v>
       </c>
-      <c r="AK14">
+      <c r="AL14">
         <v>1.384563781637522E-4</v>
       </c>
-      <c r="AL14">
+      <c r="AM14">
         <v>5.0526252963274286E-3</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>2.5096719103396089E-4</v>
       </c>
-      <c r="AN14">
+      <c r="AO14">
         <v>1.7045009814474999E-3</v>
       </c>
-      <c r="AO14">
+      <c r="AP14">
         <v>1.4521849195867858E-2</v>
       </c>
-      <c r="AP14">
+      <c r="AQ14">
         <v>1.0582886736867189E-3</v>
       </c>
-      <c r="AQ14" s="4">
+      <c r="AR14" s="4">
         <v>7.6398223281650462E-5</v>
       </c>
-      <c r="AR14" s="4">
+      <c r="AS14" s="4">
         <v>1.4284223952224014E-3</v>
       </c>
-      <c r="AS14" s="4">
+      <c r="AT14" s="4">
         <v>3.2335161057990525E-4</v>
       </c>
-      <c r="AT14" s="4">
+      <c r="AU14" s="4">
         <v>9.2590380099334864E-4</v>
       </c>
-      <c r="AU14">
+      <c r="AV14">
         <v>1.0404403176396946E-3</v>
-      </c>
-      <c r="AV14">
-        <v>2.5096719103396089E-4</v>
       </c>
       <c r="AW14">
         <v>2.5096719103396089E-4</v>
       </c>
       <c r="AX14">
+        <v>2.5096719103396089E-4</v>
+      </c>
+      <c r="AY14">
         <v>2.326725050694978E-6</v>
       </c>
-      <c r="AY14">
+      <c r="AZ14">
         <v>4.9339130582133812E-6</v>
-      </c>
-      <c r="AZ14">
-        <v>1.1155220859685694E-3</v>
       </c>
       <c r="BA14">
         <v>1.1155220859685694E-3</v>
@@ -12833,28 +12934,34 @@
         <v>1.1155220859685694E-3</v>
       </c>
       <c r="BF14">
+        <v>1.1155220859685694E-3</v>
+      </c>
+      <c r="BG14">
         <v>1.6389900374865949E-4</v>
       </c>
-      <c r="BG14">
+      <c r="BH14">
         <v>6.2734321278646725E-5</v>
       </c>
-      <c r="BH14">
+      <c r="BI14">
         <v>1.1155220859685694E-3</v>
       </c>
-      <c r="BI14">
+      <c r="BJ14">
         <v>1.8904641036896698E-5</v>
       </c>
-      <c r="BJ14">
+      <c r="BK14">
         <v>2.01041E-4</v>
       </c>
-      <c r="BK14">
+      <c r="BL14">
         <v>1.6271341968570853E-4</v>
       </c>
-      <c r="BL14">
+      <c r="BM14">
         <v>6.3347493705224476E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN14">
+        <v>3.9233022845947815E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -12870,7 +12977,7 @@
       <c r="E15" s="22">
         <v>1.8438990196320597E-4</v>
       </c>
-      <c r="F15" s="134">
+      <c r="F15" s="131">
         <v>8.3472257527739265E-4</v>
       </c>
       <c r="G15" s="22">
@@ -12954,62 +13061,62 @@
       <c r="AG15">
         <v>2.7114794461446454</v>
       </c>
-      <c r="AH15" s="22">
+      <c r="AH15" s="140">
+        <v>3.6846509333600648</v>
+      </c>
+      <c r="AI15" s="22">
         <v>3.067172810566663E-4</v>
       </c>
-      <c r="AI15">
-        <v>1.5575235226667416E-4</v>
-      </c>
-      <c r="AJ15">
+      <c r="AJ15" s="140">
+        <v>1.5578505014062489E-4</v>
+      </c>
+      <c r="AK15">
         <v>7.1601283232775145E-5</v>
       </c>
-      <c r="AK15">
+      <c r="AL15">
         <v>1.049517245304839E-4</v>
       </c>
-      <c r="AL15">
+      <c r="AM15">
         <v>1.2270097156994448E-3</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>1.6834887068156192E-4</v>
       </c>
-      <c r="AN15">
+      <c r="AO15">
         <v>9.056412863636845E-4</v>
       </c>
-      <c r="AO15">
+      <c r="AP15">
         <v>7.4082805337932394E-3</v>
       </c>
-      <c r="AP15">
+      <c r="AQ15">
         <v>8.3472257527739265E-4</v>
       </c>
-      <c r="AQ15" s="4">
+      <c r="AR15" s="4">
         <v>2.646467485885586E-5</v>
       </c>
-      <c r="AR15" s="4">
+      <c r="AS15" s="4">
         <v>6.9002810727674421E-4</v>
       </c>
-      <c r="AS15" s="4">
+      <c r="AT15" s="4">
         <v>1.5028440442550037E-4</v>
       </c>
-      <c r="AT15" s="4">
+      <c r="AU15" s="4">
         <v>4.2364544559550575E-4</v>
       </c>
-      <c r="AU15">
+      <c r="AV15">
         <v>8.1851779459990112E-4</v>
-      </c>
-      <c r="AV15">
-        <v>1.6834887068156192E-4</v>
       </c>
       <c r="AW15">
         <v>1.6834887068156192E-4</v>
       </c>
       <c r="AX15">
+        <v>1.6834887068156192E-4</v>
+      </c>
+      <c r="AY15">
         <v>1.3317401724638582E-6</v>
       </c>
-      <c r="AY15">
+      <c r="AZ15">
         <v>2.709495694275613E-6</v>
-      </c>
-      <c r="AZ15">
-        <v>8.794358938289306E-4</v>
       </c>
       <c r="BA15">
         <v>8.794358938289306E-4</v>
@@ -13027,28 +13134,34 @@
         <v>8.794358938289306E-4</v>
       </c>
       <c r="BF15">
+        <v>8.794358938289306E-4</v>
+      </c>
+      <c r="BG15">
         <v>1.2732009726717131E-4</v>
       </c>
-      <c r="BG15">
+      <c r="BH15">
         <v>4.7548857062017446E-5</v>
       </c>
-      <c r="BH15">
+      <c r="BI15">
         <v>8.794358938289306E-4</v>
       </c>
-      <c r="BI15">
+      <c r="BJ15">
         <v>1.0820388901268849E-5</v>
       </c>
-      <c r="BJ15">
+      <c r="BK15">
         <v>1.60686E-4</v>
       </c>
-      <c r="BK15">
+      <c r="BL15">
         <v>1.2817750979861499E-4</v>
       </c>
-      <c r="BL15">
+      <c r="BM15">
         <v>5.5486300276266073E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN15">
+        <v>2.0326514725382689E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -13064,7 +13177,7 @@
       <c r="E16" s="22">
         <v>1.0790959835545997E-3</v>
       </c>
-      <c r="F16" s="134">
+      <c r="F16" s="131">
         <v>1.1049620245021844E-2</v>
       </c>
       <c r="G16" s="22">
@@ -13148,62 +13261,62 @@
       <c r="AG16">
         <v>13.610201106319744</v>
       </c>
-      <c r="AH16" s="22">
+      <c r="AH16" s="140">
+        <v>23.416348896201253</v>
+      </c>
+      <c r="AI16" s="22">
         <v>1.8222658628499725E-3</v>
       </c>
-      <c r="AI16">
-        <v>6.4089140933905775E-4</v>
-      </c>
-      <c r="AJ16">
+      <c r="AJ16" s="140">
+        <v>6.4108055505771673E-4</v>
+      </c>
+      <c r="AK16">
         <v>5.0483087339241129E-4</v>
       </c>
-      <c r="AK16">
+      <c r="AL16">
         <v>1.3797051736039856E-4</v>
       </c>
-      <c r="AL16">
+      <c r="AM16">
         <v>8.3856339105434653E-3</v>
       </c>
-      <c r="AM16">
+      <c r="AN16">
         <v>1.0680267428573159E-3</v>
       </c>
-      <c r="AN16">
+      <c r="AO16">
         <v>7.2553878412718311E-3</v>
       </c>
-      <c r="AO16">
+      <c r="AP16">
         <v>1.6242981123085456</v>
       </c>
-      <c r="AP16">
+      <c r="AQ16">
         <v>1.1049620245021844E-2</v>
       </c>
-      <c r="AQ16" s="4">
+      <c r="AR16" s="4">
         <v>3.75468229155577E-5</v>
       </c>
-      <c r="AR16" s="4">
+      <c r="AS16" s="4">
         <v>9.1861320639744764E-3</v>
       </c>
-      <c r="AS16" s="4">
+      <c r="AT16" s="4">
         <v>2.4250010808802205E-2</v>
       </c>
-      <c r="AT16" s="4">
+      <c r="AU16" s="4">
         <v>3.2096943740812676E-3</v>
       </c>
-      <c r="AU16">
+      <c r="AV16">
         <v>1.0940294061138075E-2</v>
-      </c>
-      <c r="AV16">
-        <v>1.0680267428573159E-3</v>
       </c>
       <c r="AW16">
         <v>1.0680267428573159E-3</v>
       </c>
       <c r="AX16">
+        <v>1.0680267428573159E-3</v>
+      </c>
+      <c r="AY16">
         <v>1.3419259730132339E-5</v>
       </c>
-      <c r="AY16">
+      <c r="AZ16">
         <v>6.7945461187616543E-6</v>
-      </c>
-      <c r="AZ16">
-        <v>6.6987568450597376E-3</v>
       </c>
       <c r="BA16">
         <v>6.6987568450597376E-3</v>
@@ -13221,28 +13334,34 @@
         <v>6.6987568450597376E-3</v>
       </c>
       <c r="BF16">
+        <v>6.6987568450597376E-3</v>
+      </c>
+      <c r="BG16">
         <v>1.0391152025580992E-3</v>
       </c>
-      <c r="BG16">
+      <c r="BH16">
         <v>3.0192628867213963E-4</v>
       </c>
-      <c r="BH16">
+      <c r="BI16">
         <v>6.6987568450597376E-3</v>
       </c>
-      <c r="BI16">
+      <c r="BJ16">
         <v>1.0903148530732527E-4</v>
       </c>
-      <c r="BJ16">
+      <c r="BK16">
         <v>1.652819E-3</v>
       </c>
-      <c r="BK16">
+      <c r="BL16">
         <v>8.7059200446219169E-4</v>
       </c>
-      <c r="BL16">
+      <c r="BM16">
         <v>1.7710330926649157E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN16">
+        <v>1.3557166453407658E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>66</v>
       </c>
@@ -13258,7 +13377,7 @@
       <c r="E17" s="22">
         <v>3.5130761445057097E-5</v>
       </c>
-      <c r="F17" s="134">
+      <c r="F17" s="131">
         <v>4.8111856107520034E-5</v>
       </c>
       <c r="G17" s="22">
@@ -13342,62 +13461,62 @@
       <c r="AG17">
         <v>0.33504752591656944</v>
       </c>
-      <c r="AH17" s="22">
+      <c r="AH17" s="140">
+        <v>0.39065135934215078</v>
+      </c>
+      <c r="AI17" s="22">
         <v>4.5955619542805638E-5</v>
       </c>
-      <c r="AI17">
-        <v>1.8129502103015302E-5</v>
-      </c>
-      <c r="AJ17">
+      <c r="AJ17" s="140">
+        <v>1.813548940962644E-5</v>
+      </c>
+      <c r="AK17">
         <v>7.6475936623445776E-6</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>8.6013982285803297E-6</v>
       </c>
-      <c r="AL17">
+      <c r="AM17">
         <v>6.4199972524566995E-5</v>
       </c>
-      <c r="AM17">
+      <c r="AN17">
         <v>1.5318842808204928E-5</v>
       </c>
-      <c r="AN17">
+      <c r="AO17">
         <v>4.4512645820842785E-5</v>
       </c>
-      <c r="AO17">
+      <c r="AP17">
         <v>8.4312190453339313E-5</v>
       </c>
-      <c r="AP17">
+      <c r="AQ17">
         <v>4.8111856107520034E-5</v>
       </c>
-      <c r="AQ17" s="4">
+      <c r="AR17" s="4">
         <v>1.0084826813579067E-6</v>
       </c>
-      <c r="AR17" s="4">
+      <c r="AS17" s="4">
         <v>8.2766626330880094E-6</v>
       </c>
-      <c r="AS17" s="4">
+      <c r="AT17" s="4">
         <v>1.4574492333495407E-5</v>
       </c>
-      <c r="AT17" s="4">
+      <c r="AU17" s="4">
         <v>6.2850617270635867E-6</v>
       </c>
-      <c r="AU17">
+      <c r="AV17">
         <v>4.4946357995072476E-5</v>
-      </c>
-      <c r="AV17">
-        <v>1.5318842808204928E-5</v>
       </c>
       <c r="AW17">
         <v>1.5318842808204928E-5</v>
       </c>
       <c r="AX17">
+        <v>1.5318842808204928E-5</v>
+      </c>
+      <c r="AY17">
         <v>7.6091274445080203E-8</v>
       </c>
-      <c r="AY17">
+      <c r="AZ17">
         <v>1.0655147070654729E-7</v>
-      </c>
-      <c r="AZ17">
-        <v>1.1024560450050121E-4</v>
       </c>
       <c r="BA17">
         <v>1.1024560450050121E-4</v>
@@ -13415,28 +13534,34 @@
         <v>1.1024560450050121E-4</v>
       </c>
       <c r="BF17">
+        <v>1.1024560450050121E-4</v>
+      </c>
+      <c r="BG17">
         <v>1.6678591358774617E-5</v>
       </c>
-      <c r="BG17">
+      <c r="BH17">
         <v>5.1839392164824026E-6</v>
       </c>
-      <c r="BH17">
+      <c r="BI17">
         <v>1.1024560450050121E-4</v>
       </c>
-      <c r="BI17">
+      <c r="BJ17">
         <v>6.182416048662768E-7</v>
       </c>
-      <c r="BJ17">
+      <c r="BK17">
         <v>2.4223000000000002E-5</v>
       </c>
-      <c r="BK17">
+      <c r="BL17">
         <v>1.5402460347910774E-5</v>
       </c>
-      <c r="BL17">
+      <c r="BM17">
         <v>2.267359245953986E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN17">
+        <v>3.2718107917875022E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>67</v>
       </c>
@@ -13452,7 +13577,7 @@
       <c r="E18" s="22">
         <v>3.1238623176942234E-5</v>
       </c>
-      <c r="F18" s="134">
+      <c r="F18" s="131">
         <v>1.0621832498893018E-4</v>
       </c>
       <c r="G18" s="22">
@@ -13536,62 +13661,62 @@
       <c r="AG18">
         <v>0.74377470433511161</v>
       </c>
-      <c r="AH18" s="22">
+      <c r="AH18" s="140">
+        <v>1.0192401131404758</v>
+      </c>
+      <c r="AI18" s="22">
         <v>1.1205234448988939E-4</v>
       </c>
-      <c r="AI18">
-        <v>2.6305516438756624E-5</v>
-      </c>
-      <c r="AJ18">
+      <c r="AJ18" s="140">
+        <v>2.6310323667497318E-5</v>
+      </c>
+      <c r="AK18">
         <v>2.4514307433642393E-5</v>
       </c>
-      <c r="AK18">
+      <c r="AL18">
         <v>1.6411417919959357E-5</v>
       </c>
-      <c r="AL18">
+      <c r="AM18">
         <v>1.3261789974425655E-4</v>
       </c>
-      <c r="AM18">
+      <c r="AN18">
         <v>4.8671821414560816E-5</v>
       </c>
-      <c r="AN18">
+      <c r="AO18">
         <v>1.0566568758205814E-4</v>
       </c>
-      <c r="AO18">
+      <c r="AP18">
         <v>1.8068588782909787E-4</v>
       </c>
-      <c r="AP18">
+      <c r="AQ18">
         <v>1.0621832498893018E-4</v>
       </c>
-      <c r="AQ18" s="4">
+      <c r="AR18" s="4">
         <v>2.4151200263223926E-6</v>
       </c>
-      <c r="AR18" s="4">
+      <c r="AS18" s="4">
         <v>2.4164782580299077E-5</v>
       </c>
-      <c r="AS18" s="4">
+      <c r="AT18" s="4">
         <v>4.3257835022543267E-5</v>
       </c>
-      <c r="AT18" s="4">
+      <c r="AU18" s="4">
         <v>1.6206970607669284E-5</v>
       </c>
-      <c r="AU18">
+      <c r="AV18">
         <v>9.8395128927191022E-5</v>
-      </c>
-      <c r="AV18">
-        <v>4.8671821414560816E-5</v>
       </c>
       <c r="AW18">
         <v>4.8671821414560816E-5</v>
       </c>
       <c r="AX18">
+        <v>4.8671821414560816E-5</v>
+      </c>
+      <c r="AY18">
         <v>3.7696167206867435E-7</v>
       </c>
-      <c r="AY18">
+      <c r="AZ18">
         <v>1.5124048468983523E-7</v>
-      </c>
-      <c r="AZ18">
-        <v>2.7268668034746972E-4</v>
       </c>
       <c r="BA18">
         <v>2.7268668034746972E-4</v>
@@ -13609,28 +13734,34 @@
         <v>2.7268668034746972E-4</v>
       </c>
       <c r="BF18">
+        <v>2.7268668034746972E-4</v>
+      </c>
+      <c r="BG18">
         <v>4.0251380607755908E-5</v>
       </c>
-      <c r="BG18">
+      <c r="BH18">
         <v>1.375168911277876E-5</v>
       </c>
-      <c r="BH18">
+      <c r="BI18">
         <v>2.7268668034746972E-4</v>
       </c>
-      <c r="BI18">
+      <c r="BJ18">
         <v>3.0628135855579789E-6</v>
       </c>
-      <c r="BJ18">
+      <c r="BK18">
         <v>5.9191000000000003E-5</v>
       </c>
-      <c r="BK18">
+      <c r="BL18">
         <v>4.3080929272219695E-5</v>
       </c>
-      <c r="BL18">
+      <c r="BM18">
         <v>1.1238738180435919E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN18">
+        <v>5.3261285895382865E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>68</v>
       </c>
@@ -13646,7 +13777,7 @@
       <c r="E19" s="22">
         <v>2.0265281039525424E-3</v>
       </c>
-      <c r="F19" s="134">
+      <c r="F19" s="131">
         <v>3.7908790257546046E-3</v>
       </c>
       <c r="G19" s="22">
@@ -13730,62 +13861,62 @@
       <c r="AG19">
         <v>189.04492298972374</v>
       </c>
-      <c r="AH19" s="22">
+      <c r="AH19" s="140">
+        <v>223.15064256600229</v>
+      </c>
+      <c r="AI19" s="22">
         <v>1.579320164524466E-2</v>
       </c>
-      <c r="AI19">
-        <v>2.5803232307925993E-3</v>
-      </c>
-      <c r="AJ19">
+      <c r="AJ19" s="140">
+        <v>2.580565674925735E-3</v>
+      </c>
+      <c r="AK19">
         <v>3.1431483409378007E-3</v>
       </c>
-      <c r="AK19">
+      <c r="AL19">
         <v>6.7953913095346763E-4</v>
       </c>
-      <c r="AL19">
+      <c r="AM19">
         <v>1.7906358689314936E-2</v>
       </c>
-      <c r="AM19">
+      <c r="AN19">
         <v>6.1328558194932515E-3</v>
       </c>
-      <c r="AN19">
+      <c r="AO19">
         <v>1.4786114797291869E-2</v>
       </c>
-      <c r="AO19">
+      <c r="AP19">
         <v>2.0537309409465319E-2</v>
       </c>
-      <c r="AP19">
+      <c r="AQ19">
         <v>3.7908790257546046E-3</v>
       </c>
-      <c r="AQ19" s="4">
+      <c r="AR19" s="4">
         <v>4.3721739306843274E-5</v>
       </c>
-      <c r="AR19" s="4">
+      <c r="AS19" s="4">
         <v>4.0164958762704097E-3</v>
       </c>
-      <c r="AS19" s="4">
+      <c r="AT19" s="4">
         <v>2.312363438585285E-2</v>
       </c>
-      <c r="AT19" s="4">
+      <c r="AU19" s="4">
         <v>4.20452167506847E-3</v>
       </c>
-      <c r="AU19">
+      <c r="AV19">
         <v>2.1012190222127122E-3</v>
-      </c>
-      <c r="AV19">
-        <v>6.1328558194932515E-3</v>
       </c>
       <c r="AW19">
         <v>6.1328558194932515E-3</v>
       </c>
       <c r="AX19">
+        <v>6.1328558194932515E-3</v>
+      </c>
+      <c r="AY19">
         <v>4.6672099899350148E-5</v>
       </c>
-      <c r="AY19">
+      <c r="AZ19">
         <v>4.9809085410593131E-6</v>
-      </c>
-      <c r="AZ19">
-        <v>3.4177296712744172E-2</v>
       </c>
       <c r="BA19">
         <v>3.4177296712744172E-2</v>
@@ -13803,28 +13934,34 @@
         <v>3.4177296712744172E-2</v>
       </c>
       <c r="BF19">
+        <v>3.4177296712744172E-2</v>
+      </c>
+      <c r="BG19">
         <v>5.6163768386055567E-3</v>
       </c>
-      <c r="BG19">
+      <c r="BH19">
         <v>2.4549134989312366E-3</v>
       </c>
-      <c r="BH19">
+      <c r="BI19">
         <v>3.4177296712744172E-2</v>
       </c>
-      <c r="BI19">
+      <c r="BJ19">
         <v>3.7921081168221991E-4</v>
       </c>
-      <c r="BJ19">
+      <c r="BK19">
         <v>5.8936729999999994E-3</v>
       </c>
-      <c r="BK19">
+      <c r="BL19">
         <v>8.4885067131846726E-3</v>
       </c>
-      <c r="BL19">
+      <c r="BM19">
         <v>8.9030298819192874E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN19">
+        <v>1.9528710437986155E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -13840,7 +13977,7 @@
       <c r="E20" s="22">
         <v>2.6985670200181072E-3</v>
       </c>
-      <c r="F20" s="134">
+      <c r="F20" s="131">
         <v>3.5321920990798189E-5</v>
       </c>
       <c r="G20" s="22">
@@ -13924,62 +14061,62 @@
       <c r="AG20">
         <v>0.58866204659784449</v>
       </c>
-      <c r="AH20" s="22">
+      <c r="AH20" s="140">
+        <v>0.89713555715877558</v>
+      </c>
+      <c r="AI20" s="22">
         <v>1.742743859440626E-2</v>
       </c>
-      <c r="AI20">
-        <v>1.0018145421706144E-3</v>
-      </c>
-      <c r="AJ20">
+      <c r="AJ20" s="140">
+        <v>1.0023096907203865E-3</v>
+      </c>
+      <c r="AK20">
         <v>3.0014077853923169E-5</v>
       </c>
-      <c r="AK20">
+      <c r="AL20">
         <v>1.1843239562567246E-6</v>
       </c>
-      <c r="AL20">
+      <c r="AM20">
         <v>5.2328221006539869E-4</v>
       </c>
-      <c r="AM20">
+      <c r="AN20">
         <v>5.3785118551802877E-5</v>
       </c>
-      <c r="AN20">
+      <c r="AO20">
         <v>3.3911606947605884E-4</v>
       </c>
-      <c r="AO20">
+      <c r="AP20">
         <v>3.9893026804802245E-4</v>
       </c>
-      <c r="AP20">
+      <c r="AQ20">
         <v>3.5321920990798189E-5</v>
       </c>
-      <c r="AQ20" s="4">
+      <c r="AR20" s="4">
         <v>7.6381619756010868E-7</v>
       </c>
-      <c r="AR20" s="4">
+      <c r="AS20" s="4">
         <v>2.2262279430365871E-5</v>
       </c>
-      <c r="AS20" s="4">
+      <c r="AT20" s="4">
         <v>3.7538455325691253E-5</v>
       </c>
-      <c r="AT20" s="4">
+      <c r="AU20" s="4">
         <v>1.7149055177278329E-5</v>
       </c>
-      <c r="AU20">
+      <c r="AV20">
         <v>2.3823858197945876E-5</v>
-      </c>
-      <c r="AV20">
-        <v>5.3785118551802877E-5</v>
       </c>
       <c r="AW20">
         <v>5.3785118551802877E-5</v>
       </c>
       <c r="AX20">
+        <v>5.3785118551802877E-5</v>
+      </c>
+      <c r="AY20">
         <v>4.2213173274363571E-7</v>
       </c>
-      <c r="AY20">
+      <c r="AZ20">
         <v>5.6664914443380942E-8</v>
-      </c>
-      <c r="AZ20">
-        <v>2.7968853538439578E-4</v>
       </c>
       <c r="BA20">
         <v>2.7968853538439578E-4</v>
@@ -13997,28 +14134,34 @@
         <v>2.7968853538439578E-4</v>
       </c>
       <c r="BF20">
+        <v>2.7968853538439578E-4</v>
+      </c>
+      <c r="BG20">
         <v>4.2515389519619327E-5</v>
       </c>
-      <c r="BG20">
+      <c r="BH20">
         <v>1.4517663231511721E-5</v>
       </c>
-      <c r="BH20">
+      <c r="BI20">
         <v>2.7968853538439578E-4</v>
       </c>
-      <c r="BI20">
+      <c r="BJ20">
         <v>3.4298203285420399E-6</v>
       </c>
-      <c r="BJ20">
+      <c r="BK20">
         <v>2.0967329999999999E-3</v>
       </c>
-      <c r="BK20">
+      <c r="BL20">
         <v>4.3525227367842782E-5</v>
       </c>
-      <c r="BL20">
+      <c r="BM20">
         <v>6.0967430698154849E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN20">
+        <v>8.8356010400824942E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
         <v>70</v>
       </c>
@@ -14034,7 +14177,7 @@
       <c r="E21" s="30">
         <v>0.89131293645591025</v>
       </c>
-      <c r="F21" s="136">
+      <c r="F21" s="133">
         <v>1.5403860427603833</v>
       </c>
       <c r="G21" s="30">
@@ -14043,7 +14186,7 @@
       <c r="H21" s="30">
         <v>0.51476298268065945</v>
       </c>
-      <c r="I21" s="30">
+      <c r="I21" s="139">
         <v>0.65589183244261862</v>
       </c>
       <c r="J21" s="30">
@@ -14118,62 +14261,62 @@
       <c r="AG21">
         <v>78307.41826476407</v>
       </c>
-      <c r="AH21" s="30">
+      <c r="AH21" s="140">
+        <v>93797.02635737024</v>
+      </c>
+      <c r="AI21" s="30">
         <v>4.287972545719934</v>
       </c>
-      <c r="AI21">
-        <v>1.1117032316949111</v>
-      </c>
-      <c r="AJ21">
+      <c r="AJ21" s="140">
+        <v>1.1119055333036951</v>
+      </c>
+      <c r="AK21">
         <v>1.1681442085858305</v>
       </c>
-      <c r="AK21">
+      <c r="AL21">
         <v>1.2608466848423983</v>
       </c>
-      <c r="AL21">
+      <c r="AM21">
         <v>8.6223105392679198</v>
       </c>
-      <c r="AM21">
+      <c r="AN21">
         <v>2.9906430499306937</v>
       </c>
-      <c r="AN21">
+      <c r="AO21">
         <v>6.377757507508945</v>
       </c>
-      <c r="AO21">
+      <c r="AP21">
         <v>8.7784083812665976</v>
       </c>
-      <c r="AP21">
+      <c r="AQ21">
         <v>1.5403860427603833</v>
       </c>
-      <c r="AQ21" s="64">
+      <c r="AR21" s="64">
         <v>9.4362755707543489E-2</v>
       </c>
-      <c r="AR21" s="64">
+      <c r="AS21" s="64">
         <v>2.252830464041975</v>
       </c>
-      <c r="AS21" s="64">
+      <c r="AT21" s="64">
         <v>1.9042027934018182</v>
       </c>
-      <c r="AT21" s="64">
+      <c r="AU21" s="64">
         <v>0.78372738956644916</v>
       </c>
-      <c r="AU21">
+      <c r="AV21">
         <v>0.98977076923666552</v>
-      </c>
-      <c r="AV21">
-        <v>2.9906430499306933</v>
       </c>
       <c r="AW21">
         <v>2.9906430499306933</v>
       </c>
       <c r="AX21">
+        <v>2.9906430499306933</v>
+      </c>
+      <c r="AY21">
         <v>2.1196812302494747E-2</v>
       </c>
-      <c r="AY21">
+      <c r="AZ21">
         <v>3.7719393576396E-3</v>
-      </c>
-      <c r="AZ21">
-        <v>10.954043024257045</v>
       </c>
       <c r="BA21">
         <v>10.954043024257045</v>
@@ -14191,157 +14334,173 @@
         <v>10.954043024257045</v>
       </c>
       <c r="BF21">
+        <v>10.954043024257045</v>
+      </c>
+      <c r="BG21">
         <v>1.885344789686233</v>
       </c>
-      <c r="BG21">
+      <c r="BH21">
         <v>0.99108850050692909</v>
       </c>
-      <c r="BH21">
+      <c r="BI21">
         <v>10.954043024257045</v>
       </c>
-      <c r="BI21">
+      <c r="BJ21">
         <v>0.17222409995776983</v>
       </c>
-      <c r="BJ21">
+      <c r="BK21">
         <v>1.9748460000000001</v>
       </c>
-      <c r="BK21">
+      <c r="BL21">
         <v>2.4557188258542357</v>
       </c>
-      <c r="BL21">
+      <c r="BM21">
         <v>29.838516773361853</v>
       </c>
-    </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="BN21">
+        <v>2.6286261463371274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="AH22" s="140"/>
+      <c r="AJ22" s="140"/>
+    </row>
+    <row r="23" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="136" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="128"/>
-      <c r="K23" s="128"/>
-      <c r="L23" s="128"/>
-      <c r="M23" s="128"/>
-      <c r="N23" s="128"/>
-      <c r="O23" s="128"/>
-      <c r="P23" s="128"/>
-      <c r="Q23" s="128"/>
-      <c r="R23" s="128"/>
-      <c r="S23" s="128"/>
-      <c r="T23" s="128"/>
-      <c r="U23" s="128"/>
-      <c r="V23" s="128"/>
-      <c r="W23" s="128"/>
-      <c r="X23" s="128"/>
-      <c r="Y23" s="128"/>
-      <c r="Z23" s="128"/>
-      <c r="AA23" s="128"/>
-      <c r="AB23" s="128"/>
-      <c r="AC23" s="128"/>
-      <c r="AD23" s="128"/>
-      <c r="AE23" s="128"/>
-      <c r="AF23" s="128"/>
-      <c r="AI23" t="s">
-        <v>304</v>
-      </c>
-      <c r="AJ23" t="s">
-        <v>322</v>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="136"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="136"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="136"/>
+      <c r="J23" s="136"/>
+      <c r="K23" s="136"/>
+      <c r="L23" s="136"/>
+      <c r="M23" s="136"/>
+      <c r="N23" s="136"/>
+      <c r="O23" s="136"/>
+      <c r="P23" s="136"/>
+      <c r="Q23" s="136"/>
+      <c r="R23" s="136"/>
+      <c r="S23" s="136"/>
+      <c r="T23" s="136"/>
+      <c r="U23" s="136"/>
+      <c r="V23" s="136"/>
+      <c r="W23" s="136"/>
+      <c r="X23" s="136"/>
+      <c r="Y23" s="136"/>
+      <c r="Z23" s="136"/>
+      <c r="AA23" s="136"/>
+      <c r="AB23" s="136"/>
+      <c r="AC23" s="136"/>
+      <c r="AD23" s="136"/>
+      <c r="AE23" s="136"/>
+      <c r="AF23" s="136"/>
+      <c r="AH23" s="140" t="s">
+        <v>368</v>
+      </c>
+      <c r="AJ23" s="140" t="s">
+        <v>348</v>
       </c>
       <c r="AK23" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AL23" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="AM23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AN23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AO23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AP23" t="s">
+        <v>328</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>347</v>
+      </c>
+      <c r="AR23" t="s">
         <v>348</v>
       </c>
-      <c r="AQ23" t="s">
-        <v>349</v>
-      </c>
-      <c r="AR23" t="s">
-        <v>349</v>
-      </c>
       <c r="AS23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AT23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AU23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AV23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AW23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AX23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AY23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AZ23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BA23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BB23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BC23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BD23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BE23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BF23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BG23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BH23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BI23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BJ23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BK23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BL23" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.35">
-      <c r="AQ27">
+        <v>348</v>
+      </c>
+      <c r="BM23" t="s">
+        <v>348</v>
+      </c>
+      <c r="BN23" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="AR27">
         <v>99</v>
       </c>
     </row>
@@ -15477,22 +15636,22 @@
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="128"/>
-      <c r="K23" s="128"/>
-      <c r="L23" s="128"/>
-      <c r="M23" s="128"/>
-      <c r="N23" s="128"/>
-      <c r="O23" s="128"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="136"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="136"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="136"/>
+      <c r="J23" s="136"/>
+      <c r="K23" s="136"/>
+      <c r="L23" s="136"/>
+      <c r="M23" s="136"/>
+      <c r="N23" s="136"/>
+      <c r="O23" s="136"/>
       <c r="P23" t="s">
         <v>90</v>
       </c>
@@ -15528,7 +15687,7 @@
         <v>299</v>
       </c>
       <c r="D1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -15536,13 +15695,13 @@
         <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -15849,7 +16008,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B4" t="s">
         <v>117</v>
@@ -15977,7 +16136,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="126" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B20" s="69" t="s">
         <v>119</v>
@@ -16030,10 +16189,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16502,7 +16661,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B43" s="69">
         <v>44.291949816853993</v>
@@ -16513,7 +16672,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B44" s="69">
         <v>43.995102738357922</v>
@@ -16747,7 +16906,7 @@
         <v>187</v>
       </c>
       <c r="B65">
-        <v>47.141813661363628</v>
+        <v>47.141813661363599</v>
       </c>
       <c r="C65">
         <v>0.77692265667854898</v>
@@ -16776,248 +16935,259 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>189</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68">
-        <v>1.9768383817590991</v>
+      <c r="A68" s="143" t="s">
+        <v>367</v>
+      </c>
+      <c r="B68" s="140">
+        <v>119.98674372549019</v>
+      </c>
+      <c r="C68" s="140">
+        <v>9.0052398842286357E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B69">
-        <v>48.885121247479262</v>
+        <v>0</v>
       </c>
       <c r="C69">
-        <v>0.88356773166440861</v>
+        <v>1.9768383817590991</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70">
-        <v>22.648458746153963</v>
+        <v>48.885121247479262</v>
+      </c>
+      <c r="C70">
+        <v>0.88356773166440861</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71">
-        <v>26.329529071139479</v>
+        <v>22.648458746153963</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B72">
-        <v>18.707371337693861</v>
+        <v>26.329529071139479</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B73">
-        <v>12.566427590816895</v>
+        <v>18.707371337693861</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B74">
-        <v>26.329529071139479</v>
+        <v>12.566427590816895</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B75">
-        <v>11.566786665057547</v>
+        <v>26.329529071139479</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B76">
-        <v>31.342185540824094</v>
+        <v>11.566786665057547</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B77">
-        <v>31.0106439692332</v>
+        <v>31.342185540824094</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B78">
-        <v>28.609127685562171</v>
+        <v>31.0106439692332</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B79">
-        <v>33.012627597074328</v>
+        <v>28.609127685562171</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>200</v>
+      </c>
+      <c r="B80">
+        <v>33.012627597074328</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>201</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>202</v>
       </c>
-      <c r="B81">
+      <c r="B82">
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>203</v>
       </c>
-      <c r="B82">
+      <c r="B83">
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>204</v>
       </c>
-      <c r="B83">
+      <c r="B84">
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>205</v>
       </c>
-      <c r="B84">
+      <c r="B85">
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>206</v>
       </c>
-      <c r="B85">
+      <c r="B86">
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>207</v>
       </c>
-      <c r="B86">
+      <c r="B87">
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>208</v>
       </c>
-      <c r="B87">
+      <c r="B88">
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>209</v>
       </c>
-      <c r="B88">
+      <c r="B89">
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>210</v>
       </c>
-      <c r="B89">
+      <c r="B90">
         <v>14.4</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>211</v>
       </c>
-      <c r="B90">
+      <c r="B91">
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>212</v>
       </c>
-      <c r="B91">
+      <c r="B92">
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>213</v>
-      </c>
-      <c r="B92">
-        <v>16.758749999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>214</v>
       </c>
       <c r="B93">
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>214</v>
+      </c>
+      <c r="B94">
+        <v>16.758749999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>215</v>
       </c>
-      <c r="B94">
+      <c r="B95">
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>216</v>
       </c>
-      <c r="B95">
+      <c r="B96">
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="68" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="68" t="s">
         <v>219</v>
       </c>
-      <c r="C96">
+      <c r="C97">
         <v>1000</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>75</v>
       </c>
-      <c r="C97">
+      <c r="C98">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the CAP pathway (fuel distribution consistency issue NOT resolved)
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39498F3E-BFA4-4CC0-9836-7E75147DB8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23CA6AC-3D67-434C-8B5C-4F424CEEC9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" firstSheet="3" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="374">
   <si>
     <t>NG</t>
   </si>
@@ -1418,6 +1418,18 @@
   </si>
   <si>
     <t>Nitrogen Gas</t>
+  </si>
+  <si>
+    <t>Ag_Inputs</t>
+  </si>
+  <si>
+    <t>Ca(NO3)2</t>
+  </si>
+  <si>
+    <t>Renewable Diesel - Algae (BDO)</t>
+  </si>
+  <si>
+    <t>Renewable Diesel - Algae (Acids)</t>
   </si>
 </sst>
 </file>
@@ -2020,15 +2032,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="174" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2040,6 +2043,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2757,21 +2769,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
-  <dimension ref="A1:AS23"/>
+  <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM2" sqref="AM2"/>
+      <selection pane="topRight" activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="122"/>
-    <col min="41" max="41" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="122"/>
+    <col min="41" max="41" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2904,8 +2916,26 @@
       <c r="AS1" s="6" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:45" ht="78.5" x14ac:dyDescent="0.35">
+      <c r="AT1" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="AW1" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="AY1" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -3038,8 +3068,26 @@
       <c r="AS2" s="65" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT2" s="65" t="s">
+        <v>310</v>
+      </c>
+      <c r="AU2" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="AV2" s="65" t="s">
+        <v>314</v>
+      </c>
+      <c r="AW2" s="65" t="s">
+        <v>310</v>
+      </c>
+      <c r="AX2" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="AY2" s="65" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3140,7 +3188,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3272,8 +3320,28 @@
         <f>AQ4+AR4</f>
         <v>1001250.3090024699</v>
       </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AU4">
+        <v>1250.309002469897</v>
+      </c>
+      <c r="AV4">
+        <f>AT4+AU4</f>
+        <v>1001250.3090024699</v>
+      </c>
+      <c r="AW4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="AX4">
+        <v>1250.309002469897</v>
+      </c>
+      <c r="AY4">
+        <f>AW4+AX4</f>
+        <v>1001250.3090024699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3405,8 +3473,28 @@
         <f t="shared" ref="AS5:AS9" si="3">AQ5+AR5</f>
         <v>1199.1725344773329</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>1199.1725344773329</v>
+      </c>
+      <c r="AV5">
+        <f t="shared" ref="AV5:AV9" si="4">AT5+AU5</f>
+        <v>1199.1725344773329</v>
+      </c>
+      <c r="AW5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>1199.1725344773329</v>
+      </c>
+      <c r="AY5">
+        <f t="shared" ref="AY5:AY9" si="5">AW5+AX5</f>
+        <v>1199.1725344773329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3538,8 +3626,28 @@
         <f t="shared" si="3"/>
         <v>8.0912620107395146</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>8.0912620107395146</v>
+      </c>
+      <c r="AV6">
+        <f t="shared" si="4"/>
+        <v>8.0912620107395146</v>
+      </c>
+      <c r="AW6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>8.0912620107395146</v>
+      </c>
+      <c r="AY6">
+        <f t="shared" si="5"/>
+        <v>8.0912620107395146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3671,8 +3779,28 @@
         <f t="shared" si="3"/>
         <v>124.60248498831356</v>
       </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>124.60248498831356</v>
+      </c>
+      <c r="AV7">
+        <f t="shared" si="4"/>
+        <v>124.60248498831356</v>
+      </c>
+      <c r="AW7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>124.60248498831356</v>
+      </c>
+      <c r="AY7">
+        <f t="shared" si="5"/>
+        <v>124.60248498831356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3804,8 +3932,28 @@
         <f t="shared" si="3"/>
         <v>1066.4787874782799</v>
       </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>1066.4787874782799</v>
+      </c>
+      <c r="AV8">
+        <f t="shared" si="4"/>
+        <v>1066.4787874782799</v>
+      </c>
+      <c r="AW8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>1066.4787874782799</v>
+      </c>
+      <c r="AY8">
+        <f t="shared" si="5"/>
+        <v>1066.4787874782799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3937,8 +4085,28 @@
         <f t="shared" si="3"/>
         <v>2.3217600680931635E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>2.3217600680931635E-2</v>
+      </c>
+      <c r="AV9">
+        <f t="shared" si="4"/>
+        <v>2.3217600680931635E-2</v>
+      </c>
+      <c r="AW9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>2.3217600680931635E-2</v>
+      </c>
+      <c r="AY9">
+        <f t="shared" si="5"/>
+        <v>2.3217600680931635E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4070,8 +4238,28 @@
         <f>AQ10+AR10</f>
         <v>40.366758790864871</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT10">
+        <v>40.352647182660228</v>
+      </c>
+      <c r="AU10">
+        <v>1.4111608204643369E-2</v>
+      </c>
+      <c r="AV10">
+        <f>AT10+AU10</f>
+        <v>40.366758790864871</v>
+      </c>
+      <c r="AW10">
+        <v>40.352647182660228</v>
+      </c>
+      <c r="AX10">
+        <v>1.4111608204643369E-2</v>
+      </c>
+      <c r="AY10">
+        <f>AW10+AX10</f>
+        <v>40.366758790864871</v>
+      </c>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -4170,7 +4358,7 @@
         <v>0.53001711985689259</v>
       </c>
       <c r="AJ11">
-        <f t="shared" ref="AJ11:AJ21" si="4">AH11+AI11</f>
+        <f t="shared" ref="AJ11:AJ21" si="6">AH11+AI11</f>
         <v>639.63416782778677</v>
       </c>
       <c r="AK11">
@@ -4180,7 +4368,7 @@
         <v>0.19579254162294349</v>
       </c>
       <c r="AM11">
-        <f t="shared" ref="AM11:AM21" si="5">AK11+AL11</f>
+        <f t="shared" ref="AM11:AM21" si="7">AK11+AL11</f>
         <v>993.99652518923131</v>
       </c>
       <c r="AN11">
@@ -4190,7 +4378,7 @@
         <v>0.19579254162294349</v>
       </c>
       <c r="AP11">
-        <f t="shared" ref="AP11:AP21" si="6">AN11+AO11</f>
+        <f t="shared" ref="AP11:AP21" si="8">AN11+AO11</f>
         <v>993.99652518923131</v>
       </c>
       <c r="AQ11">
@@ -4200,11 +4388,31 @@
         <v>0.19579254162294349</v>
       </c>
       <c r="AS11">
-        <f t="shared" ref="AS11:AS21" si="7">AQ11+AR11</f>
+        <f t="shared" ref="AS11:AS21" si="9">AQ11+AR11</f>
         <v>993.99652518923131</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT11">
+        <v>993.80073264760836</v>
+      </c>
+      <c r="AU11">
+        <v>0.19579254162294349</v>
+      </c>
+      <c r="AV11">
+        <f t="shared" ref="AV11:AV21" si="10">AT11+AU11</f>
+        <v>993.99652518923131</v>
+      </c>
+      <c r="AW11">
+        <v>993.80073264760836</v>
+      </c>
+      <c r="AX11">
+        <v>0.19579254162294349</v>
+      </c>
+      <c r="AY11">
+        <f t="shared" ref="AY11:AY21" si="11">AW11+AX11</f>
+        <v>993.99652518923131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -4303,7 +4511,7 @@
         <v>1.4390708093838975</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.647805124275852</v>
       </c>
       <c r="AK12">
@@ -4313,7 +4521,7 @@
         <v>0.13356807901983217</v>
       </c>
       <c r="AM12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>27.521187334987346</v>
       </c>
       <c r="AN12">
@@ -4323,7 +4531,7 @@
         <v>0.13356807901983217</v>
       </c>
       <c r="AP12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>27.521187334987346</v>
       </c>
       <c r="AQ12">
@@ -4333,11 +4541,31 @@
         <v>0.13356807901983217</v>
       </c>
       <c r="AS12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>27.521187334987346</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT12">
+        <v>27.387619255967515</v>
+      </c>
+      <c r="AU12">
+        <v>0.13356807901983217</v>
+      </c>
+      <c r="AV12">
+        <f t="shared" si="10"/>
+        <v>27.521187334987346</v>
+      </c>
+      <c r="AW12">
+        <v>27.387619255967515</v>
+      </c>
+      <c r="AX12">
+        <v>0.13356807901983217</v>
+      </c>
+      <c r="AY12">
+        <f t="shared" si="11"/>
+        <v>27.521187334987346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -4436,7 +4664,7 @@
         <v>6.8025222126898502E-2</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.1121724631375205</v>
       </c>
       <c r="AK13">
@@ -4446,7 +4674,7 @@
         <v>7.5116168079741932E-3</v>
       </c>
       <c r="AM13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.4662813685889695</v>
       </c>
       <c r="AN13">
@@ -4456,7 +4684,7 @@
         <v>7.5116168079741932E-3</v>
       </c>
       <c r="AP13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.4662813685889695</v>
       </c>
       <c r="AQ13">
@@ -4466,11 +4694,31 @@
         <v>7.5116168079741932E-3</v>
       </c>
       <c r="AS13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9.4662813685889695</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT13">
+        <v>9.458769751780995</v>
+      </c>
+      <c r="AU13">
+        <v>7.5116168079741932E-3</v>
+      </c>
+      <c r="AV13">
+        <f t="shared" si="10"/>
+        <v>9.4662813685889695</v>
+      </c>
+      <c r="AW13">
+        <v>9.458769751780995</v>
+      </c>
+      <c r="AX13">
+        <v>7.5116168079741932E-3</v>
+      </c>
+      <c r="AY13">
+        <f t="shared" si="11"/>
+        <v>9.4662813685889695</v>
+      </c>
+    </row>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -4569,7 +4817,7 @@
         <v>4.6442748659862865E-2</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.7750922644483509</v>
       </c>
       <c r="AK14">
@@ -4579,7 +4827,7 @@
         <v>2.1809956805283149E-3</v>
       </c>
       <c r="AM14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.8944508672117086</v>
       </c>
       <c r="AN14">
@@ -4589,7 +4837,7 @@
         <v>2.1809956805283149E-3</v>
       </c>
       <c r="AP14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.8944508672117086</v>
       </c>
       <c r="AQ14">
@@ -4599,11 +4847,31 @@
         <v>2.1809956805283149E-3</v>
       </c>
       <c r="AS14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.8944508672117086</v>
       </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT14">
+        <v>1.8922698715311803</v>
+      </c>
+      <c r="AU14">
+        <v>2.1809956805283149E-3</v>
+      </c>
+      <c r="AV14">
+        <f t="shared" si="10"/>
+        <v>1.8944508672117086</v>
+      </c>
+      <c r="AW14">
+        <v>1.8922698715311803</v>
+      </c>
+      <c r="AX14">
+        <v>2.1809956805283149E-3</v>
+      </c>
+      <c r="AY14">
+        <f t="shared" si="11"/>
+        <v>1.8944508672117086</v>
+      </c>
+    </row>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -4702,7 +4970,7 @@
         <v>0.22128373782612412</v>
       </c>
       <c r="AJ15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.700151259382223</v>
       </c>
       <c r="AK15">
@@ -4712,7 +4980,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
       <c r="AM15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.3987418408876558E-3</v>
       </c>
       <c r="AN15">
@@ -4722,7 +4990,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
       <c r="AP15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.3987418408876558E-3</v>
       </c>
       <c r="AQ15">
@@ -4732,11 +5000,31 @@
         <v>5.3987418408876558E-3</v>
       </c>
       <c r="AS15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.3987418408876558E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT15">
+        <v>0</v>
+      </c>
+      <c r="AU15">
+        <v>5.3987418408876558E-3</v>
+      </c>
+      <c r="AV15">
+        <f t="shared" si="10"/>
+        <v>5.3987418408876558E-3</v>
+      </c>
+      <c r="AW15">
+        <v>0</v>
+      </c>
+      <c r="AX15">
+        <v>5.3987418408876558E-3</v>
+      </c>
+      <c r="AY15">
+        <f t="shared" si="11"/>
+        <v>5.3987418408876558E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -4831,7 +5119,7 @@
         <v>4.2404984619842561E-3</v>
       </c>
       <c r="AJ16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.47814997311821905</v>
       </c>
       <c r="AK16">
@@ -4841,7 +5129,7 @@
         <v>2.0959176112987082E-4</v>
       </c>
       <c r="AM16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.51231387456148403</v>
       </c>
       <c r="AN16">
@@ -4851,7 +5139,7 @@
         <v>2.0959176112987082E-4</v>
       </c>
       <c r="AP16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.51231387456148403</v>
       </c>
       <c r="AQ16">
@@ -4861,11 +5149,31 @@
         <v>2.0959176112987082E-4</v>
       </c>
       <c r="AS16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.51231387456148403</v>
       </c>
-    </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT16">
+        <v>0.51210428280035414</v>
+      </c>
+      <c r="AU16">
+        <v>2.0959176112987082E-4</v>
+      </c>
+      <c r="AV16">
+        <f t="shared" si="10"/>
+        <v>0.51231387456148403</v>
+      </c>
+      <c r="AW16">
+        <v>0.51210428280035414</v>
+      </c>
+      <c r="AX16">
+        <v>2.0959176112987082E-4</v>
+      </c>
+      <c r="AY16">
+        <f t="shared" si="11"/>
+        <v>0.51231387456148403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -4960,7 +5268,7 @@
         <v>2.0700811243651359E-2</v>
       </c>
       <c r="AJ17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.26655908652077559</v>
       </c>
       <c r="AK17">
@@ -4970,7 +5278,7 @@
         <v>3.7216049065244534E-4</v>
       </c>
       <c r="AM17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.7002199380836189E-2</v>
       </c>
       <c r="AN17">
@@ -4980,7 +5288,7 @@
         <v>3.7216049065244534E-4</v>
       </c>
       <c r="AP17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.7002199380836189E-2</v>
       </c>
       <c r="AQ17">
@@ -4990,11 +5298,31 @@
         <v>3.7216049065244534E-4</v>
       </c>
       <c r="AS17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.7002199380836189E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT17">
+        <v>7.6630038890183744E-2</v>
+      </c>
+      <c r="AU17">
+        <v>3.7216049065244534E-4</v>
+      </c>
+      <c r="AV17">
+        <f t="shared" si="10"/>
+        <v>7.7002199380836189E-2</v>
+      </c>
+      <c r="AW17">
+        <v>7.6630038890183744E-2</v>
+      </c>
+      <c r="AX17">
+        <v>3.7216049065244534E-4</v>
+      </c>
+      <c r="AY17">
+        <f t="shared" si="11"/>
+        <v>7.7002199380836189E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -5089,7 +5417,7 @@
         <v>1.0718762615156343</v>
       </c>
       <c r="AJ18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.4860014543055007</v>
       </c>
       <c r="AK18">
@@ -5099,7 +5427,7 @@
         <v>0.11248755052026857</v>
       </c>
       <c r="AM18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.11248755052026857</v>
       </c>
       <c r="AN18">
@@ -5109,7 +5437,7 @@
         <v>0.11248755052026857</v>
       </c>
       <c r="AP18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.11248755052026857</v>
       </c>
       <c r="AQ18">
@@ -5119,11 +5447,31 @@
         <v>0.11248755052026857</v>
       </c>
       <c r="AS18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.11248755052026857</v>
       </c>
-    </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT18">
+        <v>0</v>
+      </c>
+      <c r="AU18">
+        <v>0.11248755052026857</v>
+      </c>
+      <c r="AV18">
+        <f t="shared" si="10"/>
+        <v>0.11248755052026857</v>
+      </c>
+      <c r="AW18">
+        <v>0</v>
+      </c>
+      <c r="AX18">
+        <v>0.11248755052026857</v>
+      </c>
+      <c r="AY18">
+        <f t="shared" si="11"/>
+        <v>0.11248755052026857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -5218,7 +5566,7 @@
         <v>1.1802078079887578E-2</v>
       </c>
       <c r="AJ19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.92323127223800683</v>
       </c>
       <c r="AK19">
@@ -5228,7 +5576,7 @@
         <v>3.4778154884700514E-4</v>
       </c>
       <c r="AM19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.18912102284679677</v>
       </c>
       <c r="AN19">
@@ -5238,7 +5586,7 @@
         <v>3.4778154884700514E-4</v>
       </c>
       <c r="AP19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.18912102284679677</v>
       </c>
       <c r="AQ19">
@@ -5248,11 +5596,31 @@
         <v>3.4778154884700514E-4</v>
       </c>
       <c r="AS19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18912102284679677</v>
       </c>
-    </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT19">
+        <v>0.18877324129794976</v>
+      </c>
+      <c r="AU19">
+        <v>3.4778154884700514E-4</v>
+      </c>
+      <c r="AV19">
+        <f t="shared" si="10"/>
+        <v>0.18912102284679677</v>
+      </c>
+      <c r="AW19">
+        <v>0.18877324129794976</v>
+      </c>
+      <c r="AX19">
+        <v>3.4778154884700514E-4</v>
+      </c>
+      <c r="AY19">
+        <f t="shared" si="11"/>
+        <v>0.18912102284679677</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5363,7 +5731,7 @@
         <v>611.91676387079497</v>
       </c>
       <c r="AJ20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>72395.422081418714</v>
       </c>
       <c r="AK20">
@@ -5373,7 +5741,7 @@
         <v>92.564589004961775</v>
       </c>
       <c r="AM20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>75019.638597761033</v>
       </c>
       <c r="AN20">
@@ -5383,7 +5751,7 @@
         <v>92.564589004961775</v>
       </c>
       <c r="AP20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>75019.638597761033</v>
       </c>
       <c r="AQ20">
@@ -5393,11 +5761,31 @@
         <v>92.564589004961775</v>
       </c>
       <c r="AS20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>75019.638597761033</v>
       </c>
-    </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT20">
+        <v>74927.07400875607</v>
+      </c>
+      <c r="AU20">
+        <v>92.564589004961775</v>
+      </c>
+      <c r="AV20">
+        <f t="shared" si="10"/>
+        <v>75019.638597761033</v>
+      </c>
+      <c r="AW20">
+        <v>74927.07400875607</v>
+      </c>
+      <c r="AX20">
+        <v>92.564589004961775</v>
+      </c>
+      <c r="AY20">
+        <f t="shared" si="11"/>
+        <v>75019.638597761033</v>
+      </c>
+    </row>
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -5454,58 +5842,72 @@
         <v>-72964.246146966863</v>
       </c>
       <c r="AJ21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-72964.246146966863</v>
       </c>
       <c r="AK21">
         <v>-76614.526624731123</v>
       </c>
       <c r="AM21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-76614.526624731123</v>
       </c>
       <c r="AN21">
         <v>-76614.526624731123</v>
       </c>
       <c r="AP21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-76614.526624731123</v>
       </c>
       <c r="AQ21">
         <v>-76614.526624731123</v>
       </c>
       <c r="AS21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-76614.526624731123</v>
       </c>
-    </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AT21">
+        <v>-76614.526624731123</v>
+      </c>
+      <c r="AV21">
+        <f t="shared" si="10"/>
+        <v>-76614.526624731123</v>
+      </c>
+      <c r="AW21">
+        <v>-76614.526624731123</v>
+      </c>
+      <c r="AY21">
+        <f t="shared" si="11"/>
+        <v>-76614.526624731123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="P22" s="64"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="136" t="s">
+      <c r="B23" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="136"/>
-      <c r="D23" s="136"/>
-      <c r="E23" s="136"/>
-      <c r="F23" s="136"/>
-      <c r="G23" s="136"/>
-      <c r="H23" s="136"/>
-      <c r="I23" s="136"/>
-      <c r="J23" s="136"/>
-      <c r="K23" s="136"/>
-      <c r="L23" s="136"/>
-      <c r="M23" s="136"/>
-      <c r="N23" s="136"/>
-      <c r="O23" s="136"/>
-      <c r="P23" s="136"/>
-      <c r="Q23" s="136"/>
-      <c r="R23" s="136"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="141"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="141"/>
+      <c r="J23" s="141"/>
+      <c r="K23" s="141"/>
+      <c r="L23" s="141"/>
+      <c r="M23" s="141"/>
+      <c r="N23" s="141"/>
+      <c r="O23" s="141"/>
+      <c r="P23" s="141"/>
+      <c r="Q23" s="141"/>
+      <c r="R23" s="141"/>
       <c r="S23" s="35" t="s">
         <v>330</v>
       </c>
@@ -5555,12 +5957,12 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="115"/>
       <c r="B1" s="62" t="s">
         <v>93</v>
@@ -5584,7 +5986,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -5610,7 +6012,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -5636,7 +6038,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>336</v>
       </c>
@@ -5662,7 +6064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -5688,7 +6090,7 @@
         <v>2204.6226218487759</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>294</v>
       </c>
@@ -5714,7 +6116,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>295</v>
       </c>
@@ -5740,7 +6142,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>296</v>
       </c>
@@ -5779,9 +6181,9 @@
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>96</v>
       </c>
@@ -5801,7 +6203,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>97</v>
       </c>
@@ -5821,7 +6223,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>98</v>
       </c>
@@ -5841,7 +6243,7 @@
         <v>28316.847000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>99</v>
       </c>
@@ -5861,7 +6263,7 @@
         <v>28.316846999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>100</v>
       </c>
@@ -5881,7 +6283,7 @@
         <v>7.4805211375990615</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>101</v>
       </c>
@@ -5914,15 +6316,15 @@
       <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>102</v>
       </c>
@@ -5954,7 +6356,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>103</v>
       </c>
@@ -5987,7 +6389,7 @@
         <v>122481433.6265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>104</v>
       </c>
@@ -6020,7 +6422,7 @@
         <v>122481.4336265</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>105</v>
       </c>
@@ -6053,7 +6455,7 @@
         <v>122.48143362649999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>106</v>
       </c>
@@ -6086,7 +6488,7 @@
         <v>34022.620451805553</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>107</v>
       </c>
@@ -6119,7 +6521,7 @@
         <v>34.022620451805558</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
         <v>108</v>
       </c>
@@ -6151,7 +6553,7 @@
         <v>116090</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
         <v>109</v>
       </c>
@@ -6184,7 +6586,7 @@
         <v>0.11609</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
         <v>110</v>
       </c>
@@ -6217,7 +6619,7 @@
         <v>45.625085571947984</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="127" t="s">
         <v>337</v>
       </c>
@@ -6270,9 +6672,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="115" t="s">
         <v>111</v>
       </c>
@@ -6295,7 +6697,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>112</v>
       </c>
@@ -6318,7 +6720,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>113</v>
       </c>
@@ -6341,7 +6743,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>114</v>
       </c>
@@ -6364,7 +6766,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>115</v>
       </c>
@@ -6387,7 +6789,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>116</v>
       </c>
@@ -6410,7 +6812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>297</v>
       </c>
@@ -6446,13 +6848,13 @@
       <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
         <v>220</v>
       </c>
@@ -6463,7 +6865,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A2" s="94" t="s">
         <v>288</v>
       </c>
@@ -6474,7 +6876,7 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
         <v>289</v>
       </c>
@@ -6485,7 +6887,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:79" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A5" s="75" t="s">
         <v>223</v>
       </c>
@@ -6724,7 +7126,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
         <v>286</v>
       </c>
@@ -6853,7 +7255,7 @@
       <c r="BZ6" s="9"/>
       <c r="CA6" s="83"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>287</v>
       </c>
@@ -7030,7 +7432,7 @@
       <c r="BZ7" s="9"/>
       <c r="CA7" s="83"/>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
         <v>221</v>
       </c>
@@ -7267,7 +7669,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A9" s="87" t="s">
         <v>222</v>
       </c>
@@ -7396,13 +7798,13 @@
       <c r="BZ9" s="88"/>
       <c r="CA9" s="92"/>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
-      <c r="B12" s="137" t="s">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="B12" s="142" t="s">
         <v>290</v>
       </c>
       <c r="C12" s="96" t="s">
@@ -7419,8 +7821,8 @@
       <c r="L12" s="97"/>
       <c r="M12" s="98"/>
     </row>
-    <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="138"/>
+    <row r="13" spans="1:79" ht="39" x14ac:dyDescent="0.25">
+      <c r="B13" s="143"/>
       <c r="C13" s="99" t="s">
         <v>1</v>
       </c>
@@ -7455,7 +7857,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A14" s="110" t="s">
         <v>22</v>
       </c>
@@ -7496,7 +7898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A15" s="76" t="s">
         <v>23</v>
       </c>
@@ -7537,7 +7939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A16" s="76" t="s">
         <v>7</v>
       </c>
@@ -7578,7 +7980,7 @@
         <v>76.151387532990128</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="76" t="s">
         <v>24</v>
       </c>
@@ -7619,7 +8021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="76" t="s">
         <v>25</v>
       </c>
@@ -7660,7 +8062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="76" t="s">
         <v>26</v>
       </c>
@@ -7701,7 +8103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -7742,7 +8144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
@@ -7783,7 +8185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="76" t="s">
         <v>29</v>
       </c>
@@ -7824,7 +8226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="76" t="s">
         <v>30</v>
       </c>
@@ -7865,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="87" t="s">
         <v>31</v>
       </c>
@@ -7906,9 +8308,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="110"/>
-      <c r="B25" s="137" t="s">
+      <c r="B25" s="142" t="s">
         <v>290</v>
       </c>
       <c r="C25" s="96" t="s">
@@ -7925,9 +8327,9 @@
       <c r="L25" s="97"/>
       <c r="M25" s="98"/>
     </row>
-    <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A26" s="76"/>
-      <c r="B26" s="138"/>
+      <c r="B26" s="143"/>
       <c r="C26" s="99" t="s">
         <v>1</v>
       </c>
@@ -7962,7 +8364,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="110" t="s">
         <v>22</v>
       </c>
@@ -8003,7 +8405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="76" t="s">
         <v>23</v>
       </c>
@@ -8044,7 +8446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="76" t="s">
         <v>7</v>
       </c>
@@ -8085,7 +8487,7 @@
         <v>95.950748291567578</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="76" t="s">
         <v>24</v>
       </c>
@@ -8126,7 +8528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="76" t="s">
         <v>25</v>
       </c>
@@ -8167,7 +8569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="76" t="s">
         <v>26</v>
       </c>
@@ -8208,7 +8610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -8249,7 +8651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -8290,7 +8692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="76" t="s">
         <v>29</v>
       </c>
@@ -8331,7 +8733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="76" t="s">
         <v>30</v>
       </c>
@@ -8372,7 +8774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="87" t="s">
         <v>31</v>
       </c>
@@ -8430,9 +8832,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -8440,7 +8842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="112" t="s">
         <v>8</v>
       </c>
@@ -8451,7 +8853,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="112" t="s">
         <v>9</v>
       </c>
@@ -8462,7 +8864,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="112" t="s">
         <v>10</v>
       </c>
@@ -8473,7 +8875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>11</v>
       </c>
@@ -8484,7 +8886,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
         <v>12</v>
       </c>
@@ -8495,7 +8897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
         <v>13</v>
       </c>
@@ -8520,12 +8922,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -8533,7 +8935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8544,7 +8946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -8555,7 +8957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -8566,7 +8968,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -8577,7 +8979,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -8588,7 +8990,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -8612,17 +9014,17 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -8693,7 +9095,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="118" t="s">
         <v>122</v>
       </c>
@@ -8767,7 +9169,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -8841,7 +9243,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -8915,7 +9317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -8989,7 +9391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -9063,7 +9465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9137,7 +9539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -9211,7 +9613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -9285,7 +9687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -9359,7 +9761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -9433,7 +9835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -9507,7 +9909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -9581,7 +9983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -9655,7 +10057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -9729,7 +10131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -9803,7 +10205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -9877,7 +10279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -9951,7 +10353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10025,7 +10427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10099,23 +10501,23 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="136" t="s">
+      <c r="B22" s="141" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="136"/>
-      <c r="D22" s="136"/>
-      <c r="E22" s="136"/>
-      <c r="F22" s="136"/>
+      <c r="C22" s="141"/>
+      <c r="D22" s="141"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="141"/>
       <c r="G22" s="35" t="s">
         <v>334</v>
       </c>
       <c r="H22" s="35"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -10129,7 +10531,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -10143,7 +10545,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -10157,7 +10559,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -10171,7 +10573,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -10185,7 +10587,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -10199,7 +10601,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -10213,7 +10615,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -10227,7 +10629,7 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -10241,7 +10643,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -10255,7 +10657,7 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -10269,7 +10671,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -10283,7 +10685,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -10308,24 +10710,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
-  <dimension ref="A1:BN27"/>
+  <dimension ref="A1:BO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BJ1" sqref="BJ1"/>
+      <selection pane="topRight" activeCell="BO1" sqref="BO1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" customWidth="1"/>
-    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:67" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
         <v>309</v>
@@ -10423,13 +10825,13 @@
       <c r="AG1" t="s">
         <v>89</v>
       </c>
-      <c r="AH1" s="140" t="s">
+      <c r="AH1" s="137" t="s">
         <v>367</v>
       </c>
       <c r="AI1" s="117" t="s">
         <v>303</v>
       </c>
-      <c r="AJ1" s="140" t="s">
+      <c r="AJ1" s="137" t="s">
         <v>150</v>
       </c>
       <c r="AK1" t="s">
@@ -10522,8 +10924,11 @@
       <c r="BN1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:67" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
@@ -10623,13 +11028,13 @@
       <c r="AG2" s="119" t="s">
         <v>184</v>
       </c>
-      <c r="AH2" s="142" t="s">
+      <c r="AH2" s="139" t="s">
         <v>184</v>
       </c>
       <c r="AI2" s="117" t="s">
         <v>306</v>
       </c>
-      <c r="AJ2" s="140" t="s">
+      <c r="AJ2" s="137" t="s">
         <v>306</v>
       </c>
       <c r="AK2" s="117" t="s">
@@ -10722,8 +11127,11 @@
       <c r="BN2" s="119" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO2" s="119" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -10823,13 +11231,13 @@
       <c r="AG3" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="AH3" s="141" t="s">
+      <c r="AH3" s="138" t="s">
         <v>109</v>
       </c>
       <c r="AI3" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="AJ3" s="141" t="s">
+      <c r="AJ3" s="138" t="s">
         <v>93</v>
       </c>
       <c r="AK3" s="20" t="s">
@@ -10922,8 +11330,11 @@
       <c r="BN3" s="20" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO3" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -11023,13 +11434,13 @@
       <c r="AG4">
         <v>1315314.5481741754</v>
       </c>
-      <c r="AH4" s="140">
+      <c r="AH4" s="137">
         <v>1577047.8115483243</v>
       </c>
       <c r="AI4" s="22">
         <v>99.15771301835683</v>
       </c>
-      <c r="AJ4" s="140">
+      <c r="AJ4" s="137">
         <v>48.309136220851776</v>
       </c>
       <c r="AK4">
@@ -11122,8 +11533,11 @@
       <c r="BN4">
         <v>69.378860802973378</v>
       </c>
-    </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO4">
+        <v>9.9750188696234865</v>
+      </c>
+    </row>
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -11223,13 +11637,13 @@
       <c r="AG5">
         <v>1311743.8531964528</v>
       </c>
-      <c r="AH5" s="140">
+      <c r="AH5" s="137">
         <v>1517324.445253175</v>
       </c>
       <c r="AI5" s="22">
         <v>99.10102802045931</v>
       </c>
-      <c r="AJ5" s="140">
+      <c r="AJ5" s="137">
         <v>14.315311187199075</v>
       </c>
       <c r="AK5">
@@ -11322,8 +11736,11 @@
       <c r="BN5">
         <v>66.562363858854823</v>
       </c>
-    </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO5">
+        <v>9.9099322935660243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -11423,13 +11840,13 @@
       <c r="AG6">
         <v>4999.13237353164</v>
       </c>
-      <c r="AH6" s="140">
+      <c r="AH6" s="137">
         <v>83636.313938146748</v>
       </c>
       <c r="AI6" s="22">
         <v>7.6154275905965907E-2</v>
       </c>
-      <c r="AJ6" s="140">
+      <c r="AJ6" s="137">
         <v>1.0137246040480141</v>
       </c>
       <c r="AK6">
@@ -11522,8 +11939,11 @@
       <c r="BN6">
         <v>3.5388428925359858</v>
       </c>
-    </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO6">
+        <v>9.314408223966951E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -11623,13 +12043,13 @@
       <c r="AG7">
         <v>1301825.3866966912</v>
       </c>
-      <c r="AH7" s="140">
+      <c r="AH7" s="137">
         <v>1425319.0641897889</v>
       </c>
       <c r="AI7" s="22">
         <v>87.624663165139467</v>
       </c>
-      <c r="AJ7" s="140">
+      <c r="AJ7" s="137">
         <v>11.763196513266807</v>
       </c>
       <c r="AK7">
@@ -11722,8 +12142,11 @@
       <c r="BN7">
         <v>47.175363754400323</v>
       </c>
-    </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO7">
+        <v>8.6071446539691561</v>
+      </c>
+    </row>
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -11823,13 +12246,13 @@
       <c r="AG8">
         <v>4919.3341262300773</v>
       </c>
-      <c r="AH8" s="140">
+      <c r="AH8" s="137">
         <v>8369.0671252394204</v>
       </c>
       <c r="AI8" s="22">
         <v>11.400210579413892</v>
       </c>
-      <c r="AJ8" s="140">
+      <c r="AJ8" s="137">
         <v>1.5383900698842508</v>
       </c>
       <c r="AK8">
@@ -11922,8 +12345,11 @@
       <c r="BN8">
         <v>15.848157211918526</v>
       </c>
-    </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO8">
+        <v>1.2096435573571984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -12023,13 +12449,13 @@
       <c r="AG9">
         <v>26.022097330325355</v>
       </c>
-      <c r="AH9" s="140">
+      <c r="AH9" s="137">
         <v>49.472223700978624</v>
       </c>
       <c r="AI9" s="22">
         <v>2.8948575569389908E-3</v>
       </c>
-      <c r="AJ9" s="140">
+      <c r="AJ9" s="137">
         <v>1.0528740521994456E-2</v>
       </c>
       <c r="AK9">
@@ -12122,8 +12548,11 @@
       <c r="BN9">
         <v>1.2571786330539047E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO9">
+        <v>1.2210379021022032E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>59</v>
       </c>
@@ -12157,11 +12586,11 @@
       <c r="AC10" s="33"/>
       <c r="AD10" s="33"/>
       <c r="AE10" s="33"/>
-      <c r="AH10" s="140"/>
+      <c r="AH10" s="137"/>
       <c r="AI10" s="26"/>
-      <c r="AJ10" s="140"/>
-    </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="AJ10" s="137"/>
+    </row>
+    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>60</v>
       </c>
@@ -12261,13 +12690,13 @@
       <c r="AG11">
         <v>10.275322226239604</v>
       </c>
-      <c r="AH11" s="140">
+      <c r="AH11" s="137">
         <v>12.100690959036683</v>
       </c>
       <c r="AI11" s="22">
         <v>3.2710763129870442E-3</v>
       </c>
-      <c r="AJ11" s="140">
+      <c r="AJ11" s="137">
         <v>1.5333537460206102E-3</v>
       </c>
       <c r="AK11">
@@ -12360,8 +12789,11 @@
       <c r="BN11">
         <v>9.6751445371123475E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO11">
+        <v>1.1708326982510144E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -12461,13 +12893,13 @@
       <c r="AG12">
         <v>16.062252431105641</v>
       </c>
-      <c r="AH12" s="140">
+      <c r="AH12" s="137">
         <v>22.481656351880339</v>
       </c>
       <c r="AI12" s="22">
         <v>4.4788457908180607E-3</v>
       </c>
-      <c r="AJ12" s="140">
+      <c r="AJ12" s="137">
         <v>1.0672619853839356E-3</v>
       </c>
       <c r="AK12">
@@ -12560,8 +12992,11 @@
       <c r="BN12">
         <v>6.9227894123971819E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO12">
+        <v>1.3246978822933949E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -12661,13 +13096,13 @@
       <c r="AG13">
         <v>21.007515266850735</v>
       </c>
-      <c r="AH13" s="140">
+      <c r="AH13" s="137">
         <v>32.505122182253004</v>
       </c>
       <c r="AI13" s="22">
         <v>3.5928608420523145E-2</v>
       </c>
-      <c r="AJ13" s="140">
+      <c r="AJ13" s="137">
         <v>2.2653418147137137E-3</v>
       </c>
       <c r="AK13">
@@ -12760,8 +13195,11 @@
       <c r="BN13">
         <v>3.724647449968985E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO13">
+        <v>1.813605257613188E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -12861,13 +13299,13 @@
       <c r="AG14">
         <v>2.8401050053824055</v>
       </c>
-      <c r="AH14" s="140">
+      <c r="AH14" s="137">
         <v>4.5403634527468109</v>
       </c>
       <c r="AI14" s="22">
         <v>3.2848921981275752E-4</v>
       </c>
-      <c r="AJ14" s="140">
+      <c r="AJ14" s="137">
         <v>4.1719548987732114E-4</v>
       </c>
       <c r="AK14">
@@ -12960,8 +13398,11 @@
       <c r="BN14">
         <v>3.9233022845947815E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO14">
+        <v>7.6792485564078277E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -13061,13 +13502,13 @@
       <c r="AG15">
         <v>2.7114794461446454</v>
       </c>
-      <c r="AH15" s="140">
+      <c r="AH15" s="137">
         <v>3.6846509333600648</v>
       </c>
       <c r="AI15" s="22">
         <v>3.067172810566663E-4</v>
       </c>
-      <c r="AJ15" s="140">
+      <c r="AJ15" s="137">
         <v>1.5578505014062489E-4</v>
       </c>
       <c r="AK15">
@@ -13160,8 +13601,11 @@
       <c r="BN15">
         <v>2.0326514725382689E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO15">
+        <v>6.6674042219136396E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -13261,13 +13705,13 @@
       <c r="AG16">
         <v>13.610201106319744</v>
       </c>
-      <c r="AH16" s="140">
+      <c r="AH16" s="137">
         <v>23.416348896201253</v>
       </c>
       <c r="AI16" s="22">
         <v>1.8222658628499725E-3</v>
       </c>
-      <c r="AJ16" s="140">
+      <c r="AJ16" s="137">
         <v>6.4108055505771673E-4</v>
       </c>
       <c r="AK16">
@@ -13360,8 +13804,11 @@
       <c r="BN16">
         <v>1.3557166453407658E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO16">
+        <v>5.5307439159581304E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>66</v>
       </c>
@@ -13461,13 +13908,13 @@
       <c r="AG17">
         <v>0.33504752591656944</v>
       </c>
-      <c r="AH17" s="140">
+      <c r="AH17" s="137">
         <v>0.39065135934215078</v>
       </c>
       <c r="AI17" s="22">
         <v>4.5955619542805638E-5</v>
       </c>
-      <c r="AJ17" s="140">
+      <c r="AJ17" s="137">
         <v>1.813548940962644E-5</v>
       </c>
       <c r="AK17">
@@ -13560,8 +14007,11 @@
       <c r="BN17">
         <v>3.2718107917875022E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO17">
+        <v>1.0214514606039252E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>67</v>
       </c>
@@ -13661,13 +14111,13 @@
       <c r="AG18">
         <v>0.74377470433511161</v>
       </c>
-      <c r="AH18" s="140">
+      <c r="AH18" s="137">
         <v>1.0192401131404758</v>
       </c>
       <c r="AI18" s="22">
         <v>1.1205234448988939E-4</v>
       </c>
-      <c r="AJ18" s="140">
+      <c r="AJ18" s="137">
         <v>2.6310323667497318E-5</v>
       </c>
       <c r="AK18">
@@ -13760,8 +14210,11 @@
       <c r="BN18">
         <v>5.3261285895382865E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO18">
+        <v>2.6458634401739373E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>68</v>
       </c>
@@ -13861,13 +14314,13 @@
       <c r="AG19">
         <v>189.04492298972374</v>
       </c>
-      <c r="AH19" s="140">
+      <c r="AH19" s="137">
         <v>223.15064256600229</v>
       </c>
       <c r="AI19" s="22">
         <v>1.579320164524466E-2</v>
       </c>
-      <c r="AJ19" s="140">
+      <c r="AJ19" s="137">
         <v>2.580565674925735E-3</v>
       </c>
       <c r="AK19">
@@ -13960,8 +14413,11 @@
       <c r="BN19">
         <v>1.9528710437986155E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO19">
+        <v>1.7288576101387265E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -14061,13 +14517,13 @@
       <c r="AG20">
         <v>0.58866204659784449</v>
       </c>
-      <c r="AH20" s="140">
+      <c r="AH20" s="137">
         <v>0.89713555715877558</v>
       </c>
       <c r="AI20" s="22">
         <v>1.742743859440626E-2</v>
       </c>
-      <c r="AJ20" s="140">
+      <c r="AJ20" s="137">
         <v>1.0023096907203865E-3</v>
       </c>
       <c r="AK20">
@@ -14160,8 +14616,11 @@
       <c r="BN20">
         <v>8.8356010400824942E-5</v>
       </c>
-    </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO20">
+        <v>3.6636240073674802E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>70</v>
       </c>
@@ -14186,7 +14645,7 @@
       <c r="H21" s="30">
         <v>0.51476298268065945</v>
       </c>
-      <c r="I21" s="139">
+      <c r="I21" s="136">
         <v>0.65589183244261862</v>
       </c>
       <c r="J21" s="30">
@@ -14261,13 +14720,13 @@
       <c r="AG21">
         <v>78307.41826476407</v>
       </c>
-      <c r="AH21" s="140">
+      <c r="AH21" s="137">
         <v>93797.02635737024</v>
       </c>
       <c r="AI21" s="30">
         <v>4.287972545719934</v>
       </c>
-      <c r="AJ21" s="140">
+      <c r="AJ21" s="137">
         <v>1.1119055333036951</v>
       </c>
       <c r="AK21">
@@ -14360,52 +14819,55 @@
       <c r="BN21">
         <v>2.6286261463371274</v>
       </c>
-    </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.35">
-      <c r="AH22" s="140"/>
-      <c r="AJ22" s="140"/>
-    </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO21">
+        <v>0.88119803944701025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AH22" s="137"/>
+      <c r="AJ22" s="137"/>
+    </row>
+    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="136" t="s">
+      <c r="B23" s="141" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="136"/>
-      <c r="D23" s="136"/>
-      <c r="E23" s="136"/>
-      <c r="F23" s="136"/>
-      <c r="G23" s="136"/>
-      <c r="H23" s="136"/>
-      <c r="I23" s="136"/>
-      <c r="J23" s="136"/>
-      <c r="K23" s="136"/>
-      <c r="L23" s="136"/>
-      <c r="M23" s="136"/>
-      <c r="N23" s="136"/>
-      <c r="O23" s="136"/>
-      <c r="P23" s="136"/>
-      <c r="Q23" s="136"/>
-      <c r="R23" s="136"/>
-      <c r="S23" s="136"/>
-      <c r="T23" s="136"/>
-      <c r="U23" s="136"/>
-      <c r="V23" s="136"/>
-      <c r="W23" s="136"/>
-      <c r="X23" s="136"/>
-      <c r="Y23" s="136"/>
-      <c r="Z23" s="136"/>
-      <c r="AA23" s="136"/>
-      <c r="AB23" s="136"/>
-      <c r="AC23" s="136"/>
-      <c r="AD23" s="136"/>
-      <c r="AE23" s="136"/>
-      <c r="AF23" s="136"/>
-      <c r="AH23" s="140" t="s">
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="141"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="141"/>
+      <c r="J23" s="141"/>
+      <c r="K23" s="141"/>
+      <c r="L23" s="141"/>
+      <c r="M23" s="141"/>
+      <c r="N23" s="141"/>
+      <c r="O23" s="141"/>
+      <c r="P23" s="141"/>
+      <c r="Q23" s="141"/>
+      <c r="R23" s="141"/>
+      <c r="S23" s="141"/>
+      <c r="T23" s="141"/>
+      <c r="U23" s="141"/>
+      <c r="V23" s="141"/>
+      <c r="W23" s="141"/>
+      <c r="X23" s="141"/>
+      <c r="Y23" s="141"/>
+      <c r="Z23" s="141"/>
+      <c r="AA23" s="141"/>
+      <c r="AB23" s="141"/>
+      <c r="AC23" s="141"/>
+      <c r="AD23" s="141"/>
+      <c r="AE23" s="141"/>
+      <c r="AF23" s="141"/>
+      <c r="AH23" s="137" t="s">
         <v>368</v>
       </c>
-      <c r="AJ23" s="140" t="s">
+      <c r="AJ23" s="137" t="s">
         <v>348</v>
       </c>
       <c r="AK23" t="s">
@@ -14498,8 +14960,11 @@
       <c r="BN23" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BO23" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
       <c r="AR27">
         <v>99</v>
       </c>
@@ -14521,9 +14986,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -14531,7 +14996,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -14540,7 +15005,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -14549,7 +15014,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -14558,7 +15023,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -14567,7 +15032,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>79</v>
       </c>
@@ -14588,9 +15053,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -14640,7 +15105,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -14690,7 +15155,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -14743,7 +15208,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="112" t="s">
         <v>8</v>
       </c>
@@ -14794,7 +15259,7 @@
       </c>
       <c r="Q4" s="114"/>
     </row>
-    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>9</v>
       </c>
@@ -14845,7 +15310,7 @@
       </c>
       <c r="Q5" s="114"/>
     </row>
-    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
         <v>10</v>
       </c>
@@ -14896,7 +15361,7 @@
       </c>
       <c r="Q6" s="114"/>
     </row>
-    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
         <v>11</v>
       </c>
@@ -14947,7 +15412,7 @@
       </c>
       <c r="Q7" s="114"/>
     </row>
-    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="112" t="s">
         <v>12</v>
       </c>
@@ -14998,7 +15463,7 @@
       </c>
       <c r="Q8" s="114"/>
     </row>
-    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="112" t="s">
         <v>13</v>
       </c>
@@ -15049,7 +15514,7 @@
       </c>
       <c r="Q9" s="114"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -15100,7 +15565,7 @@
       </c>
       <c r="Q10" s="67"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -15151,7 +15616,7 @@
       </c>
       <c r="Q11" s="67"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -15202,7 +15667,7 @@
       </c>
       <c r="Q12" s="67"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -15253,7 +15718,7 @@
       </c>
       <c r="Q13" s="67"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -15304,7 +15769,7 @@
       </c>
       <c r="Q14" s="67"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -15355,7 +15820,7 @@
       </c>
       <c r="Q15" s="67"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -15406,7 +15871,7 @@
       </c>
       <c r="Q16" s="67"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -15457,7 +15922,7 @@
       </c>
       <c r="Q17" s="67"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -15508,7 +15973,7 @@
       </c>
       <c r="Q18" s="67"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -15559,7 +16024,7 @@
       </c>
       <c r="Q19" s="67"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -15614,7 +16079,7 @@
         <v>3.3478260869565215</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -15628,30 +16093,30 @@
       <c r="N21" s="64"/>
       <c r="O21" s="64"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="M22" s="64"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="136" t="s">
+      <c r="B23" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="136"/>
-      <c r="D23" s="136"/>
-      <c r="E23" s="136"/>
-      <c r="F23" s="136"/>
-      <c r="G23" s="136"/>
-      <c r="H23" s="136"/>
-      <c r="I23" s="136"/>
-      <c r="J23" s="136"/>
-      <c r="K23" s="136"/>
-      <c r="L23" s="136"/>
-      <c r="M23" s="136"/>
-      <c r="N23" s="136"/>
-      <c r="O23" s="136"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="141"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="141"/>
+      <c r="J23" s="141"/>
+      <c r="K23" s="141"/>
+      <c r="L23" s="141"/>
+      <c r="M23" s="141"/>
+      <c r="N23" s="141"/>
+      <c r="O23" s="141"/>
       <c r="P23" t="s">
         <v>90</v>
       </c>
@@ -15674,12 +16139,12 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>298</v>
       </c>
@@ -15690,7 +16155,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -15704,7 +16169,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -15718,7 +16183,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -15732,7 +16197,7 @@
         <v>362403.00757167325</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -15746,7 +16211,7 @@
         <v>344979.42656462023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -15760,7 +16225,7 @@
         <v>24381.856026689315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -15774,7 +16239,7 @@
         <v>254462.26606022959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -15788,7 +16253,7 @@
         <v>66135.304477701342</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -15802,7 +16267,7 @@
         <v>59.889274923371126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -15816,7 +16281,7 @@
         <v>24.470884336712146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -15830,7 +16295,7 @@
         <v>34.134614130073174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -15844,7 +16309,7 @@
         <v>-15.759603589368934</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -15858,7 +16323,7 @@
         <v>8.6858851249063438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -15872,7 +16337,7 @@
         <v>6.9883164862451217</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -15886,7 +16351,7 @@
         <v>58.328462296040968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -15900,7 +16365,7 @@
         <v>0.49662761207225459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -15914,7 +16379,7 @@
         <v>1.1283578872130025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -15928,7 +16393,7 @@
         <v>57.127332585038609</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -15942,7 +16407,7 @@
         <v>-82.715827114534676</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -15956,7 +16421,7 @@
         <v>22763.019075759898</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -15980,9 +16445,9 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -15990,7 +16455,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -15998,7 +16463,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -16006,7 +16471,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>336</v>
       </c>
@@ -16014,7 +16479,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -16022,7 +16487,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>294</v>
       </c>
@@ -16030,7 +16495,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>97</v>
       </c>
@@ -16038,7 +16503,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>98</v>
       </c>
@@ -16046,7 +16511,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>99</v>
       </c>
@@ -16054,7 +16519,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>100</v>
       </c>
@@ -16062,7 +16527,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>101</v>
       </c>
@@ -16070,7 +16535,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>103</v>
       </c>
@@ -16078,7 +16543,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>104</v>
       </c>
@@ -16086,7 +16551,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>105</v>
       </c>
@@ -16094,7 +16559,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
         <v>106</v>
       </c>
@@ -16102,7 +16567,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="s">
         <v>107</v>
       </c>
@@ -16110,7 +16575,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>108</v>
       </c>
@@ -16118,7 +16583,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>109</v>
       </c>
@@ -16126,7 +16591,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>110</v>
       </c>
@@ -16134,7 +16599,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="126" t="s">
         <v>337</v>
       </c>
@@ -16142,7 +16607,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>112</v>
       </c>
@@ -16150,7 +16615,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="s">
         <v>113</v>
       </c>
@@ -16158,7 +16623,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="62" t="s">
         <v>114</v>
       </c>
@@ -16166,7 +16631,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>115</v>
       </c>
@@ -16174,7 +16639,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
         <v>116</v>
       </c>
@@ -16189,18 +16654,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="68" t="s">
         <v>186</v>
       </c>
@@ -16208,7 +16673,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -16219,7 +16684,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -16230,7 +16695,7 @@
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
         <v>127</v>
       </c>
@@ -16241,7 +16706,7 @@
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
         <v>128</v>
       </c>
@@ -16252,7 +16717,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
         <v>129</v>
       </c>
@@ -16263,7 +16728,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
         <v>130</v>
       </c>
@@ -16274,7 +16739,7 @@
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
         <v>131</v>
       </c>
@@ -16285,7 +16750,7 @@
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
         <v>132</v>
       </c>
@@ -16296,7 +16761,7 @@
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
         <v>133</v>
       </c>
@@ -16307,7 +16772,7 @@
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="69" t="s">
         <v>134</v>
       </c>
@@ -16318,7 +16783,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -16329,7 +16794,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="69" t="s">
         <v>136</v>
       </c>
@@ -16340,7 +16805,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="69" t="s">
         <v>137</v>
       </c>
@@ -16351,7 +16816,7 @@
         <v>755.86244135709444</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="69" t="s">
         <v>138</v>
       </c>
@@ -16362,7 +16827,7 @@
         <v>762.55920427134606</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
         <v>139</v>
       </c>
@@ -16373,7 +16838,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
         <v>140</v>
       </c>
@@ -16384,7 +16849,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
         <v>141</v>
       </c>
@@ -16395,7 +16860,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="68" t="s">
         <v>1</v>
       </c>
@@ -16406,7 +16871,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -16417,7 +16882,7 @@
         <v>725.15243391008278</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -16428,7 +16893,7 @@
         <v>748.62596861099109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -16439,7 +16904,7 @@
         <v>801.99999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -16450,7 +16915,7 @@
         <v>791.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -16461,7 +16926,7 @@
         <v>700.32025584540236</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -16472,7 +16937,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -16483,7 +16948,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -16494,7 +16959,7 @@
         <v>794.1013538556316</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -16505,7 +16970,7 @@
         <v>789.34625592835232</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -16516,7 +16981,7 @@
         <v>809.68750817282455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -16527,7 +16992,7 @@
         <v>783.00612535864673</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -16538,7 +17003,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -16549,7 +17014,7 @@
         <v>508.00296189766453</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>155</v>
       </c>
@@ -16560,7 +17025,7 @@
         <v>428.22298556220187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -16571,7 +17036,7 @@
         <v>665.18536560495022</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -16582,7 +17047,7 @@
         <v>859.88020851632757</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -16593,7 +17058,7 @@
         <v>887.88245186586084</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -16604,7 +17069,7 @@
         <v>797.00724703341325</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -16615,7 +17080,7 @@
         <v>748.92792354647884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -16626,7 +17091,7 @@
         <v>778.77937164550963</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>162</v>
       </c>
@@ -16637,7 +17102,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -16648,7 +17113,7 @@
         <v>798.04417121416941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -16659,7 +17124,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>338</v>
       </c>
@@ -16670,7 +17135,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>339</v>
       </c>
@@ -16681,513 +17146,535 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>372</v>
+      </c>
+      <c r="B45" s="69">
+        <v>43.975450721892244</v>
+      </c>
+      <c r="C45">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>373</v>
+      </c>
+      <c r="B46" s="69">
+        <v>43.819577184272568</v>
+      </c>
+      <c r="C46">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>164</v>
       </c>
-      <c r="B45">
+      <c r="B47">
         <v>38.180512527472686</v>
       </c>
-      <c r="C45">
+      <c r="C47">
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>165</v>
       </c>
-      <c r="B46">
+      <c r="B48">
         <v>37.300256882262083</v>
       </c>
-      <c r="C46">
+      <c r="C48">
         <v>716.69892648380858</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>166</v>
       </c>
-      <c r="B47">
+      <c r="B49">
         <v>36.889328265240245</v>
       </c>
-      <c r="C47">
+      <c r="C49">
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>167</v>
       </c>
-      <c r="B48">
+      <c r="B50">
         <v>39.429337036099838</v>
       </c>
-      <c r="C48">
+      <c r="C50">
         <v>756.99999999999989</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>168</v>
       </c>
-      <c r="B49">
+      <c r="B51">
         <v>10.040313081123244</v>
       </c>
-      <c r="C49">
+      <c r="C51">
         <v>70.798124695046326</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>169</v>
       </c>
-      <c r="B50">
+      <c r="B52">
         <v>30.792488052730107</v>
       </c>
-      <c r="C50">
+      <c r="C52">
         <v>742.58779297677324</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>170</v>
       </c>
-      <c r="B51">
+      <c r="B53">
         <v>31.839314137909518</v>
       </c>
-      <c r="C51">
+      <c r="C53">
         <v>742.32362086970215</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>171</v>
       </c>
-      <c r="B52">
+      <c r="B54">
         <v>33.077070766926674</v>
       </c>
-      <c r="C52">
+      <c r="C54">
         <v>769.53334789802227</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>172</v>
       </c>
-      <c r="B53">
+      <c r="B55">
         <v>31.263230600468017</v>
       </c>
-      <c r="C53">
+      <c r="C55">
         <v>584.61287294827434</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>173</v>
       </c>
-      <c r="B54">
+      <c r="B56">
         <v>29.646904789703584</v>
       </c>
-      <c r="C54">
+      <c r="C56">
         <v>559.51652277652283</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>174</v>
       </c>
-      <c r="B55">
+      <c r="B57">
         <v>31.510123545085804</v>
       </c>
-      <c r="C55">
+      <c r="C57">
         <v>595.17975723111715</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>175</v>
       </c>
-      <c r="B56">
+      <c r="B58">
         <v>27.734307445397814</v>
       </c>
-      <c r="C56">
+      <c r="C58">
         <v>507.21044557645126</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>176</v>
       </c>
-      <c r="B57">
+      <c r="B59">
         <v>27.548680827882244</v>
       </c>
-      <c r="C57">
+      <c r="C59">
         <v>668.88377510394514</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>177</v>
       </c>
-      <c r="B58">
+      <c r="B60">
         <v>34.60609523247426</v>
       </c>
-      <c r="C58">
+      <c r="C60">
         <v>654.80340179705718</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>178</v>
       </c>
-      <c r="B59">
+      <c r="B61">
         <v>36.455478031346189</v>
       </c>
-      <c r="C59">
+      <c r="C61">
         <v>688.85095964480468</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>179</v>
       </c>
-      <c r="B60">
+      <c r="B62">
         <v>38.505872853524245</v>
       </c>
-      <c r="C60">
+      <c r="C62">
         <v>737.59071339941693</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>180</v>
       </c>
-      <c r="B61">
+      <c r="B63">
         <v>39.773165285279561</v>
       </c>
-      <c r="C61">
+      <c r="C63">
         <v>765.47381512866104</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>181</v>
       </c>
-      <c r="B62">
+      <c r="B64">
         <v>38.281904677575831</v>
       </c>
-      <c r="C62">
+      <c r="C64">
         <v>731.67589538225809</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>182</v>
       </c>
-      <c r="B63">
+      <c r="B65">
         <v>31.369932808387436</v>
       </c>
-      <c r="C63">
+      <c r="C65">
         <v>800.00032424653136</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>183</v>
       </c>
-      <c r="B64">
+      <c r="B66">
         <v>38.180512527472686</v>
       </c>
-      <c r="C64">
+      <c r="C66">
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>187</v>
       </c>
-      <c r="B65">
+      <c r="B67">
         <v>47.141813661363599</v>
       </c>
-      <c r="C65">
+      <c r="C67">
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>188</v>
       </c>
-      <c r="B66">
+      <c r="B68">
         <v>49.999999999999993</v>
       </c>
-      <c r="C66">
+      <c r="C68">
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="68" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="B67">
+      <c r="B69">
         <v>119.98674372549019</v>
       </c>
-      <c r="C67">
+      <c r="C69">
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="143" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="140" t="s">
         <v>367</v>
       </c>
-      <c r="B68" s="140">
+      <c r="B70" s="137">
         <v>119.98674372549019</v>
       </c>
-      <c r="C68" s="140">
+      <c r="C70" s="137">
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>189</v>
       </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-      <c r="C69">
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>190</v>
       </c>
-      <c r="B70">
+      <c r="B72">
         <v>48.885121247479262</v>
       </c>
-      <c r="C70">
+      <c r="C72">
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>191</v>
       </c>
-      <c r="B71">
+      <c r="B73">
         <v>22.648458746153963</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>192</v>
       </c>
-      <c r="B72">
+      <c r="B74">
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>193</v>
       </c>
-      <c r="B73">
+      <c r="B75">
         <v>18.707371337693861</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>194</v>
       </c>
-      <c r="B74">
+      <c r="B76">
         <v>12.566427590816895</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>195</v>
       </c>
-      <c r="B75">
+      <c r="B77">
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>196</v>
       </c>
-      <c r="B76">
+      <c r="B78">
         <v>11.566786665057547</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>197</v>
       </c>
-      <c r="B77">
+      <c r="B79">
         <v>31.342185540824094</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>198</v>
       </c>
-      <c r="B78">
+      <c r="B80">
         <v>31.0106439692332</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>199</v>
       </c>
-      <c r="B79">
+      <c r="B81">
         <v>28.609127685562171</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>200</v>
       </c>
-      <c r="B80">
+      <c r="B82">
         <v>33.012627597074328</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>201</v>
       </c>
-      <c r="B81">
+      <c r="B83">
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>202</v>
       </c>
-      <c r="B82">
+      <c r="B84">
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>203</v>
       </c>
-      <c r="B83">
+      <c r="B85">
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>204</v>
       </c>
-      <c r="B84">
+      <c r="B86">
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>205</v>
       </c>
-      <c r="B85">
+      <c r="B87">
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>206</v>
       </c>
-      <c r="B86">
+      <c r="B88">
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>207</v>
       </c>
-      <c r="B87">
+      <c r="B89">
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>208</v>
       </c>
-      <c r="B88">
+      <c r="B90">
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>209</v>
       </c>
-      <c r="B89">
+      <c r="B91">
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>210</v>
       </c>
-      <c r="B90">
+      <c r="B92">
         <v>14.4</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>211</v>
       </c>
-      <c r="B91">
+      <c r="B93">
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>212</v>
       </c>
-      <c r="B92">
+      <c r="B94">
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>213</v>
       </c>
-      <c r="B93">
+      <c r="B95">
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>214</v>
       </c>
-      <c r="B94">
+      <c r="B96">
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>215</v>
       </c>
-      <c r="B95">
+      <c r="B97">
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>216</v>
       </c>
-      <c r="B96">
+      <c r="B98">
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="68" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="68" t="s">
         <v>219</v>
       </c>
-      <c r="C97">
+      <c r="C99">
         <v>1000</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>75</v>
       </c>
-      <c r="C98">
+      <c r="C100">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding the Algae HTL pathway
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23CA6AC-3D67-434C-8B5C-4F424CEEC9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B18F0DF-5C29-4270-97F5-742394E2AEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" activeTab="13" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="373">
   <si>
     <t>NG</t>
   </si>
@@ -1091,9 +1091,6 @@
   </si>
   <si>
     <t>Biochar</t>
-  </si>
-  <si>
-    <t>Algae Biomass</t>
   </si>
   <si>
     <t>Vegetable Oil</t>
@@ -1498,7 +1495,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1574,6 +1571,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1761,7 +1764,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2051,6 +2054,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2771,19 +2777,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="122"/>
-    <col min="41" max="41" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="122"/>
+    <col min="41" max="41" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" ht="26.5" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2839,46 +2845,46 @@
         <v>14</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AE1" s="6" t="s">
         <v>48</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AG1" s="117" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AH1" s="6" t="s">
         <v>164</v>
@@ -2899,43 +2905,43 @@
         <v>242</v>
       </c>
       <c r="AN1" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AR1" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AS1" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="AQ1" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="AR1" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="AS1" s="6" t="s">
-        <v>339</v>
-      </c>
       <c r="AT1" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="AW1" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AX1" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AY1" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="AW1" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="AX1" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="AY1" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="2" spans="1:51" ht="77.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:51" ht="78.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -2952,13 +2958,13 @@
         <v>20</v>
       </c>
       <c r="G2" s="121" t="s">
+        <v>310</v>
+      </c>
+      <c r="H2" s="121" t="s">
         <v>311</v>
       </c>
-      <c r="H2" s="121" t="s">
-        <v>312</v>
-      </c>
       <c r="I2" s="121" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J2" s="65" t="s">
         <v>80</v>
@@ -2988,7 +2994,7 @@
         <v>86</v>
       </c>
       <c r="S2" s="65" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T2" s="65" t="s">
         <v>80</v>
@@ -3018,7 +3024,7 @@
         <v>86</v>
       </c>
       <c r="AC2" s="65" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AD2" s="65" t="s">
         <v>91</v>
@@ -3027,67 +3033,67 @@
         <v>92</v>
       </c>
       <c r="AF2" s="65" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AG2" s="65" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AH2" s="65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AI2" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="AJ2" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="AJ2" s="65" t="s">
-        <v>314</v>
-      </c>
       <c r="AK2" s="65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AL2" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="AM2" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="AM2" s="65" t="s">
-        <v>314</v>
-      </c>
       <c r="AN2" s="65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AO2" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="AP2" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="AP2" s="65" t="s">
-        <v>314</v>
-      </c>
       <c r="AQ2" s="65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AR2" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="AS2" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="AS2" s="65" t="s">
-        <v>314</v>
-      </c>
       <c r="AT2" s="65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AU2" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="AV2" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="AV2" s="65" t="s">
-        <v>314</v>
-      </c>
       <c r="AW2" s="65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AX2" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="AY2" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="AY2" s="65" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3341,7 +3347,7 @@
         <v>1001250.3090024699</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>1199.1725344773329</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3647,7 +3653,7 @@
         <v>8.0912620107395146</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3800,7 +3806,7 @@
         <v>124.60248498831356</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3953,7 +3959,7 @@
         <v>1066.4787874782799</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -4106,7 +4112,7 @@
         <v>2.3217600680931635E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4259,7 +4265,7 @@
         <v>40.366758790864871</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -4412,7 +4418,7 @@
         <v>993.99652518923131</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -4565,7 +4571,7 @@
         <v>27.521187334987346</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -4718,7 +4724,7 @@
         <v>9.4662813685889695</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -4871,7 +4877,7 @@
         <v>1.8944508672117086</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -5024,7 +5030,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -5173,7 +5179,7 @@
         <v>0.51231387456148403</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -5322,7 +5328,7 @@
         <v>7.7002199380836189E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -5471,7 +5477,7 @@
         <v>0.11248755052026857</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -5620,7 +5626,7 @@
         <v>0.18912102284679677</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5785,7 +5791,7 @@
         <v>75019.638597761033</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -5881,11 +5887,11 @@
         <v>-76614.526624731123</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="P22" s="64"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -5909,10 +5915,10 @@
       <c r="Q23" s="141"/>
       <c r="R23" s="141"/>
       <c r="S23" s="35" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="T23" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="U23" s="35"/>
       <c r="V23" s="35"/>
@@ -5927,7 +5933,7 @@
         <v>90</v>
       </c>
       <c r="AI23" s="69" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AJ23" s="69"/>
       <c r="AK23" s="69"/>
@@ -5935,7 +5941,7 @@
       <c r="AM23" s="69"/>
       <c r="AN23" s="69"/>
       <c r="AO23" s="69" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AP23" s="69"/>
     </row>
@@ -5957,12 +5963,12 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="115"/>
       <c r="B1" s="62" t="s">
         <v>93</v>
@@ -5971,22 +5977,22 @@
         <v>94</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E1" s="62" t="s">
         <v>95</v>
       </c>
       <c r="F1" s="62" t="s">
+        <v>293</v>
+      </c>
+      <c r="G1" s="62" t="s">
         <v>294</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="H1" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="H1" s="62" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -6012,7 +6018,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -6038,9 +6044,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B4" s="40">
         <v>9.9999999999999995E-7</v>
@@ -6064,7 +6070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -6090,9 +6096,9 @@
         <v>2204.6226218487759</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B6" s="40">
         <v>1.102311310924388E-6</v>
@@ -6116,9 +6122,9 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B7">
         <v>1.102311310924388E-6</v>
@@ -6142,9 +6148,9 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B8">
         <v>9.9999999999999995E-7</v>
@@ -6181,9 +6187,9 @@
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>96</v>
       </c>
@@ -6203,7 +6209,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>97</v>
       </c>
@@ -6223,7 +6229,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="60" t="s">
         <v>98</v>
       </c>
@@ -6243,7 +6249,7 @@
         <v>28316.847000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="60" t="s">
         <v>99</v>
       </c>
@@ -6263,7 +6269,7 @@
         <v>28.316846999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="60" t="s">
         <v>100</v>
       </c>
@@ -6283,7 +6289,7 @@
         <v>7.4805211375990615</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="61" t="s">
         <v>101</v>
       </c>
@@ -6316,15 +6322,15 @@
       <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>102</v>
       </c>
@@ -6353,10 +6359,10 @@
         <v>110</v>
       </c>
       <c r="J1" s="126" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>103</v>
       </c>
@@ -6389,7 +6395,7 @@
         <v>122481433.6265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="60" t="s">
         <v>104</v>
       </c>
@@ -6422,7 +6428,7 @@
         <v>122481.4336265</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="60" t="s">
         <v>105</v>
       </c>
@@ -6455,7 +6461,7 @@
         <v>122.48143362649999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="60" t="s">
         <v>106</v>
       </c>
@@ -6488,7 +6494,7 @@
         <v>34022.620451805553</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="60" t="s">
         <v>107</v>
       </c>
@@ -6521,7 +6527,7 @@
         <v>34.022620451805558</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="60" t="s">
         <v>108</v>
       </c>
@@ -6553,7 +6559,7 @@
         <v>116090</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="60" t="s">
         <v>109</v>
       </c>
@@ -6586,7 +6592,7 @@
         <v>0.11609</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="61" t="s">
         <v>110</v>
       </c>
@@ -6619,9 +6625,9 @@
         <v>45.625085571947984</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="127" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B10" s="69">
         <f>1/J2</f>
@@ -6672,9 +6678,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="115" t="s">
         <v>111</v>
       </c>
@@ -6694,10 +6700,10 @@
         <v>116</v>
       </c>
       <c r="G1" s="62" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>112</v>
       </c>
@@ -6720,7 +6726,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>113</v>
       </c>
@@ -6743,7 +6749,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
         <v>114</v>
       </c>
@@ -6766,7 +6772,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>115</v>
       </c>
@@ -6789,7 +6795,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
         <v>116</v>
       </c>
@@ -6812,9 +6818,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B7">
         <v>6.2137273664980671E-7</v>
@@ -6844,17 +6850,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F07116-128C-456A-A5F4-E4321BD8FA65}">
   <dimension ref="A1:CA37"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AF13" sqref="AF13"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="93" t="s">
         <v>220</v>
       </c>
@@ -6865,9 +6871,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A2" s="94" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B2" s="2">
         <v>17919.85304059858</v>
@@ -6876,9 +6882,9 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A3" s="95" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B3" s="73">
         <v>14222.105587776652</v>
@@ -6887,7 +6893,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:79" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A5" s="75" t="s">
         <v>223</v>
       </c>
@@ -6976,13 +6982,13 @@
         <v>244</v>
       </c>
       <c r="AD5" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="AE5" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="AE5" s="17" t="s">
-        <v>299</v>
-      </c>
       <c r="AF5" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AG5" s="17" t="s">
         <v>245</v>
@@ -7032,65 +7038,65 @@
       <c r="AV5" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="AW5" s="17" t="s">
+      <c r="AW5" s="144" t="s">
+        <v>347</v>
+      </c>
+      <c r="AX5" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="AX5" s="17" t="s">
+      <c r="AY5" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="AY5" s="17" t="s">
+      <c r="AZ5" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="AZ5" s="17" t="s">
+      <c r="BA5" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="BA5" s="17" t="s">
+      <c r="BB5" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="BB5" s="17" t="s">
+      <c r="BC5" s="17" t="s">
         <v>266</v>
-      </c>
-      <c r="BC5" s="17" t="s">
-        <v>267</v>
       </c>
       <c r="BD5" s="17" t="s">
         <v>39</v>
       </c>
       <c r="BE5" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="BF5" s="17" t="s">
         <v>268</v>
-      </c>
-      <c r="BF5" s="17" t="s">
-        <v>269</v>
       </c>
       <c r="BG5" s="17" t="s">
         <v>42</v>
       </c>
       <c r="BH5" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI5" s="17" t="s">
         <v>270</v>
-      </c>
-      <c r="BI5" s="17" t="s">
-        <v>271</v>
       </c>
       <c r="BJ5" s="17" t="s">
         <v>204</v>
       </c>
       <c r="BK5" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="BL5" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="BL5" s="17" t="s">
+      <c r="BM5" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="BM5" s="17" t="s">
+      <c r="BN5" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="BN5" s="17" t="s">
+      <c r="BO5" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="BO5" s="17" t="s">
+      <c r="BP5" s="17" t="s">
         <v>276</v>
-      </c>
-      <c r="BP5" s="17" t="s">
-        <v>277</v>
       </c>
       <c r="BQ5" s="17" t="s">
         <v>143</v>
@@ -7099,36 +7105,36 @@
         <v>207</v>
       </c>
       <c r="BS5" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="BT5" s="17" t="s">
         <v>175</v>
       </c>
       <c r="BU5" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="BV5" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="BV5" s="17" t="s">
+      <c r="BW5" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="BW5" s="17" t="s">
+      <c r="BX5" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="BX5" s="17" t="s">
+      <c r="BY5" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="BY5" s="17" t="s">
+      <c r="BZ5" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="BZ5" s="17" t="s">
+      <c r="CA5" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="CA5" s="18" t="s">
+    </row>
+    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
+      <c r="A6" s="76" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
-        <v>286</v>
       </c>
       <c r="B6" s="77">
         <v>133526.27602620388</v>
@@ -7255,9 +7261,9 @@
       <c r="BZ6" s="9"/>
       <c r="CA6" s="83"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A7" s="76" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7" s="78">
         <v>22500</v>
@@ -7432,7 +7438,7 @@
       <c r="BZ7" s="9"/>
       <c r="CA7" s="83"/>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A8" s="76" t="s">
         <v>221</v>
       </c>
@@ -7669,7 +7675,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A9" s="87" t="s">
         <v>222</v>
       </c>
@@ -7798,17 +7804,17 @@
       <c r="BZ9" s="88"/>
       <c r="CA9" s="92"/>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
       <c r="B12" s="142" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="96" t="s">
         <v>290</v>
-      </c>
-      <c r="C12" s="96" t="s">
-        <v>291</v>
       </c>
       <c r="D12" s="97"/>
       <c r="E12" s="97"/>
@@ -7821,7 +7827,7 @@
       <c r="L12" s="97"/>
       <c r="M12" s="98"/>
     </row>
-    <row r="13" spans="1:79" ht="39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
       <c r="B13" s="143"/>
       <c r="C13" s="99" t="s">
         <v>1</v>
@@ -7833,7 +7839,7 @@
         <v>233</v>
       </c>
       <c r="F13" s="100" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G13" s="100" t="s">
         <v>150</v>
@@ -7857,7 +7863,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A14" s="110" t="s">
         <v>22</v>
       </c>
@@ -7898,7 +7904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A15" s="76" t="s">
         <v>23</v>
       </c>
@@ -7939,7 +7945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A16" s="76" t="s">
         <v>7</v>
       </c>
@@ -7980,7 +7986,7 @@
         <v>76.151387532990128</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="76" t="s">
         <v>24</v>
       </c>
@@ -8021,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="76" t="s">
         <v>25</v>
       </c>
@@ -8062,7 +8068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="76" t="s">
         <v>26</v>
       </c>
@@ -8103,7 +8109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -8144,7 +8150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
@@ -8185,7 +8191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="76" t="s">
         <v>29</v>
       </c>
@@ -8226,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="76" t="s">
         <v>30</v>
       </c>
@@ -8267,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="87" t="s">
         <v>31</v>
       </c>
@@ -8308,13 +8314,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="110"/>
       <c r="B25" s="142" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" s="96" t="s">
         <v>290</v>
-      </c>
-      <c r="C25" s="96" t="s">
-        <v>291</v>
       </c>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
@@ -8327,7 +8333,7 @@
       <c r="L25" s="97"/>
       <c r="M25" s="98"/>
     </row>
-    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="76"/>
       <c r="B26" s="143"/>
       <c r="C26" s="99" t="s">
@@ -8340,7 +8346,7 @@
         <v>233</v>
       </c>
       <c r="F26" s="100" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G26" s="100" t="s">
         <v>150</v>
@@ -8364,7 +8370,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="110" t="s">
         <v>22</v>
       </c>
@@ -8405,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="76" t="s">
         <v>23</v>
       </c>
@@ -8446,7 +8452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="76" t="s">
         <v>7</v>
       </c>
@@ -8487,7 +8493,7 @@
         <v>95.950748291567578</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="76" t="s">
         <v>24</v>
       </c>
@@ -8528,7 +8534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="76" t="s">
         <v>25</v>
       </c>
@@ -8569,7 +8575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="76" t="s">
         <v>26</v>
       </c>
@@ -8610,7 +8616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -8651,7 +8657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -8692,7 +8698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="76" t="s">
         <v>29</v>
       </c>
@@ -8733,7 +8739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="76" t="s">
         <v>30</v>
       </c>
@@ -8774,7 +8780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="87" t="s">
         <v>31</v>
       </c>
@@ -8832,9 +8838,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -8842,7 +8848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="112" t="s">
         <v>8</v>
       </c>
@@ -8853,7 +8859,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="112" t="s">
         <v>9</v>
       </c>
@@ -8864,7 +8870,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="112" t="s">
         <v>10</v>
       </c>
@@ -8875,7 +8881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="112" t="s">
         <v>11</v>
       </c>
@@ -8886,7 +8892,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="112" t="s">
         <v>12</v>
       </c>
@@ -8897,7 +8903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="112" t="s">
         <v>13</v>
       </c>
@@ -8922,12 +8928,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -8935,7 +8941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8946,7 +8952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -8957,7 +8963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -8968,7 +8974,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -8979,7 +8985,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -8990,7 +8996,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -9014,17 +9020,17 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -9032,31 +9038,31 @@
         <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H1" t="s">
         <v>242</v>
       </c>
       <c r="I1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J1" t="s">
         <v>338</v>
       </c>
-      <c r="J1" t="s">
-        <v>339</v>
-      </c>
       <c r="K1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M1" t="s">
         <v>22</v>
@@ -9092,10 +9098,10 @@
         <v>31</v>
       </c>
       <c r="X1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="118" t="s">
         <v>122</v>
       </c>
@@ -9127,49 +9133,49 @@
         <v>184</v>
       </c>
       <c r="K2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="R2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="U2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="V2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="W2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="X2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -9243,7 +9249,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -9317,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -9391,7 +9397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -9465,7 +9471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9539,7 +9545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -9613,7 +9619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -9687,7 +9693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -9761,7 +9767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -9835,7 +9841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -9909,7 +9915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -9983,7 +9989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -10057,7 +10063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -10131,7 +10137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -10205,7 +10211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -10279,7 +10285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -10353,7 +10359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10427,7 +10433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10501,7 +10507,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -10513,11 +10519,11 @@
       <c r="E22" s="141"/>
       <c r="F22" s="141"/>
       <c r="G22" s="35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H22" s="35"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -10531,7 +10537,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -10545,7 +10551,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -10559,7 +10565,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -10573,7 +10579,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -10587,7 +10593,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -10601,7 +10607,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -10615,7 +10621,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -10629,7 +10635,7 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -10643,7 +10649,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -10657,7 +10663,7 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -10671,7 +10677,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -10685,7 +10691,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -10717,20 +10723,20 @@
       <selection pane="topRight" activeCell="BO1" sqref="BO1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>71</v>
@@ -10760,7 +10766,7 @@
         <v>45</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M1" s="17" t="s">
         <v>46</v>
@@ -10772,7 +10778,7 @@
         <v>48</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q1" s="17" t="s">
         <v>49</v>
@@ -10799,7 +10805,7 @@
         <v>56</v>
       </c>
       <c r="Y1" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Z1" s="17" t="s">
         <v>57</v>
@@ -10814,7 +10820,7 @@
         <v>73</v>
       </c>
       <c r="AD1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AE1" t="s">
         <v>74</v>
@@ -10826,156 +10832,156 @@
         <v>89</v>
       </c>
       <c r="AH1" s="137" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AI1" s="117" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AJ1" s="137" t="s">
         <v>150</v>
       </c>
       <c r="AK1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AL1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AM1" s="124" t="s">
+        <v>324</v>
+      </c>
+      <c r="AN1" s="124" t="s">
         <v>325</v>
       </c>
-      <c r="AN1" s="124" t="s">
+      <c r="AO1" s="124" t="s">
         <v>326</v>
       </c>
-      <c r="AO1" s="124" t="s">
-        <v>327</v>
-      </c>
       <c r="AP1" s="124" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AQ1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AR1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AS1" t="s">
         <v>343</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>344</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>345</v>
       </c>
-      <c r="AU1" t="s">
-        <v>346</v>
-      </c>
       <c r="AV1" s="134" t="s">
+        <v>348</v>
+      </c>
+      <c r="AW1" s="134" t="s">
         <v>349</v>
       </c>
-      <c r="AW1" s="134" t="s">
+      <c r="AX1" s="134" t="s">
         <v>350</v>
       </c>
-      <c r="AX1" s="134" t="s">
+      <c r="AY1" s="135" t="s">
         <v>351</v>
       </c>
-      <c r="AY1" s="135" t="s">
+      <c r="AZ1" s="135" t="s">
         <v>352</v>
       </c>
-      <c r="AZ1" s="135" t="s">
+      <c r="BA1" s="135" t="s">
         <v>353</v>
       </c>
-      <c r="BA1" s="135" t="s">
+      <c r="BB1" s="135" t="s">
         <v>354</v>
       </c>
-      <c r="BB1" s="135" t="s">
+      <c r="BC1" s="135" t="s">
         <v>355</v>
       </c>
-      <c r="BC1" s="135" t="s">
+      <c r="BD1" s="135" t="s">
         <v>356</v>
       </c>
-      <c r="BD1" s="135" t="s">
+      <c r="BE1" s="135" t="s">
         <v>357</v>
       </c>
-      <c r="BE1" s="135" t="s">
+      <c r="BF1" s="135" t="s">
         <v>358</v>
       </c>
-      <c r="BF1" s="135" t="s">
+      <c r="BG1" s="135" t="s">
         <v>359</v>
       </c>
-      <c r="BG1" s="135" t="s">
+      <c r="BH1" s="135" t="s">
         <v>360</v>
       </c>
-      <c r="BH1" s="135" t="s">
+      <c r="BI1" s="135" t="s">
         <v>361</v>
       </c>
-      <c r="BI1" s="135" t="s">
+      <c r="BJ1" s="135" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK1" s="135" t="s">
         <v>362</v>
       </c>
-      <c r="BJ1" s="135" t="s">
-        <v>369</v>
-      </c>
-      <c r="BK1" s="135" t="s">
+      <c r="BL1" s="135" t="s">
         <v>363</v>
       </c>
-      <c r="BL1" s="135" t="s">
+      <c r="BM1" s="135" t="s">
         <v>364</v>
       </c>
-      <c r="BM1" s="135" t="s">
+      <c r="BN1" t="s">
         <v>365</v>
       </c>
-      <c r="BN1" t="s">
-        <v>366</v>
-      </c>
       <c r="BO1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="2" spans="1:67" ht="26.25" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F2" s="129" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P2" s="65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q2" s="65" t="s">
         <v>2</v>
@@ -10993,34 +10999,34 @@
         <v>2</v>
       </c>
       <c r="V2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="W2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="X2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Y2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AA2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AB2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AC2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AD2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AF2" s="119" t="s">
         <v>219</v>
@@ -11032,106 +11038,106 @@
         <v>184</v>
       </c>
       <c r="AI2" s="117" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AJ2" s="137" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AK2" s="117" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AL2" s="117" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AM2" s="117" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AN2" s="117" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AO2" s="117" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AP2" s="117" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AQ2" s="117" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AR2" s="117" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AS2" s="117" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AT2" s="117" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AU2" s="117" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AW2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AX2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AY2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AZ2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BA2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BB2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BC2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BD2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BE2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BF2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BG2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BH2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BI2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BJ2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BK2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BL2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BM2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BN2" s="119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BO2" s="119" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -11334,7 +11340,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -11537,7 +11543,7 @@
         <v>9.9750188696234865</v>
       </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -11740,7 +11746,7 @@
         <v>9.9099322935660243</v>
       </c>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -11943,7 +11949,7 @@
         <v>9.314408223966951E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -12146,7 +12152,7 @@
         <v>8.6071446539691561</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -12349,7 +12355,7 @@
         <v>1.2096435573571984</v>
       </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -12552,7 +12558,7 @@
         <v>1.2210379021022032E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>59</v>
       </c>
@@ -12590,7 +12596,7 @@
       <c r="AI10" s="26"/>
       <c r="AJ10" s="137"/>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>60</v>
       </c>
@@ -12793,7 +12799,7 @@
         <v>1.1708326982510144E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -12996,7 +13002,7 @@
         <v>1.3246978822933949E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -13199,7 +13205,7 @@
         <v>1.813605257613188E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -13402,7 +13408,7 @@
         <v>7.6792485564078277E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -13605,7 +13611,7 @@
         <v>6.6674042219136396E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -13808,7 +13814,7 @@
         <v>5.5307439159581304E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>66</v>
       </c>
@@ -14011,7 +14017,7 @@
         <v>1.0214514606039252E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>67</v>
       </c>
@@ -14214,7 +14220,7 @@
         <v>2.6458634401739373E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>68</v>
       </c>
@@ -14417,7 +14423,7 @@
         <v>1.7288576101387265E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -14620,7 +14626,7 @@
         <v>3.6636240073674802E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
         <v>70</v>
       </c>
@@ -14823,11 +14829,11 @@
         <v>0.88119803944701025</v>
       </c>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:67" x14ac:dyDescent="0.35">
       <c r="AH22" s="137"/>
       <c r="AJ22" s="137"/>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -14865,106 +14871,106 @@
       <c r="AE23" s="141"/>
       <c r="AF23" s="141"/>
       <c r="AH23" s="137" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AJ23" s="137" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AL23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AM23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AN23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AO23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AP23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AQ23" t="s">
+        <v>346</v>
+      </c>
+      <c r="AR23" t="s">
         <v>347</v>
       </c>
-      <c r="AR23" t="s">
-        <v>348</v>
-      </c>
       <c r="AS23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AT23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AU23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AV23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AW23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AX23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AY23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AZ23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BA23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BB23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BC23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BD23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BE23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BF23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BG23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BH23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BI23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BJ23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BK23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BL23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BM23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BN23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BO23" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="27" spans="1:67" x14ac:dyDescent="0.35">
       <c r="AR27">
         <v>99</v>
       </c>
@@ -14986,9 +14992,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -14996,7 +15002,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -15005,7 +15011,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -15014,7 +15020,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -15023,7 +15029,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -15032,7 +15038,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="34" t="s">
         <v>79</v>
       </c>
@@ -15053,9 +15059,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -15105,7 +15111,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="78.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -15155,7 +15161,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -15208,7 +15214,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="112" t="s">
         <v>8</v>
       </c>
@@ -15259,7 +15265,7 @@
       </c>
       <c r="Q4" s="114"/>
     </row>
-    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="112" t="s">
         <v>9</v>
       </c>
@@ -15310,7 +15316,7 @@
       </c>
       <c r="Q5" s="114"/>
     </row>
-    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="112" t="s">
         <v>10</v>
       </c>
@@ -15361,7 +15367,7 @@
       </c>
       <c r="Q6" s="114"/>
     </row>
-    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="112" t="s">
         <v>11</v>
       </c>
@@ -15412,7 +15418,7 @@
       </c>
       <c r="Q7" s="114"/>
     </row>
-    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="112" t="s">
         <v>12</v>
       </c>
@@ -15463,7 +15469,7 @@
       </c>
       <c r="Q8" s="114"/>
     </row>
-    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="112" t="s">
         <v>13</v>
       </c>
@@ -15514,7 +15520,7 @@
       </c>
       <c r="Q9" s="114"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -15565,7 +15571,7 @@
       </c>
       <c r="Q10" s="67"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -15616,7 +15622,7 @@
       </c>
       <c r="Q11" s="67"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -15667,7 +15673,7 @@
       </c>
       <c r="Q12" s="67"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -15718,7 +15724,7 @@
       </c>
       <c r="Q13" s="67"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -15769,7 +15775,7 @@
       </c>
       <c r="Q14" s="67"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -15820,7 +15826,7 @@
       </c>
       <c r="Q15" s="67"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -15871,7 +15877,7 @@
       </c>
       <c r="Q16" s="67"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -15922,7 +15928,7 @@
       </c>
       <c r="Q17" s="67"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -15973,7 +15979,7 @@
       </c>
       <c r="Q18" s="67"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -16024,7 +16030,7 @@
       </c>
       <c r="Q19" s="67"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -16079,7 +16085,7 @@
         <v>3.3478260869565215</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -16093,11 +16099,11 @@
       <c r="N21" s="64"/>
       <c r="O21" s="64"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="M22" s="64"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -16139,51 +16145,51 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1" t="s">
         <v>298</v>
       </c>
-      <c r="C1" t="s">
-        <v>299</v>
-      </c>
       <c r="D1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -16197,7 +16203,7 @@
         <v>362403.00757167325</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -16211,7 +16217,7 @@
         <v>344979.42656462023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -16225,7 +16231,7 @@
         <v>24381.856026689315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -16239,7 +16245,7 @@
         <v>254462.26606022959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -16253,7 +16259,7 @@
         <v>66135.304477701342</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -16267,7 +16273,7 @@
         <v>59.889274923371126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -16281,7 +16287,7 @@
         <v>24.470884336712146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -16295,7 +16301,7 @@
         <v>34.134614130073174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -16309,7 +16315,7 @@
         <v>-15.759603589368934</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -16323,7 +16329,7 @@
         <v>8.6858851249063438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -16337,7 +16343,7 @@
         <v>6.9883164862451217</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -16351,7 +16357,7 @@
         <v>58.328462296040968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -16365,7 +16371,7 @@
         <v>0.49662761207225459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -16379,7 +16385,7 @@
         <v>1.1283578872130025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -16393,7 +16399,7 @@
         <v>57.127332585038609</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -16407,7 +16413,7 @@
         <v>-82.715827114534676</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -16421,7 +16427,7 @@
         <v>22763.019075759898</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -16445,9 +16451,9 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -16455,7 +16461,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -16463,7 +16469,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -16471,15 +16477,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -16487,15 +16493,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
         <v>97</v>
       </c>
@@ -16503,7 +16509,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
         <v>98</v>
       </c>
@@ -16511,7 +16517,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="62" t="s">
         <v>99</v>
       </c>
@@ -16519,7 +16525,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="62" t="s">
         <v>100</v>
       </c>
@@ -16527,7 +16533,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
         <v>101</v>
       </c>
@@ -16535,7 +16541,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="62" t="s">
         <v>103</v>
       </c>
@@ -16543,7 +16549,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="62" t="s">
         <v>104</v>
       </c>
@@ -16551,7 +16557,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="62" t="s">
         <v>105</v>
       </c>
@@ -16559,7 +16565,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="62" t="s">
         <v>106</v>
       </c>
@@ -16567,7 +16573,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="62" t="s">
         <v>107</v>
       </c>
@@ -16575,7 +16581,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="62" t="s">
         <v>108</v>
       </c>
@@ -16583,7 +16589,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="62" t="s">
         <v>109</v>
       </c>
@@ -16591,7 +16597,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="62" t="s">
         <v>110</v>
       </c>
@@ -16599,15 +16605,15 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="126" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B20" s="69" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="62" t="s">
         <v>112</v>
       </c>
@@ -16615,7 +16621,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="62" t="s">
         <v>113</v>
       </c>
@@ -16623,7 +16629,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="62" t="s">
         <v>114</v>
       </c>
@@ -16631,7 +16637,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="62" t="s">
         <v>115</v>
       </c>
@@ -16639,7 +16645,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="62" t="s">
         <v>116</v>
       </c>
@@ -16660,12 +16666,12 @@
       <selection activeCell="A45" sqref="A45:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="68" t="s">
         <v>186</v>
       </c>
@@ -16673,7 +16679,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -16684,7 +16690,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -16695,7 +16701,7 @@
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="69" t="s">
         <v>127</v>
       </c>
@@ -16706,7 +16712,7 @@
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="69" t="s">
         <v>128</v>
       </c>
@@ -16717,7 +16723,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="69" t="s">
         <v>129</v>
       </c>
@@ -16728,7 +16734,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="69" t="s">
         <v>130</v>
       </c>
@@ -16739,7 +16745,7 @@
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="69" t="s">
         <v>131</v>
       </c>
@@ -16750,7 +16756,7 @@
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="69" t="s">
         <v>132</v>
       </c>
@@ -16761,7 +16767,7 @@
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="69" t="s">
         <v>133</v>
       </c>
@@ -16772,7 +16778,7 @@
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="69" t="s">
         <v>134</v>
       </c>
@@ -16783,7 +16789,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -16794,7 +16800,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="69" t="s">
         <v>136</v>
       </c>
@@ -16805,7 +16811,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="69" t="s">
         <v>137</v>
       </c>
@@ -16816,7 +16822,7 @@
         <v>755.86244135709444</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="69" t="s">
         <v>138</v>
       </c>
@@ -16827,7 +16833,7 @@
         <v>762.55920427134606</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="69" t="s">
         <v>139</v>
       </c>
@@ -16838,7 +16844,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="69" t="s">
         <v>140</v>
       </c>
@@ -16849,7 +16855,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="69" t="s">
         <v>141</v>
       </c>
@@ -16860,7 +16866,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="68" t="s">
         <v>1</v>
       </c>
@@ -16871,7 +16877,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -16882,7 +16888,7 @@
         <v>725.15243391008278</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -16893,7 +16899,7 @@
         <v>748.62596861099109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -16904,7 +16910,7 @@
         <v>801.99999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -16915,7 +16921,7 @@
         <v>791.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -16926,7 +16932,7 @@
         <v>700.32025584540236</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -16937,7 +16943,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -16948,7 +16954,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -16959,7 +16965,7 @@
         <v>794.1013538556316</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -16970,7 +16976,7 @@
         <v>789.34625592835232</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -16981,7 +16987,7 @@
         <v>809.68750817282455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -16992,7 +16998,7 @@
         <v>783.00612535864673</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -17003,7 +17009,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -17014,7 +17020,7 @@
         <v>508.00296189766453</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>155</v>
       </c>
@@ -17025,7 +17031,7 @@
         <v>428.22298556220187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -17036,7 +17042,7 @@
         <v>665.18536560495022</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -17047,7 +17053,7 @@
         <v>859.88020851632757</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -17058,7 +17064,7 @@
         <v>887.88245186586084</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -17069,7 +17075,7 @@
         <v>797.00724703341325</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -17080,7 +17086,7 @@
         <v>748.92792354647884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -17091,7 +17097,7 @@
         <v>778.77937164550963</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>162</v>
       </c>
@@ -17102,7 +17108,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -17113,7 +17119,7 @@
         <v>798.04417121416941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -17124,9 +17130,9 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B43" s="69">
         <v>44.291949816853993</v>
@@ -17135,9 +17141,9 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B44" s="69">
         <v>43.995102738357922</v>
@@ -17146,9 +17152,9 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B45" s="69">
         <v>43.975450721892244</v>
@@ -17157,9 +17163,9 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B46" s="69">
         <v>43.819577184272568</v>
@@ -17168,7 +17174,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>164</v>
       </c>
@@ -17179,7 +17185,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>165</v>
       </c>
@@ -17190,7 +17196,7 @@
         <v>716.69892648380858</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>166</v>
       </c>
@@ -17201,7 +17207,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>167</v>
       </c>
@@ -17212,7 +17218,7 @@
         <v>756.99999999999989</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -17223,7 +17229,7 @@
         <v>70.798124695046326</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -17234,7 +17240,7 @@
         <v>742.58779297677324</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -17245,7 +17251,7 @@
         <v>742.32362086970215</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -17256,7 +17262,7 @@
         <v>769.53334789802227</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -17267,7 +17273,7 @@
         <v>584.61287294827434</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>173</v>
       </c>
@@ -17278,7 +17284,7 @@
         <v>559.51652277652283</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -17289,7 +17295,7 @@
         <v>595.17975723111715</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -17300,7 +17306,7 @@
         <v>507.21044557645126</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>176</v>
       </c>
@@ -17311,7 +17317,7 @@
         <v>668.88377510394514</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>177</v>
       </c>
@@ -17322,7 +17328,7 @@
         <v>654.80340179705718</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>178</v>
       </c>
@@ -17333,7 +17339,7 @@
         <v>688.85095964480468</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -17344,7 +17350,7 @@
         <v>737.59071339941693</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>180</v>
       </c>
@@ -17355,7 +17361,7 @@
         <v>765.47381512866104</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -17366,7 +17372,7 @@
         <v>731.67589538225809</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>182</v>
       </c>
@@ -17377,7 +17383,7 @@
         <v>800.00032424653136</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>183</v>
       </c>
@@ -17388,7 +17394,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -17399,7 +17405,7 @@
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>188</v>
       </c>
@@ -17410,7 +17416,7 @@
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="68" t="s">
         <v>89</v>
       </c>
@@ -17421,9 +17427,9 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="140" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B70" s="137">
         <v>119.98674372549019</v>
@@ -17432,7 +17438,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -17443,7 +17449,7 @@
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -17454,7 +17460,7 @@
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -17462,7 +17468,7 @@
         <v>22.648458746153963</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>192</v>
       </c>
@@ -17470,7 +17476,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>193</v>
       </c>
@@ -17478,7 +17484,7 @@
         <v>18.707371337693861</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>194</v>
       </c>
@@ -17486,7 +17492,7 @@
         <v>12.566427590816895</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>195</v>
       </c>
@@ -17494,7 +17500,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -17502,7 +17508,7 @@
         <v>11.566786665057547</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>197</v>
       </c>
@@ -17510,7 +17516,7 @@
         <v>31.342185540824094</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>198</v>
       </c>
@@ -17518,7 +17524,7 @@
         <v>31.0106439692332</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>199</v>
       </c>
@@ -17526,7 +17532,7 @@
         <v>28.609127685562171</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>200</v>
       </c>
@@ -17534,7 +17540,7 @@
         <v>33.012627597074328</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>201</v>
       </c>
@@ -17542,7 +17548,7 @@
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>202</v>
       </c>
@@ -17550,7 +17556,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -17558,7 +17564,7 @@
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>204</v>
       </c>
@@ -17566,7 +17572,7 @@
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>205</v>
       </c>
@@ -17574,7 +17580,7 @@
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>206</v>
       </c>
@@ -17582,7 +17588,7 @@
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>207</v>
       </c>
@@ -17590,7 +17596,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>208</v>
       </c>
@@ -17598,7 +17604,7 @@
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -17606,7 +17612,7 @@
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>210</v>
       </c>
@@ -17614,7 +17620,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>211</v>
       </c>
@@ -17622,7 +17628,7 @@
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>212</v>
       </c>
@@ -17630,7 +17636,7 @@
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>213</v>
       </c>
@@ -17638,7 +17644,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>214</v>
       </c>
@@ -17646,7 +17652,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>215</v>
       </c>
@@ -17654,7 +17660,7 @@
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>216</v>
       </c>
@@ -17662,7 +17668,7 @@
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="68" t="s">
         <v>219</v>
       </c>
@@ -17670,7 +17676,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Adding the algae HTL pathway ... continued
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B18F0DF-5C29-4270-97F5-742394E2AEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21175302-5B51-4165-B5DC-117117F30EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" activeTab="13" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="375">
   <si>
     <t>NG</t>
   </si>
@@ -1427,6 +1427,12 @@
   </si>
   <si>
     <t>Renewable Diesel - Algae (Acids)</t>
+  </si>
+  <si>
+    <t>MgO</t>
+  </si>
+  <si>
+    <t>NaCl</t>
   </si>
 </sst>
 </file>
@@ -2046,6 +2052,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2054,9 +2063,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2782,14 +2788,14 @@
       <selection pane="topRight" activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="122"/>
-    <col min="41" max="41" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="122"/>
+    <col min="41" max="41" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2941,7 +2947,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -3093,7 +3099,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3194,7 +3200,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3347,7 +3353,7 @@
         <v>1001250.3090024699</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3500,7 +3506,7 @@
         <v>1199.1725344773329</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3653,7 +3659,7 @@
         <v>8.0912620107395146</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3806,7 +3812,7 @@
         <v>124.60248498831356</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3959,7 +3965,7 @@
         <v>1066.4787874782799</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -4112,7 +4118,7 @@
         <v>2.3217600680931635E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4265,7 +4271,7 @@
         <v>40.366758790864871</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -4418,7 +4424,7 @@
         <v>993.99652518923131</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -4571,7 +4577,7 @@
         <v>27.521187334987346</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -4724,7 +4730,7 @@
         <v>9.4662813685889695</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -4877,7 +4883,7 @@
         <v>1.8944508672117086</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -5030,7 +5036,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -5179,7 +5185,7 @@
         <v>0.51231387456148403</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -5328,7 +5334,7 @@
         <v>7.7002199380836189E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -5477,7 +5483,7 @@
         <v>0.11248755052026857</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -5626,7 +5632,7 @@
         <v>0.18912102284679677</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5791,7 +5797,7 @@
         <v>75019.638597761033</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -5887,33 +5893,33 @@
         <v>-76614.526624731123</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="P22" s="64"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="141" t="s">
+      <c r="B23" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
-      <c r="J23" s="141"/>
-      <c r="K23" s="141"/>
-      <c r="L23" s="141"/>
-      <c r="M23" s="141"/>
-      <c r="N23" s="141"/>
-      <c r="O23" s="141"/>
-      <c r="P23" s="141"/>
-      <c r="Q23" s="141"/>
-      <c r="R23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="142"/>
+      <c r="J23" s="142"/>
+      <c r="K23" s="142"/>
+      <c r="L23" s="142"/>
+      <c r="M23" s="142"/>
+      <c r="N23" s="142"/>
+      <c r="O23" s="142"/>
+      <c r="P23" s="142"/>
+      <c r="Q23" s="142"/>
+      <c r="R23" s="142"/>
       <c r="S23" s="35" t="s">
         <v>329</v>
       </c>
@@ -5963,12 +5969,12 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="115"/>
       <c r="B1" s="62" t="s">
         <v>93</v>
@@ -5992,7 +5998,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -6018,7 +6024,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -6044,7 +6050,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>335</v>
       </c>
@@ -6070,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -6096,7 +6102,7 @@
         <v>2204.6226218487759</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>293</v>
       </c>
@@ -6122,7 +6128,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>294</v>
       </c>
@@ -6148,7 +6154,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>295</v>
       </c>
@@ -6187,9 +6193,9 @@
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>96</v>
       </c>
@@ -6209,7 +6215,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>97</v>
       </c>
@@ -6229,7 +6235,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>98</v>
       </c>
@@ -6249,7 +6255,7 @@
         <v>28316.847000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>99</v>
       </c>
@@ -6269,7 +6275,7 @@
         <v>28.316846999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>100</v>
       </c>
@@ -6289,7 +6295,7 @@
         <v>7.4805211375990615</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>101</v>
       </c>
@@ -6322,15 +6328,15 @@
       <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>102</v>
       </c>
@@ -6362,7 +6368,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>103</v>
       </c>
@@ -6395,7 +6401,7 @@
         <v>122481433.6265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>104</v>
       </c>
@@ -6428,7 +6434,7 @@
         <v>122481.4336265</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>105</v>
       </c>
@@ -6461,7 +6467,7 @@
         <v>122.48143362649999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>106</v>
       </c>
@@ -6494,7 +6500,7 @@
         <v>34022.620451805553</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>107</v>
       </c>
@@ -6527,7 +6533,7 @@
         <v>34.022620451805558</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
         <v>108</v>
       </c>
@@ -6559,7 +6565,7 @@
         <v>116090</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
         <v>109</v>
       </c>
@@ -6592,7 +6598,7 @@
         <v>0.11609</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
         <v>110</v>
       </c>
@@ -6625,7 +6631,7 @@
         <v>45.625085571947984</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="127" t="s">
         <v>336</v>
       </c>
@@ -6678,9 +6684,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="115" t="s">
         <v>111</v>
       </c>
@@ -6703,7 +6709,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>112</v>
       </c>
@@ -6726,7 +6732,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>113</v>
       </c>
@@ -6749,7 +6755,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>114</v>
       </c>
@@ -6772,7 +6778,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>115</v>
       </c>
@@ -6795,7 +6801,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>116</v>
       </c>
@@ -6818,7 +6824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>296</v>
       </c>
@@ -6850,17 +6856,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F07116-128C-456A-A5F4-E4321BD8FA65}">
   <dimension ref="A1:CA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
         <v>220</v>
       </c>
@@ -6871,7 +6877,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A2" s="94" t="s">
         <v>287</v>
       </c>
@@ -6882,7 +6888,7 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
         <v>288</v>
       </c>
@@ -6893,7 +6899,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:79" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A5" s="75" t="s">
         <v>223</v>
       </c>
@@ -7038,7 +7044,7 @@
       <c r="AV5" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="AW5" s="144" t="s">
+      <c r="AW5" s="141" t="s">
         <v>347</v>
       </c>
       <c r="AX5" s="17" t="s">
@@ -7132,7 +7138,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
         <v>285</v>
       </c>
@@ -7261,7 +7267,7 @@
       <c r="BZ6" s="9"/>
       <c r="CA6" s="83"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>286</v>
       </c>
@@ -7438,7 +7444,7 @@
       <c r="BZ7" s="9"/>
       <c r="CA7" s="83"/>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
         <v>221</v>
       </c>
@@ -7675,7 +7681,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A9" s="87" t="s">
         <v>222</v>
       </c>
@@ -7804,13 +7810,13 @@
       <c r="BZ9" s="88"/>
       <c r="CA9" s="92"/>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
-      <c r="B12" s="142" t="s">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="B12" s="143" t="s">
         <v>289</v>
       </c>
       <c r="C12" s="96" t="s">
@@ -7827,8 +7833,8 @@
       <c r="L12" s="97"/>
       <c r="M12" s="98"/>
     </row>
-    <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="143"/>
+    <row r="13" spans="1:79" ht="39" x14ac:dyDescent="0.25">
+      <c r="B13" s="144"/>
       <c r="C13" s="99" t="s">
         <v>1</v>
       </c>
@@ -7863,7 +7869,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A14" s="110" t="s">
         <v>22</v>
       </c>
@@ -7904,7 +7910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A15" s="76" t="s">
         <v>23</v>
       </c>
@@ -7945,7 +7951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A16" s="76" t="s">
         <v>7</v>
       </c>
@@ -7986,7 +7992,7 @@
         <v>76.151387532990128</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="76" t="s">
         <v>24</v>
       </c>
@@ -8027,7 +8033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="76" t="s">
         <v>25</v>
       </c>
@@ -8068,7 +8074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="76" t="s">
         <v>26</v>
       </c>
@@ -8109,7 +8115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -8150,7 +8156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
@@ -8191,7 +8197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="76" t="s">
         <v>29</v>
       </c>
@@ -8232,7 +8238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="76" t="s">
         <v>30</v>
       </c>
@@ -8273,7 +8279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="87" t="s">
         <v>31</v>
       </c>
@@ -8314,9 +8320,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="110"/>
-      <c r="B25" s="142" t="s">
+      <c r="B25" s="143" t="s">
         <v>289</v>
       </c>
       <c r="C25" s="96" t="s">
@@ -8333,9 +8339,9 @@
       <c r="L25" s="97"/>
       <c r="M25" s="98"/>
     </row>
-    <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A26" s="76"/>
-      <c r="B26" s="143"/>
+      <c r="B26" s="144"/>
       <c r="C26" s="99" t="s">
         <v>1</v>
       </c>
@@ -8370,7 +8376,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="110" t="s">
         <v>22</v>
       </c>
@@ -8411,7 +8417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="76" t="s">
         <v>23</v>
       </c>
@@ -8452,7 +8458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="76" t="s">
         <v>7</v>
       </c>
@@ -8493,7 +8499,7 @@
         <v>95.950748291567578</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="76" t="s">
         <v>24</v>
       </c>
@@ -8534,7 +8540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="76" t="s">
         <v>25</v>
       </c>
@@ -8575,7 +8581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="76" t="s">
         <v>26</v>
       </c>
@@ -8616,7 +8622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -8657,7 +8663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -8698,7 +8704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="76" t="s">
         <v>29</v>
       </c>
@@ -8739,7 +8745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="76" t="s">
         <v>30</v>
       </c>
@@ -8780,7 +8786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="87" t="s">
         <v>31</v>
       </c>
@@ -8838,9 +8844,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -8848,7 +8854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="112" t="s">
         <v>8</v>
       </c>
@@ -8859,7 +8865,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="112" t="s">
         <v>9</v>
       </c>
@@ -8870,7 +8876,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="112" t="s">
         <v>10</v>
       </c>
@@ -8881,7 +8887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>11</v>
       </c>
@@ -8892,7 +8898,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
         <v>12</v>
       </c>
@@ -8903,7 +8909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
         <v>13</v>
       </c>
@@ -8928,12 +8934,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -8941,7 +8947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8952,7 +8958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -8963,7 +8969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -8974,7 +8980,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -8985,7 +8991,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -8996,7 +9002,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -9020,17 +9026,17 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -9101,7 +9107,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="118" t="s">
         <v>122</v>
       </c>
@@ -9175,7 +9181,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -9249,7 +9255,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -9323,7 +9329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -9397,7 +9403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -9471,7 +9477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9545,7 +9551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -9619,7 +9625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -9693,7 +9699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -9767,7 +9773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -9841,7 +9847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -9915,7 +9921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -9989,7 +9995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -10063,7 +10069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -10137,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -10211,7 +10217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -10285,7 +10291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -10359,7 +10365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10433,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10507,23 +10513,23 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="141" t="s">
+      <c r="B22" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="141"/>
-      <c r="F22" s="141"/>
+      <c r="C22" s="142"/>
+      <c r="D22" s="142"/>
+      <c r="E22" s="142"/>
+      <c r="F22" s="142"/>
       <c r="G22" s="35" t="s">
         <v>333</v>
       </c>
       <c r="H22" s="35"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -10537,7 +10543,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -10551,7 +10557,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -10565,7 +10571,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -10579,7 +10585,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -10593,7 +10599,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -10607,7 +10613,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -10621,7 +10627,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -10635,7 +10641,7 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -10649,7 +10655,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -10663,7 +10669,7 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -10677,7 +10683,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -10691,7 +10697,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -10716,24 +10722,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
-  <dimension ref="A1:BO27"/>
+  <dimension ref="A1:BQ27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BO1" sqref="BO1"/>
+      <selection pane="topRight" activeCell="BQ23" sqref="BQ23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" customWidth="1"/>
-    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:69" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
         <v>308</v>
@@ -10933,8 +10939,14 @@
       <c r="BO1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP1" t="s">
+        <v>373</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2" spans="1:69" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
@@ -11136,8 +11148,14 @@
       <c r="BO2" s="119" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP2" s="119" t="s">
+        <v>305</v>
+      </c>
+      <c r="BQ2" s="119" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -11339,8 +11357,14 @@
       <c r="BO3" s="20" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ3" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -11542,8 +11566,14 @@
       <c r="BO4">
         <v>9.9750188696234865</v>
       </c>
-    </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP4">
+        <v>9.5108303722001502</v>
+      </c>
+      <c r="BQ4">
+        <v>3.2282836457015942</v>
+      </c>
+    </row>
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -11745,8 +11775,14 @@
       <c r="BO5">
         <v>9.9099322935660243</v>
       </c>
-    </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP5">
+        <v>9.5037991779901425</v>
+      </c>
+      <c r="BQ5">
+        <v>3.0728681340416055</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -11948,8 +11984,14 @@
       <c r="BO6">
         <v>9.314408223966951E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP6">
+        <v>9.814155860263277E-3</v>
+      </c>
+      <c r="BQ6">
+        <v>0.50413295762414023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -12151,8 +12193,14 @@
       <c r="BO7">
         <v>8.6071446539691561</v>
       </c>
-    </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP7">
+        <v>9.3789910121123334</v>
+      </c>
+      <c r="BQ7">
+        <v>1.5123986505927864</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -12354,8 +12402,14 @@
       <c r="BO8">
         <v>1.2096435573571984</v>
       </c>
-    </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP8">
+        <v>0.11499401001754572</v>
+      </c>
+      <c r="BQ8">
+        <v>1.0563365258246789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -12557,8 +12611,14 @@
       <c r="BO9">
         <v>1.2210379021022032E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP9">
+        <v>2.9151282887827102E-5</v>
+      </c>
+      <c r="BQ9">
+        <v>5.6136052454827743E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>59</v>
       </c>
@@ -12595,8 +12655,11 @@
       <c r="AH10" s="137"/>
       <c r="AI10" s="26"/>
       <c r="AJ10" s="137"/>
-    </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BQ10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>60</v>
       </c>
@@ -12798,8 +12861,14 @@
       <c r="BO11">
         <v>1.1708326982510144E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP11">
+        <v>1.1048894219065913E-4</v>
+      </c>
+      <c r="BQ11">
+        <v>6.0986993193583903E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -13001,8 +13070,14 @@
       <c r="BO12">
         <v>1.3246978822933949E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP12">
+        <v>4.8275492204424793E-4</v>
+      </c>
+      <c r="BQ12">
+        <v>2.0719796655857878E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -13204,8 +13279,14 @@
       <c r="BO13">
         <v>1.813605257613188E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP13">
+        <v>6.5001141161784726E-4</v>
+      </c>
+      <c r="BQ13">
+        <v>1.0111465275939799E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -13407,8 +13488,14 @@
       <c r="BO14">
         <v>7.6792485564078277E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP14">
+        <v>3.4079574042148611E-5</v>
+      </c>
+      <c r="BQ14">
+        <v>8.1861576543595249E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -13610,8 +13697,14 @@
       <c r="BO15">
         <v>6.6674042219136396E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP15">
+        <v>3.331330013852727E-5</v>
+      </c>
+      <c r="BQ15">
+        <v>7.181414584611474E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -13813,8 +13906,14 @@
       <c r="BO16">
         <v>5.5307439159581304E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP16">
+        <v>9.7559788461663695E-5</v>
+      </c>
+      <c r="BQ16">
+        <v>6.0405047745250632E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>66</v>
       </c>
@@ -14016,8 +14115,14 @@
       <c r="BO17">
         <v>1.0214514606039252E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP17">
+        <v>5.7981173811555583E-6</v>
+      </c>
+      <c r="BQ17">
+        <v>1.1211156972976533E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>67</v>
       </c>
@@ -14219,8 +14324,14 @@
       <c r="BO18">
         <v>2.6458634401739373E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP18">
+        <v>1.4054144835976559E-5</v>
+      </c>
+      <c r="BQ18">
+        <v>2.7441649209226465E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>68</v>
       </c>
@@ -14422,8 +14533,14 @@
       <c r="BO19">
         <v>1.7288576101387265E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP19">
+        <v>1.863156302317926E-3</v>
+      </c>
+      <c r="BQ19">
+        <v>4.5597517783716818E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -14625,8 +14742,14 @@
       <c r="BO20">
         <v>3.6636240073674802E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP20">
+        <v>1.6828234446617456E-5</v>
+      </c>
+      <c r="BQ20">
+        <v>4.7430396768858183E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>70</v>
       </c>
@@ -14828,48 +14951,54 @@
       <c r="BO21">
         <v>0.88119803944701025</v>
       </c>
-    </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP21">
+        <v>0.56574062825797522</v>
+      </c>
+      <c r="BQ21">
+        <v>0.22607654837045763</v>
+      </c>
+    </row>
+    <row r="22" spans="1:69" x14ac:dyDescent="0.25">
       <c r="AH22" s="137"/>
       <c r="AJ22" s="137"/>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="141" t="s">
+      <c r="B23" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
-      <c r="J23" s="141"/>
-      <c r="K23" s="141"/>
-      <c r="L23" s="141"/>
-      <c r="M23" s="141"/>
-      <c r="N23" s="141"/>
-      <c r="O23" s="141"/>
-      <c r="P23" s="141"/>
-      <c r="Q23" s="141"/>
-      <c r="R23" s="141"/>
-      <c r="S23" s="141"/>
-      <c r="T23" s="141"/>
-      <c r="U23" s="141"/>
-      <c r="V23" s="141"/>
-      <c r="W23" s="141"/>
-      <c r="X23" s="141"/>
-      <c r="Y23" s="141"/>
-      <c r="Z23" s="141"/>
-      <c r="AA23" s="141"/>
-      <c r="AB23" s="141"/>
-      <c r="AC23" s="141"/>
-      <c r="AD23" s="141"/>
-      <c r="AE23" s="141"/>
-      <c r="AF23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="142"/>
+      <c r="J23" s="142"/>
+      <c r="K23" s="142"/>
+      <c r="L23" s="142"/>
+      <c r="M23" s="142"/>
+      <c r="N23" s="142"/>
+      <c r="O23" s="142"/>
+      <c r="P23" s="142"/>
+      <c r="Q23" s="142"/>
+      <c r="R23" s="142"/>
+      <c r="S23" s="142"/>
+      <c r="T23" s="142"/>
+      <c r="U23" s="142"/>
+      <c r="V23" s="142"/>
+      <c r="W23" s="142"/>
+      <c r="X23" s="142"/>
+      <c r="Y23" s="142"/>
+      <c r="Z23" s="142"/>
+      <c r="AA23" s="142"/>
+      <c r="AB23" s="142"/>
+      <c r="AC23" s="142"/>
+      <c r="AD23" s="142"/>
+      <c r="AE23" s="142"/>
+      <c r="AF23" s="142"/>
       <c r="AH23" s="137" t="s">
         <v>367</v>
       </c>
@@ -14969,8 +15098,14 @@
       <c r="BO23" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BP23" t="s">
+        <v>347</v>
+      </c>
+      <c r="BQ23" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:69" x14ac:dyDescent="0.25">
       <c r="AR27">
         <v>99</v>
       </c>
@@ -14992,9 +15127,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -15002,7 +15137,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -15011,7 +15146,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -15020,7 +15155,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -15029,7 +15164,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -15038,7 +15173,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>79</v>
       </c>
@@ -15059,9 +15194,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -15111,7 +15246,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -15161,7 +15296,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -15214,7 +15349,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="112" t="s">
         <v>8</v>
       </c>
@@ -15265,7 +15400,7 @@
       </c>
       <c r="Q4" s="114"/>
     </row>
-    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>9</v>
       </c>
@@ -15316,7 +15451,7 @@
       </c>
       <c r="Q5" s="114"/>
     </row>
-    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
         <v>10</v>
       </c>
@@ -15367,7 +15502,7 @@
       </c>
       <c r="Q6" s="114"/>
     </row>
-    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
         <v>11</v>
       </c>
@@ -15418,7 +15553,7 @@
       </c>
       <c r="Q7" s="114"/>
     </row>
-    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="112" t="s">
         <v>12</v>
       </c>
@@ -15469,7 +15604,7 @@
       </c>
       <c r="Q8" s="114"/>
     </row>
-    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="112" t="s">
         <v>13</v>
       </c>
@@ -15520,7 +15655,7 @@
       </c>
       <c r="Q9" s="114"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -15571,7 +15706,7 @@
       </c>
       <c r="Q10" s="67"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -15622,7 +15757,7 @@
       </c>
       <c r="Q11" s="67"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -15673,7 +15808,7 @@
       </c>
       <c r="Q12" s="67"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -15724,7 +15859,7 @@
       </c>
       <c r="Q13" s="67"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -15775,7 +15910,7 @@
       </c>
       <c r="Q14" s="67"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -15826,7 +15961,7 @@
       </c>
       <c r="Q15" s="67"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -15877,7 +16012,7 @@
       </c>
       <c r="Q16" s="67"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -15928,7 +16063,7 @@
       </c>
       <c r="Q17" s="67"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -15979,7 +16114,7 @@
       </c>
       <c r="Q18" s="67"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -16030,7 +16165,7 @@
       </c>
       <c r="Q19" s="67"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -16085,7 +16220,7 @@
         <v>3.3478260869565215</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -16099,30 +16234,30 @@
       <c r="N21" s="64"/>
       <c r="O21" s="64"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="M22" s="64"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="141" t="s">
+      <c r="B23" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
-      <c r="J23" s="141"/>
-      <c r="K23" s="141"/>
-      <c r="L23" s="141"/>
-      <c r="M23" s="141"/>
-      <c r="N23" s="141"/>
-      <c r="O23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="142"/>
+      <c r="J23" s="142"/>
+      <c r="K23" s="142"/>
+      <c r="L23" s="142"/>
+      <c r="M23" s="142"/>
+      <c r="N23" s="142"/>
+      <c r="O23" s="142"/>
       <c r="P23" t="s">
         <v>90</v>
       </c>
@@ -16145,12 +16280,12 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>297</v>
       </c>
@@ -16161,7 +16296,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -16175,7 +16310,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -16189,7 +16324,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -16203,7 +16338,7 @@
         <v>362403.00757167325</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -16217,7 +16352,7 @@
         <v>344979.42656462023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -16231,7 +16366,7 @@
         <v>24381.856026689315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -16245,7 +16380,7 @@
         <v>254462.26606022959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -16259,7 +16394,7 @@
         <v>66135.304477701342</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -16273,7 +16408,7 @@
         <v>59.889274923371126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -16287,7 +16422,7 @@
         <v>24.470884336712146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -16301,7 +16436,7 @@
         <v>34.134614130073174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -16315,7 +16450,7 @@
         <v>-15.759603589368934</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -16329,7 +16464,7 @@
         <v>8.6858851249063438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -16343,7 +16478,7 @@
         <v>6.9883164862451217</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -16357,7 +16492,7 @@
         <v>58.328462296040968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -16371,7 +16506,7 @@
         <v>0.49662761207225459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -16385,7 +16520,7 @@
         <v>1.1283578872130025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -16399,7 +16534,7 @@
         <v>57.127332585038609</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -16413,7 +16548,7 @@
         <v>-82.715827114534676</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -16427,7 +16562,7 @@
         <v>22763.019075759898</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -16451,9 +16586,9 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -16461,7 +16596,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -16469,7 +16604,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -16477,7 +16612,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>335</v>
       </c>
@@ -16485,7 +16620,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -16493,7 +16628,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>293</v>
       </c>
@@ -16501,7 +16636,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>97</v>
       </c>
@@ -16509,7 +16644,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>98</v>
       </c>
@@ -16517,7 +16652,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>99</v>
       </c>
@@ -16525,7 +16660,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>100</v>
       </c>
@@ -16533,7 +16668,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>101</v>
       </c>
@@ -16541,7 +16676,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>103</v>
       </c>
@@ -16549,7 +16684,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>104</v>
       </c>
@@ -16557,7 +16692,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>105</v>
       </c>
@@ -16565,7 +16700,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
         <v>106</v>
       </c>
@@ -16573,7 +16708,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="s">
         <v>107</v>
       </c>
@@ -16581,7 +16716,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>108</v>
       </c>
@@ -16589,7 +16724,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>109</v>
       </c>
@@ -16597,7 +16732,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>110</v>
       </c>
@@ -16605,7 +16740,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="126" t="s">
         <v>336</v>
       </c>
@@ -16613,7 +16748,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>112</v>
       </c>
@@ -16621,7 +16756,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="s">
         <v>113</v>
       </c>
@@ -16629,7 +16764,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="62" t="s">
         <v>114</v>
       </c>
@@ -16637,7 +16772,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>115</v>
       </c>
@@ -16645,7 +16780,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
         <v>116</v>
       </c>
@@ -16666,12 +16801,12 @@
       <selection activeCell="A45" sqref="A45:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="68" t="s">
         <v>186</v>
       </c>
@@ -16679,7 +16814,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -16690,7 +16825,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -16701,7 +16836,7 @@
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
         <v>127</v>
       </c>
@@ -16712,7 +16847,7 @@
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
         <v>128</v>
       </c>
@@ -16723,7 +16858,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
         <v>129</v>
       </c>
@@ -16734,7 +16869,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
         <v>130</v>
       </c>
@@ -16745,7 +16880,7 @@
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
         <v>131</v>
       </c>
@@ -16756,7 +16891,7 @@
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
         <v>132</v>
       </c>
@@ -16767,7 +16902,7 @@
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
         <v>133</v>
       </c>
@@ -16778,7 +16913,7 @@
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="69" t="s">
         <v>134</v>
       </c>
@@ -16789,7 +16924,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -16800,7 +16935,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="69" t="s">
         <v>136</v>
       </c>
@@ -16811,7 +16946,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="69" t="s">
         <v>137</v>
       </c>
@@ -16822,7 +16957,7 @@
         <v>755.86244135709444</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="69" t="s">
         <v>138</v>
       </c>
@@ -16833,7 +16968,7 @@
         <v>762.55920427134606</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
         <v>139</v>
       </c>
@@ -16844,7 +16979,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
         <v>140</v>
       </c>
@@ -16855,7 +16990,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
         <v>141</v>
       </c>
@@ -16866,7 +17001,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="68" t="s">
         <v>1</v>
       </c>
@@ -16877,7 +17012,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -16888,7 +17023,7 @@
         <v>725.15243391008278</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -16899,7 +17034,7 @@
         <v>748.62596861099109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -16910,7 +17045,7 @@
         <v>801.99999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -16921,7 +17056,7 @@
         <v>791.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -16932,7 +17067,7 @@
         <v>700.32025584540236</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -16943,7 +17078,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -16954,7 +17089,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -16965,7 +17100,7 @@
         <v>794.1013538556316</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -16976,7 +17111,7 @@
         <v>789.34625592835232</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -16987,7 +17122,7 @@
         <v>809.68750817282455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -16998,7 +17133,7 @@
         <v>783.00612535864673</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -17009,7 +17144,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -17020,7 +17155,7 @@
         <v>508.00296189766453</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>155</v>
       </c>
@@ -17031,7 +17166,7 @@
         <v>428.22298556220187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -17042,7 +17177,7 @@
         <v>665.18536560495022</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -17053,7 +17188,7 @@
         <v>859.88020851632757</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -17064,7 +17199,7 @@
         <v>887.88245186586084</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -17075,7 +17210,7 @@
         <v>797.00724703341325</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -17086,7 +17221,7 @@
         <v>748.92792354647884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -17097,7 +17232,7 @@
         <v>778.77937164550963</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>162</v>
       </c>
@@ -17108,7 +17243,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -17119,7 +17254,7 @@
         <v>798.04417121416941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -17130,7 +17265,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>337</v>
       </c>
@@ -17141,7 +17276,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>338</v>
       </c>
@@ -17152,7 +17287,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>371</v>
       </c>
@@ -17163,7 +17298,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>372</v>
       </c>
@@ -17174,7 +17309,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>164</v>
       </c>
@@ -17185,7 +17320,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>165</v>
       </c>
@@ -17196,7 +17331,7 @@
         <v>716.69892648380858</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>166</v>
       </c>
@@ -17207,7 +17342,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>167</v>
       </c>
@@ -17218,7 +17353,7 @@
         <v>756.99999999999989</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -17229,7 +17364,7 @@
         <v>70.798124695046326</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -17240,7 +17375,7 @@
         <v>742.58779297677324</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -17251,7 +17386,7 @@
         <v>742.32362086970215</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -17262,7 +17397,7 @@
         <v>769.53334789802227</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -17273,7 +17408,7 @@
         <v>584.61287294827434</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>173</v>
       </c>
@@ -17284,7 +17419,7 @@
         <v>559.51652277652283</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -17295,7 +17430,7 @@
         <v>595.17975723111715</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -17306,7 +17441,7 @@
         <v>507.21044557645126</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>176</v>
       </c>
@@ -17317,7 +17452,7 @@
         <v>668.88377510394514</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>177</v>
       </c>
@@ -17328,7 +17463,7 @@
         <v>654.80340179705718</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>178</v>
       </c>
@@ -17339,7 +17474,7 @@
         <v>688.85095964480468</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -17350,7 +17485,7 @@
         <v>737.59071339941693</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>180</v>
       </c>
@@ -17361,7 +17496,7 @@
         <v>765.47381512866104</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -17372,7 +17507,7 @@
         <v>731.67589538225809</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>182</v>
       </c>
@@ -17383,7 +17518,7 @@
         <v>800.00032424653136</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>183</v>
       </c>
@@ -17394,7 +17529,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -17405,7 +17540,7 @@
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>188</v>
       </c>
@@ -17416,7 +17551,7 @@
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="68" t="s">
         <v>89</v>
       </c>
@@ -17427,7 +17562,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="140" t="s">
         <v>366</v>
       </c>
@@ -17438,7 +17573,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -17449,7 +17584,7 @@
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -17460,7 +17595,7 @@
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -17468,7 +17603,7 @@
         <v>22.648458746153963</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>192</v>
       </c>
@@ -17476,7 +17611,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>193</v>
       </c>
@@ -17484,7 +17619,7 @@
         <v>18.707371337693861</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>194</v>
       </c>
@@ -17492,7 +17627,7 @@
         <v>12.566427590816895</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>195</v>
       </c>
@@ -17500,7 +17635,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -17508,7 +17643,7 @@
         <v>11.566786665057547</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>197</v>
       </c>
@@ -17516,7 +17651,7 @@
         <v>31.342185540824094</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>198</v>
       </c>
@@ -17524,7 +17659,7 @@
         <v>31.0106439692332</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>199</v>
       </c>
@@ -17532,7 +17667,7 @@
         <v>28.609127685562171</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>200</v>
       </c>
@@ -17540,7 +17675,7 @@
         <v>33.012627597074328</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>201</v>
       </c>
@@ -17548,7 +17683,7 @@
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>202</v>
       </c>
@@ -17556,7 +17691,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -17564,7 +17699,7 @@
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>204</v>
       </c>
@@ -17572,7 +17707,7 @@
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>205</v>
       </c>
@@ -17580,7 +17715,7 @@
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>206</v>
       </c>
@@ -17588,7 +17723,7 @@
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>207</v>
       </c>
@@ -17596,7 +17731,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>208</v>
       </c>
@@ -17604,7 +17739,7 @@
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -17612,7 +17747,7 @@
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>210</v>
       </c>
@@ -17620,7 +17755,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>211</v>
       </c>
@@ -17628,7 +17763,7 @@
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>212</v>
       </c>
@@ -17636,7 +17771,7 @@
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>213</v>
       </c>
@@ -17644,7 +17779,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>214</v>
       </c>
@@ -17652,7 +17787,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>215</v>
       </c>
@@ -17660,7 +17795,7 @@
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>216</v>
       </c>
@@ -17668,7 +17803,7 @@
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="68" t="s">
         <v>219</v>
       </c>
@@ -17676,7 +17811,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Adding the Algae HTL pathway ...Continued
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21175302-5B51-4165-B5DC-117117F30EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679CCC45-B9A1-4CD5-A222-4288E0ABE757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="375">
   <si>
     <t>NG</t>
   </si>
@@ -2788,14 +2788,14 @@
       <selection pane="topRight" activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="122"/>
-    <col min="41" max="41" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="122"/>
+    <col min="41" max="41" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" ht="26.5" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" ht="78.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>1001250.3090024699</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>1199.1725344773329</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>8.0912620107395146</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>124.60248498831356</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>1066.4787874782799</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>2.3217600680931635E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>40.366758790864871</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>993.99652518923131</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>27.521187334987346</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>9.4662813685889695</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>1.8944508672117086</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>0.51231387456148403</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>7.7002199380836189E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>0.11248755052026857</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>0.18912102284679677</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>75019.638597761033</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -5893,11 +5893,11 @@
         <v>-76614.526624731123</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="P22" s="64"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -5969,12 +5969,12 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="115"/>
       <c r="B1" s="62" t="s">
         <v>93</v>
@@ -5998,7 +5998,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
         <v>335</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>2204.6226218487759</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
         <v>293</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
         <v>294</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
         <v>295</v>
       </c>
@@ -6193,9 +6193,9 @@
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>96</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>97</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="60" t="s">
         <v>98</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>28316.847000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="60" t="s">
         <v>99</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>28.316846999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="60" t="s">
         <v>100</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>7.4805211375990615</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="61" t="s">
         <v>101</v>
       </c>
@@ -6328,15 +6328,15 @@
       <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>102</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>103</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>122481433.6265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="60" t="s">
         <v>104</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>122481.4336265</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="60" t="s">
         <v>105</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>122.48143362649999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="60" t="s">
         <v>106</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>34022.620451805553</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="60" t="s">
         <v>107</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>34.022620451805558</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="60" t="s">
         <v>108</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>116090</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="60" t="s">
         <v>109</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>0.11609</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="61" t="s">
         <v>110</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>45.625085571947984</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="127" t="s">
         <v>336</v>
       </c>
@@ -6684,9 +6684,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="115" t="s">
         <v>111</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>112</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>113</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
         <v>114</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>115</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
         <v>116</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
         <v>296</v>
       </c>
@@ -6860,13 +6860,13 @@
       <selection activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="93" t="s">
         <v>220</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A2" s="94" t="s">
         <v>287</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A3" s="95" t="s">
         <v>288</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:79" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A5" s="75" t="s">
         <v>223</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A6" s="76" t="s">
         <v>285</v>
       </c>
@@ -7267,7 +7267,7 @@
       <c r="BZ6" s="9"/>
       <c r="CA6" s="83"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A7" s="76" t="s">
         <v>286</v>
       </c>
@@ -7444,7 +7444,7 @@
       <c r="BZ7" s="9"/>
       <c r="CA7" s="83"/>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A8" s="76" t="s">
         <v>221</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A9" s="87" t="s">
         <v>222</v>
       </c>
@@ -7810,12 +7810,12 @@
       <c r="BZ9" s="88"/>
       <c r="CA9" s="92"/>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
       <c r="B12" s="143" t="s">
         <v>289</v>
       </c>
@@ -7833,7 +7833,7 @@
       <c r="L12" s="97"/>
       <c r="M12" s="98"/>
     </row>
-    <row r="13" spans="1:79" ht="39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
       <c r="B13" s="144"/>
       <c r="C13" s="99" t="s">
         <v>1</v>
@@ -7869,7 +7869,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A14" s="110" t="s">
         <v>22</v>
       </c>
@@ -7910,7 +7910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A15" s="76" t="s">
         <v>23</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A16" s="76" t="s">
         <v>7</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>76.151387532990128</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="76" t="s">
         <v>24</v>
       </c>
@@ -8033,7 +8033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="76" t="s">
         <v>25</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="76" t="s">
         <v>26</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -8156,7 +8156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
@@ -8197,7 +8197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="76" t="s">
         <v>29</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="76" t="s">
         <v>30</v>
       </c>
@@ -8279,7 +8279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="87" t="s">
         <v>31</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="110"/>
       <c r="B25" s="143" t="s">
         <v>289</v>
@@ -8339,7 +8339,7 @@
       <c r="L25" s="97"/>
       <c r="M25" s="98"/>
     </row>
-    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="76"/>
       <c r="B26" s="144"/>
       <c r="C26" s="99" t="s">
@@ -8376,7 +8376,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="110" t="s">
         <v>22</v>
       </c>
@@ -8417,7 +8417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="76" t="s">
         <v>23</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="76" t="s">
         <v>7</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>95.950748291567578</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="76" t="s">
         <v>24</v>
       </c>
@@ -8540,7 +8540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="76" t="s">
         <v>25</v>
       </c>
@@ -8581,7 +8581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="76" t="s">
         <v>26</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="76" t="s">
         <v>29</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="76" t="s">
         <v>30</v>
       </c>
@@ -8786,7 +8786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="87" t="s">
         <v>31</v>
       </c>
@@ -8844,9 +8844,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -8854,7 +8854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="112" t="s">
         <v>8</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="112" t="s">
         <v>9</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="112" t="s">
         <v>10</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="112" t="s">
         <v>11</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="112" t="s">
         <v>12</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="112" t="s">
         <v>13</v>
       </c>
@@ -8934,12 +8934,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8958,7 +8958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -8980,7 +8980,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -8991,7 +8991,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -9002,7 +9002,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -9026,17 +9026,17 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="118" t="s">
         <v>122</v>
       </c>
@@ -9181,7 +9181,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -9255,7 +9255,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -9477,7 +9477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9551,7 +9551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -9699,7 +9699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -9773,7 +9773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -9847,7 +9847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -9921,7 +9921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -9995,7 +9995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -10069,7 +10069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -10143,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -10217,7 +10217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -10291,7 +10291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10439,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10513,7 +10513,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -10529,7 +10529,7 @@
       </c>
       <c r="H22" s="35"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -10543,7 +10543,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -10557,7 +10557,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -10571,7 +10571,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -10585,7 +10585,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -10599,7 +10599,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -10613,7 +10613,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -10627,7 +10627,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -10641,7 +10641,7 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -10655,7 +10655,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -10669,7 +10669,7 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -10683,7 +10683,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -10697,7 +10697,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -10722,24 +10722,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
-  <dimension ref="A1:BQ27"/>
+  <dimension ref="A1:BR27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BQ23" sqref="BQ23"/>
+      <selection pane="topRight" activeCell="BS12" sqref="BS12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
         <v>308</v>
@@ -10945,8 +10945,11 @@
       <c r="BQ1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="2" spans="1:69" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="BR1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
@@ -11154,8 +11157,11 @@
       <c r="BQ2" s="119" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR2" s="119" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -11363,8 +11369,11 @@
       <c r="BQ3" s="20" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR3" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -11572,8 +11581,11 @@
       <c r="BQ4">
         <v>3.2282836457015942</v>
       </c>
-    </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR4">
+        <v>29.226475858183772</v>
+      </c>
+    </row>
+    <row r="5" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -11781,8 +11793,11 @@
       <c r="BQ5">
         <v>3.0728681340416055</v>
       </c>
-    </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR5">
+        <v>27.68007234257048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -11990,8 +12005,11 @@
       <c r="BQ6">
         <v>0.50413295762414023</v>
       </c>
-    </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR6">
+        <v>2.1637867344060759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -12199,8 +12217,11 @@
       <c r="BQ7">
         <v>1.5123986505927864</v>
       </c>
-    </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR7">
+        <v>18.983121758092206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -12408,8 +12429,11 @@
       <c r="BQ8">
         <v>1.0563365258246789</v>
       </c>
-    </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR8">
+        <v>6.5331638500721958</v>
+      </c>
+    </row>
+    <row r="9" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -12617,8 +12641,11 @@
       <c r="BQ9">
         <v>5.6136052454827743E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR9">
+        <v>1.2931339474403903E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>59</v>
       </c>
@@ -12655,11 +12682,8 @@
       <c r="AH10" s="137"/>
       <c r="AI10" s="26"/>
       <c r="AJ10" s="137"/>
-      <c r="BQ10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>60</v>
       </c>
@@ -12867,8 +12891,11 @@
       <c r="BQ11">
         <v>6.0986993193583903E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR11">
+        <v>1.5369575444769657E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -13076,8 +13103,11 @@
       <c r="BQ12">
         <v>2.0719796655857878E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR12">
+        <v>2.3767403603346744E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -13285,8 +13315,11 @@
       <c r="BQ13">
         <v>1.0111465275939799E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR13">
+        <v>6.3420799050257172E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -13494,8 +13527,11 @@
       <c r="BQ14">
         <v>8.1861576543595249E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR14">
+        <v>1.3985631716786429E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -13703,8 +13739,11 @@
       <c r="BQ15">
         <v>7.181414584611474E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR15">
+        <v>1.1023100446641545E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -13912,8 +13951,11 @@
       <c r="BQ16">
         <v>6.0405047745250632E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR16">
+        <v>1.4622443754029444E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>66</v>
       </c>
@@ -14121,8 +14163,11 @@
       <c r="BQ17">
         <v>1.1211156972976533E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR17">
+        <v>6.2816299281138246E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>67</v>
       </c>
@@ -14330,8 +14375,11 @@
       <c r="BQ18">
         <v>2.7441649209226465E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR18">
+        <v>1.384465768977587E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>68</v>
       </c>
@@ -14539,8 +14587,11 @@
       <c r="BQ19">
         <v>4.5597517783716818E-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR19">
+        <v>4.4791265345305257E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -14748,8 +14799,11 @@
       <c r="BQ20">
         <v>4.7430396768858183E-6</v>
       </c>
-    </row>
-    <row r="21" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR20">
+        <v>4.3182873037403548E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
         <v>70</v>
       </c>
@@ -14957,12 +15011,15 @@
       <c r="BQ21">
         <v>0.22607654837045763</v>
       </c>
-    </row>
-    <row r="22" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR21">
+        <v>1.8656888381642496</v>
+      </c>
+    </row>
+    <row r="22" spans="1:70" x14ac:dyDescent="0.35">
       <c r="AH22" s="137"/>
       <c r="AJ22" s="137"/>
     </row>
-    <row r="23" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -15104,8 +15161,11 @@
       <c r="BQ23" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="27" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR23" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="AR27">
         <v>99</v>
       </c>
@@ -15127,9 +15187,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -15137,7 +15197,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -15146,7 +15206,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -15155,7 +15215,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -15164,7 +15224,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -15173,7 +15233,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="34" t="s">
         <v>79</v>
       </c>
@@ -15194,9 +15254,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -15246,7 +15306,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="78.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -15296,7 +15356,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -15349,7 +15409,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="112" t="s">
         <v>8</v>
       </c>
@@ -15400,7 +15460,7 @@
       </c>
       <c r="Q4" s="114"/>
     </row>
-    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="112" t="s">
         <v>9</v>
       </c>
@@ -15451,7 +15511,7 @@
       </c>
       <c r="Q5" s="114"/>
     </row>
-    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="112" t="s">
         <v>10</v>
       </c>
@@ -15502,7 +15562,7 @@
       </c>
       <c r="Q6" s="114"/>
     </row>
-    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="112" t="s">
         <v>11</v>
       </c>
@@ -15553,7 +15613,7 @@
       </c>
       <c r="Q7" s="114"/>
     </row>
-    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="112" t="s">
         <v>12</v>
       </c>
@@ -15604,7 +15664,7 @@
       </c>
       <c r="Q8" s="114"/>
     </row>
-    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="112" t="s">
         <v>13</v>
       </c>
@@ -15655,7 +15715,7 @@
       </c>
       <c r="Q9" s="114"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -15706,7 +15766,7 @@
       </c>
       <c r="Q10" s="67"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -15757,7 +15817,7 @@
       </c>
       <c r="Q11" s="67"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -15808,7 +15868,7 @@
       </c>
       <c r="Q12" s="67"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -15859,7 +15919,7 @@
       </c>
       <c r="Q13" s="67"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -15910,7 +15970,7 @@
       </c>
       <c r="Q14" s="67"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -15961,7 +16021,7 @@
       </c>
       <c r="Q15" s="67"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -16012,7 +16072,7 @@
       </c>
       <c r="Q16" s="67"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -16063,7 +16123,7 @@
       </c>
       <c r="Q17" s="67"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -16114,7 +16174,7 @@
       </c>
       <c r="Q18" s="67"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -16165,7 +16225,7 @@
       </c>
       <c r="Q19" s="67"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -16220,7 +16280,7 @@
         <v>3.3478260869565215</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -16234,11 +16294,11 @@
       <c r="N21" s="64"/>
       <c r="O21" s="64"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="M22" s="64"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -16280,12 +16340,12 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>297</v>
       </c>
@@ -16296,7 +16356,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -16310,7 +16370,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -16324,7 +16384,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -16338,7 +16398,7 @@
         <v>362403.00757167325</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -16352,7 +16412,7 @@
         <v>344979.42656462023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -16366,7 +16426,7 @@
         <v>24381.856026689315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -16380,7 +16440,7 @@
         <v>254462.26606022959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -16394,7 +16454,7 @@
         <v>66135.304477701342</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -16408,7 +16468,7 @@
         <v>59.889274923371126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -16422,7 +16482,7 @@
         <v>24.470884336712146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -16436,7 +16496,7 @@
         <v>34.134614130073174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -16450,7 +16510,7 @@
         <v>-15.759603589368934</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -16464,7 +16524,7 @@
         <v>8.6858851249063438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -16478,7 +16538,7 @@
         <v>6.9883164862451217</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -16492,7 +16552,7 @@
         <v>58.328462296040968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -16506,7 +16566,7 @@
         <v>0.49662761207225459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -16520,7 +16580,7 @@
         <v>1.1283578872130025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -16534,7 +16594,7 @@
         <v>57.127332585038609</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -16548,7 +16608,7 @@
         <v>-82.715827114534676</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -16562,7 +16622,7 @@
         <v>22763.019075759898</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -16586,9 +16646,9 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -16596,7 +16656,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -16604,7 +16664,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -16612,7 +16672,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
         <v>335</v>
       </c>
@@ -16620,7 +16680,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -16628,7 +16688,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
         <v>293</v>
       </c>
@@ -16636,7 +16696,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
         <v>97</v>
       </c>
@@ -16644,7 +16704,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
         <v>98</v>
       </c>
@@ -16652,7 +16712,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="62" t="s">
         <v>99</v>
       </c>
@@ -16660,7 +16720,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="62" t="s">
         <v>100</v>
       </c>
@@ -16668,7 +16728,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
         <v>101</v>
       </c>
@@ -16676,7 +16736,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="62" t="s">
         <v>103</v>
       </c>
@@ -16684,7 +16744,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="62" t="s">
         <v>104</v>
       </c>
@@ -16692,7 +16752,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="62" t="s">
         <v>105</v>
       </c>
@@ -16700,7 +16760,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="62" t="s">
         <v>106</v>
       </c>
@@ -16708,7 +16768,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="62" t="s">
         <v>107</v>
       </c>
@@ -16716,7 +16776,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="62" t="s">
         <v>108</v>
       </c>
@@ -16724,7 +16784,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="62" t="s">
         <v>109</v>
       </c>
@@ -16732,7 +16792,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="62" t="s">
         <v>110</v>
       </c>
@@ -16740,7 +16800,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="126" t="s">
         <v>336</v>
       </c>
@@ -16748,7 +16808,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="62" t="s">
         <v>112</v>
       </c>
@@ -16756,7 +16816,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="62" t="s">
         <v>113</v>
       </c>
@@ -16764,7 +16824,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="62" t="s">
         <v>114</v>
       </c>
@@ -16772,7 +16832,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="62" t="s">
         <v>115</v>
       </c>
@@ -16780,7 +16840,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="62" t="s">
         <v>116</v>
       </c>
@@ -16801,12 +16861,12 @@
       <selection activeCell="A45" sqref="A45:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="68" t="s">
         <v>186</v>
       </c>
@@ -16814,7 +16874,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -16825,7 +16885,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -16836,7 +16896,7 @@
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="69" t="s">
         <v>127</v>
       </c>
@@ -16847,7 +16907,7 @@
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="69" t="s">
         <v>128</v>
       </c>
@@ -16858,7 +16918,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="69" t="s">
         <v>129</v>
       </c>
@@ -16869,7 +16929,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="69" t="s">
         <v>130</v>
       </c>
@@ -16880,7 +16940,7 @@
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="69" t="s">
         <v>131</v>
       </c>
@@ -16891,7 +16951,7 @@
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="69" t="s">
         <v>132</v>
       </c>
@@ -16902,7 +16962,7 @@
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="69" t="s">
         <v>133</v>
       </c>
@@ -16913,7 +16973,7 @@
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="69" t="s">
         <v>134</v>
       </c>
@@ -16924,7 +16984,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -16935,7 +16995,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="69" t="s">
         <v>136</v>
       </c>
@@ -16946,7 +17006,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="69" t="s">
         <v>137</v>
       </c>
@@ -16957,7 +17017,7 @@
         <v>755.86244135709444</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="69" t="s">
         <v>138</v>
       </c>
@@ -16968,7 +17028,7 @@
         <v>762.55920427134606</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="69" t="s">
         <v>139</v>
       </c>
@@ -16979,7 +17039,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="69" t="s">
         <v>140</v>
       </c>
@@ -16990,7 +17050,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="69" t="s">
         <v>141</v>
       </c>
@@ -17001,7 +17061,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="68" t="s">
         <v>1</v>
       </c>
@@ -17012,7 +17072,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -17023,7 +17083,7 @@
         <v>725.15243391008278</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -17034,7 +17094,7 @@
         <v>748.62596861099109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -17045,7 +17105,7 @@
         <v>801.99999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -17056,7 +17116,7 @@
         <v>791.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -17067,7 +17127,7 @@
         <v>700.32025584540236</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -17078,7 +17138,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -17089,7 +17149,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -17100,7 +17160,7 @@
         <v>794.1013538556316</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -17111,7 +17171,7 @@
         <v>789.34625592835232</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -17122,7 +17182,7 @@
         <v>809.68750817282455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -17133,7 +17193,7 @@
         <v>783.00612535864673</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -17144,7 +17204,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -17155,7 +17215,7 @@
         <v>508.00296189766453</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>155</v>
       </c>
@@ -17166,7 +17226,7 @@
         <v>428.22298556220187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -17177,7 +17237,7 @@
         <v>665.18536560495022</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -17188,7 +17248,7 @@
         <v>859.88020851632757</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -17199,7 +17259,7 @@
         <v>887.88245186586084</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -17210,7 +17270,7 @@
         <v>797.00724703341325</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -17221,7 +17281,7 @@
         <v>748.92792354647884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -17232,7 +17292,7 @@
         <v>778.77937164550963</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>162</v>
       </c>
@@ -17243,7 +17303,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -17254,7 +17314,7 @@
         <v>798.04417121416941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -17265,7 +17325,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>337</v>
       </c>
@@ -17276,7 +17336,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>338</v>
       </c>
@@ -17287,7 +17347,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>371</v>
       </c>
@@ -17298,7 +17358,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>372</v>
       </c>
@@ -17309,7 +17369,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>164</v>
       </c>
@@ -17320,7 +17380,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>165</v>
       </c>
@@ -17331,7 +17391,7 @@
         <v>716.69892648380858</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>166</v>
       </c>
@@ -17342,7 +17402,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>167</v>
       </c>
@@ -17353,7 +17413,7 @@
         <v>756.99999999999989</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -17364,7 +17424,7 @@
         <v>70.798124695046326</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -17375,7 +17435,7 @@
         <v>742.58779297677324</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -17386,7 +17446,7 @@
         <v>742.32362086970215</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -17397,7 +17457,7 @@
         <v>769.53334789802227</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -17408,7 +17468,7 @@
         <v>584.61287294827434</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>173</v>
       </c>
@@ -17419,7 +17479,7 @@
         <v>559.51652277652283</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -17430,7 +17490,7 @@
         <v>595.17975723111715</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -17441,7 +17501,7 @@
         <v>507.21044557645126</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>176</v>
       </c>
@@ -17452,7 +17512,7 @@
         <v>668.88377510394514</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>177</v>
       </c>
@@ -17463,7 +17523,7 @@
         <v>654.80340179705718</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>178</v>
       </c>
@@ -17474,7 +17534,7 @@
         <v>688.85095964480468</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -17485,7 +17545,7 @@
         <v>737.59071339941693</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>180</v>
       </c>
@@ -17496,7 +17556,7 @@
         <v>765.47381512866104</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -17507,7 +17567,7 @@
         <v>731.67589538225809</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>182</v>
       </c>
@@ -17518,7 +17578,7 @@
         <v>800.00032424653136</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>183</v>
       </c>
@@ -17529,7 +17589,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -17540,7 +17600,7 @@
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>188</v>
       </c>
@@ -17551,7 +17611,7 @@
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="68" t="s">
         <v>89</v>
       </c>
@@ -17562,7 +17622,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="140" t="s">
         <v>366</v>
       </c>
@@ -17573,7 +17633,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -17584,7 +17644,7 @@
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -17595,7 +17655,7 @@
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -17603,7 +17663,7 @@
         <v>22.648458746153963</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>192</v>
       </c>
@@ -17611,7 +17671,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>193</v>
       </c>
@@ -17619,7 +17679,7 @@
         <v>18.707371337693861</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>194</v>
       </c>
@@ -17627,7 +17687,7 @@
         <v>12.566427590816895</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>195</v>
       </c>
@@ -17635,7 +17695,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -17643,7 +17703,7 @@
         <v>11.566786665057547</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>197</v>
       </c>
@@ -17651,7 +17711,7 @@
         <v>31.342185540824094</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>198</v>
       </c>
@@ -17659,7 +17719,7 @@
         <v>31.0106439692332</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>199</v>
       </c>
@@ -17667,7 +17727,7 @@
         <v>28.609127685562171</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>200</v>
       </c>
@@ -17675,7 +17735,7 @@
         <v>33.012627597074328</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>201</v>
       </c>
@@ -17683,7 +17743,7 @@
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>202</v>
       </c>
@@ -17691,7 +17751,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -17699,7 +17759,7 @@
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>204</v>
       </c>
@@ -17707,7 +17767,7 @@
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>205</v>
       </c>
@@ -17715,7 +17775,7 @@
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>206</v>
       </c>
@@ -17723,7 +17783,7 @@
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>207</v>
       </c>
@@ -17731,7 +17791,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>208</v>
       </c>
@@ -17739,7 +17799,7 @@
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -17747,7 +17807,7 @@
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>210</v>
       </c>
@@ -17755,7 +17815,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>211</v>
       </c>
@@ -17763,7 +17823,7 @@
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>212</v>
       </c>
@@ -17771,7 +17831,7 @@
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>213</v>
       </c>
@@ -17779,7 +17839,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>214</v>
       </c>
@@ -17787,7 +17847,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>215</v>
       </c>
@@ -17795,7 +17855,7 @@
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>216</v>
       </c>
@@ -17803,7 +17863,7 @@
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="68" t="s">
         <v>219</v>
       </c>
@@ -17811,7 +17871,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
1. Added urban emission factors to the LCI files, 2. Modify emission_factor function to account for urban emissions from dirct input for emissions and sequestrations
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2749084-BC40-48B1-9ADB-7C901F8007BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474D63F9-11B2-48D1-934F-E0C18441A862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -2111,6 +2111,10 @@
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2119,10 +2123,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2851,14 +2851,14 @@
       <selection pane="topRight" activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="122"/>
-    <col min="41" max="41" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="122"/>
+    <col min="41" max="41" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>1001250.3090024699</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>1199.1725344773329</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>8.0912620107395146</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>124.60248498831356</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>1066.4787874782799</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>2.3217600680931635E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>40.366758790864871</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>993.99652518923131</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>27.521187334987346</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>9.4662813685889695</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>1.8944508672117086</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>0.51231387456148403</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>7.7002199380836189E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>0.11248755052026857</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>0.18912102284679677</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>75019.638597761033</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -5956,33 +5956,33 @@
         <v>-76614.526624731123</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="P22" s="64"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="149" t="s">
+      <c r="B23" s="151" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="149"/>
-      <c r="D23" s="149"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="149"/>
-      <c r="G23" s="149"/>
-      <c r="H23" s="149"/>
-      <c r="I23" s="149"/>
-      <c r="J23" s="149"/>
-      <c r="K23" s="149"/>
-      <c r="L23" s="149"/>
-      <c r="M23" s="149"/>
-      <c r="N23" s="149"/>
-      <c r="O23" s="149"/>
-      <c r="P23" s="149"/>
-      <c r="Q23" s="149"/>
-      <c r="R23" s="149"/>
+      <c r="C23" s="151"/>
+      <c r="D23" s="151"/>
+      <c r="E23" s="151"/>
+      <c r="F23" s="151"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="151"/>
+      <c r="J23" s="151"/>
+      <c r="K23" s="151"/>
+      <c r="L23" s="151"/>
+      <c r="M23" s="151"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="151"/>
+      <c r="P23" s="151"/>
+      <c r="Q23" s="151"/>
+      <c r="R23" s="151"/>
       <c r="S23" s="35" t="s">
         <v>329</v>
       </c>
@@ -6032,12 +6032,12 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="115"/>
       <c r="B1" s="62" t="s">
         <v>93</v>
@@ -6061,7 +6061,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>335</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>2204.6226218487759</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>293</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>294</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>295</v>
       </c>
@@ -6256,9 +6256,9 @@
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>96</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>97</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>98</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>28316.847000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>99</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>28.316846999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>100</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>7.4805211375990615</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>101</v>
       </c>
@@ -6391,15 +6391,15 @@
       <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>102</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>103</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>122481433.6265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>104</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>122481.4336265</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>105</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>122.48143362649999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>106</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>34022.620451805553</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>107</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>34.022620451805558</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
         <v>108</v>
       </c>
@@ -6628,7 +6628,7 @@
         <v>116090</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
         <v>109</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>0.11609</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
         <v>110</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>45.625085571947984</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="127" t="s">
         <v>336</v>
       </c>
@@ -6747,9 +6747,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="115" t="s">
         <v>111</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>112</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>113</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>114</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>115</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>116</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>296</v>
       </c>
@@ -6923,13 +6923,13 @@
       <selection activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
         <v>220</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A2" s="94" t="s">
         <v>287</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
         <v>288</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:79" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A5" s="75" t="s">
         <v>223</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
         <v>285</v>
       </c>
@@ -7330,7 +7330,7 @@
       <c r="BZ6" s="9"/>
       <c r="CA6" s="83"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>286</v>
       </c>
@@ -7507,7 +7507,7 @@
       <c r="BZ7" s="9"/>
       <c r="CA7" s="83"/>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
         <v>221</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A9" s="87" t="s">
         <v>222</v>
       </c>
@@ -7873,13 +7873,13 @@
       <c r="BZ9" s="88"/>
       <c r="CA9" s="92"/>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
-      <c r="B12" s="150" t="s">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="B12" s="152" t="s">
         <v>289</v>
       </c>
       <c r="C12" s="96" t="s">
@@ -7896,8 +7896,8 @@
       <c r="L12" s="97"/>
       <c r="M12" s="98"/>
     </row>
-    <row r="13" spans="1:79" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="151"/>
+    <row r="13" spans="1:79" ht="39" x14ac:dyDescent="0.25">
+      <c r="B13" s="153"/>
       <c r="C13" s="99" t="s">
         <v>1</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A14" s="110" t="s">
         <v>22</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A15" s="76" t="s">
         <v>23</v>
       </c>
@@ -8014,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A16" s="76" t="s">
         <v>7</v>
       </c>
@@ -8055,7 +8055,7 @@
         <v>76.151387532990128</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="76" t="s">
         <v>24</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="76" t="s">
         <v>25</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="76" t="s">
         <v>26</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
@@ -8260,7 +8260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="76" t="s">
         <v>29</v>
       </c>
@@ -8301,7 +8301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="76" t="s">
         <v>30</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="87" t="s">
         <v>31</v>
       </c>
@@ -8383,9 +8383,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="110"/>
-      <c r="B25" s="150" t="s">
+      <c r="B25" s="152" t="s">
         <v>289</v>
       </c>
       <c r="C25" s="96" t="s">
@@ -8402,9 +8402,9 @@
       <c r="L25" s="97"/>
       <c r="M25" s="98"/>
     </row>
-    <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A26" s="76"/>
-      <c r="B26" s="151"/>
+      <c r="B26" s="153"/>
       <c r="C26" s="99" t="s">
         <v>1</v>
       </c>
@@ -8439,7 +8439,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="110" t="s">
         <v>22</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="76" t="s">
         <v>23</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="76" t="s">
         <v>7</v>
       </c>
@@ -8562,7 +8562,7 @@
         <v>95.950748291567578</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="76" t="s">
         <v>24</v>
       </c>
@@ -8603,7 +8603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="76" t="s">
         <v>25</v>
       </c>
@@ -8644,7 +8644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="76" t="s">
         <v>26</v>
       </c>
@@ -8685,7 +8685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -8726,7 +8726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="76" t="s">
         <v>29</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="76" t="s">
         <v>30</v>
       </c>
@@ -8849,7 +8849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="87" t="s">
         <v>31</v>
       </c>
@@ -8907,9 +8907,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -8917,7 +8917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="112" t="s">
         <v>8</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="112" t="s">
         <v>9</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="112" t="s">
         <v>10</v>
       </c>
@@ -8950,7 +8950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>11</v>
       </c>
@@ -8961,7 +8961,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
         <v>12</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
         <v>13</v>
       </c>
@@ -8997,12 +8997,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -9010,7 +9010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -9032,7 +9032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -9065,7 +9065,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -9085,21 +9085,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -9170,7 +9170,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="118" t="s">
         <v>122</v>
       </c>
@@ -9244,7 +9244,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -9318,7 +9318,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -9466,7 +9466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -9688,7 +9688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -9762,7 +9762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -9836,7 +9836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -9910,7 +9910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -10058,7 +10058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -10132,7 +10132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -10206,7 +10206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -10354,7 +10354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -10428,7 +10428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10502,7 +10502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10576,12 +10576,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="76" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="142" t="s">
         <v>376</v>
       </c>
@@ -10619,7 +10619,7 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -10655,7 +10655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="142" t="s">
         <v>377</v>
       </c>
@@ -10696,7 +10696,7 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -10729,7 +10729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="142" t="s">
         <v>378</v>
       </c>
@@ -10773,7 +10773,7 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24">
         <v>0</v>
@@ -10803,7 +10803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="142" t="s">
         <v>379</v>
       </c>
@@ -10850,7 +10850,7 @@
         <v>0</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -10877,7 +10877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="142" t="s">
         <v>380</v>
       </c>
@@ -10927,7 +10927,7 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26">
         <v>0</v>
@@ -10951,7 +10951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="142" t="s">
         <v>381</v>
       </c>
@@ -11004,7 +11004,7 @@
         <v>0</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S27">
         <v>0</v>
@@ -11025,7 +11025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="142" t="s">
         <v>382</v>
       </c>
@@ -11081,7 +11081,7 @@
         <v>0</v>
       </c>
       <c r="S28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -11099,7 +11099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="143" t="s">
         <v>383</v>
       </c>
@@ -11158,7 +11158,7 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29">
         <v>0</v>
@@ -11173,27 +11173,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
       <c r="B31" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="149" t="s">
+      <c r="C31" s="151" t="s">
         <v>384</v>
       </c>
-      <c r="D31" s="149"/>
-      <c r="E31" s="149"/>
+      <c r="D31" s="151"/>
+      <c r="E31" s="151"/>
       <c r="G31" s="35" t="s">
         <v>333</v>
       </c>
       <c r="H31" s="35"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -11207,7 +11207,7 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -11221,7 +11221,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -11235,7 +11235,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -11249,7 +11249,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -11263,7 +11263,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -11277,7 +11277,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -11291,7 +11291,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -11305,7 +11305,7 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -11319,7 +11319,7 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -11333,7 +11333,7 @@
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -11347,7 +11347,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -11361,7 +11361,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -11388,22 +11388,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
   <dimension ref="A1:BR32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AT1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="BO24" sqref="BO24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" customWidth="1"/>
-    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:70" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
         <v>308</v>
@@ -11613,7 +11613,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:70" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -12037,7 +12037,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -12249,7 +12249,7 @@
         <v>29.226475858183772</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -12461,7 +12461,7 @@
         <v>27.68007234257048</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -12673,7 +12673,7 @@
         <v>2.1637867344060759</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -12885,7 +12885,7 @@
         <v>18.983121758092206</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -13097,7 +13097,7 @@
         <v>6.5331638500721958</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -13309,7 +13309,7 @@
         <v>1.2931339474403903E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>59</v>
       </c>
@@ -13348,7 +13348,7 @@
       <c r="AJ10" s="137"/>
       <c r="AK10" s="145"/>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>60</v>
       </c>
@@ -13560,7 +13560,7 @@
         <v>1.5369575444769657E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -13772,7 +13772,7 @@
         <v>2.3767403603346744E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -13984,7 +13984,7 @@
         <v>6.3420799050257172E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -14196,7 +14196,7 @@
         <v>1.3985631716786429E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -14408,7 +14408,7 @@
         <v>1.1023100446641545E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -14620,7 +14620,7 @@
         <v>1.4622443754029444E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>66</v>
       </c>
@@ -14832,7 +14832,7 @@
         <v>6.2816299281138246E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>67</v>
       </c>
@@ -15044,7 +15044,7 @@
         <v>1.384465768977587E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>68</v>
       </c>
@@ -15256,7 +15256,7 @@
         <v>4.4791265345305257E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -15468,7 +15468,7 @@
         <v>4.3182873037403548E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>70</v>
       </c>
@@ -15680,7 +15680,7 @@
         <v>1.8656888381642496</v>
       </c>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A22" s="76" t="s">
         <v>375</v>
       </c>
@@ -15724,7 +15724,7 @@
       <c r="AT22" s="64"/>
       <c r="AU22" s="64"/>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" s="142" t="s">
         <v>376</v>
       </c>
@@ -15737,7 +15737,7 @@
       <c r="D23" s="22">
         <v>2.2183972612377794E-5</v>
       </c>
-      <c r="E23" s="153">
+      <c r="E23" s="150">
         <v>1.682069501830573E-5</v>
       </c>
       <c r="F23" s="22">
@@ -15854,7 +15854,7 @@
       <c r="AQ23">
         <v>2.799058377780967E-5</v>
       </c>
-      <c r="AR23" s="152">
+      <c r="AR23" s="149">
         <v>4.4004992061689248E-5</v>
       </c>
       <c r="AS23" s="148">
@@ -15863,7 +15863,7 @@
       <c r="AT23" s="148">
         <v>5.7539331296186584E-4</v>
       </c>
-      <c r="AU23" s="152">
+      <c r="AU23" s="149">
         <v>9.3345353840135853E-6</v>
       </c>
       <c r="AV23">
@@ -15936,7 +15936,7 @@
         <v>3.5515149979386286E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A24" s="142" t="s">
         <v>377</v>
       </c>
@@ -16148,7 +16148,7 @@
         <v>1.090336568096634E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A25" s="142" t="s">
         <v>378</v>
       </c>
@@ -16360,7 +16360,7 @@
         <v>3.3685121043801309E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A26" s="142" t="s">
         <v>379</v>
       </c>
@@ -16572,7 +16572,7 @@
         <v>2.702203671489133E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A27" s="142" t="s">
         <v>380</v>
       </c>
@@ -16784,7 +16784,7 @@
         <v>2.3849770757134076E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" s="142" t="s">
         <v>381</v>
       </c>
@@ -16996,7 +16996,7 @@
         <v>1.9778305848322815E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A29" s="142" t="s">
         <v>382</v>
       </c>
@@ -17208,7 +17208,7 @@
         <v>2.6907087561252384E-6</v>
       </c>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A30" s="143" t="s">
         <v>383</v>
       </c>
@@ -17420,48 +17420,48 @@
         <v>8.1834506459948039E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
       <c r="AH31" s="137"/>
       <c r="AJ31" s="137"/>
       <c r="AK31" s="145"/>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="149" t="s">
+      <c r="B32" s="151" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="149"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="149"/>
-      <c r="G32" s="149"/>
-      <c r="H32" s="149"/>
-      <c r="I32" s="149"/>
-      <c r="J32" s="149"/>
-      <c r="K32" s="149"/>
-      <c r="L32" s="149"/>
-      <c r="M32" s="149"/>
-      <c r="N32" s="149"/>
-      <c r="O32" s="149"/>
-      <c r="P32" s="149"/>
-      <c r="Q32" s="149"/>
-      <c r="R32" s="149"/>
-      <c r="S32" s="149"/>
-      <c r="T32" s="149"/>
-      <c r="U32" s="149"/>
-      <c r="V32" s="149"/>
-      <c r="W32" s="149"/>
-      <c r="X32" s="149"/>
-      <c r="Y32" s="149"/>
-      <c r="Z32" s="149"/>
-      <c r="AA32" s="149"/>
-      <c r="AB32" s="149"/>
-      <c r="AC32" s="149"/>
-      <c r="AD32" s="149"/>
-      <c r="AE32" s="149"/>
-      <c r="AF32" s="149"/>
+      <c r="C32" s="151"/>
+      <c r="D32" s="151"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="151"/>
+      <c r="G32" s="151"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="151"/>
+      <c r="J32" s="151"/>
+      <c r="K32" s="151"/>
+      <c r="L32" s="151"/>
+      <c r="M32" s="151"/>
+      <c r="N32" s="151"/>
+      <c r="O32" s="151"/>
+      <c r="P32" s="151"/>
+      <c r="Q32" s="151"/>
+      <c r="R32" s="151"/>
+      <c r="S32" s="151"/>
+      <c r="T32" s="151"/>
+      <c r="U32" s="151"/>
+      <c r="V32" s="151"/>
+      <c r="W32" s="151"/>
+      <c r="X32" s="151"/>
+      <c r="Y32" s="151"/>
+      <c r="Z32" s="151"/>
+      <c r="AA32" s="151"/>
+      <c r="AB32" s="151"/>
+      <c r="AC32" s="151"/>
+      <c r="AD32" s="151"/>
+      <c r="AE32" s="151"/>
+      <c r="AF32" s="151"/>
       <c r="AH32" s="137" t="s">
         <v>367</v>
       </c>
@@ -17588,9 +17588,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -17598,7 +17598,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -17607,7 +17607,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -17616,7 +17616,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -17625,7 +17625,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -17634,7 +17634,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>79</v>
       </c>
@@ -17655,9 +17655,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -17707,7 +17707,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -17757,7 +17757,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -17810,7 +17810,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="112" t="s">
         <v>8</v>
       </c>
@@ -17861,7 +17861,7 @@
       </c>
       <c r="Q4" s="114"/>
     </row>
-    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>9</v>
       </c>
@@ -17912,7 +17912,7 @@
       </c>
       <c r="Q5" s="114"/>
     </row>
-    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
         <v>10</v>
       </c>
@@ -17963,7 +17963,7 @@
       </c>
       <c r="Q6" s="114"/>
     </row>
-    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
         <v>11</v>
       </c>
@@ -18014,7 +18014,7 @@
       </c>
       <c r="Q7" s="114"/>
     </row>
-    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="112" t="s">
         <v>12</v>
       </c>
@@ -18065,7 +18065,7 @@
       </c>
       <c r="Q8" s="114"/>
     </row>
-    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="112" t="s">
         <v>13</v>
       </c>
@@ -18116,7 +18116,7 @@
       </c>
       <c r="Q9" s="114"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -18167,7 +18167,7 @@
       </c>
       <c r="Q10" s="67"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -18218,7 +18218,7 @@
       </c>
       <c r="Q11" s="67"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -18269,7 +18269,7 @@
       </c>
       <c r="Q12" s="67"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -18320,7 +18320,7 @@
       </c>
       <c r="Q13" s="67"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -18371,7 +18371,7 @@
       </c>
       <c r="Q14" s="67"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -18422,7 +18422,7 @@
       </c>
       <c r="Q15" s="67"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -18473,7 +18473,7 @@
       </c>
       <c r="Q16" s="67"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -18524,7 +18524,7 @@
       </c>
       <c r="Q17" s="67"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -18575,7 +18575,7 @@
       </c>
       <c r="Q18" s="67"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -18626,7 +18626,7 @@
       </c>
       <c r="Q19" s="67"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -18681,7 +18681,7 @@
         <v>3.3478260869565215</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -18695,30 +18695,30 @@
       <c r="N21" s="64"/>
       <c r="O21" s="64"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="M22" s="64"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="149" t="s">
+      <c r="B23" s="151" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="149"/>
-      <c r="D23" s="149"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="149"/>
-      <c r="G23" s="149"/>
-      <c r="H23" s="149"/>
-      <c r="I23" s="149"/>
-      <c r="J23" s="149"/>
-      <c r="K23" s="149"/>
-      <c r="L23" s="149"/>
-      <c r="M23" s="149"/>
-      <c r="N23" s="149"/>
-      <c r="O23" s="149"/>
+      <c r="C23" s="151"/>
+      <c r="D23" s="151"/>
+      <c r="E23" s="151"/>
+      <c r="F23" s="151"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="151"/>
+      <c r="J23" s="151"/>
+      <c r="K23" s="151"/>
+      <c r="L23" s="151"/>
+      <c r="M23" s="151"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="151"/>
       <c r="P23" t="s">
         <v>90</v>
       </c>
@@ -18741,14 +18741,14 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>297</v>
       </c>
@@ -18759,7 +18759,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -18773,7 +18773,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -18787,7 +18787,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -18801,7 +18801,7 @@
         <v>362403.00757167325</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -18815,7 +18815,7 @@
         <v>344979.42656462023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -18829,7 +18829,7 @@
         <v>24381.856026689315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -18843,7 +18843,7 @@
         <v>254462.26606022959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -18857,7 +18857,7 @@
         <v>66135.304477701342</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -18871,7 +18871,7 @@
         <v>59.889274923371126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -18885,7 +18885,7 @@
         <v>24.470884336712146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -18899,7 +18899,7 @@
         <v>34.134614130073174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -18913,7 +18913,7 @@
         <v>-15.759603589368934</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -18927,7 +18927,7 @@
         <v>8.6858851249063438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -18941,7 +18941,7 @@
         <v>6.9883164862451217</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -18955,7 +18955,7 @@
         <v>58.328462296040968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -18969,7 +18969,7 @@
         <v>0.49662761207225459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -18983,7 +18983,7 @@
         <v>1.1283578872130025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -18997,7 +18997,7 @@
         <v>57.127332585038609</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -19011,7 +19011,7 @@
         <v>-82.715827114534676</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -19025,12 +19025,12 @@
         <v>22763.019075759898</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="76" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="142" t="s">
         <v>376</v>
       </c>
@@ -19044,7 +19044,7 @@
         <v>0.37034943531993869</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="142" t="s">
         <v>377</v>
       </c>
@@ -19058,7 +19058,7 @@
         <v>1.274407618987647</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="142" t="s">
         <v>378</v>
       </c>
@@ -19072,7 +19072,7 @@
         <v>3.1302091249900932</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="142" t="s">
         <v>379</v>
       </c>
@@ -19086,7 +19086,7 @@
         <v>0.24682227388035821</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="142" t="s">
         <v>380</v>
       </c>
@@ -19100,7 +19100,7 @@
         <v>0.21415419754922327</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="142" t="s">
         <v>381</v>
       </c>
@@ -19114,7 +19114,7 @@
         <v>1.7961904743782098</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="142" t="s">
         <v>382</v>
       </c>
@@ -19128,7 +19128,7 @@
         <v>2.2352473934910237E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="143" t="s">
         <v>383</v>
       </c>
@@ -19142,7 +19142,7 @@
         <v>7.0223242933031296E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -19166,9 +19166,9 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -19176,7 +19176,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -19184,7 +19184,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -19192,7 +19192,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>335</v>
       </c>
@@ -19200,7 +19200,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -19208,7 +19208,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>293</v>
       </c>
@@ -19216,7 +19216,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>97</v>
       </c>
@@ -19224,7 +19224,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>98</v>
       </c>
@@ -19232,7 +19232,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>99</v>
       </c>
@@ -19240,7 +19240,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>100</v>
       </c>
@@ -19248,7 +19248,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>101</v>
       </c>
@@ -19256,7 +19256,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>103</v>
       </c>
@@ -19264,7 +19264,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>104</v>
       </c>
@@ -19272,7 +19272,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>105</v>
       </c>
@@ -19280,7 +19280,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
         <v>106</v>
       </c>
@@ -19288,7 +19288,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="s">
         <v>107</v>
       </c>
@@ -19296,7 +19296,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>108</v>
       </c>
@@ -19304,7 +19304,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>109</v>
       </c>
@@ -19312,7 +19312,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>110</v>
       </c>
@@ -19320,7 +19320,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="126" t="s">
         <v>336</v>
       </c>
@@ -19328,7 +19328,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>112</v>
       </c>
@@ -19336,7 +19336,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="s">
         <v>113</v>
       </c>
@@ -19344,7 +19344,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="62" t="s">
         <v>114</v>
       </c>
@@ -19352,7 +19352,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>115</v>
       </c>
@@ -19360,7 +19360,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
         <v>116</v>
       </c>
@@ -19381,12 +19381,12 @@
       <selection activeCell="A45" sqref="A45:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="68" t="s">
         <v>186</v>
       </c>
@@ -19394,7 +19394,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -19405,7 +19405,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -19416,7 +19416,7 @@
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
         <v>127</v>
       </c>
@@ -19427,7 +19427,7 @@
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
         <v>128</v>
       </c>
@@ -19438,7 +19438,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
         <v>129</v>
       </c>
@@ -19449,7 +19449,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
         <v>130</v>
       </c>
@@ -19460,7 +19460,7 @@
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
         <v>131</v>
       </c>
@@ -19471,7 +19471,7 @@
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
         <v>132</v>
       </c>
@@ -19482,7 +19482,7 @@
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="69" t="s">
         <v>133</v>
       </c>
@@ -19493,7 +19493,7 @@
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="69" t="s">
         <v>134</v>
       </c>
@@ -19504,7 +19504,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -19515,7 +19515,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="69" t="s">
         <v>136</v>
       </c>
@@ -19526,7 +19526,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="69" t="s">
         <v>137</v>
       </c>
@@ -19537,7 +19537,7 @@
         <v>755.86244135709444</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="69" t="s">
         <v>138</v>
       </c>
@@ -19548,7 +19548,7 @@
         <v>762.55920427134606</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
         <v>139</v>
       </c>
@@ -19559,7 +19559,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
         <v>140</v>
       </c>
@@ -19570,7 +19570,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
         <v>141</v>
       </c>
@@ -19581,7 +19581,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="68" t="s">
         <v>1</v>
       </c>
@@ -19592,7 +19592,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -19603,7 +19603,7 @@
         <v>725.15243391008278</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -19614,7 +19614,7 @@
         <v>748.62596861099109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -19625,7 +19625,7 @@
         <v>801.99999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -19636,7 +19636,7 @@
         <v>791.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -19647,7 +19647,7 @@
         <v>700.32025584540236</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -19658,7 +19658,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -19669,7 +19669,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -19680,7 +19680,7 @@
         <v>794.1013538556316</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -19691,7 +19691,7 @@
         <v>789.34625592835232</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -19702,7 +19702,7 @@
         <v>809.68750817282455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -19713,7 +19713,7 @@
         <v>783.00612535864673</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -19724,7 +19724,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -19735,7 +19735,7 @@
         <v>508.00296189766453</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>155</v>
       </c>
@@ -19746,7 +19746,7 @@
         <v>428.22298556220187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -19757,7 +19757,7 @@
         <v>665.18536560495022</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -19768,7 +19768,7 @@
         <v>859.88020851632757</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -19779,7 +19779,7 @@
         <v>887.88245186586084</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -19790,7 +19790,7 @@
         <v>797.00724703341325</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -19801,7 +19801,7 @@
         <v>748.92792354647884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -19812,7 +19812,7 @@
         <v>778.77937164550963</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>162</v>
       </c>
@@ -19823,7 +19823,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -19834,7 +19834,7 @@
         <v>798.04417121416941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -19845,7 +19845,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>337</v>
       </c>
@@ -19856,7 +19856,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>338</v>
       </c>
@@ -19867,7 +19867,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>371</v>
       </c>
@@ -19878,7 +19878,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>372</v>
       </c>
@@ -19889,7 +19889,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>164</v>
       </c>
@@ -19900,7 +19900,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>165</v>
       </c>
@@ -19911,7 +19911,7 @@
         <v>716.69892648380858</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>166</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>167</v>
       </c>
@@ -19933,7 +19933,7 @@
         <v>756.99999999999989</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -19944,7 +19944,7 @@
         <v>70.798124695046326</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -19955,7 +19955,7 @@
         <v>742.58779297677324</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -19966,7 +19966,7 @@
         <v>742.32362086970215</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -19977,7 +19977,7 @@
         <v>769.53334789802227</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -19988,7 +19988,7 @@
         <v>584.61287294827434</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>173</v>
       </c>
@@ -19999,7 +19999,7 @@
         <v>559.51652277652283</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -20010,7 +20010,7 @@
         <v>595.17975723111715</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -20021,7 +20021,7 @@
         <v>507.21044557645126</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>176</v>
       </c>
@@ -20032,7 +20032,7 @@
         <v>668.88377510394514</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>177</v>
       </c>
@@ -20043,7 +20043,7 @@
         <v>654.80340179705718</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>178</v>
       </c>
@@ -20054,7 +20054,7 @@
         <v>688.85095964480468</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -20065,7 +20065,7 @@
         <v>737.59071339941693</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>180</v>
       </c>
@@ -20076,7 +20076,7 @@
         <v>765.47381512866104</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -20087,7 +20087,7 @@
         <v>731.67589538225809</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>182</v>
       </c>
@@ -20098,7 +20098,7 @@
         <v>800.00032424653136</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>183</v>
       </c>
@@ -20109,7 +20109,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -20120,7 +20120,7 @@
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>188</v>
       </c>
@@ -20131,7 +20131,7 @@
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="68" t="s">
         <v>89</v>
       </c>
@@ -20142,7 +20142,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="140" t="s">
         <v>366</v>
       </c>
@@ -20153,7 +20153,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -20164,7 +20164,7 @@
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -20175,7 +20175,7 @@
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -20183,7 +20183,7 @@
         <v>22.648458746153963</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>192</v>
       </c>
@@ -20191,7 +20191,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>193</v>
       </c>
@@ -20199,7 +20199,7 @@
         <v>18.707371337693861</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>194</v>
       </c>
@@ -20207,7 +20207,7 @@
         <v>12.566427590816895</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>195</v>
       </c>
@@ -20215,7 +20215,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -20223,7 +20223,7 @@
         <v>11.566786665057547</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>197</v>
       </c>
@@ -20231,7 +20231,7 @@
         <v>31.342185540824094</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>198</v>
       </c>
@@ -20239,7 +20239,7 @@
         <v>31.0106439692332</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>199</v>
       </c>
@@ -20247,7 +20247,7 @@
         <v>28.609127685562171</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>200</v>
       </c>
@@ -20255,7 +20255,7 @@
         <v>33.012627597074328</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>201</v>
       </c>
@@ -20263,7 +20263,7 @@
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>202</v>
       </c>
@@ -20271,7 +20271,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -20279,7 +20279,7 @@
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>204</v>
       </c>
@@ -20287,7 +20287,7 @@
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>205</v>
       </c>
@@ -20295,7 +20295,7 @@
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>206</v>
       </c>
@@ -20303,7 +20303,7 @@
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>207</v>
       </c>
@@ -20311,7 +20311,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>208</v>
       </c>
@@ -20319,7 +20319,7 @@
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -20327,7 +20327,7 @@
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>210</v>
       </c>
@@ -20335,7 +20335,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>211</v>
       </c>
@@ -20343,7 +20343,7 @@
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>212</v>
       </c>
@@ -20351,7 +20351,7 @@
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>213</v>
       </c>
@@ -20359,7 +20359,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>214</v>
       </c>
@@ -20367,7 +20367,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>215</v>
       </c>
@@ -20375,7 +20375,7 @@
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>216</v>
       </c>
@@ -20383,7 +20383,7 @@
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="68" t="s">
         <v>219</v>
       </c>
@@ -20391,7 +20391,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Added payload of renewable diesels to the file
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474D63F9-11B2-48D1-934F-E0C18441A862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FB001F-E901-4A9E-AE9C-900D436B56CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="13" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="385">
   <si>
     <t>NG</t>
   </si>
@@ -2851,14 +2851,14 @@
       <selection pane="topRight" activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="122"/>
-    <col min="41" max="41" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="122"/>
+    <col min="41" max="41" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" ht="26.5" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" ht="78.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>1001250.3090024699</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>1199.1725344773329</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>8.0912620107395146</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>124.60248498831356</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>1066.4787874782799</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>2.3217600680931635E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>40.366758790864871</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>993.99652518923131</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>27.521187334987346</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>9.4662813685889695</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>1.8944508672117086</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>5.3987418408876558E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>0.51231387456148403</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>7.7002199380836189E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>0.11248755052026857</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>0.18912102284679677</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>75019.638597761033</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -5956,11 +5956,11 @@
         <v>-76614.526624731123</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="P22" s="64"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -6032,12 +6032,12 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="115"/>
       <c r="B1" s="62" t="s">
         <v>93</v>
@@ -6061,7 +6061,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
         <v>335</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>2204.6226218487759</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
         <v>293</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
         <v>294</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>1.1023113109243878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
         <v>295</v>
       </c>
@@ -6256,9 +6256,9 @@
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>96</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>97</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="60" t="s">
         <v>98</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>28316.847000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="60" t="s">
         <v>99</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>28.316846999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="60" t="s">
         <v>100</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>7.4805211375990615</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="61" t="s">
         <v>101</v>
       </c>
@@ -6391,15 +6391,15 @@
       <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>102</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>103</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>122481433.6265</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="60" t="s">
         <v>104</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>122481.4336265</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="60" t="s">
         <v>105</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>122.48143362649999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="60" t="s">
         <v>106</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>34022.620451805553</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="60" t="s">
         <v>107</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>34.022620451805558</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="60" t="s">
         <v>108</v>
       </c>
@@ -6628,7 +6628,7 @@
         <v>116090</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="60" t="s">
         <v>109</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>0.11609</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="61" t="s">
         <v>110</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>45.625085571947984</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="127" t="s">
         <v>336</v>
       </c>
@@ -6747,9 +6747,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="115" t="s">
         <v>111</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>112</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>113</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
         <v>114</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>115</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
         <v>116</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
         <v>296</v>
       </c>
@@ -6917,19 +6917,19 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F07116-128C-456A-A5F4-E4321BD8FA65}">
-  <dimension ref="A1:CA37"/>
+  <dimension ref="A1:CE37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF22" sqref="AF22"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="93" t="s">
         <v>220</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A2" s="94" t="s">
         <v>287</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>19855.30899836577</v>
       </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A3" s="95" t="s">
         <v>288</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>18556.36354987455</v>
       </c>
     </row>
-    <row r="5" spans="1:79" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:83" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A5" s="75" t="s">
         <v>223</v>
       </c>
@@ -7033,175 +7033,187 @@
         <v>242</v>
       </c>
       <c r="X5" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y5" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="Z5" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="AA5" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="AB5" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="Y5" s="17" t="s">
+      <c r="AC5" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="Z5" s="17" t="s">
+      <c r="AD5" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="AA5" s="17" t="s">
+      <c r="AE5" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="AB5" s="17" t="s">
+      <c r="AF5" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="AC5" s="17" t="s">
+      <c r="AG5" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="AD5" s="17" t="s">
+      <c r="AH5" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="AE5" s="17" t="s">
+      <c r="AI5" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="AF5" s="17" t="s">
+      <c r="AJ5" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="AG5" s="17" t="s">
+      <c r="AK5" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="AH5" s="17" t="s">
+      <c r="AL5" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="AI5" s="17" t="s">
+      <c r="AM5" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="AJ5" s="17" t="s">
+      <c r="AN5" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="AK5" s="17" t="s">
+      <c r="AO5" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="AL5" s="17" t="s">
+      <c r="AP5" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="AM5" s="17" t="s">
+      <c r="AQ5" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="AN5" s="17" t="s">
+      <c r="AR5" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="AO5" s="17" t="s">
+      <c r="AS5" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="AP5" s="17" t="s">
+      <c r="AT5" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="AQ5" s="17" t="s">
+      <c r="AU5" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="AR5" s="17" t="s">
+      <c r="AV5" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="AS5" s="17" t="s">
+      <c r="AW5" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="AT5" s="17" t="s">
+      <c r="AX5" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="AU5" s="17" t="s">
+      <c r="AY5" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="AV5" s="17" t="s">
+      <c r="AZ5" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="AW5" s="141" t="s">
+      <c r="BA5" s="141" t="s">
         <v>347</v>
       </c>
-      <c r="AX5" s="17" t="s">
+      <c r="BB5" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="AY5" s="17" t="s">
+      <c r="BC5" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="AZ5" s="17" t="s">
+      <c r="BD5" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="BA5" s="17" t="s">
+      <c r="BE5" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="BB5" s="17" t="s">
+      <c r="BF5" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="BC5" s="17" t="s">
+      <c r="BG5" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="BD5" s="17" t="s">
+      <c r="BH5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="BE5" s="17" t="s">
+      <c r="BI5" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="BF5" s="17" t="s">
+      <c r="BJ5" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="BG5" s="17" t="s">
+      <c r="BK5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="BH5" s="17" t="s">
+      <c r="BL5" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="BI5" s="17" t="s">
+      <c r="BM5" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="BJ5" s="17" t="s">
+      <c r="BN5" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="BK5" s="17" t="s">
+      <c r="BO5" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="BL5" s="17" t="s">
+      <c r="BP5" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="BM5" s="17" t="s">
+      <c r="BQ5" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="BN5" s="17" t="s">
+      <c r="BR5" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="BO5" s="17" t="s">
+      <c r="BS5" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="BP5" s="17" t="s">
+      <c r="BT5" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="BQ5" s="17" t="s">
+      <c r="BU5" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="BR5" s="17" t="s">
+      <c r="BV5" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="BS5" s="17" t="s">
+      <c r="BW5" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="BT5" s="17" t="s">
+      <c r="BX5" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="BU5" s="17" t="s">
+      <c r="BY5" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="BV5" s="17" t="s">
+      <c r="BZ5" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="BW5" s="17" t="s">
+      <c r="CA5" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="BX5" s="17" t="s">
+      <c r="CB5" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="BY5" s="17" t="s">
+      <c r="CC5" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="BZ5" s="17" t="s">
+      <c r="CD5" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="CA5" s="18" t="s">
+      <c r="CE5" s="18" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A6" s="76" t="s">
         <v>285</v>
       </c>
@@ -7260,13 +7272,13 @@
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
-      <c r="Y6" s="78">
-        <v>65000</v>
-      </c>
+      <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
+      <c r="AC6" s="78">
+        <v>65000</v>
+      </c>
       <c r="AD6" s="9"/>
       <c r="AE6" s="9"/>
       <c r="AF6" s="9"/>
@@ -7275,26 +7287,26 @@
       <c r="AI6" s="9"/>
       <c r="AJ6" s="9"/>
       <c r="AK6" s="9"/>
-      <c r="AL6" s="78">
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="78">
         <v>150000</v>
       </c>
-      <c r="AM6" s="9"/>
-      <c r="AN6" s="7"/>
-      <c r="AO6" s="9"/>
-      <c r="AP6" s="9"/>
       <c r="AQ6" s="9"/>
-      <c r="AR6" s="9"/>
-      <c r="AS6" s="79">
+      <c r="AR6" s="7"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="79">
         <v>100000</v>
       </c>
-      <c r="AT6" s="79">
+      <c r="AX6" s="79">
         <v>100000</v>
       </c>
-      <c r="AU6" s="80"/>
-      <c r="AV6" s="9"/>
-      <c r="AW6" s="9"/>
-      <c r="AX6" s="9"/>
-      <c r="AY6" s="9"/>
+      <c r="AY6" s="80"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
       <c r="BB6" s="9"/>
@@ -7308,29 +7320,33 @@
       <c r="BJ6" s="9"/>
       <c r="BK6" s="9"/>
       <c r="BL6" s="9"/>
-      <c r="BM6" s="7"/>
+      <c r="BM6" s="9"/>
       <c r="BN6" s="9"/>
-      <c r="BO6" s="81">
+      <c r="BO6" s="9"/>
+      <c r="BP6" s="9"/>
+      <c r="BQ6" s="7"/>
+      <c r="BR6" s="9"/>
+      <c r="BS6" s="81">
         <v>100000</v>
       </c>
-      <c r="BP6" s="7"/>
-      <c r="BQ6" s="82">
+      <c r="BT6" s="7"/>
+      <c r="BU6" s="82">
         <v>90000</v>
       </c>
-      <c r="BR6" s="9"/>
-      <c r="BS6" s="7"/>
-      <c r="BT6" s="82">
+      <c r="BV6" s="9"/>
+      <c r="BW6" s="7"/>
+      <c r="BX6" s="82">
         <v>80000</v>
       </c>
-      <c r="BU6" s="9"/>
-      <c r="BV6" s="9"/>
-      <c r="BW6" s="9"/>
-      <c r="BX6" s="9"/>
       <c r="BY6" s="9"/>
       <c r="BZ6" s="9"/>
-      <c r="CA6" s="83"/>
-    </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CA6" s="9"/>
+      <c r="CB6" s="9"/>
+      <c r="CC6" s="9"/>
+      <c r="CD6" s="9"/>
+      <c r="CE6" s="83"/>
+    </row>
+    <row r="7" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A7" s="76" t="s">
         <v>286</v>
       </c>
@@ -7399,20 +7415,20 @@
       <c r="X7" s="9">
         <v>20000</v>
       </c>
-      <c r="Y7" s="78">
+      <c r="Y7" s="9">
+        <v>20000</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>20000</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>20000</v>
+      </c>
+      <c r="AB7" s="9">
+        <v>20000</v>
+      </c>
+      <c r="AC7" s="78">
         <v>22500</v>
-      </c>
-      <c r="Z7" s="78">
-        <v>20000</v>
-      </c>
-      <c r="AA7" s="78">
-        <v>20000</v>
-      </c>
-      <c r="AB7" s="78">
-        <v>20000</v>
-      </c>
-      <c r="AC7" s="78">
-        <v>20000</v>
       </c>
       <c r="AD7" s="78">
         <v>20000</v>
@@ -7426,49 +7442,57 @@
       <c r="AG7" s="78">
         <v>20000</v>
       </c>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="9"/>
+      <c r="AH7" s="78">
+        <v>20000</v>
+      </c>
+      <c r="AI7" s="78">
+        <v>20000</v>
+      </c>
+      <c r="AJ7" s="78">
+        <v>20000</v>
+      </c>
       <c r="AK7" s="78">
         <v>20000</v>
       </c>
       <c r="AL7" s="9"/>
-      <c r="AM7" s="78">
-        <v>20000</v>
-      </c>
-      <c r="AN7" s="78">
-        <v>20000</v>
-      </c>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
       <c r="AO7" s="78">
         <v>20000</v>
       </c>
-      <c r="AP7" s="78">
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="78">
+        <v>20000</v>
+      </c>
+      <c r="AR7" s="78">
+        <v>20000</v>
+      </c>
+      <c r="AS7" s="78">
+        <v>20000</v>
+      </c>
+      <c r="AT7" s="78">
         <v>30000</v>
       </c>
-      <c r="AQ7" s="9"/>
-      <c r="AR7" s="78">
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="78">
         <v>30000</v>
       </c>
-      <c r="AS7" s="78">
+      <c r="AW7" s="78">
         <v>22500</v>
       </c>
-      <c r="AT7" s="78">
+      <c r="AX7" s="78">
         <v>20000</v>
       </c>
-      <c r="AU7" s="78">
+      <c r="AY7" s="78">
         <v>20000</v>
       </c>
-      <c r="AV7" s="78">
+      <c r="AZ7" s="78">
         <v>20000</v>
       </c>
-      <c r="AW7" s="9"/>
-      <c r="AX7" s="78">
+      <c r="BA7" s="9"/>
+      <c r="BB7" s="78">
         <v>22500</v>
       </c>
-      <c r="AY7" s="9"/>
-      <c r="AZ7" s="9"/>
-      <c r="BA7" s="9"/>
-      <c r="BB7" s="9"/>
       <c r="BC7" s="9"/>
       <c r="BD7" s="9"/>
       <c r="BE7" s="9"/>
@@ -7476,38 +7500,42 @@
       <c r="BG7" s="9"/>
       <c r="BH7" s="9"/>
       <c r="BI7" s="9"/>
-      <c r="BJ7" s="78">
+      <c r="BJ7" s="9"/>
+      <c r="BK7" s="9"/>
+      <c r="BL7" s="9"/>
+      <c r="BM7" s="9"/>
+      <c r="BN7" s="78">
         <v>20000</v>
       </c>
-      <c r="BK7" s="9"/>
-      <c r="BL7" s="78">
+      <c r="BO7" s="9"/>
+      <c r="BP7" s="78">
         <v>20000</v>
       </c>
-      <c r="BM7" s="9"/>
-      <c r="BN7" s="78"/>
-      <c r="BO7" s="9"/>
-      <c r="BP7" s="7"/>
-      <c r="BQ7" s="78">
+      <c r="BQ7" s="9"/>
+      <c r="BR7" s="78"/>
+      <c r="BS7" s="9"/>
+      <c r="BT7" s="7"/>
+      <c r="BU7" s="78">
         <v>19000</v>
       </c>
-      <c r="BR7" s="78">
+      <c r="BV7" s="78">
         <v>20000</v>
       </c>
-      <c r="BS7" s="7"/>
-      <c r="BT7" s="78">
+      <c r="BW7" s="7"/>
+      <c r="BX7" s="78">
         <v>18000</v>
       </c>
-      <c r="BU7" s="78">
+      <c r="BY7" s="78">
         <v>20000</v>
       </c>
-      <c r="BV7" s="9"/>
-      <c r="BW7" s="9"/>
-      <c r="BX7" s="9"/>
-      <c r="BY7" s="9"/>
       <c r="BZ7" s="9"/>
-      <c r="CA7" s="83"/>
-    </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CA7" s="9"/>
+      <c r="CB7" s="9"/>
+      <c r="CC7" s="9"/>
+      <c r="CD7" s="9"/>
+      <c r="CE7" s="83"/>
+    </row>
+    <row r="8" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A8" s="76" t="s">
         <v>221</v>
       </c>
@@ -7580,53 +7608,53 @@
       <c r="X8" s="9">
         <v>25</v>
       </c>
-      <c r="Y8" s="78">
+      <c r="Y8" s="9">
+        <v>25</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>25</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>25</v>
+      </c>
+      <c r="AC8" s="78">
         <v>22.5</v>
       </c>
-      <c r="Z8" s="78">
+      <c r="AD8" s="78">
         <v>17.5</v>
       </c>
-      <c r="AA8" s="78">
+      <c r="AE8" s="78">
         <v>17.5</v>
       </c>
-      <c r="AB8" s="78">
+      <c r="AF8" s="78">
         <v>25</v>
       </c>
-      <c r="AC8" s="78">
+      <c r="AG8" s="78">
         <v>15</v>
       </c>
-      <c r="AD8" s="116">
+      <c r="AH8" s="116">
         <v>17.684999999999999</v>
       </c>
-      <c r="AE8" s="116">
+      <c r="AI8" s="116">
         <v>20.889521999999999</v>
       </c>
-      <c r="AF8" s="116">
+      <c r="AJ8" s="116">
         <v>17.684999999999999</v>
       </c>
-      <c r="AG8" s="78">
+      <c r="AK8" s="78">
         <v>17.5</v>
-      </c>
-      <c r="AH8" s="78">
-        <v>25</v>
-      </c>
-      <c r="AI8" s="78">
-        <v>17</v>
-      </c>
-      <c r="AJ8" s="78">
-        <v>17</v>
-      </c>
-      <c r="AK8" s="78">
-        <v>15</v>
       </c>
       <c r="AL8" s="78">
         <v>25</v>
       </c>
       <c r="AM8" s="78">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AN8" s="78">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AO8" s="78">
         <v>15</v>
@@ -7635,13 +7663,13 @@
         <v>25</v>
       </c>
       <c r="AQ8" s="78">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AR8" s="78">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AS8" s="78">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AT8" s="78">
         <v>25</v>
@@ -7650,7 +7678,7 @@
         <v>25</v>
       </c>
       <c r="AV8" s="78">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AW8" s="78">
         <v>25</v>
@@ -7662,7 +7690,7 @@
         <v>25</v>
       </c>
       <c r="AZ8" s="78">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="BA8" s="78">
         <v>25</v>
@@ -7671,16 +7699,16 @@
         <v>25</v>
       </c>
       <c r="BC8" s="78">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="BD8" s="78">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="BE8" s="78">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="BF8" s="78">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="BG8" s="78">
         <v>23</v>
@@ -7692,59 +7720,71 @@
         <v>23</v>
       </c>
       <c r="BJ8" s="78">
+        <v>23</v>
+      </c>
+      <c r="BK8" s="78">
+        <v>23</v>
+      </c>
+      <c r="BL8" s="78">
+        <v>23</v>
+      </c>
+      <c r="BM8" s="78">
+        <v>23</v>
+      </c>
+      <c r="BN8" s="78">
         <v>25</v>
       </c>
-      <c r="BK8" s="78">
+      <c r="BO8" s="78">
         <v>25</v>
       </c>
-      <c r="BL8" s="78">
+      <c r="BP8" s="78">
         <v>20</v>
       </c>
-      <c r="BM8" s="84">
+      <c r="BQ8" s="84">
         <v>23</v>
       </c>
-      <c r="BN8" s="78">
+      <c r="BR8" s="78">
         <v>21.75</v>
       </c>
-      <c r="BO8" s="7"/>
-      <c r="BP8" s="85">
+      <c r="BS8" s="7"/>
+      <c r="BT8" s="85">
         <v>23</v>
       </c>
-      <c r="BQ8" s="78">
+      <c r="BU8" s="78">
         <v>22</v>
       </c>
-      <c r="BR8" s="81">
+      <c r="BV8" s="81">
         <v>17.62</v>
       </c>
-      <c r="BS8" s="85">
+      <c r="BW8" s="85">
         <v>17.68</v>
       </c>
-      <c r="BT8" s="78">
+      <c r="BX8" s="78">
         <v>20</v>
       </c>
-      <c r="BU8" s="78">
+      <c r="BY8" s="78">
         <v>17.62</v>
-      </c>
-      <c r="BV8" s="78">
-        <v>24</v>
-      </c>
-      <c r="BW8" s="78">
-        <v>15</v>
-      </c>
-      <c r="BX8" s="78">
-        <v>15</v>
-      </c>
-      <c r="BY8" s="78">
-        <v>21</v>
       </c>
       <c r="BZ8" s="78">
         <v>24</v>
       </c>
-      <c r="CA8" s="86">
+      <c r="CA8" s="78">
+        <v>15</v>
+      </c>
+      <c r="CB8" s="78">
+        <v>15</v>
+      </c>
+      <c r="CC8" s="78">
+        <v>21</v>
+      </c>
+      <c r="CD8" s="78">
+        <v>24</v>
+      </c>
+      <c r="CE8" s="86">
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A9" s="87" t="s">
         <v>222</v>
       </c>
@@ -7777,9 +7817,7 @@
       <c r="V9" s="88"/>
       <c r="W9" s="88"/>
       <c r="X9" s="88"/>
-      <c r="Y9" s="89">
-        <v>8</v>
-      </c>
+      <c r="Y9" s="88"/>
       <c r="Z9" s="88"/>
       <c r="AA9" s="88"/>
       <c r="AB9" s="88"/>
@@ -7789,50 +7827,44 @@
       <c r="AD9" s="88"/>
       <c r="AE9" s="88"/>
       <c r="AF9" s="88"/>
-      <c r="AG9" s="88"/>
+      <c r="AG9" s="89">
+        <v>8</v>
+      </c>
       <c r="AH9" s="88"/>
       <c r="AI9" s="88"/>
       <c r="AJ9" s="88"/>
-      <c r="AK9" s="89">
-        <v>8</v>
-      </c>
-      <c r="AL9" s="89">
-        <v>8</v>
-      </c>
-      <c r="AM9" s="89">
-        <v>8</v>
-      </c>
-      <c r="AN9" s="89">
-        <v>8</v>
-      </c>
+      <c r="AK9" s="88"/>
+      <c r="AL9" s="88"/>
+      <c r="AM9" s="88"/>
+      <c r="AN9" s="88"/>
       <c r="AO9" s="89">
         <v>8</v>
       </c>
-      <c r="AP9" s="88"/>
-      <c r="AQ9" s="88"/>
-      <c r="AR9" s="88"/>
-      <c r="AS9" s="90"/>
-      <c r="AT9" s="90"/>
-      <c r="AU9" s="90"/>
+      <c r="AP9" s="89">
+        <v>8</v>
+      </c>
+      <c r="AQ9" s="89">
+        <v>8</v>
+      </c>
+      <c r="AR9" s="89">
+        <v>8</v>
+      </c>
+      <c r="AS9" s="89">
+        <v>8</v>
+      </c>
+      <c r="AT9" s="88"/>
+      <c r="AU9" s="88"/>
       <c r="AV9" s="88"/>
-      <c r="AW9" s="89">
-        <v>8</v>
-      </c>
-      <c r="AX9" s="88"/>
-      <c r="AY9" s="88"/>
+      <c r="AW9" s="90"/>
+      <c r="AX9" s="90"/>
+      <c r="AY9" s="90"/>
       <c r="AZ9" s="88"/>
       <c r="BA9" s="89">
         <v>8</v>
       </c>
-      <c r="BB9" s="89">
-        <v>8</v>
-      </c>
-      <c r="BC9" s="89">
-        <v>8</v>
-      </c>
-      <c r="BD9" s="89">
-        <v>8</v>
-      </c>
+      <c r="BB9" s="88"/>
+      <c r="BC9" s="88"/>
+      <c r="BD9" s="88"/>
       <c r="BE9" s="89">
         <v>8</v>
       </c>
@@ -7848,37 +7880,49 @@
       <c r="BI9" s="89">
         <v>8</v>
       </c>
-      <c r="BJ9" s="88"/>
-      <c r="BK9" s="88"/>
-      <c r="BL9" s="88">
+      <c r="BJ9" s="89">
+        <v>8</v>
+      </c>
+      <c r="BK9" s="89">
+        <v>8</v>
+      </c>
+      <c r="BL9" s="89">
+        <v>8</v>
+      </c>
+      <c r="BM9" s="89">
+        <v>8</v>
+      </c>
+      <c r="BN9" s="88"/>
+      <c r="BO9" s="88"/>
+      <c r="BP9" s="88">
         <v>5</v>
       </c>
-      <c r="BM9" s="91">
+      <c r="BQ9" s="91">
         <v>8</v>
       </c>
-      <c r="BN9" s="88"/>
-      <c r="BO9" s="90"/>
-      <c r="BP9" s="90"/>
-      <c r="BQ9" s="88"/>
       <c r="BR9" s="88"/>
       <c r="BS9" s="90"/>
-      <c r="BT9" s="88"/>
+      <c r="BT9" s="90"/>
       <c r="BU9" s="88"/>
       <c r="BV9" s="88"/>
-      <c r="BW9" s="88">
-        <v>8</v>
-      </c>
+      <c r="BW9" s="90"/>
       <c r="BX9" s="88"/>
       <c r="BY9" s="88"/>
       <c r="BZ9" s="88"/>
-      <c r="CA9" s="92"/>
-    </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CA9" s="88">
+        <v>8</v>
+      </c>
+      <c r="CB9" s="88"/>
+      <c r="CC9" s="88"/>
+      <c r="CD9" s="88"/>
+      <c r="CE9" s="92"/>
+    </row>
+    <row r="11" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.35">
       <c r="B12" s="152" t="s">
         <v>289</v>
       </c>
@@ -7896,7 +7940,7 @@
       <c r="L12" s="97"/>
       <c r="M12" s="98"/>
     </row>
-    <row r="13" spans="1:79" ht="39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:83" ht="39.5" x14ac:dyDescent="0.35">
       <c r="B13" s="153"/>
       <c r="C13" s="99" t="s">
         <v>1</v>
@@ -7932,7 +7976,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A14" s="110" t="s">
         <v>22</v>
       </c>
@@ -7973,7 +8017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A15" s="76" t="s">
         <v>23</v>
       </c>
@@ -8014,7 +8058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A16" s="76" t="s">
         <v>7</v>
       </c>
@@ -8055,7 +8099,7 @@
         <v>76.151387532990128</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="76" t="s">
         <v>24</v>
       </c>
@@ -8096,7 +8140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="76" t="s">
         <v>25</v>
       </c>
@@ -8137,7 +8181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="76" t="s">
         <v>26</v>
       </c>
@@ -8178,7 +8222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -8219,7 +8263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
@@ -8260,7 +8304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="76" t="s">
         <v>29</v>
       </c>
@@ -8301,7 +8345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="76" t="s">
         <v>30</v>
       </c>
@@ -8342,7 +8386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="87" t="s">
         <v>31</v>
       </c>
@@ -8383,7 +8427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="110"/>
       <c r="B25" s="152" t="s">
         <v>289</v>
@@ -8402,7 +8446,7 @@
       <c r="L25" s="97"/>
       <c r="M25" s="98"/>
     </row>
-    <row r="26" spans="1:13" ht="39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A26" s="76"/>
       <c r="B26" s="153"/>
       <c r="C26" s="99" t="s">
@@ -8439,7 +8483,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="110" t="s">
         <v>22</v>
       </c>
@@ -8480,7 +8524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="76" t="s">
         <v>23</v>
       </c>
@@ -8521,7 +8565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="76" t="s">
         <v>7</v>
       </c>
@@ -8562,7 +8606,7 @@
         <v>95.950748291567578</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="76" t="s">
         <v>24</v>
       </c>
@@ -8603,7 +8647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="76" t="s">
         <v>25</v>
       </c>
@@ -8644,7 +8688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="76" t="s">
         <v>26</v>
       </c>
@@ -8685,7 +8729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -8726,7 +8770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -8767,7 +8811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="76" t="s">
         <v>29</v>
       </c>
@@ -8808,7 +8852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="76" t="s">
         <v>30</v>
       </c>
@@ -8849,7 +8893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="87" t="s">
         <v>31</v>
       </c>
@@ -8907,9 +8951,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -8917,7 +8961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="112" t="s">
         <v>8</v>
       </c>
@@ -8928,7 +8972,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="112" t="s">
         <v>9</v>
       </c>
@@ -8939,7 +8983,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="112" t="s">
         <v>10</v>
       </c>
@@ -8950,7 +8994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="112" t="s">
         <v>11</v>
       </c>
@@ -8961,7 +9005,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="112" t="s">
         <v>12</v>
       </c>
@@ -8972,7 +9016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="112" t="s">
         <v>13</v>
       </c>
@@ -8997,12 +9041,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -9010,7 +9054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -9021,7 +9065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -9032,7 +9076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -9043,7 +9087,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -9054,7 +9098,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -9065,7 +9109,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -9085,21 +9129,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -9170,7 +9214,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="118" t="s">
         <v>122</v>
       </c>
@@ -9244,7 +9288,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -9318,7 +9362,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -9392,7 +9436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -9466,7 +9510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -9540,7 +9584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9614,7 +9658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -9688,7 +9732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -9762,7 +9806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -9836,7 +9880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -9910,7 +9954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -9984,7 +10028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -10058,7 +10102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -10132,7 +10176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -10206,7 +10250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -10280,7 +10324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -10354,7 +10398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -10428,7 +10472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -10502,7 +10546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -10576,12 +10620,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="76" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="142" t="s">
         <v>376</v>
       </c>
@@ -10655,7 +10699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" s="142" t="s">
         <v>377</v>
       </c>
@@ -10729,7 +10773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" s="142" t="s">
         <v>378</v>
       </c>
@@ -10803,7 +10847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="142" t="s">
         <v>379</v>
       </c>
@@ -10877,7 +10921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" s="142" t="s">
         <v>380</v>
       </c>
@@ -10951,7 +10995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" s="142" t="s">
         <v>381</v>
       </c>
@@ -11025,7 +11069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="142" t="s">
         <v>382</v>
       </c>
@@ -11099,7 +11143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" s="143" t="s">
         <v>383</v>
       </c>
@@ -11173,10 +11217,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -11193,7 +11237,7 @@
       </c>
       <c r="H31" s="35"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -11207,7 +11251,7 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -11221,7 +11265,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -11235,7 +11279,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -11249,7 +11293,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -11263,7 +11307,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -11277,7 +11321,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -11291,7 +11335,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -11305,7 +11349,7 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -11319,7 +11363,7 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -11333,7 +11377,7 @@
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -11347,7 +11391,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -11361,7 +11405,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -11393,17 +11437,17 @@
       <selection pane="topRight" activeCell="BO24" sqref="BO24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
         <v>308</v>
@@ -11613,7 +11657,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:70" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
@@ -11825,7 +11869,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -12037,7 +12081,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -12249,7 +12293,7 @@
         <v>29.226475858183772</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -12461,7 +12505,7 @@
         <v>27.68007234257048</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -12673,7 +12717,7 @@
         <v>2.1637867344060759</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -12885,7 +12929,7 @@
         <v>18.983121758092206</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -13097,7 +13141,7 @@
         <v>6.5331638500721958</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -13309,7 +13353,7 @@
         <v>1.2931339474403903E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>59</v>
       </c>
@@ -13348,7 +13392,7 @@
       <c r="AJ10" s="137"/>
       <c r="AK10" s="145"/>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>60</v>
       </c>
@@ -13560,7 +13604,7 @@
         <v>1.5369575444769657E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>61</v>
       </c>
@@ -13772,7 +13816,7 @@
         <v>2.3767403603346744E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>62</v>
       </c>
@@ -13984,7 +14028,7 @@
         <v>6.3420799050257172E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -14196,7 +14240,7 @@
         <v>1.3985631716786429E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>64</v>
       </c>
@@ -14408,7 +14452,7 @@
         <v>1.1023100446641545E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
@@ -14620,7 +14664,7 @@
         <v>1.4622443754029444E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>66</v>
       </c>
@@ -14832,7 +14876,7 @@
         <v>6.2816299281138246E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>67</v>
       </c>
@@ -15044,7 +15088,7 @@
         <v>1.384465768977587E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>68</v>
       </c>
@@ -15256,7 +15300,7 @@
         <v>4.4791265345305257E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -15468,7 +15512,7 @@
         <v>4.3182873037403548E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
         <v>70</v>
       </c>
@@ -15680,7 +15724,7 @@
         <v>1.8656888381642496</v>
       </c>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A22" s="76" t="s">
         <v>375</v>
       </c>
@@ -15724,7 +15768,7 @@
       <c r="AT22" s="64"/>
       <c r="AU22" s="64"/>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" s="142" t="s">
         <v>376</v>
       </c>
@@ -15936,7 +15980,7 @@
         <v>3.5515149979386286E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A24" s="142" t="s">
         <v>377</v>
       </c>
@@ -16148,7 +16192,7 @@
         <v>1.090336568096634E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A25" s="142" t="s">
         <v>378</v>
       </c>
@@ -16360,7 +16404,7 @@
         <v>3.3685121043801309E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A26" s="142" t="s">
         <v>379</v>
       </c>
@@ -16572,7 +16616,7 @@
         <v>2.702203671489133E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A27" s="142" t="s">
         <v>380</v>
       </c>
@@ -16784,7 +16828,7 @@
         <v>2.3849770757134076E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A28" s="142" t="s">
         <v>381</v>
       </c>
@@ -16996,7 +17040,7 @@
         <v>1.9778305848322815E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A29" s="142" t="s">
         <v>382</v>
       </c>
@@ -17208,7 +17252,7 @@
         <v>2.6907087561252384E-6</v>
       </c>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A30" s="143" t="s">
         <v>383</v>
       </c>
@@ -17420,12 +17464,12 @@
         <v>8.1834506459948039E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
       <c r="AH31" s="137"/>
       <c r="AJ31" s="137"/>
       <c r="AK31" s="145"/>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -17588,9 +17632,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -17598,7 +17642,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -17607,7 +17651,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -17616,7 +17660,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -17625,7 +17669,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -17634,7 +17678,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="34" t="s">
         <v>79</v>
       </c>
@@ -17655,9 +17699,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -17707,7 +17751,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="78.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
@@ -17757,7 +17801,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -17810,7 +17854,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="112" t="s">
         <v>8</v>
       </c>
@@ -17861,7 +17905,7 @@
       </c>
       <c r="Q4" s="114"/>
     </row>
-    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="112" t="s">
         <v>9</v>
       </c>
@@ -17912,7 +17956,7 @@
       </c>
       <c r="Q5" s="114"/>
     </row>
-    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="112" t="s">
         <v>10</v>
       </c>
@@ -17963,7 +18007,7 @@
       </c>
       <c r="Q6" s="114"/>
     </row>
-    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="112" t="s">
         <v>11</v>
       </c>
@@ -18014,7 +18058,7 @@
       </c>
       <c r="Q7" s="114"/>
     </row>
-    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="112" t="s">
         <v>12</v>
       </c>
@@ -18065,7 +18109,7 @@
       </c>
       <c r="Q8" s="114"/>
     </row>
-    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="112" t="s">
         <v>13</v>
       </c>
@@ -18116,7 +18160,7 @@
       </c>
       <c r="Q9" s="114"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -18167,7 +18211,7 @@
       </c>
       <c r="Q10" s="67"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -18218,7 +18262,7 @@
       </c>
       <c r="Q11" s="67"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -18269,7 +18313,7 @@
       </c>
       <c r="Q12" s="67"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -18320,7 +18364,7 @@
       </c>
       <c r="Q13" s="67"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -18371,7 +18415,7 @@
       </c>
       <c r="Q14" s="67"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
@@ -18422,7 +18466,7 @@
       </c>
       <c r="Q15" s="67"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -18473,7 +18517,7 @@
       </c>
       <c r="Q16" s="67"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -18524,7 +18568,7 @@
       </c>
       <c r="Q17" s="67"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -18575,7 +18619,7 @@
       </c>
       <c r="Q18" s="67"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -18626,7 +18670,7 @@
       </c>
       <c r="Q19" s="67"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -18681,7 +18725,7 @@
         <v>3.3478260869565215</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -18695,11 +18739,11 @@
       <c r="N21" s="64"/>
       <c r="O21" s="64"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="M22" s="64"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -18741,14 +18785,14 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>297</v>
       </c>
@@ -18759,7 +18803,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -18773,7 +18817,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>125</v>
       </c>
@@ -18787,7 +18831,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -18801,7 +18845,7 @@
         <v>362403.00757167325</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -18815,7 +18859,7 @@
         <v>344979.42656462023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -18829,7 +18873,7 @@
         <v>24381.856026689315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -18843,7 +18887,7 @@
         <v>254462.26606022959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -18857,7 +18901,7 @@
         <v>66135.304477701342</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -18871,7 +18915,7 @@
         <v>59.889274923371126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -18885,7 +18929,7 @@
         <v>24.470884336712146</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -18899,7 +18943,7 @@
         <v>34.134614130073174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -18913,7 +18957,7 @@
         <v>-15.759603589368934</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -18927,7 +18971,7 @@
         <v>8.6858851249063438</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -18941,7 +18985,7 @@
         <v>6.9883164862451217</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -18955,7 +18999,7 @@
         <v>58.328462296040968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -18969,7 +19013,7 @@
         <v>0.49662761207225459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -18983,7 +19027,7 @@
         <v>1.1283578872130025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -18997,7 +19041,7 @@
         <v>57.127332585038609</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -19011,7 +19055,7 @@
         <v>-82.715827114534676</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -19025,12 +19069,12 @@
         <v>22763.019075759898</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="76" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="142" t="s">
         <v>376</v>
       </c>
@@ -19044,7 +19088,7 @@
         <v>0.37034943531993869</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="142" t="s">
         <v>377</v>
       </c>
@@ -19058,7 +19102,7 @@
         <v>1.274407618987647</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="142" t="s">
         <v>378</v>
       </c>
@@ -19072,7 +19116,7 @@
         <v>3.1302091249900932</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="142" t="s">
         <v>379</v>
       </c>
@@ -19086,7 +19130,7 @@
         <v>0.24682227388035821</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="142" t="s">
         <v>380</v>
       </c>
@@ -19100,7 +19144,7 @@
         <v>0.21415419754922327</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="142" t="s">
         <v>381</v>
       </c>
@@ -19114,7 +19158,7 @@
         <v>1.7961904743782098</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="142" t="s">
         <v>382</v>
       </c>
@@ -19128,7 +19172,7 @@
         <v>2.2352473934910237E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="143" t="s">
         <v>383</v>
       </c>
@@ -19142,7 +19186,7 @@
         <v>7.0223242933031296E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -19166,9 +19210,9 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -19176,7 +19220,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>93</v>
       </c>
@@ -19184,7 +19228,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="62" t="s">
         <v>94</v>
       </c>
@@ -19192,7 +19236,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="62" t="s">
         <v>335</v>
       </c>
@@ -19200,7 +19244,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
         <v>95</v>
       </c>
@@ -19208,7 +19252,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
         <v>293</v>
       </c>
@@ -19216,7 +19260,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
         <v>97</v>
       </c>
@@ -19224,7 +19268,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
         <v>98</v>
       </c>
@@ -19232,7 +19276,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="62" t="s">
         <v>99</v>
       </c>
@@ -19240,7 +19284,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="62" t="s">
         <v>100</v>
       </c>
@@ -19248,7 +19292,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
         <v>101</v>
       </c>
@@ -19256,7 +19300,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="62" t="s">
         <v>103</v>
       </c>
@@ -19264,7 +19308,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="62" t="s">
         <v>104</v>
       </c>
@@ -19272,7 +19316,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="62" t="s">
         <v>105</v>
       </c>
@@ -19280,7 +19324,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="62" t="s">
         <v>106</v>
       </c>
@@ -19288,7 +19332,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="62" t="s">
         <v>107</v>
       </c>
@@ -19296,7 +19340,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="62" t="s">
         <v>108</v>
       </c>
@@ -19304,7 +19348,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="62" t="s">
         <v>109</v>
       </c>
@@ -19312,7 +19356,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="62" t="s">
         <v>110</v>
       </c>
@@ -19320,7 +19364,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="126" t="s">
         <v>336</v>
       </c>
@@ -19328,7 +19372,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="62" t="s">
         <v>112</v>
       </c>
@@ -19336,7 +19380,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="62" t="s">
         <v>113</v>
       </c>
@@ -19344,7 +19388,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="62" t="s">
         <v>114</v>
       </c>
@@ -19352,7 +19396,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="62" t="s">
         <v>115</v>
       </c>
@@ -19360,7 +19404,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="62" t="s">
         <v>116</v>
       </c>
@@ -19381,12 +19425,12 @@
       <selection activeCell="A45" sqref="A45:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="68" t="s">
         <v>186</v>
       </c>
@@ -19394,7 +19438,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -19405,7 +19449,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -19416,7 +19460,7 @@
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="69" t="s">
         <v>127</v>
       </c>
@@ -19427,7 +19471,7 @@
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="69" t="s">
         <v>128</v>
       </c>
@@ -19438,7 +19482,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="69" t="s">
         <v>129</v>
       </c>
@@ -19449,7 +19493,7 @@
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="69" t="s">
         <v>130</v>
       </c>
@@ -19460,7 +19504,7 @@
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="69" t="s">
         <v>131</v>
       </c>
@@ -19471,7 +19515,7 @@
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="69" t="s">
         <v>132</v>
       </c>
@@ -19482,7 +19526,7 @@
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="69" t="s">
         <v>133</v>
       </c>
@@ -19493,7 +19537,7 @@
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="69" t="s">
         <v>134</v>
       </c>
@@ -19504,7 +19548,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -19515,7 +19559,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="69" t="s">
         <v>136</v>
       </c>
@@ -19526,7 +19570,7 @@
         <v>749.07638827065296</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="69" t="s">
         <v>137</v>
       </c>
@@ -19537,7 +19581,7 @@
         <v>755.86244135709444</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="69" t="s">
         <v>138</v>
       </c>
@@ -19548,7 +19592,7 @@
         <v>762.55920427134606</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="69" t="s">
         <v>139</v>
       </c>
@@ -19559,7 +19603,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="69" t="s">
         <v>140</v>
       </c>
@@ -19570,7 +19614,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="69" t="s">
         <v>141</v>
       </c>
@@ -19581,7 +19625,7 @@
         <v>836.63306309407369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="68" t="s">
         <v>1</v>
       </c>
@@ -19592,7 +19636,7 @@
         <v>846.93577526984518</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -19603,7 +19647,7 @@
         <v>725.15243391008278</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -19614,7 +19658,7 @@
         <v>748.62596861099109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -19625,7 +19669,7 @@
         <v>801.99999999999989</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -19636,7 +19680,7 @@
         <v>791.99999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -19647,7 +19691,7 @@
         <v>700.32025584540236</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -19658,7 +19702,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -19669,7 +19713,7 @@
         <v>991.17374573064865</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -19680,7 +19724,7 @@
         <v>794.1013538556316</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -19691,7 +19735,7 @@
         <v>789.34625592835232</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -19702,7 +19746,7 @@
         <v>809.68750817282455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -19713,7 +19757,7 @@
         <v>783.00612535864673</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -19724,7 +19768,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -19735,7 +19779,7 @@
         <v>508.00296189766453</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>155</v>
       </c>
@@ -19746,7 +19790,7 @@
         <v>428.22298556220187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -19757,7 +19801,7 @@
         <v>665.18536560495022</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -19768,7 +19812,7 @@
         <v>859.88020851632757</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -19779,7 +19823,7 @@
         <v>887.88245186586084</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -19790,7 +19834,7 @@
         <v>797.00724703341325</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -19801,7 +19845,7 @@
         <v>748.92792354647884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -19812,7 +19856,7 @@
         <v>778.77937164550963</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>162</v>
       </c>
@@ -19823,7 +19867,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -19834,7 +19878,7 @@
         <v>798.04417121416941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -19845,7 +19889,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>337</v>
       </c>
@@ -19856,7 +19900,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>338</v>
       </c>
@@ -19867,7 +19911,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>371</v>
       </c>
@@ -19878,7 +19922,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>372</v>
       </c>
@@ -19889,7 +19933,7 @@
         <v>793.37856525946859</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>164</v>
       </c>
@@ -19900,7 +19944,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>165</v>
       </c>
@@ -19911,7 +19955,7 @@
         <v>716.69892648380858</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>166</v>
       </c>
@@ -19922,7 +19966,7 @@
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>167</v>
       </c>
@@ -19933,7 +19977,7 @@
         <v>756.99999999999989</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -19944,7 +19988,7 @@
         <v>70.798124695046326</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -19955,7 +19999,7 @@
         <v>742.58779297677324</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -19966,7 +20010,7 @@
         <v>742.32362086970215</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -19977,7 +20021,7 @@
         <v>769.53334789802227</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -19988,7 +20032,7 @@
         <v>584.61287294827434</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>173</v>
       </c>
@@ -19999,7 +20043,7 @@
         <v>559.51652277652283</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -20010,7 +20054,7 @@
         <v>595.17975723111715</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -20021,7 +20065,7 @@
         <v>507.21044557645126</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>176</v>
       </c>
@@ -20032,7 +20076,7 @@
         <v>668.88377510394514</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>177</v>
       </c>
@@ -20043,7 +20087,7 @@
         <v>654.80340179705718</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>178</v>
       </c>
@@ -20054,7 +20098,7 @@
         <v>688.85095964480468</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -20065,7 +20109,7 @@
         <v>737.59071339941693</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>180</v>
       </c>
@@ -20076,7 +20120,7 @@
         <v>765.47381512866104</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -20087,7 +20131,7 @@
         <v>731.67589538225809</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>182</v>
       </c>
@@ -20098,7 +20142,7 @@
         <v>800.00032424653136</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>183</v>
       </c>
@@ -20109,7 +20153,7 @@
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -20120,7 +20164,7 @@
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>188</v>
       </c>
@@ -20131,7 +20175,7 @@
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="68" t="s">
         <v>89</v>
       </c>
@@ -20142,7 +20186,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="140" t="s">
         <v>366</v>
       </c>
@@ -20153,7 +20197,7 @@
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -20164,7 +20208,7 @@
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -20175,7 +20219,7 @@
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -20183,7 +20227,7 @@
         <v>22.648458746153963</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>192</v>
       </c>
@@ -20191,7 +20235,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>193</v>
       </c>
@@ -20199,7 +20243,7 @@
         <v>18.707371337693861</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>194</v>
       </c>
@@ -20207,7 +20251,7 @@
         <v>12.566427590816895</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>195</v>
       </c>
@@ -20215,7 +20259,7 @@
         <v>26.329529071139479</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -20223,7 +20267,7 @@
         <v>11.566786665057547</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>197</v>
       </c>
@@ -20231,7 +20275,7 @@
         <v>31.342185540824094</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>198</v>
       </c>
@@ -20239,7 +20283,7 @@
         <v>31.0106439692332</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>199</v>
       </c>
@@ -20247,7 +20291,7 @@
         <v>28.609127685562171</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>200</v>
       </c>
@@ -20255,7 +20299,7 @@
         <v>33.012627597074328</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>201</v>
       </c>
@@ -20263,7 +20307,7 @@
         <v>17.905547955535493</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>202</v>
       </c>
@@ -20271,7 +20315,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -20279,7 +20323,7 @@
         <v>16.801860958276258</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>204</v>
       </c>
@@ -20287,7 +20331,7 @@
         <v>17.842745955691449</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>205</v>
       </c>
@@ -20295,7 +20339,7 @@
         <v>17.11470795749937</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>206</v>
       </c>
@@ -20303,7 +20347,7 @@
         <v>20.107106950068403</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>207</v>
       </c>
@@ -20311,7 +20355,7 @@
         <v>18.52542695399616</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>208</v>
       </c>
@@ -20319,7 +20363,7 @@
         <v>17.444999956679162</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -20327,7 +20371,7 @@
         <v>15.647058823529411</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>210</v>
       </c>
@@ -20335,7 +20379,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>211</v>
       </c>
@@ -20343,7 +20387,7 @@
         <v>22.000366940104676</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>212</v>
       </c>
@@ -20351,7 +20395,7 @@
         <v>14.864999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>213</v>
       </c>
@@ -20359,7 +20403,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>214</v>
       </c>
@@ -20367,7 +20411,7 @@
         <v>16.758749999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>215</v>
       </c>
@@ -20375,7 +20419,7 @@
         <v>13.036809815950916</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>216</v>
       </c>
@@ -20383,7 +20427,7 @@
         <v>16.462585034013607</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="68" t="s">
         <v>219</v>
       </c>
@@ -20391,7 +20435,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
1. Updated biomass inventory data for biochem pathways; 2. Fixed typos in the files (bichem to biochem)
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AB66B8-D5E6-4911-8FE7-6C14E7642863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CF7654-108A-470D-A13F-0AF65DFD8E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
@@ -1312,9 +1312,6 @@
     <t>GGE</t>
   </si>
   <si>
-    <t>Renewable Diesel - Bichem (BDO)</t>
-  </si>
-  <si>
     <t>Renewable Diesel - Biochem (Acids)</t>
   </si>
   <si>
@@ -1466,6 +1463,9 @@
   </si>
   <si>
     <t>Functional Unit</t>
+  </si>
+  <si>
+    <t>Renewable Diesel - Biochem (BDO)</t>
   </si>
 </sst>
 </file>
@@ -2824,7 +2824,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AW3" sqref="AW3:AY3"/>
+      <selection pane="topRight" activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2950,40 +2950,40 @@
         <v>242</v>
       </c>
       <c r="AN1" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AR1" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AS1" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="AQ1" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="AR1" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="AS1" s="6" t="s">
-        <v>332</v>
-      </c>
       <c r="AT1" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="AW1" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AX1" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AY1" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="AW1" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="AX1" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="AY1" s="6" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:51" ht="78.5" x14ac:dyDescent="0.35">
@@ -3012,10 +3012,10 @@
         <v>305</v>
       </c>
       <c r="J2" s="65" t="s">
+        <v>376</v>
+      </c>
+      <c r="K2" s="65" t="s">
         <v>377</v>
-      </c>
-      <c r="K2" s="65" t="s">
-        <v>378</v>
       </c>
       <c r="L2" s="65" t="s">
         <v>82</v>
@@ -3042,10 +3042,10 @@
         <v>322</v>
       </c>
       <c r="T2" s="65" t="s">
+        <v>376</v>
+      </c>
+      <c r="U2" s="65" t="s">
         <v>377</v>
-      </c>
-      <c r="U2" s="65" t="s">
-        <v>378</v>
       </c>
       <c r="V2" s="65" t="s">
         <v>82</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>109</v>
@@ -7063,16 +7063,16 @@
         <v>242</v>
       </c>
       <c r="X5" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y5" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="Y5" s="17" t="s">
-        <v>332</v>
-      </c>
       <c r="Z5" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="AA5" s="17" t="s">
         <v>363</v>
-      </c>
-      <c r="AA5" s="17" t="s">
-        <v>364</v>
       </c>
       <c r="AB5" s="17" t="s">
         <v>164</v>
@@ -7150,7 +7150,7 @@
         <v>260</v>
       </c>
       <c r="BA5" s="137" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BB5" s="17" t="s">
         <v>261</v>
@@ -7949,7 +7949,7 @@
     </row>
     <row r="11" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:83" x14ac:dyDescent="0.35">
@@ -7957,7 +7957,7 @@
         <v>289</v>
       </c>
       <c r="C12" s="96" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D12" s="97"/>
       <c r="E12" s="97"/>
@@ -8463,7 +8463,7 @@
         <v>289</v>
       </c>
       <c r="C25" s="96" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
@@ -9181,7 +9181,7 @@
         <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E1" t="s">
         <v>325</v>
@@ -9196,10 +9196,10 @@
         <v>242</v>
       </c>
       <c r="I1" t="s">
+        <v>382</v>
+      </c>
+      <c r="J1" t="s">
         <v>331</v>
-      </c>
-      <c r="J1" t="s">
-        <v>332</v>
       </c>
       <c r="K1" t="s">
         <v>312</v>
@@ -9246,7 +9246,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s">
         <v>109</v>
@@ -10578,12 +10578,12 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" s="76" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="138" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B21">
         <v>2.7655646829798428</v>
@@ -10657,7 +10657,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="138" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B22">
         <v>1.8625224624391841</v>
@@ -10731,7 +10731,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" s="138" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B23">
         <v>2.8473649419529896</v>
@@ -10805,7 +10805,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" s="138" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B24">
         <v>0.49856107045690662</v>
@@ -10879,7 +10879,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="138" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B25">
         <v>0.42888718671683485</v>
@@ -10953,7 +10953,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" s="138" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B26">
         <v>1.0198572582099572</v>
@@ -11027,7 +11027,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" s="138" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B27">
         <v>5.4460967964926707E-2</v>
@@ -11101,7 +11101,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="139" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B28">
         <v>7.7076176183809256E-2</v>
@@ -11184,7 +11184,7 @@
         <v>123</v>
       </c>
       <c r="C30" s="147" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D30" s="147"/>
       <c r="E30" s="147"/>
@@ -11502,7 +11502,7 @@
         <v>89</v>
       </c>
       <c r="AH1" s="134" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AI1" s="117" t="s">
         <v>300</v>
@@ -11529,85 +11529,85 @@
         <v>317</v>
       </c>
       <c r="AQ1" t="s">
+        <v>333</v>
+      </c>
+      <c r="AR1" t="s">
         <v>334</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>335</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>336</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>337</v>
       </c>
-      <c r="AU1" t="s">
-        <v>338</v>
-      </c>
       <c r="AV1" s="131" t="s">
+        <v>340</v>
+      </c>
+      <c r="AW1" s="131" t="s">
         <v>341</v>
       </c>
-      <c r="AW1" s="131" t="s">
+      <c r="AX1" s="131" t="s">
         <v>342</v>
       </c>
-      <c r="AX1" s="131" t="s">
+      <c r="AY1" s="132" t="s">
         <v>343</v>
       </c>
-      <c r="AY1" s="132" t="s">
+      <c r="AZ1" s="132" t="s">
         <v>344</v>
       </c>
-      <c r="AZ1" s="132" t="s">
+      <c r="BA1" s="132" t="s">
         <v>345</v>
       </c>
-      <c r="BA1" s="132" t="s">
+      <c r="BB1" s="132" t="s">
         <v>346</v>
       </c>
-      <c r="BB1" s="132" t="s">
+      <c r="BC1" s="132" t="s">
         <v>347</v>
       </c>
-      <c r="BC1" s="132" t="s">
+      <c r="BD1" s="132" t="s">
         <v>348</v>
       </c>
-      <c r="BD1" s="132" t="s">
+      <c r="BE1" s="132" t="s">
         <v>349</v>
       </c>
-      <c r="BE1" s="132" t="s">
+      <c r="BF1" s="132" t="s">
         <v>350</v>
       </c>
-      <c r="BF1" s="132" t="s">
+      <c r="BG1" s="132" t="s">
         <v>351</v>
       </c>
-      <c r="BG1" s="132" t="s">
+      <c r="BH1" s="132" t="s">
         <v>352</v>
       </c>
-      <c r="BH1" s="132" t="s">
+      <c r="BI1" s="132" t="s">
         <v>353</v>
       </c>
-      <c r="BI1" s="132" t="s">
+      <c r="BJ1" s="132" t="s">
+        <v>359</v>
+      </c>
+      <c r="BK1" s="132" t="s">
         <v>354</v>
       </c>
-      <c r="BJ1" s="132" t="s">
-        <v>360</v>
-      </c>
-      <c r="BK1" s="132" t="s">
+      <c r="BL1" s="132" t="s">
         <v>355</v>
       </c>
-      <c r="BL1" s="132" t="s">
+      <c r="BM1" s="132" t="s">
         <v>356</v>
       </c>
-      <c r="BM1" s="132" t="s">
+      <c r="BN1" t="s">
         <v>357</v>
       </c>
-      <c r="BN1" t="s">
-        <v>358</v>
-      </c>
       <c r="BO1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="BP1" t="s">
+        <v>364</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>365</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>366</v>
       </c>
       <c r="BR1" t="s">
         <v>50</v>
@@ -11615,7 +11615,7 @@
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>93</v>
@@ -15470,7 +15470,7 @@
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A21" s="76" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
@@ -15514,7 +15514,7 @@
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A22" s="138" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B22" s="22">
         <v>1.6475121459595702E-6</v>
@@ -15726,7 +15726,7 @@
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" s="138" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B23" s="22">
         <v>3.0399408312257672E-6</v>
@@ -15938,7 +15938,7 @@
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A24" s="138" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B24" s="22">
         <v>1.7869631031761375E-5</v>
@@ -16150,7 +16150,7 @@
     </row>
     <row r="25" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A25" s="138" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B25" s="22">
         <v>1.3358914550832159E-6</v>
@@ -16362,7 +16362,7 @@
     </row>
     <row r="26" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A26" s="138" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B26" s="22">
         <v>1.2100049326248854E-6</v>
@@ -16574,7 +16574,7 @@
     </row>
     <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A27" s="138" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B27" s="22">
         <v>9.1315061995251688E-6</v>
@@ -16786,7 +16786,7 @@
     </row>
     <row r="28" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A28" s="138" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B28" s="22">
         <v>1.5662485543207782E-7</v>
@@ -16998,7 +16998,7 @@
     </row>
     <row r="29" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A29" s="139" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B29" s="30">
         <v>4.6137457863884076E-7</v>
@@ -17251,10 +17251,10 @@
       <c r="AE31" s="147"/>
       <c r="AF31" s="147"/>
       <c r="AH31" s="134" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AJ31" s="134" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AK31" s="141" t="s">
         <v>314</v>
@@ -17275,88 +17275,88 @@
         <v>321</v>
       </c>
       <c r="AQ31" t="s">
+        <v>338</v>
+      </c>
+      <c r="AR31" t="s">
         <v>339</v>
       </c>
-      <c r="AR31" t="s">
-        <v>340</v>
-      </c>
       <c r="AS31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AT31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AU31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AV31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AW31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AX31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AY31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AZ31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BA31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BB31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BC31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BD31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BE31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BF31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BG31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BH31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BI31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BJ31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BK31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BL31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BM31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BN31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BO31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="BP31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BQ31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BR31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -18549,7 +18549,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s">
         <v>291</v>
@@ -18801,12 +18801,12 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="76" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="138" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B21">
         <v>0.37034943531993869</v>
@@ -18820,7 +18820,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="138" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B22">
         <v>1.274407618987647</v>
@@ -18834,7 +18834,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="138" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B23">
         <v>3.1302091249900932</v>
@@ -18848,7 +18848,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="138" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B24">
         <v>0.24682227388035821</v>
@@ -18862,7 +18862,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="138" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B25">
         <v>0.21415419754922327</v>
@@ -18876,7 +18876,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="138" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B26">
         <v>1.7961904743782098</v>
@@ -18890,7 +18890,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="138" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B27">
         <v>2.2352473934910237E-2</v>
@@ -18904,7 +18904,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="139" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B28">
         <v>7.0223242933031296E-2</v>
@@ -19621,7 +19621,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>331</v>
+        <v>382</v>
       </c>
       <c r="B43" s="69">
         <v>44.291949816853993</v>
@@ -19632,7 +19632,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B44" s="69">
         <v>43.995102738357922</v>
@@ -19643,7 +19643,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B45" s="69">
         <v>43.975450721892244</v>
@@ -19654,7 +19654,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B46" s="69">
         <v>43.819577184272568</v>
@@ -19918,7 +19918,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="136" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B70" s="134">
         <v>119.98674372549019</v>

</xml_diff>

<commit_message>
Minor update: added urban emissions of fuel distribution to the background GREET2021 data for comparing biochem pathways
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping.xlsx
+++ b/Lookup table_prototyping.xlsx
@@ -1,37 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CF7654-108A-470D-A13F-0AF65DFD8E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7924AA2E-0464-4AB2-90F7-C4FE0E4327CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Production" sheetId="2" r:id="rId3"/>
-    <sheet name="Chemicals" sheetId="5" r:id="rId4"/>
-    <sheet name="Other" sheetId="4" r:id="rId5"/>
-    <sheet name="End use" sheetId="3" state="hidden" r:id="rId6"/>
-    <sheet name="Feedstock" sheetId="15" r:id="rId7"/>
-    <sheet name="Units" sheetId="10" r:id="rId8"/>
-    <sheet name="Fuel specs" sheetId="11" r:id="rId9"/>
-    <sheet name="Mass" sheetId="6" r:id="rId10"/>
-    <sheet name="Volume" sheetId="7" r:id="rId11"/>
-    <sheet name="Energy" sheetId="8" r:id="rId12"/>
-    <sheet name="Length" sheetId="9" r:id="rId13"/>
-    <sheet name="Transportation" sheetId="12" r:id="rId14"/>
-    <sheet name="End use supplement" sheetId="13" r:id="rId15"/>
+    <sheet name="Fuel dist urban" sheetId="16" r:id="rId3"/>
+    <sheet name="Production" sheetId="2" r:id="rId4"/>
+    <sheet name="Chemicals" sheetId="5" r:id="rId5"/>
+    <sheet name="Other" sheetId="4" r:id="rId6"/>
+    <sheet name="End use" sheetId="3" state="hidden" r:id="rId7"/>
+    <sheet name="Feedstock" sheetId="15" r:id="rId8"/>
+    <sheet name="Units" sheetId="10" r:id="rId9"/>
+    <sheet name="Fuel specs" sheetId="11" r:id="rId10"/>
+    <sheet name="Mass" sheetId="6" r:id="rId11"/>
+    <sheet name="Volume" sheetId="7" r:id="rId12"/>
+    <sheet name="Energy" sheetId="8" r:id="rId13"/>
+    <sheet name="Length" sheetId="9" r:id="rId14"/>
+    <sheet name="Transportation" sheetId="12" r:id="rId15"/>
+    <sheet name="End use supplement" sheetId="13" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
     <definedName name="g2T">[1]Fuel_Specs!$B$175</definedName>
@@ -43,6 +45,7 @@
     <definedName name="mmBTU2BTU">[1]Fuel_Specs!$H$190</definedName>
     <definedName name="MT2g">[1]Fuel_Specs!$D$171</definedName>
     <definedName name="MT2T">[2]Fuel_Specs!$D$175</definedName>
+    <definedName name="t2g" localSheetId="2">#REF!</definedName>
     <definedName name="t2g">Other!$B$8</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
@@ -159,6 +162,24 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={F0C05CB8-4FDE-46EC-8173-80CAA713821E}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F0C05CB8-4FDE-46EC-8173-80CAA713821E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is 2022 data, not reverted to 2011 yet.  Just for testing.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={044CB3AF-6283-4031-8C05-A50B4C478E65}</author>
     <author>tc={AC7E57AA-E1E8-4F84-B9FC-C85A72059020}</author>
     <author>tc={DE17457E-03BF-4211-B5F5-8525E651A0CD}</author>
@@ -238,7 +259,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={AB144FDA-22B0-44A8-8FFE-47B0095C1B54}</author>
@@ -298,7 +319,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={3EAA6704-9DE5-43CA-95E4-FB464F0E000B}</author>
@@ -317,7 +338,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="383">
   <si>
     <t>NG</t>
   </si>
@@ -1486,7 +1507,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
     <numFmt numFmtId="174" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1524,6 +1545,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -1801,7 +1828,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2100,6 +2127,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2120,7 +2150,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Overview"/>
@@ -2269,7 +2299,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Overview"/>
@@ -2402,6 +2432,46 @@
       <sheetData sheetId="55" refreshError="1"/>
       <sheetData sheetId="56" refreshError="1"/>
       <sheetData sheetId="57" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="End use test"/>
+      <sheetName val="Fuel dist urban"/>
+      <sheetName val="Production"/>
+      <sheetName val="Chemicals"/>
+      <sheetName val="End use"/>
+      <sheetName val="Feedstock"/>
+      <sheetName val="Units"/>
+      <sheetName val="Fuel specs"/>
+      <sheetName val="Mass"/>
+      <sheetName val="Volume"/>
+      <sheetName val="Energy"/>
+      <sheetName val="Length"/>
+      <sheetName val="Transportation"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2707,7 +2777,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2756,6 +2826,14 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2023-01-23T16:44:57.18" personId="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" id="{F0C05CB8-4FDE-46EC-8173-80CAA713821E}">
+    <text>This is 2022 data, not reverted to 2011 yet.  Just for testing.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="K1" personId="{C9416A2D-8241-4F20-804B-D394F6D9AB2A}" id="{044CB3AF-6283-4031-8C05-A50B4C478E65}">
     <text>CO2 transportation for algae cultivation is used here as surrogate.</text>
   </threadedComment>
@@ -2784,7 +2862,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="G2" personId="{52F93C99-6E2F-47FF-A86C-9CFC6703D7FF}" id="{AB144FDA-22B0-44A8-8FFE-47B0095C1B54}">
     <text>Emsisions factors are for large industrial boilers. 
@@ -2810,7 +2888,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A2" dT="2022-01-26T21:12:20.99" personId="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" id="{3EAA6704-9DE5-43CA-95E4-FB464F0E000B}">
     <text>These values are added manually.</text>
@@ -2822,7 +2900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AN1" sqref="AN1"/>
     </sheetView>
@@ -6055,6 +6133,1037 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
+  <dimension ref="A1:C100"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" s="68" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3">
+        <v>42.686144171450856</v>
+      </c>
+      <c r="C3">
+        <v>846.6716031627742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="69">
+        <v>44.468682566682403</v>
+      </c>
+      <c r="C4" s="69">
+        <v>862.78610169410933</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="69">
+        <v>50.159067341356092</v>
+      </c>
+      <c r="C5" s="69">
+        <v>1014.3369175627239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="69">
+        <v>50.159067341356092</v>
+      </c>
+      <c r="C6" s="69">
+        <v>1014.3369175627239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="69">
+        <v>47.796561156394887</v>
+      </c>
+      <c r="C7" s="69">
+        <v>924.72851371056413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="69">
+        <v>42.284046724818751</v>
+      </c>
+      <c r="C8" s="69">
+        <v>715.64223805552433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="69">
+        <v>41.346637144473675</v>
+      </c>
+      <c r="C9" s="69">
+        <v>815.56195965417839</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="69">
+        <v>40.32341453625299</v>
+      </c>
+      <c r="C10" s="69">
+        <v>788.30083565459597</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="69">
+        <v>38.215735920904834</v>
+      </c>
+      <c r="C11" s="69">
+        <v>744.70116983334174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12">
+        <v>36.933051359779093</v>
+      </c>
+      <c r="C12">
+        <v>749.07638827065296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="69">
+        <v>36.933051359779093</v>
+      </c>
+      <c r="C13" s="69">
+        <v>749.07638827065296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="69" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="69">
+        <v>34.943581428237124</v>
+      </c>
+      <c r="C14" s="69">
+        <v>755.86244135709444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="69">
+        <v>32.980288732636502</v>
+      </c>
+      <c r="C15" s="69">
+        <v>762.55920427134606</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="69">
+        <v>42.284531648205927</v>
+      </c>
+      <c r="C16" s="69">
+        <v>836.63306309407369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="69" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="69">
+        <v>42.626181307031878</v>
+      </c>
+      <c r="C17" s="69">
+        <v>846.93577526984518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="69">
+        <v>42.284531648205927</v>
+      </c>
+      <c r="C18" s="69">
+        <v>836.63306309407369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>42.626181307031878</v>
+      </c>
+      <c r="C19">
+        <v>846.93577526984518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20">
+        <v>38.488964112948509</v>
+      </c>
+      <c r="C20">
+        <v>725.15243391008278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21">
+        <v>38.922651269814651</v>
+      </c>
+      <c r="C21">
+        <v>748.62596861099109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22">
+        <v>40.920706293416544</v>
+      </c>
+      <c r="C22">
+        <v>801.99999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23">
+        <v>40.504015809547568</v>
+      </c>
+      <c r="C23">
+        <v>791.99999999999989</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24">
+        <v>36.711334911700462</v>
+      </c>
+      <c r="C24">
+        <v>700.32025584540236</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25">
+        <v>46.202729987714299</v>
+      </c>
+      <c r="C25">
+        <v>991.17374573064865</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26">
+        <v>46.202729987714299</v>
+      </c>
+      <c r="C26">
+        <v>991.17374573064865</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27">
+        <v>18.846161439157566</v>
+      </c>
+      <c r="C27">
+        <v>794.1013538556316</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28">
+        <v>25.127117950234005</v>
+      </c>
+      <c r="C28">
+        <v>789.34625592835232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29">
+        <v>32.865401215741031</v>
+      </c>
+      <c r="C29">
+        <v>809.68750817282455</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30">
+        <v>27.364626409656783</v>
+      </c>
+      <c r="C30">
+        <v>783.00612535864673</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31">
+        <v>38.215735920904834</v>
+      </c>
+      <c r="C31">
+        <v>744.70116983334174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32">
+        <v>27.964740860374413</v>
+      </c>
+      <c r="C32">
+        <v>508.00296189766453</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33">
+        <v>24.597121095787827</v>
+      </c>
+      <c r="C33">
+        <v>428.22298556220187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34">
+        <v>22.69110756333853</v>
+      </c>
+      <c r="C34">
+        <v>665.18536560495022</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35">
+        <v>23.767560801872072</v>
+      </c>
+      <c r="C35">
+        <v>859.88020851632757</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36">
+        <v>39.354735372074877</v>
+      </c>
+      <c r="C36">
+        <v>887.88245186586084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37">
+        <v>40.711000614508571</v>
+      </c>
+      <c r="C37">
+        <v>797.00724703341325</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38">
+        <v>38.53472160535101</v>
+      </c>
+      <c r="C38">
+        <v>748.92792354647884</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39">
+        <v>40.453244380327611</v>
+      </c>
+      <c r="C39">
+        <v>778.77937164550963</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>162</v>
+      </c>
+      <c r="B40">
+        <v>43.400833892223638</v>
+      </c>
+      <c r="C40">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41">
+        <v>40.954601653198118</v>
+      </c>
+      <c r="C41">
+        <v>798.04417121416941</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>242</v>
+      </c>
+      <c r="B42" s="69">
+        <v>44.291949816853993</v>
+      </c>
+      <c r="C42">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>382</v>
+      </c>
+      <c r="B43" s="69">
+        <v>44.291949816853993</v>
+      </c>
+      <c r="C43">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>331</v>
+      </c>
+      <c r="B44" s="69">
+        <v>43.995102738357922</v>
+      </c>
+      <c r="C44">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>362</v>
+      </c>
+      <c r="B45" s="69">
+        <v>43.975450721892244</v>
+      </c>
+      <c r="C45">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>363</v>
+      </c>
+      <c r="B46" s="69">
+        <v>43.819577184272568</v>
+      </c>
+      <c r="C46">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>164</v>
+      </c>
+      <c r="B47">
+        <v>38.180512527472686</v>
+      </c>
+      <c r="C47">
+        <v>747.6070630111235</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>165</v>
+      </c>
+      <c r="B48">
+        <v>37.300256882262083</v>
+      </c>
+      <c r="C48">
+        <v>716.69892648380858</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>166</v>
+      </c>
+      <c r="B49">
+        <v>36.889328265240245</v>
+      </c>
+      <c r="C49">
+        <v>744.70116983334174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>167</v>
+      </c>
+      <c r="B50">
+        <v>39.429337036099838</v>
+      </c>
+      <c r="C50">
+        <v>756.99999999999989</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51">
+        <v>10.040313081123244</v>
+      </c>
+      <c r="C51">
+        <v>70.798124695046326</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>169</v>
+      </c>
+      <c r="B52">
+        <v>30.792488052730107</v>
+      </c>
+      <c r="C52">
+        <v>742.58779297677324</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53">
+        <v>31.839314137909518</v>
+      </c>
+      <c r="C53">
+        <v>742.32362086970215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>171</v>
+      </c>
+      <c r="B54">
+        <v>33.077070766926674</v>
+      </c>
+      <c r="C54">
+        <v>769.53334789802227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55">
+        <v>31.263230600468017</v>
+      </c>
+      <c r="C55">
+        <v>584.61287294827434</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56">
+        <v>29.646904789703584</v>
+      </c>
+      <c r="C56">
+        <v>559.51652277652283</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>174</v>
+      </c>
+      <c r="B57">
+        <v>31.510123545085804</v>
+      </c>
+      <c r="C57">
+        <v>595.17975723111715</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>175</v>
+      </c>
+      <c r="B58">
+        <v>27.734307445397814</v>
+      </c>
+      <c r="C58">
+        <v>507.21044557645126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>176</v>
+      </c>
+      <c r="B59">
+        <v>27.548680827882244</v>
+      </c>
+      <c r="C59">
+        <v>668.88377510394514</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60">
+        <v>34.60609523247426</v>
+      </c>
+      <c r="C60">
+        <v>654.80340179705718</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>178</v>
+      </c>
+      <c r="B61">
+        <v>36.455478031346189</v>
+      </c>
+      <c r="C61">
+        <v>688.85095964480468</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62">
+        <v>38.505872853524245</v>
+      </c>
+      <c r="C62">
+        <v>737.59071339941693</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63">
+        <v>39.773165285279561</v>
+      </c>
+      <c r="C63">
+        <v>765.47381512866104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>181</v>
+      </c>
+      <c r="B64">
+        <v>38.281904677575831</v>
+      </c>
+      <c r="C64">
+        <v>731.67589538225809</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>182</v>
+      </c>
+      <c r="B65">
+        <v>31.369932808387436</v>
+      </c>
+      <c r="C65">
+        <v>800.00032424653136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>183</v>
+      </c>
+      <c r="B66">
+        <v>38.180512527472686</v>
+      </c>
+      <c r="C66">
+        <v>747.6070630111235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67">
+        <v>47.141813661363599</v>
+      </c>
+      <c r="C67">
+        <v>0.77692265667854898</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>188</v>
+      </c>
+      <c r="B68">
+        <v>49.999999999999993</v>
+      </c>
+      <c r="C68">
+        <v>0.71699999999999986</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69">
+        <v>119.98674372549019</v>
+      </c>
+      <c r="C69">
+        <v>9.0052398842286357E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="136" t="s">
+        <v>358</v>
+      </c>
+      <c r="B70" s="134">
+        <v>119.98674372549019</v>
+      </c>
+      <c r="C70" s="134">
+        <v>9.0052398842286357E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>189</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>1.9768383817590991</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72">
+        <v>48.885121247479262</v>
+      </c>
+      <c r="C72">
+        <v>0.88356773166440861</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73">
+        <v>22.648458746153963</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74">
+        <v>26.329529071139479</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75">
+        <v>18.707371337693861</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>194</v>
+      </c>
+      <c r="B76">
+        <v>12.566427590816895</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>195</v>
+      </c>
+      <c r="B77">
+        <v>26.329529071139479</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>196</v>
+      </c>
+      <c r="B78">
+        <v>11.566786665057547</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>197</v>
+      </c>
+      <c r="B79">
+        <v>31.342185540824094</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80">
+        <v>31.0106439692332</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>199</v>
+      </c>
+      <c r="B81">
+        <v>28.609127685562171</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82">
+        <v>33.012627597074328</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>201</v>
+      </c>
+      <c r="B83">
+        <v>17.905547955535493</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>202</v>
+      </c>
+      <c r="B84">
+        <v>18.52542695399616</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>203</v>
+      </c>
+      <c r="B85">
+        <v>16.801860958276258</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>204</v>
+      </c>
+      <c r="B86">
+        <v>17.842745955691449</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>205</v>
+      </c>
+      <c r="B87">
+        <v>17.11470795749937</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>206</v>
+      </c>
+      <c r="B88">
+        <v>20.107106950068403</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>207</v>
+      </c>
+      <c r="B89">
+        <v>18.52542695399616</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>208</v>
+      </c>
+      <c r="B90">
+        <v>17.444999956679162</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>209</v>
+      </c>
+      <c r="B91">
+        <v>15.647058823529411</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>210</v>
+      </c>
+      <c r="B92">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>211</v>
+      </c>
+      <c r="B93">
+        <v>22.000366940104676</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>212</v>
+      </c>
+      <c r="B94">
+        <v>14.864999999999997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>213</v>
+      </c>
+      <c r="B95">
+        <v>16.758749999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>214</v>
+      </c>
+      <c r="B96">
+        <v>16.758749999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>215</v>
+      </c>
+      <c r="B97">
+        <v>13.036809815950916</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>216</v>
+      </c>
+      <c r="B98">
+        <v>16.462585034013607</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="68" t="s">
+        <v>219</v>
+      </c>
+      <c r="C99">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>75</v>
+      </c>
+      <c r="C100">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C295DD4-7C09-4646-A296-16CD0AFAEC63}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -6278,7 +7387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8F5E2C-DDF2-4E57-AD59-B511AD831FCD}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -6413,7 +7522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02D7542-6EF2-41EA-86E3-98DE7161C9DB}">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -6769,7 +7878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01334582-9977-4CFE-91E6-70D92C4489D0}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -6945,7 +8054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F07116-128C-456A-A5F4-E4321BD8FA65}">
   <dimension ref="A1:CE37"/>
   <sheetViews>
@@ -8973,7 +10082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83661039-7356-4024-8E14-826D73D1CFCD}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -9156,6 +10265,767 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C897779-42DB-4A8F-A187-9EBE1CDEE719}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="150" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="150" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1" s="150" t="s">
+        <v>382</v>
+      </c>
+      <c r="E1" s="150" t="s">
+        <v>331</v>
+      </c>
+      <c r="F1" s="150" t="s">
+        <v>362</v>
+      </c>
+      <c r="G1" s="150" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="65" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>308</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>308</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>308</v>
+      </c>
+      <c r="F2" s="65" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" s="65" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9339.5518419730979</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5093.7824552240209</v>
+      </c>
+      <c r="D4" s="3">
+        <f>C4</f>
+        <v>5093.7824552240209</v>
+      </c>
+      <c r="E4" s="3">
+        <f>C4</f>
+        <v>5093.7824552240209</v>
+      </c>
+      <c r="F4" s="3">
+        <f>C4</f>
+        <v>5093.7824552240209</v>
+      </c>
+      <c r="G4" s="3">
+        <f>C4</f>
+        <v>5093.7824552240209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8169.6873553428004</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5023.1958652604862</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D20" si="0">C5</f>
+        <v>5023.1958652604862</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E20" si="1">C5</f>
+        <v>5023.1958652604862</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F20" si="2">C5</f>
+        <v>5023.1958652604862</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:G20" si="3">C5</f>
+        <v>5023.1958652604862</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1989.4630119087635</v>
+      </c>
+      <c r="C6" s="3">
+        <v>41.657173986229949</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>41.657173986229949</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>41.657173986229949</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>41.657173986229949</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="3"/>
+        <v>41.657173986229949</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2794.9003158789556</v>
+      </c>
+      <c r="C7" s="3">
+        <v>527.78573845908159</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>527.78573845908159</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>527.78573845908159</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>527.78573845908159</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="3"/>
+        <v>527.78573845908159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3385.324027555082</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4453.7529528151745</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>4453.7529528151745</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>4453.7529528151745</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>4453.7529528151745</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="3"/>
+        <v>4453.7529528151745</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.53885408384714351</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9.869537321209304E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>9.869537321209304E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>9.869537321209304E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>9.869537321209304E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="3"/>
+        <v>9.869537321209304E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.12683831523481029</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.1883133447180589</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1883133447180589</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1883133447180589</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1883133447180589</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1883133447180589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.54395091021563391</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.60557378989801824</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.60557378989801824</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.60557378989801824</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.60557378989801824</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="3"/>
+        <v>0.60557378989801824</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.4670490677357695</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.3472060329660924</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3472060329660924</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3472060329660924</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3472060329660924</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3472060329660924</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7.2523053711609858E-2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4.077408879999693E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>4.077408879999693E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>4.077408879999693E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>4.077408879999693E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="3"/>
+        <v>4.077408879999693E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4.8091315083300508E-2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2.866035992117464E-2</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>2.866035992117464E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>2.866035992117464E-2</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>2.866035992117464E-2</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="3"/>
+        <v>2.866035992117464E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.25121575444697092</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2.4510023670013949E-2</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>2.4510023670013949E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4510023670013949E-2</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>2.4510023670013949E-2</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4510023670013949E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3">
+        <v>4.2349995275388881E-3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3.3183046022218594E-3</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>3.3183046022218594E-3</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>3.3183046022218594E-3</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>3.3183046022218594E-3</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="3"/>
+        <v>3.3183046022218594E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2.0560277799938402E-2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1.5425727512154881E-2</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5425727512154881E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>1.5425727512154881E-2</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5425727512154881E-2</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5425727512154881E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.0961495941820574</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.48940655600260441</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48940655600260441</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>0.48940655600260441</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>0.48940655600260441</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="3"/>
+        <v>0.48940655600260441</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.2419532449195709E-2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>5.8402637809921217E-3</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>5.8402637809921217E-3</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>5.8402637809921217E-3</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>5.8402637809921217E-3</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="3"/>
+        <v>5.8402637809921217E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3">
+        <v>633.15471120171344</v>
+      </c>
+      <c r="C20" s="3">
+        <v>387.85040331686662</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>387.85040331686662</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>387.85040331686662</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>387.85040331686662</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="3"/>
+        <v>387.85040331686662</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B21">
+        <v>2.1781234690476294E-2</v>
+      </c>
+      <c r="C21">
+        <v>0.26551552589021865</v>
+      </c>
+      <c r="D21">
+        <f>C21</f>
+        <v>0.26551552589021865</v>
+      </c>
+      <c r="E21">
+        <f>C21</f>
+        <v>0.26551552589021865</v>
+      </c>
+      <c r="F21">
+        <f>C21</f>
+        <v>0.26551552589021865</v>
+      </c>
+      <c r="G21">
+        <f>C21</f>
+        <v>0.26551552589021865</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B22">
+        <v>0.18381159698546526</v>
+      </c>
+      <c r="C22">
+        <v>0.17288665151109295</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22:D28" si="4">C22</f>
+        <v>0.17288665151109295</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:E28" si="5">C22</f>
+        <v>0.17288665151109295</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:F28" si="6">C22</f>
+        <v>0.17288665151109295</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G28" si="7">C22</f>
+        <v>0.17288665151109295</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B23">
+        <v>0.26679009552113131</v>
+      </c>
+      <c r="C23">
+        <v>0.21330355735173617</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="4"/>
+        <v>0.21330355735173617</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="5"/>
+        <v>0.21330355735173617</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="6"/>
+        <v>0.21330355735173617</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>0.21330355735173617</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B24">
+        <v>1.6067527224713878E-2</v>
+      </c>
+      <c r="C24">
+        <v>9.4740252492059081E-3</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="4"/>
+        <v>9.4740252492059081E-3</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="5"/>
+        <v>9.4740252492059081E-3</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="6"/>
+        <v>9.4740252492059081E-3</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="7"/>
+        <v>9.4740252492059081E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B25">
+        <v>1.0925985281165002E-2</v>
+      </c>
+      <c r="C25">
+        <v>5.0442745092267195E-3</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="4"/>
+        <v>5.0442745092267195E-3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="5"/>
+        <v>5.0442745092267195E-3</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="6"/>
+        <v>5.0442745092267195E-3</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="7"/>
+        <v>5.0442745092267195E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B26">
+        <v>7.5973312175973959E-2</v>
+      </c>
+      <c r="C26">
+        <v>5.2423279836688944E-3</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="4"/>
+        <v>5.2423279836688944E-3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="5"/>
+        <v>5.2423279836688944E-3</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="6"/>
+        <v>5.2423279836688944E-3</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="7"/>
+        <v>5.2423279836688944E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B27">
+        <v>7.7626034636698693E-4</v>
+      </c>
+      <c r="C27">
+        <v>5.4229333446464761E-4</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="4"/>
+        <v>5.4229333446464761E-4</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="5"/>
+        <v>5.4229333446464761E-4</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="6"/>
+        <v>5.4229333446464761E-4</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="7"/>
+        <v>5.4229333446464761E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B28">
+        <v>3.3865871217684512E-3</v>
+      </c>
+      <c r="C28">
+        <v>1.8571109385136862E-3</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="4"/>
+        <v>1.8571109385136862E-3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="5"/>
+        <v>1.8571109385136862E-3</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="6"/>
+        <v>1.8571109385136862E-3</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="7"/>
+        <v>1.8571109385136862E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
   <dimension ref="A1:X44"/>
   <sheetViews>
@@ -11384,7 +13254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
   <dimension ref="A1:BR31"/>
   <sheetViews>
@@ -17368,7 +19238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0314A913-1E2B-402E-8225-BB138359D3D4}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -17435,7 +19305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F728B1BE-12B0-4F72-A3B0-228655F7F3FD}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
@@ -18521,7 +20391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2275C5-799F-4B1B-8AD1-776CB314922E}">
   <dimension ref="A1:D30"/>
   <sheetViews>
@@ -18932,7 +20802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912BA9E3-4DC6-4F1B-8852-1658C2A4C23D}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -19145,1035 +21015,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
-  <dimension ref="A1:C100"/>
-  <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3">
-        <v>42.686144171450856</v>
-      </c>
-      <c r="C3">
-        <v>846.6716031627742</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="69" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="69">
-        <v>44.468682566682403</v>
-      </c>
-      <c r="C4" s="69">
-        <v>862.78610169410933</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="69" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" s="69">
-        <v>50.159067341356092</v>
-      </c>
-      <c r="C5" s="69">
-        <v>1014.3369175627239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" s="69">
-        <v>50.159067341356092</v>
-      </c>
-      <c r="C6" s="69">
-        <v>1014.3369175627239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="69">
-        <v>47.796561156394887</v>
-      </c>
-      <c r="C7" s="69">
-        <v>924.72851371056413</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="69">
-        <v>42.284046724818751</v>
-      </c>
-      <c r="C8" s="69">
-        <v>715.64223805552433</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="69" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" s="69">
-        <v>41.346637144473675</v>
-      </c>
-      <c r="C9" s="69">
-        <v>815.56195965417839</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="69" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="69">
-        <v>40.32341453625299</v>
-      </c>
-      <c r="C10" s="69">
-        <v>788.30083565459597</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="69" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="69">
-        <v>38.215735920904834</v>
-      </c>
-      <c r="C11" s="69">
-        <v>744.70116983334174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12">
-        <v>36.933051359779093</v>
-      </c>
-      <c r="C12">
-        <v>749.07638827065296</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="69" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="69">
-        <v>36.933051359779093</v>
-      </c>
-      <c r="C13" s="69">
-        <v>749.07638827065296</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="69" t="s">
-        <v>137</v>
-      </c>
-      <c r="B14" s="69">
-        <v>34.943581428237124</v>
-      </c>
-      <c r="C14" s="69">
-        <v>755.86244135709444</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="69" t="s">
-        <v>138</v>
-      </c>
-      <c r="B15" s="69">
-        <v>32.980288732636502</v>
-      </c>
-      <c r="C15" s="69">
-        <v>762.55920427134606</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" s="69">
-        <v>42.284531648205927</v>
-      </c>
-      <c r="C16" s="69">
-        <v>836.63306309407369</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="69">
-        <v>42.626181307031878</v>
-      </c>
-      <c r="C17" s="69">
-        <v>846.93577526984518</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" s="69">
-        <v>42.284531648205927</v>
-      </c>
-      <c r="C18" s="69">
-        <v>836.63306309407369</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>42.626181307031878</v>
-      </c>
-      <c r="C19">
-        <v>846.93577526984518</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B20">
-        <v>38.488964112948509</v>
-      </c>
-      <c r="C20">
-        <v>725.15243391008278</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21">
-        <v>38.922651269814651</v>
-      </c>
-      <c r="C21">
-        <v>748.62596861099109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>144</v>
-      </c>
-      <c r="B22">
-        <v>40.920706293416544</v>
-      </c>
-      <c r="C22">
-        <v>801.99999999999989</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>145</v>
-      </c>
-      <c r="B23">
-        <v>40.504015809547568</v>
-      </c>
-      <c r="C23">
-        <v>791.99999999999989</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>146</v>
-      </c>
-      <c r="B24">
-        <v>36.711334911700462</v>
-      </c>
-      <c r="C24">
-        <v>700.32025584540236</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>147</v>
-      </c>
-      <c r="B25">
-        <v>46.202729987714299</v>
-      </c>
-      <c r="C25">
-        <v>991.17374573064865</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B26">
-        <v>46.202729987714299</v>
-      </c>
-      <c r="C26">
-        <v>991.17374573064865</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27">
-        <v>18.846161439157566</v>
-      </c>
-      <c r="C27">
-        <v>794.1013538556316</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>150</v>
-      </c>
-      <c r="B28">
-        <v>25.127117950234005</v>
-      </c>
-      <c r="C28">
-        <v>789.34625592835232</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B29">
-        <v>32.865401215741031</v>
-      </c>
-      <c r="C29">
-        <v>809.68750817282455</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30">
-        <v>27.364626409656783</v>
-      </c>
-      <c r="C30">
-        <v>783.00612535864673</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>153</v>
-      </c>
-      <c r="B31">
-        <v>38.215735920904834</v>
-      </c>
-      <c r="C31">
-        <v>744.70116983334174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>154</v>
-      </c>
-      <c r="B32">
-        <v>27.964740860374413</v>
-      </c>
-      <c r="C32">
-        <v>508.00296189766453</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>155</v>
-      </c>
-      <c r="B33">
-        <v>24.597121095787827</v>
-      </c>
-      <c r="C33">
-        <v>428.22298556220187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>156</v>
-      </c>
-      <c r="B34">
-        <v>22.69110756333853</v>
-      </c>
-      <c r="C34">
-        <v>665.18536560495022</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>157</v>
-      </c>
-      <c r="B35">
-        <v>23.767560801872072</v>
-      </c>
-      <c r="C35">
-        <v>859.88020851632757</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>158</v>
-      </c>
-      <c r="B36">
-        <v>39.354735372074877</v>
-      </c>
-      <c r="C36">
-        <v>887.88245186586084</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>159</v>
-      </c>
-      <c r="B37">
-        <v>40.711000614508571</v>
-      </c>
-      <c r="C37">
-        <v>797.00724703341325</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>160</v>
-      </c>
-      <c r="B38">
-        <v>38.53472160535101</v>
-      </c>
-      <c r="C38">
-        <v>748.92792354647884</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>161</v>
-      </c>
-      <c r="B39">
-        <v>40.453244380327611</v>
-      </c>
-      <c r="C39">
-        <v>778.77937164550963</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>162</v>
-      </c>
-      <c r="B40">
-        <v>43.400833892223638</v>
-      </c>
-      <c r="C40">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>163</v>
-      </c>
-      <c r="B41">
-        <v>40.954601653198118</v>
-      </c>
-      <c r="C41">
-        <v>798.04417121416941</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>242</v>
-      </c>
-      <c r="B42" s="69">
-        <v>44.291949816853993</v>
-      </c>
-      <c r="C42">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>382</v>
-      </c>
-      <c r="B43" s="69">
-        <v>44.291949816853993</v>
-      </c>
-      <c r="C43">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>331</v>
-      </c>
-      <c r="B44" s="69">
-        <v>43.995102738357922</v>
-      </c>
-      <c r="C44">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>362</v>
-      </c>
-      <c r="B45" s="69">
-        <v>43.975450721892244</v>
-      </c>
-      <c r="C45">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>363</v>
-      </c>
-      <c r="B46" s="69">
-        <v>43.819577184272568</v>
-      </c>
-      <c r="C46">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>164</v>
-      </c>
-      <c r="B47">
-        <v>38.180512527472686</v>
-      </c>
-      <c r="C47">
-        <v>747.6070630111235</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>165</v>
-      </c>
-      <c r="B48">
-        <v>37.300256882262083</v>
-      </c>
-      <c r="C48">
-        <v>716.69892648380858</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>166</v>
-      </c>
-      <c r="B49">
-        <v>36.889328265240245</v>
-      </c>
-      <c r="C49">
-        <v>744.70116983334174</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>167</v>
-      </c>
-      <c r="B50">
-        <v>39.429337036099838</v>
-      </c>
-      <c r="C50">
-        <v>756.99999999999989</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51">
-        <v>10.040313081123244</v>
-      </c>
-      <c r="C51">
-        <v>70.798124695046326</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>169</v>
-      </c>
-      <c r="B52">
-        <v>30.792488052730107</v>
-      </c>
-      <c r="C52">
-        <v>742.58779297677324</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>170</v>
-      </c>
-      <c r="B53">
-        <v>31.839314137909518</v>
-      </c>
-      <c r="C53">
-        <v>742.32362086970215</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>171</v>
-      </c>
-      <c r="B54">
-        <v>33.077070766926674</v>
-      </c>
-      <c r="C54">
-        <v>769.53334789802227</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>172</v>
-      </c>
-      <c r="B55">
-        <v>31.263230600468017</v>
-      </c>
-      <c r="C55">
-        <v>584.61287294827434</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>173</v>
-      </c>
-      <c r="B56">
-        <v>29.646904789703584</v>
-      </c>
-      <c r="C56">
-        <v>559.51652277652283</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>174</v>
-      </c>
-      <c r="B57">
-        <v>31.510123545085804</v>
-      </c>
-      <c r="C57">
-        <v>595.17975723111715</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>175</v>
-      </c>
-      <c r="B58">
-        <v>27.734307445397814</v>
-      </c>
-      <c r="C58">
-        <v>507.21044557645126</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>176</v>
-      </c>
-      <c r="B59">
-        <v>27.548680827882244</v>
-      </c>
-      <c r="C59">
-        <v>668.88377510394514</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>177</v>
-      </c>
-      <c r="B60">
-        <v>34.60609523247426</v>
-      </c>
-      <c r="C60">
-        <v>654.80340179705718</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>178</v>
-      </c>
-      <c r="B61">
-        <v>36.455478031346189</v>
-      </c>
-      <c r="C61">
-        <v>688.85095964480468</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>179</v>
-      </c>
-      <c r="B62">
-        <v>38.505872853524245</v>
-      </c>
-      <c r="C62">
-        <v>737.59071339941693</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>180</v>
-      </c>
-      <c r="B63">
-        <v>39.773165285279561</v>
-      </c>
-      <c r="C63">
-        <v>765.47381512866104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64">
-        <v>38.281904677575831</v>
-      </c>
-      <c r="C64">
-        <v>731.67589538225809</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>182</v>
-      </c>
-      <c r="B65">
-        <v>31.369932808387436</v>
-      </c>
-      <c r="C65">
-        <v>800.00032424653136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>183</v>
-      </c>
-      <c r="B66">
-        <v>38.180512527472686</v>
-      </c>
-      <c r="C66">
-        <v>747.6070630111235</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>187</v>
-      </c>
-      <c r="B67">
-        <v>47.141813661363599</v>
-      </c>
-      <c r="C67">
-        <v>0.77692265667854898</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>188</v>
-      </c>
-      <c r="B68">
-        <v>49.999999999999993</v>
-      </c>
-      <c r="C68">
-        <v>0.71699999999999986</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="B69">
-        <v>119.98674372549019</v>
-      </c>
-      <c r="C69">
-        <v>9.0052398842286357E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="136" t="s">
-        <v>358</v>
-      </c>
-      <c r="B70" s="134">
-        <v>119.98674372549019</v>
-      </c>
-      <c r="C70" s="134">
-        <v>9.0052398842286357E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>189</v>
-      </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="C71">
-        <v>1.9768383817590991</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>190</v>
-      </c>
-      <c r="B72">
-        <v>48.885121247479262</v>
-      </c>
-      <c r="C72">
-        <v>0.88356773166440861</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>191</v>
-      </c>
-      <c r="B73">
-        <v>22.648458746153963</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>192</v>
-      </c>
-      <c r="B74">
-        <v>26.329529071139479</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>193</v>
-      </c>
-      <c r="B75">
-        <v>18.707371337693861</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>194</v>
-      </c>
-      <c r="B76">
-        <v>12.566427590816895</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>195</v>
-      </c>
-      <c r="B77">
-        <v>26.329529071139479</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>196</v>
-      </c>
-      <c r="B78">
-        <v>11.566786665057547</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>197</v>
-      </c>
-      <c r="B79">
-        <v>31.342185540824094</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>198</v>
-      </c>
-      <c r="B80">
-        <v>31.0106439692332</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>199</v>
-      </c>
-      <c r="B81">
-        <v>28.609127685562171</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>200</v>
-      </c>
-      <c r="B82">
-        <v>33.012627597074328</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>201</v>
-      </c>
-      <c r="B83">
-        <v>17.905547955535493</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>202</v>
-      </c>
-      <c r="B84">
-        <v>18.52542695399616</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>203</v>
-      </c>
-      <c r="B85">
-        <v>16.801860958276258</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>204</v>
-      </c>
-      <c r="B86">
-        <v>17.842745955691449</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>205</v>
-      </c>
-      <c r="B87">
-        <v>17.11470795749937</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>206</v>
-      </c>
-      <c r="B88">
-        <v>20.107106950068403</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>207</v>
-      </c>
-      <c r="B89">
-        <v>18.52542695399616</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>208</v>
-      </c>
-      <c r="B90">
-        <v>17.444999956679162</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>209</v>
-      </c>
-      <c r="B91">
-        <v>15.647058823529411</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>210</v>
-      </c>
-      <c r="B92">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>211</v>
-      </c>
-      <c r="B93">
-        <v>22.000366940104676</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>212</v>
-      </c>
-      <c r="B94">
-        <v>14.864999999999997</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>213</v>
-      </c>
-      <c r="B95">
-        <v>16.758749999999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>214</v>
-      </c>
-      <c r="B96">
-        <v>16.758749999999999</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>215</v>
-      </c>
-      <c r="B97">
-        <v>13.036809815950916</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>216</v>
-      </c>
-      <c r="B98">
-        <v>16.462585034013607</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="68" t="s">
-        <v>219</v>
-      </c>
-      <c r="C99">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>75</v>
-      </c>
-      <c r="C100">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>